<commit_message>
i373--TMP reusable feature added
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_example/standard_suite/diamond_regression.xlsx
+++ b/tmp_client/doc/TMP_example/standard_suite/diamond_regression.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\repository\tmp_client\doc\TMP_example\standard_suite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="40MRd5r6vR/eXVUGbL7aEMM1NO6mwC4SojgFQmqHtZOqnQZBLsdr03u6GYWM/ftoMUNBO+KP7cdpMmOVZ0x4WQ==" workbookSaltValue="I+dbibQaVxj+tsXuP7uNKg==" workbookSpinCount="100000" lockStructure="1"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="sXipEUe4ofmbJ/VNsEp+rzubWcfs6D2Dd011fah7XjWPwWDEMNPI+WgbTdHC9ocktcX0RezfEDwP38HjohLwAA==" workbookSaltValue="V2+JL2w8HFZBCHZgrfWRgg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13740"/>
   </bookViews>
@@ -19,22 +19,22 @@
     <sheet name="comments" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">case!$A$2:$AE$46</definedName>
-    <definedName name="Z_16B2C8B3_13FA_43FB_96C1_3763C72619A6_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AE$2</definedName>
-    <definedName name="Z_179F0E1F_F6F7_410E_B883_54B8A90BA550_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AE$2</definedName>
-    <definedName name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AE$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">case!$A$2:$AF$46</definedName>
+    <definedName name="Z_16B2C8B3_13FA_43FB_96C1_3763C72619A6_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AF$2</definedName>
+    <definedName name="Z_179F0E1F_F6F7_410E_B883_54B8A90BA550_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AF$2</definedName>
+    <definedName name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AF$46</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
   <customWorkbookViews>
-    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="3"/>
+    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="3" showComments="commIndAndComment"/>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
     <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="344">
   <si>
     <t>[suite_info]</t>
   </si>
@@ -709,9 +709,6 @@
   </si>
   <si>
     <t>general_group</t>
-  </si>
-  <si>
-    <t>Preference/ClientPreference(Note.3)</t>
   </si>
   <si>
     <t>case_mode</t>
@@ -755,9 +752,6 @@
   <si>
     <t>2. The following environment variables will be ignored due to Core Script processing method:
 LM_LICENSE_FILE,TW_PAP_VERBOSE,LSC_RECORD_CPUMEM,SEDISABLE,LSC_REPORT_MEMORY,DISABLE_TMCHECK</t>
-  </si>
-  <si>
-    <t>3. Preference/ClientPreference only for TMP client runtime use, 'ClientPreference' will be deprecated later</t>
   </si>
   <si>
     <t>Table 3</t>
@@ -1069,6 +1063,15 @@
   </si>
   <si>
     <t>Machine account support</t>
+  </si>
+  <si>
+    <t>Reusable</t>
+  </si>
+  <si>
+    <t>3. Preference only for TMP client runtime use</t>
+  </si>
+  <si>
+    <t>Reusable column added</t>
   </si>
 </sst>
 </file>
@@ -1642,7 +1645,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5">
       <alignment vertical="center"/>
@@ -1897,6 +1900,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="33" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1909,109 +1915,115 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -3327,6 +3339,36 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>	Smoke: test case need to be smoke or not in final cycle, see table1 for available value. shown on page</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	Reusable:test case can be reusable or not for derivative device, see table1 for available value. shown on page</a:t>
           </a:r>
           <a:endParaRPr lang="zh-CN" altLang="zh-CN">
             <a:effectLst/>
@@ -4311,13 +4353,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>192</xdr:row>
+      <xdr:row>193</xdr:row>
       <xdr:rowOff>140970</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>904875</xdr:colOff>
-      <xdr:row>200</xdr:row>
+      <xdr:row>201</xdr:row>
       <xdr:rowOff>102870</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4524,8 +4566,8 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{0FB28824-15BE-430D-BD95-CDA8C60DAB9A}">
-  <header guid="{0FB28824-15BE-430D-BD95-CDA8C60DAB9A}" dateTime="2021-06-10T14:59:24" maxSheetId="5" userName="Jason Wang" r:id="rId1">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{A5694B8A-CCC3-4ACD-8EF2-0CB46AEC2CBD}">
+  <header guid="{A5694B8A-CCC3-4ACD-8EF2-0CB46AEC2CBD}" dateTime="2021-10-18T15:36:01" maxSheetId="5" userName="Jason Wang" r:id="rId1">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -4834,9 +4876,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -4850,7 +4890,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="59" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4858,7 +4898,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4874,12 +4914,12 @@
         <v>4</v>
       </c>
       <c r="B4" s="59" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="B5" s="59" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4900,7 +4940,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="59" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4926,13 +4966,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="B4" sqref="B4"/>
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+      <selection activeCell="B35" sqref="B35"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
-      <selection activeCell="B35" sqref="B35"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="B4" sqref="B4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -4945,13 +4985,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:AE46"/>
+  <dimension ref="A1:AF46"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="T3" sqref="T3"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4968,59 +5008,61 @@
     <col min="10" max="10" width="9.85546875" style="59" customWidth="1"/>
     <col min="11" max="11" width="12" style="59" customWidth="1"/>
     <col min="12" max="12" width="9.5703125" style="60" customWidth="1"/>
-    <col min="13" max="13" width="38" style="59" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" style="59" customWidth="1"/>
-    <col min="15" max="15" width="30.28515625" style="59" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" style="59" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" style="59" customWidth="1"/>
-    <col min="18" max="18" width="13" style="59" customWidth="1"/>
-    <col min="19" max="20" width="9.7109375" style="59" customWidth="1"/>
-    <col min="21" max="21" width="9.42578125" style="59" customWidth="1"/>
-    <col min="22" max="22" width="11" style="59" customWidth="1"/>
-    <col min="23" max="23" width="11.7109375" style="59" customWidth="1"/>
-    <col min="24" max="29" width="9" style="59"/>
-    <col min="30" max="30" width="10.140625" style="59" customWidth="1"/>
-    <col min="31" max="16384" width="9" style="59"/>
+    <col min="13" max="13" width="11.140625" style="60" customWidth="1"/>
+    <col min="14" max="14" width="38" style="59" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" style="59" customWidth="1"/>
+    <col min="16" max="16" width="30.28515625" style="59" customWidth="1"/>
+    <col min="17" max="17" width="17.28515625" style="59" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" style="59" customWidth="1"/>
+    <col min="19" max="19" width="13" style="59" customWidth="1"/>
+    <col min="20" max="21" width="9.7109375" style="59" customWidth="1"/>
+    <col min="22" max="22" width="9.42578125" style="59" customWidth="1"/>
+    <col min="23" max="23" width="11" style="59" customWidth="1"/>
+    <col min="24" max="24" width="11.7109375" style="59" customWidth="1"/>
+    <col min="25" max="30" width="9" style="59"/>
+    <col min="31" max="31" width="10.140625" style="59" customWidth="1"/>
+    <col min="32" max="16384" width="9" style="59"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="58" customFormat="1">
-      <c r="A1" s="86" t="s">
+    <row r="1" spans="1:32" s="58" customFormat="1">
+      <c r="A1" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="87"/>
-      <c r="S1" s="87"/>
-      <c r="T1" s="87"/>
-      <c r="U1" s="87"/>
-      <c r="V1" s="87"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="88"/>
+      <c r="J1" s="88"/>
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
+      <c r="M1" s="88"/>
+      <c r="N1" s="88"/>
+      <c r="O1" s="88"/>
+      <c r="P1" s="88"/>
+      <c r="Q1" s="88"/>
+      <c r="R1" s="88"/>
+      <c r="S1" s="88"/>
+      <c r="T1" s="88"/>
+      <c r="U1" s="88"/>
+      <c r="V1" s="88"/>
       <c r="W1" s="88"/>
-      <c r="X1" s="89" t="s">
+      <c r="X1" s="89"/>
+      <c r="Y1" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="Y1" s="89"/>
-      <c r="Z1" s="89"/>
-      <c r="AA1" s="89"/>
-      <c r="AB1" s="89"/>
-      <c r="AC1" s="89"/>
-      <c r="AD1" s="89"/>
-      <c r="AE1" s="89"/>
-    </row>
-    <row r="2" spans="1:31" s="58" customFormat="1">
+      <c r="Z1" s="90"/>
+      <c r="AA1" s="90"/>
+      <c r="AB1" s="90"/>
+      <c r="AC1" s="90"/>
+      <c r="AD1" s="90"/>
+      <c r="AE1" s="90"/>
+      <c r="AF1" s="90"/>
+    </row>
+    <row r="2" spans="1:32" s="58" customFormat="1">
       <c r="A2" s="61" t="s">
         <v>14</v>
       </c>
@@ -5057,65 +5099,68 @@
       <c r="L2" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="61" t="s">
+      <c r="M2" s="62" t="s">
+        <v>341</v>
+      </c>
+      <c r="N2" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="61" t="s">
+      <c r="O2" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="61" t="s">
+      <c r="P2" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="61" t="s">
+      <c r="Q2" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="61" t="s">
+      <c r="R2" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="61" t="s">
+      <c r="S2" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="S2" s="61" t="s">
+      <c r="T2" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="61" t="s">
-        <v>322</v>
-      </c>
       <c r="U2" s="61" t="s">
+        <v>320</v>
+      </c>
+      <c r="V2" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="V2" s="61" t="s">
+      <c r="W2" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="W2" s="61" t="s">
+      <c r="X2" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="X2" s="61" t="s">
+      <c r="Y2" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="Y2" s="61" t="s">
+      <c r="Z2" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="Z2" s="61" t="s">
+      <c r="AA2" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="AA2" s="61" t="s">
+      <c r="AB2" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="AB2" s="61" t="s">
+      <c r="AC2" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="AC2" s="61" t="s">
+      <c r="AD2" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="AD2" s="61" t="s">
+      <c r="AE2" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="AE2" s="61" t="s">
+      <c r="AF2" s="61" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:32">
       <c r="A3" s="59">
         <v>1</v>
       </c>
@@ -5143,17 +5188,17 @@
       <c r="J3" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O3" s="59" t="s">
+      <c r="P3" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="P3" s="59" t="s">
+      <c r="Q3" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="S3" s="59" t="s">
+      <c r="T3" s="59" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:31">
+    <row r="4" spans="1:32">
       <c r="A4" s="59">
         <v>2</v>
       </c>
@@ -5181,11 +5226,11 @@
       <c r="J4" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O4" s="59" t="s">
+      <c r="P4" s="59" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:31">
+    <row r="5" spans="1:32">
       <c r="A5" s="59">
         <v>3</v>
       </c>
@@ -5213,11 +5258,11 @@
       <c r="J5" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O5" s="59" t="s">
+      <c r="P5" s="59" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:32">
       <c r="A6" s="59">
         <v>4</v>
       </c>
@@ -5246,7 +5291,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:32">
       <c r="A7" s="59">
         <v>5</v>
       </c>
@@ -5275,7 +5320,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:32">
       <c r="A8" s="59">
         <v>6</v>
       </c>
@@ -5304,7 +5349,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:32">
       <c r="A9" s="59">
         <v>7</v>
       </c>
@@ -5333,7 +5378,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:31">
+    <row r="10" spans="1:32">
       <c r="A10" s="59">
         <v>8</v>
       </c>
@@ -5361,11 +5406,11 @@
       <c r="J10" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O10" s="59" t="s">
+      <c r="P10" s="59" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:32">
       <c r="A11" s="59">
         <v>9</v>
       </c>
@@ -5394,7 +5439,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:32">
       <c r="A12" s="59">
         <v>10</v>
       </c>
@@ -5423,7 +5468,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:31">
+    <row r="13" spans="1:32">
       <c r="A13" s="59">
         <v>11</v>
       </c>
@@ -5452,7 +5497,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:31">
+    <row r="14" spans="1:32">
       <c r="A14" s="59">
         <v>12</v>
       </c>
@@ -5481,7 +5526,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:31">
+    <row r="15" spans="1:32">
       <c r="A15" s="59">
         <v>13</v>
       </c>
@@ -5509,11 +5554,11 @@
       <c r="J15" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O15" s="59" t="s">
+      <c r="P15" s="59" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:31">
+    <row r="16" spans="1:32">
       <c r="A16" s="59">
         <v>14</v>
       </c>
@@ -5541,11 +5586,11 @@
       <c r="J16" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O16" s="59" t="s">
+      <c r="P16" s="59" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:18">
       <c r="A17" s="59">
         <v>15</v>
       </c>
@@ -5573,11 +5618,11 @@
       <c r="J17" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O17" s="59" t="s">
+      <c r="P17" s="59" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:18">
       <c r="A18" s="59">
         <v>16</v>
       </c>
@@ -5606,7 +5651,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:18">
       <c r="A19" s="59">
         <v>17</v>
       </c>
@@ -5634,11 +5679,11 @@
       <c r="J19" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O19" s="59" t="s">
+      <c r="P19" s="59" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:18">
       <c r="A20" s="59">
         <v>18</v>
       </c>
@@ -5667,7 +5712,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:18">
       <c r="A21" s="59">
         <v>19</v>
       </c>
@@ -5695,14 +5740,14 @@
       <c r="J21" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O21" s="59" t="s">
+      <c r="P21" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="Q21" s="59" t="s">
+      <c r="R21" s="59" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:18">
       <c r="A22" s="59">
         <v>20</v>
       </c>
@@ -5730,14 +5775,14 @@
       <c r="J22" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O22" s="59" t="s">
+      <c r="P22" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="P22" s="59" t="s">
+      <c r="Q22" s="59" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:18">
       <c r="A23" s="59">
         <v>21</v>
       </c>
@@ -5765,14 +5810,14 @@
       <c r="J23" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O23" s="59" t="s">
+      <c r="P23" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="P23" s="59" t="s">
+      <c r="Q23" s="59" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:18">
       <c r="A24" s="59">
         <v>22</v>
       </c>
@@ -5800,14 +5845,14 @@
       <c r="J24" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O24" s="59" t="s">
+      <c r="P24" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="P24" s="59" t="s">
+      <c r="Q24" s="59" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:18">
       <c r="A25" s="59">
         <v>23</v>
       </c>
@@ -5835,14 +5880,14 @@
       <c r="J25" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O25" s="59" t="s">
+      <c r="P25" s="59" t="s">
         <v>90</v>
       </c>
-      <c r="P25" s="59" t="s">
+      <c r="Q25" s="59" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:18">
       <c r="A26" s="59">
         <v>24</v>
       </c>
@@ -5870,14 +5915,14 @@
       <c r="J26" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O26" s="59" t="s">
+      <c r="P26" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="Q26" s="59" t="s">
+      <c r="R26" s="59" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:18">
       <c r="A27" s="59">
         <v>25</v>
       </c>
@@ -5905,14 +5950,14 @@
       <c r="J27" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O27" s="59" t="s">
+      <c r="P27" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="P27" s="59" t="s">
+      <c r="Q27" s="59" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:18">
       <c r="A28" s="59">
         <v>26</v>
       </c>
@@ -5940,14 +5985,14 @@
       <c r="J28" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O28" s="59" t="s">
+      <c r="P28" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="P28" s="59" t="s">
+      <c r="Q28" s="59" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:18">
       <c r="A29" s="59">
         <v>27</v>
       </c>
@@ -5975,14 +6020,14 @@
       <c r="J29" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O29" s="59" t="s">
+      <c r="P29" s="59" t="s">
         <v>90</v>
       </c>
-      <c r="P29" s="59" t="s">
+      <c r="Q29" s="59" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:18">
       <c r="A30" s="59">
         <v>28</v>
       </c>
@@ -6010,14 +6055,14 @@
       <c r="J30" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O30" s="59" t="s">
+      <c r="P30" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="Q30" s="59" t="s">
+      <c r="R30" s="59" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:18">
       <c r="A31" s="59">
         <v>29</v>
       </c>
@@ -6045,14 +6090,14 @@
       <c r="J31" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O31" s="59" t="s">
+      <c r="P31" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="P31" s="59" t="s">
+      <c r="Q31" s="59" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:18">
       <c r="A32" s="59">
         <v>30</v>
       </c>
@@ -6080,14 +6125,14 @@
       <c r="J32" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O32" s="59" t="s">
+      <c r="P32" s="59" t="s">
         <v>100</v>
       </c>
-      <c r="P32" s="59" t="s">
+      <c r="Q32" s="59" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:16">
       <c r="A33" s="59">
         <v>31</v>
       </c>
@@ -6115,11 +6160,11 @@
       <c r="J33" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O33" s="59" t="s">
+      <c r="P33" s="59" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:16">
       <c r="A34" s="59">
         <v>32</v>
       </c>
@@ -6147,11 +6192,11 @@
       <c r="J34" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O34" s="59" t="s">
+      <c r="P34" s="59" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:16">
       <c r="A35" s="59">
         <v>33</v>
       </c>
@@ -6179,11 +6224,11 @@
       <c r="J35" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O35" s="59" t="s">
+      <c r="P35" s="59" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:16">
       <c r="A36" s="59">
         <v>34</v>
       </c>
@@ -6211,11 +6256,11 @@
       <c r="J36" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O36" s="59" t="s">
+      <c r="P36" s="59" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:16">
       <c r="A37" s="59">
         <v>35</v>
       </c>
@@ -6243,11 +6288,11 @@
       <c r="J37" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O37" s="59" t="s">
+      <c r="P37" s="59" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:16">
       <c r="A38" s="59">
         <v>36</v>
       </c>
@@ -6275,11 +6320,11 @@
       <c r="J38" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O38" s="59" t="s">
+      <c r="P38" s="59" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:16">
       <c r="A39" s="59">
         <v>37</v>
       </c>
@@ -6307,11 +6352,11 @@
       <c r="J39" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O39" s="59" t="s">
+      <c r="P39" s="59" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:16">
       <c r="A40" s="59">
         <v>38</v>
       </c>
@@ -6339,11 +6384,11 @@
       <c r="J40" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O40" s="59" t="s">
+      <c r="P40" s="59" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:16">
       <c r="A41" s="59">
         <v>39</v>
       </c>
@@ -6371,11 +6416,11 @@
       <c r="J41" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O41" s="59" t="s">
+      <c r="P41" s="59" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:16">
       <c r="A42" s="59">
         <v>40</v>
       </c>
@@ -6403,11 +6448,11 @@
       <c r="J42" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O42" s="59" t="s">
+      <c r="P42" s="59" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:16">
       <c r="A43" s="59">
         <v>41</v>
       </c>
@@ -6435,11 +6480,11 @@
       <c r="J43" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O43" s="59" t="s">
+      <c r="P43" s="59" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:16">
       <c r="A44" s="59">
         <v>42</v>
       </c>
@@ -6468,7 +6513,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:16">
       <c r="A45" s="59">
         <v>43</v>
       </c>
@@ -6496,11 +6541,11 @@
       <c r="J45" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O45" s="59" t="s">
+      <c r="P45" s="59" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:16">
       <c r="A46" s="59">
         <v>44</v>
       </c>
@@ -6528,20 +6573,27 @@
       <c r="J46" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O46" s="59" t="s">
+      <c r="P46" s="59" t="s">
         <v>132</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="w3hzLRIZQs2OCo+gOq6y+7pYsPrB2OQJ9K8otGIWyN2fO4ZszAE4hICBModvrzYm14kQD00caij1zHZ8JrwNZw==" saltValue="e2kEBt19h9WsbWZKJxfJPw==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <autoFilter ref="A2:AE46"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Sju3pjEnjegba3BrZLImZ+xscQ9MLEq+i8mDO7rXFn4S3yXv8zWb4HaF0uC2YruSs8wkV8FCIxY7a0fvnwVXFw==" saltValue="mZmUchosJ60PlKqUXOSzGQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <autoFilter ref="A2:AF46"/>
   <customSheetViews>
     <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="T3" sqref="T3"/>
+      <selection pane="bottomRight" activeCell="N7" sqref="N7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
-      <autoFilter ref="A2:AE46"/>
+      <autoFilter ref="A2:AF46"/>
+    </customSheetView>
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen"/>
+      <selection activeCell="C23" sqref="C23"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait"/>
+      <autoFilter ref="A2:Y2"/>
     </customSheetView>
     <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen"/>
@@ -6550,23 +6602,16 @@
       <pageSetup paperSize="9" orientation="portrait"/>
       <autoFilter ref="A2:Y2"/>
     </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen"/>
-      <selection activeCell="C23" sqref="C23"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait"/>
-      <autoFilter ref="A2:Y2"/>
-    </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
-    <mergeCell ref="A1:W1"/>
-    <mergeCell ref="X1:AE1"/>
+    <mergeCell ref="A1:X1"/>
+    <mergeCell ref="Y1:AF1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:I1 M1:W1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:I1 N1:X1">
       <formula1>$F$119:$J$119</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X1:AB1 AE1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y1:AC1 AF1">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -6574,7 +6619,7 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>description!$F$122:$H$122</xm:f>
@@ -6601,9 +6646,9 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>description!$F$141:$H$141</xm:f>
+            <xm:f>description!$F$142:$H$142</xm:f>
           </x14:formula1>
-          <xm:sqref>AC1:AC1048576</xm:sqref>
+          <xm:sqref>AD1:AD1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -6619,9 +6664,15 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>description!$F$142:$H$142</xm:f>
+            <xm:f>description!$F$143:$H$143</xm:f>
           </x14:formula1>
-          <xm:sqref>AD1:AD1048576</xm:sqref>
+          <xm:sqref>AE1:AE1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>description!$F$124:$H$124</xm:f>
+          </x14:formula1>
+          <xm:sqref>M1:M1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6632,11 +6683,9 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:N249"/>
+  <dimension ref="A1:N251"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -6658,7 +6707,7 @@
         <v>133</v>
       </c>
       <c r="B1" s="2">
-        <v>1.2</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -6666,7 +6715,7 @@
         <v>29</v>
       </c>
       <c r="B2" s="3">
-        <v>44357</v>
+        <v>44487</v>
       </c>
     </row>
     <row r="107" spans="1:14" ht="12.75" customHeight="1"/>
@@ -6696,17 +6745,17 @@
       <c r="E111" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="F111" s="121" t="s">
+      <c r="F111" s="91" t="s">
         <v>140</v>
       </c>
-      <c r="G111" s="122"/>
-      <c r="H111" s="122"/>
-      <c r="I111" s="122"/>
-      <c r="J111" s="122"/>
-      <c r="K111" s="122"/>
-      <c r="L111" s="122"/>
-      <c r="M111" s="122"/>
-      <c r="N111" s="123"/>
+      <c r="G111" s="92"/>
+      <c r="H111" s="92"/>
+      <c r="I111" s="92"/>
+      <c r="J111" s="92"/>
+      <c r="K111" s="92"/>
+      <c r="L111" s="92"/>
+      <c r="M111" s="92"/>
+      <c r="N111" s="93"/>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="6" t="s">
@@ -7048,10 +7097,10 @@
     </row>
     <row r="124" spans="1:14">
       <c r="A124" s="8" t="s">
-        <v>4</v>
+        <v>341</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C124" s="9" t="s">
         <v>142</v>
@@ -7059,11 +7108,15 @@
       <c r="D124" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="E124" s="9"/>
+      <c r="E124" s="9" t="s">
+        <v>129</v>
+      </c>
       <c r="F124" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="G124" s="9"/>
+        <v>129</v>
+      </c>
+      <c r="G124" s="9" t="s">
+        <v>142</v>
+      </c>
       <c r="H124" s="9"/>
       <c r="I124" s="9"/>
       <c r="J124" s="9"/>
@@ -7074,7 +7127,7 @@
     </row>
     <row r="125" spans="1:14">
       <c r="A125" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B125" s="9" t="s">
         <v>146</v>
@@ -7100,7 +7153,7 @@
     </row>
     <row r="126" spans="1:14">
       <c r="A126" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B126" s="9" t="s">
         <v>146</v>
@@ -7126,7 +7179,7 @@
     </row>
     <row r="127" spans="1:14">
       <c r="A127" s="8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B127" s="9" t="s">
         <v>146</v>
@@ -7152,7 +7205,7 @@
     </row>
     <row r="128" spans="1:14">
       <c r="A128" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B128" s="9" t="s">
         <v>146</v>
@@ -7178,7 +7231,7 @@
     </row>
     <row r="129" spans="1:14">
       <c r="A129" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B129" s="9" t="s">
         <v>146</v>
@@ -7204,7 +7257,7 @@
     </row>
     <row r="130" spans="1:14">
       <c r="A130" s="8" t="s">
-        <v>156</v>
+        <v>10</v>
       </c>
       <c r="B130" s="9" t="s">
         <v>146</v>
@@ -7230,19 +7283,21 @@
     </row>
     <row r="131" spans="1:14">
       <c r="A131" s="8" t="s">
-        <v>26</v>
+        <v>156</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C131" s="9" t="s">
         <v>142</v>
       </c>
       <c r="D131" s="9" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="E131" s="9"/>
-      <c r="F131" s="9"/>
+      <c r="F131" s="9" t="s">
+        <v>155</v>
+      </c>
       <c r="G131" s="9"/>
       <c r="H131" s="9"/>
       <c r="I131" s="9"/>
@@ -7253,8 +7308,8 @@
       <c r="N131" s="11"/>
     </row>
     <row r="132" spans="1:14">
-      <c r="A132" s="76" t="s">
-        <v>322</v>
+      <c r="A132" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="B132" s="9" t="s">
         <v>143</v>
@@ -7263,11 +7318,9 @@
         <v>142</v>
       </c>
       <c r="D132" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E132" s="77" t="s">
-        <v>323</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="E132" s="9"/>
       <c r="F132" s="9"/>
       <c r="G132" s="9"/>
       <c r="H132" s="9"/>
@@ -7279,8 +7332,8 @@
       <c r="N132" s="11"/>
     </row>
     <row r="133" spans="1:14">
-      <c r="A133" s="8" t="s">
-        <v>27</v>
+      <c r="A133" s="76" t="s">
+        <v>320</v>
       </c>
       <c r="B133" s="9" t="s">
         <v>143</v>
@@ -7291,7 +7344,9 @@
       <c r="D133" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="E133" s="9"/>
+      <c r="E133" s="77" t="s">
+        <v>321</v>
+      </c>
       <c r="F133" s="9"/>
       <c r="G133" s="9"/>
       <c r="H133" s="9"/>
@@ -7304,7 +7359,7 @@
     </row>
     <row r="134" spans="1:14">
       <c r="A134" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B134" s="9" t="s">
         <v>143</v>
@@ -7313,7 +7368,7 @@
         <v>142</v>
       </c>
       <c r="D134" s="9" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="E134" s="9"/>
       <c r="F134" s="9"/>
@@ -7328,7 +7383,7 @@
     </row>
     <row r="135" spans="1:14">
       <c r="A135" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B135" s="9" t="s">
         <v>143</v>
@@ -7352,7 +7407,7 @@
     </row>
     <row r="136" spans="1:14">
       <c r="A136" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B136" s="9" t="s">
         <v>143</v>
@@ -7361,7 +7416,7 @@
         <v>142</v>
       </c>
       <c r="D136" s="9" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="E136" s="9"/>
       <c r="F136" s="9"/>
@@ -7376,10 +7431,10 @@
     </row>
     <row r="137" spans="1:14">
       <c r="A137" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="C137" s="9" t="s">
         <v>142</v>
@@ -7400,7 +7455,7 @@
     </row>
     <row r="138" spans="1:14">
       <c r="A138" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B138" s="9" t="s">
         <v>157</v>
@@ -7424,7 +7479,7 @@
     </row>
     <row r="139" spans="1:14">
       <c r="A139" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B139" s="9" t="s">
         <v>157</v>
@@ -7448,7 +7503,7 @@
     </row>
     <row r="140" spans="1:14">
       <c r="A140" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B140" s="9" t="s">
         <v>157</v>
@@ -7472,10 +7527,10 @@
     </row>
     <row r="141" spans="1:14">
       <c r="A141" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="C141" s="9" t="s">
         <v>142</v>
@@ -7483,18 +7538,10 @@
       <c r="D141" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="E141" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="F141" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="G141" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="H141" s="9" t="s">
-        <v>158</v>
-      </c>
+      <c r="E141" s="9"/>
+      <c r="F141" s="9"/>
+      <c r="G141" s="9"/>
+      <c r="H141" s="9"/>
       <c r="I141" s="9"/>
       <c r="J141" s="9"/>
       <c r="K141" s="9"/>
@@ -7503,128 +7550,136 @@
       <c r="N141" s="11"/>
     </row>
     <row r="142" spans="1:14">
-      <c r="A142" s="12" t="s">
+      <c r="A142" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B142" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C142" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D142" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E142" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="F142" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G142" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="H142" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="I142" s="9"/>
+      <c r="J142" s="9"/>
+      <c r="K142" s="9"/>
+      <c r="L142" s="9"/>
+      <c r="M142" s="9"/>
+      <c r="N142" s="11"/>
+    </row>
+    <row r="143" spans="1:14">
+      <c r="A143" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B142" s="13" t="s">
+      <c r="B143" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="C142" s="13" t="s">
+      <c r="C143" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="D142" s="13" t="s">
+      <c r="D143" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="E142" s="13" t="s">
+      <c r="E143" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="F142" s="13" t="s">
+      <c r="F143" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="G142" s="13" t="s">
+      <c r="G143" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="H142" s="13" t="s">
+      <c r="H143" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="I142" s="13"/>
-      <c r="J142" s="13"/>
-      <c r="K142" s="13"/>
-      <c r="L142" s="13"/>
-      <c r="M142" s="13"/>
-      <c r="N142" s="23"/>
-    </row>
-    <row r="143" spans="1:14">
-      <c r="A143" s="14" t="s">
+      <c r="I143" s="13"/>
+      <c r="J143" s="13"/>
+      <c r="K143" s="13"/>
+      <c r="L143" s="13"/>
+      <c r="M143" s="13"/>
+      <c r="N143" s="23"/>
+    </row>
+    <row r="144" spans="1:14">
+      <c r="A144" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B143" s="15" t="s">
+      <c r="B144" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="C143" s="15" t="s">
+      <c r="C144" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="D143" s="15" t="s">
+      <c r="D144" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="E143" s="15"/>
-      <c r="F143" s="15"/>
-      <c r="G143" s="15"/>
-      <c r="H143" s="15"/>
-      <c r="I143" s="15"/>
-      <c r="J143" s="15"/>
-      <c r="K143" s="15"/>
-      <c r="L143" s="15"/>
-      <c r="M143" s="15"/>
-      <c r="N143" s="28"/>
-    </row>
-    <row r="146" spans="1:8">
-      <c r="A146" s="1" t="s">
+      <c r="E144" s="15"/>
+      <c r="F144" s="15"/>
+      <c r="G144" s="15"/>
+      <c r="H144" s="15"/>
+      <c r="I144" s="15"/>
+      <c r="J144" s="15"/>
+      <c r="K144" s="15"/>
+      <c r="L144" s="15"/>
+      <c r="M144" s="15"/>
+      <c r="N144" s="28"/>
+    </row>
+    <row r="147" spans="1:8">
+      <c r="A147" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B146" s="1" t="s">
+      <c r="B147" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="147" spans="1:8">
-      <c r="A147" s="16" t="s">
+    <row r="148" spans="1:8">
+      <c r="A148" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="B147" s="17" t="s">
+      <c r="B148" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C147" s="17" t="s">
+      <c r="C148" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="D147" s="17" t="s">
+      <c r="D148" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="E147" s="17" t="s">
+      <c r="E148" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="F147" s="17" t="s">
+      <c r="F148" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="G147" s="17" t="s">
+      <c r="G148" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="H147" s="18" t="s">
+      <c r="H148" s="18" t="s">
         <v>167</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8">
-      <c r="A148" s="19">
-        <v>1</v>
-      </c>
-      <c r="B148" s="90" t="s">
-        <v>4</v>
-      </c>
-      <c r="C148" s="63" t="s">
-        <v>168</v>
-      </c>
-      <c r="D148" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E148" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F148" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="G148" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="H148" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="149" spans="1:8">
       <c r="A149" s="19">
-        <v>2</v>
-      </c>
-      <c r="B149" s="91"/>
-      <c r="C149" s="21" t="s">
-        <v>173</v>
+        <v>1</v>
+      </c>
+      <c r="B149" s="122" t="s">
+        <v>4</v>
+      </c>
+      <c r="C149" s="63" t="s">
+        <v>168</v>
       </c>
       <c r="D149" s="21" t="s">
         <v>169</v>
@@ -7633,27 +7688,31 @@
         <v>169</v>
       </c>
       <c r="F149" s="21" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="G149" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="H149" s="11"/>
+      <c r="H149" s="1" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="150" spans="1:8">
       <c r="A150" s="19">
-        <v>3</v>
-      </c>
-      <c r="B150" s="91"/>
+        <v>2</v>
+      </c>
+      <c r="B150" s="123"/>
       <c r="C150" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D150" s="21"/>
+        <v>173</v>
+      </c>
+      <c r="D150" s="21" t="s">
+        <v>169</v>
+      </c>
       <c r="E150" s="21" t="s">
         <v>169</v>
       </c>
       <c r="F150" s="21" t="s">
-        <v>310</v>
+        <v>174</v>
       </c>
       <c r="G150" s="21" t="s">
         <v>171</v>
@@ -7662,35 +7721,31 @@
     </row>
     <row r="151" spans="1:8">
       <c r="A151" s="19">
-        <v>4</v>
-      </c>
-      <c r="B151" s="91"/>
+        <v>3</v>
+      </c>
+      <c r="B151" s="123"/>
       <c r="C151" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="D151" s="21" t="s">
-        <v>169</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D151" s="21"/>
       <c r="E151" s="21" t="s">
         <v>169</v>
       </c>
       <c r="F151" s="21" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="G151" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="H151" s="11" t="s">
-        <v>176</v>
-      </c>
+      <c r="H151" s="11"/>
     </row>
     <row r="152" spans="1:8">
       <c r="A152" s="19">
-        <v>5</v>
-      </c>
-      <c r="B152" s="91"/>
-      <c r="C152" s="63" t="s">
-        <v>177</v>
+        <v>4</v>
+      </c>
+      <c r="B152" s="123"/>
+      <c r="C152" s="21" t="s">
+        <v>175</v>
       </c>
       <c r="D152" s="21" t="s">
         <v>169</v>
@@ -7699,22 +7754,22 @@
         <v>169</v>
       </c>
       <c r="F152" s="21" t="s">
-        <v>178</v>
+        <v>309</v>
       </c>
       <c r="G152" s="21" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="H152" s="11" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="153" spans="1:8">
       <c r="A153" s="19">
-        <v>6</v>
-      </c>
-      <c r="B153" s="91"/>
+        <v>5</v>
+      </c>
+      <c r="B153" s="123"/>
       <c r="C153" s="63" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D153" s="21" t="s">
         <v>169</v>
@@ -7723,10 +7778,10 @@
         <v>169</v>
       </c>
       <c r="F153" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="G153" s="71" t="s">
-        <v>309</v>
+        <v>178</v>
+      </c>
+      <c r="G153" s="21" t="s">
+        <v>179</v>
       </c>
       <c r="H153" s="11" t="s">
         <v>180</v>
@@ -7734,11 +7789,11 @@
     </row>
     <row r="154" spans="1:8">
       <c r="A154" s="19">
-        <v>7</v>
-      </c>
-      <c r="B154" s="91"/>
-      <c r="C154" s="21" t="s">
-        <v>183</v>
+        <v>6</v>
+      </c>
+      <c r="B154" s="123"/>
+      <c r="C154" s="63" t="s">
+        <v>181</v>
       </c>
       <c r="D154" s="21" t="s">
         <v>169</v>
@@ -7747,20 +7802,22 @@
         <v>169</v>
       </c>
       <c r="F154" s="21" t="s">
-        <v>312</v>
-      </c>
-      <c r="G154" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="H154" s="11"/>
+        <v>182</v>
+      </c>
+      <c r="G154" s="71" t="s">
+        <v>307</v>
+      </c>
+      <c r="H154" s="11" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="155" spans="1:8">
       <c r="A155" s="19">
-        <v>8</v>
-      </c>
-      <c r="B155" s="91"/>
-      <c r="C155" s="63" t="s">
-        <v>184</v>
+        <v>7</v>
+      </c>
+      <c r="B155" s="123"/>
+      <c r="C155" s="21" t="s">
+        <v>183</v>
       </c>
       <c r="D155" s="21" t="s">
         <v>169</v>
@@ -7768,23 +7825,21 @@
       <c r="E155" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="F155" s="21">
-        <v>3071</v>
+      <c r="F155" s="21" t="s">
+        <v>310</v>
       </c>
       <c r="G155" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="H155" s="11" t="s">
-        <v>176</v>
-      </c>
+      <c r="H155" s="11"/>
     </row>
     <row r="156" spans="1:8">
       <c r="A156" s="19">
-        <v>9</v>
-      </c>
-      <c r="B156" s="91"/>
+        <v>8</v>
+      </c>
+      <c r="B156" s="123"/>
       <c r="C156" s="63" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D156" s="21" t="s">
         <v>169</v>
@@ -7792,23 +7847,23 @@
       <c r="E156" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="F156" s="21" t="s">
-        <v>178</v>
+      <c r="F156" s="21">
+        <v>3071</v>
       </c>
       <c r="G156" s="21" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="H156" s="11" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="157" spans="1:8">
       <c r="A157" s="19">
-        <v>10</v>
-      </c>
-      <c r="B157" s="91"/>
-      <c r="C157" s="21" t="s">
-        <v>186</v>
+        <v>9</v>
+      </c>
+      <c r="B157" s="123"/>
+      <c r="C157" s="63" t="s">
+        <v>185</v>
       </c>
       <c r="D157" s="21" t="s">
         <v>169</v>
@@ -7817,10 +7872,10 @@
         <v>169</v>
       </c>
       <c r="F157" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="G157" s="71" t="s">
-        <v>309</v>
+        <v>178</v>
+      </c>
+      <c r="G157" s="21" t="s">
+        <v>179</v>
       </c>
       <c r="H157" s="11" t="s">
         <v>180</v>
@@ -7828,11 +7883,11 @@
     </row>
     <row r="158" spans="1:8">
       <c r="A158" s="19">
-        <v>11</v>
-      </c>
-      <c r="B158" s="91"/>
+        <v>10</v>
+      </c>
+      <c r="B158" s="123"/>
       <c r="C158" s="21" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D158" s="21" t="s">
         <v>169</v>
@@ -7841,70 +7896,68 @@
         <v>169</v>
       </c>
       <c r="F158" s="21" t="s">
-        <v>313</v>
-      </c>
-      <c r="G158" s="21" t="s">
-        <v>171</v>
+        <v>182</v>
+      </c>
+      <c r="G158" s="71" t="s">
+        <v>307</v>
       </c>
       <c r="H158" s="11" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
     </row>
     <row r="159" spans="1:8">
       <c r="A159" s="19">
-        <v>12</v>
-      </c>
-      <c r="B159" s="91"/>
+        <v>11</v>
+      </c>
+      <c r="B159" s="123"/>
       <c r="C159" s="21" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D159" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="E159" s="21"/>
+      <c r="E159" s="21" t="s">
+        <v>169</v>
+      </c>
       <c r="F159" s="21" t="s">
-        <v>190</v>
+        <v>311</v>
       </c>
       <c r="G159" s="21" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="H159" s="11" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="160" spans="1:8">
       <c r="A160" s="19">
-        <v>13</v>
-      </c>
-      <c r="B160" s="98"/>
+        <v>12</v>
+      </c>
+      <c r="B160" s="123"/>
       <c r="C160" s="21" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D160" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="E160" s="21" t="s">
-        <v>169</v>
-      </c>
+      <c r="E160" s="21"/>
       <c r="F160" s="21" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="G160" s="21" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="H160" s="11" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="161" spans="1:8">
       <c r="A161" s="19">
-        <v>14</v>
-      </c>
-      <c r="B161" s="99" t="s">
-        <v>5</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B161" s="108"/>
       <c r="C161" s="21" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D161" s="21" t="s">
         <v>169</v>
@@ -7913,22 +7966,24 @@
         <v>169</v>
       </c>
       <c r="F161" s="21" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="G161" s="21" t="s">
-        <v>171</v>
+        <v>195</v>
       </c>
       <c r="H161" s="11" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="162" spans="1:8">
       <c r="A162" s="19">
-        <v>15</v>
-      </c>
-      <c r="B162" s="96"/>
+        <v>14</v>
+      </c>
+      <c r="B162" s="103" t="s">
+        <v>5</v>
+      </c>
       <c r="C162" s="21" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D162" s="21" t="s">
         <v>169</v>
@@ -7937,24 +7992,22 @@
         <v>169</v>
       </c>
       <c r="F162" s="21" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G162" s="21" t="s">
         <v>171</v>
       </c>
       <c r="H162" s="11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="163" spans="1:8">
-      <c r="A163" s="68">
-        <v>16</v>
-      </c>
-      <c r="B163" s="90" t="s">
-        <v>6</v>
-      </c>
+      <c r="A163" s="19">
+        <v>15</v>
+      </c>
+      <c r="B163" s="104"/>
       <c r="C163" s="21" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D163" s="21" t="s">
         <v>169</v>
@@ -7963,64 +8016,68 @@
         <v>169</v>
       </c>
       <c r="F163" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="G163" s="67" t="s">
+        <v>200</v>
+      </c>
+      <c r="G163" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="H163" s="11"/>
+      <c r="H163" s="11" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="164" spans="1:8">
       <c r="A164" s="68">
-        <v>17</v>
-      </c>
-      <c r="B164" s="100"/>
-      <c r="C164" s="67" t="s">
-        <v>307</v>
-      </c>
-      <c r="D164" s="66" t="s">
+        <v>16</v>
+      </c>
+      <c r="B164" s="122" t="s">
+        <v>6</v>
+      </c>
+      <c r="C164" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="D164" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="E164" s="66" t="s">
+      <c r="E164" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="F164" s="66"/>
+      <c r="F164" s="21" t="s">
+        <v>203</v>
+      </c>
       <c r="G164" s="67" t="s">
         <v>171</v>
       </c>
-      <c r="H164" s="70" t="s">
-        <v>308</v>
-      </c>
+      <c r="H164" s="11"/>
     </row>
     <row r="165" spans="1:8">
       <c r="A165" s="68">
-        <v>18</v>
-      </c>
-      <c r="B165" s="98"/>
-      <c r="C165" s="63" t="s">
-        <v>204</v>
-      </c>
-      <c r="D165" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B165" s="124"/>
+      <c r="C165" s="67" t="s">
+        <v>305</v>
+      </c>
+      <c r="D165" s="66" t="s">
         <v>169</v>
       </c>
-      <c r="E165" s="21" t="s">
+      <c r="E165" s="66" t="s">
         <v>169</v>
       </c>
-      <c r="F165" s="21"/>
-      <c r="G165" s="21" t="s">
-        <v>205</v>
-      </c>
-      <c r="H165" s="11"/>
+      <c r="F165" s="66"/>
+      <c r="G165" s="67" t="s">
+        <v>171</v>
+      </c>
+      <c r="H165" s="70" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="166" spans="1:8">
       <c r="A166" s="68">
-        <v>19</v>
-      </c>
-      <c r="B166" s="99" t="s">
-        <v>8</v>
-      </c>
-      <c r="C166" s="21" t="s">
-        <v>206</v>
+        <v>18</v>
+      </c>
+      <c r="B166" s="108"/>
+      <c r="C166" s="63" t="s">
+        <v>204</v>
       </c>
       <c r="D166" s="21" t="s">
         <v>169</v>
@@ -8028,21 +8085,21 @@
       <c r="E166" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="F166" s="21" t="s">
-        <v>207</v>
-      </c>
+      <c r="F166" s="21"/>
       <c r="G166" s="21" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H166" s="11"/>
     </row>
     <row r="167" spans="1:8">
       <c r="A167" s="68">
-        <v>20</v>
-      </c>
-      <c r="B167" s="96"/>
+        <v>19</v>
+      </c>
+      <c r="B167" s="103" t="s">
+        <v>8</v>
+      </c>
       <c r="C167" s="21" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D167" s="21" t="s">
         <v>169</v>
@@ -8050,7 +8107,9 @@
       <c r="E167" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="F167" s="21"/>
+      <c r="F167" s="21" t="s">
+        <v>207</v>
+      </c>
       <c r="G167" s="21" t="s">
         <v>208</v>
       </c>
@@ -8058,11 +8117,11 @@
     </row>
     <row r="168" spans="1:8">
       <c r="A168" s="68">
-        <v>21</v>
-      </c>
-      <c r="B168" s="96"/>
+        <v>20</v>
+      </c>
+      <c r="B168" s="104"/>
       <c r="C168" s="21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D168" s="21" t="s">
         <v>169</v>
@@ -8078,11 +8137,11 @@
     </row>
     <row r="169" spans="1:8">
       <c r="A169" s="68">
-        <v>22</v>
-      </c>
-      <c r="B169" s="96"/>
+        <v>21</v>
+      </c>
+      <c r="B169" s="104"/>
       <c r="C169" s="21" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D169" s="21" t="s">
         <v>169</v>
@@ -8098,11 +8157,11 @@
     </row>
     <row r="170" spans="1:8">
       <c r="A170" s="68">
-        <v>23</v>
-      </c>
-      <c r="B170" s="96"/>
+        <v>22</v>
+      </c>
+      <c r="B170" s="104"/>
       <c r="C170" s="21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D170" s="21" t="s">
         <v>169</v>
@@ -8118,11 +8177,11 @@
     </row>
     <row r="171" spans="1:8">
       <c r="A171" s="68">
-        <v>24</v>
-      </c>
-      <c r="B171" s="96"/>
+        <v>23</v>
+      </c>
+      <c r="B171" s="104"/>
       <c r="C171" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D171" s="21" t="s">
         <v>169</v>
@@ -8138,11 +8197,11 @@
     </row>
     <row r="172" spans="1:8">
       <c r="A172" s="68">
-        <v>25</v>
-      </c>
-      <c r="B172" s="96"/>
+        <v>24</v>
+      </c>
+      <c r="B172" s="104"/>
       <c r="C172" s="21" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D172" s="21" t="s">
         <v>169</v>
@@ -8157,12 +8216,12 @@
       <c r="H172" s="11"/>
     </row>
     <row r="173" spans="1:8">
-      <c r="A173" s="81">
-        <v>26</v>
-      </c>
-      <c r="B173" s="96"/>
+      <c r="A173" s="68">
+        <v>25</v>
+      </c>
+      <c r="B173" s="104"/>
       <c r="C173" s="21" t="s">
-        <v>47</v>
+        <v>214</v>
       </c>
       <c r="D173" s="21" t="s">
         <v>169</v>
@@ -8176,15 +8235,13 @@
       </c>
       <c r="H173" s="11"/>
     </row>
-    <row r="174" spans="1:8" ht="45">
+    <row r="174" spans="1:8">
       <c r="A174" s="81">
-        <v>27</v>
-      </c>
-      <c r="B174" s="99" t="s">
-        <v>9</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B174" s="104"/>
       <c r="C174" s="21" t="s">
-        <v>215</v>
+        <v>47</v>
       </c>
       <c r="D174" s="21" t="s">
         <v>169</v>
@@ -8192,21 +8249,21 @@
       <c r="E174" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="F174" s="69" t="s">
-        <v>331</v>
-      </c>
-      <c r="G174" s="85" t="s">
-        <v>336</v>
+      <c r="F174" s="21"/>
+      <c r="G174" s="21" t="s">
+        <v>208</v>
       </c>
       <c r="H174" s="11"/>
     </row>
-    <row r="175" spans="1:8">
+    <row r="175" spans="1:8" ht="45">
       <c r="A175" s="81">
-        <v>28</v>
-      </c>
-      <c r="B175" s="96"/>
-      <c r="C175" s="63" t="s">
-        <v>216</v>
+        <v>27</v>
+      </c>
+      <c r="B175" s="103" t="s">
+        <v>9</v>
+      </c>
+      <c r="C175" s="21" t="s">
+        <v>215</v>
       </c>
       <c r="D175" s="21" t="s">
         <v>169</v>
@@ -8214,43 +8271,43 @@
       <c r="E175" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="F175" s="63" t="s">
-        <v>217</v>
-      </c>
-      <c r="G175" s="63" t="s">
-        <v>218</v>
+      <c r="F175" s="69" t="s">
+        <v>329</v>
+      </c>
+      <c r="G175" s="85" t="s">
+        <v>334</v>
       </c>
       <c r="H175" s="11"/>
     </row>
     <row r="176" spans="1:8">
       <c r="A176" s="81">
-        <v>29</v>
-      </c>
-      <c r="B176" s="96"/>
-      <c r="C176" s="80" t="s">
-        <v>337</v>
-      </c>
-      <c r="D176" s="78" t="s">
+        <v>28</v>
+      </c>
+      <c r="B176" s="104"/>
+      <c r="C176" s="63" t="s">
+        <v>216</v>
+      </c>
+      <c r="D176" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="E176" s="78" t="s">
+      <c r="E176" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="F176" s="80" t="s">
+      <c r="F176" s="63" t="s">
         <v>217</v>
       </c>
-      <c r="G176" s="80" t="s">
-        <v>338</v>
+      <c r="G176" s="63" t="s">
+        <v>218</v>
       </c>
       <c r="H176" s="11"/>
     </row>
     <row r="177" spans="1:8">
       <c r="A177" s="81">
-        <v>30</v>
-      </c>
-      <c r="B177" s="96"/>
+        <v>29</v>
+      </c>
+      <c r="B177" s="104"/>
       <c r="C177" s="80" t="s">
-        <v>219</v>
+        <v>335</v>
       </c>
       <c r="D177" s="78" t="s">
         <v>169</v>
@@ -8259,20 +8316,20 @@
         <v>169</v>
       </c>
       <c r="F177" s="80" t="s">
-        <v>332</v>
+        <v>217</v>
       </c>
       <c r="G177" s="80" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="H177" s="11"/>
     </row>
     <row r="178" spans="1:8">
       <c r="A178" s="81">
-        <v>31</v>
-      </c>
-      <c r="B178" s="96"/>
+        <v>30</v>
+      </c>
+      <c r="B178" s="104"/>
       <c r="C178" s="80" t="s">
-        <v>334</v>
+        <v>219</v>
       </c>
       <c r="D178" s="78" t="s">
         <v>169</v>
@@ -8280,45 +8337,43 @@
       <c r="E178" s="78" t="s">
         <v>169</v>
       </c>
-      <c r="F178" s="80">
-        <v>64</v>
+      <c r="F178" s="80" t="s">
+        <v>330</v>
       </c>
       <c r="G178" s="80" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="H178" s="11"/>
     </row>
     <row r="179" spans="1:8">
       <c r="A179" s="81">
-        <v>32</v>
-      </c>
-      <c r="B179" s="96"/>
+        <v>31</v>
+      </c>
+      <c r="B179" s="104"/>
       <c r="C179" s="80" t="s">
-        <v>335</v>
-      </c>
-      <c r="D179" s="21" t="s">
+        <v>332</v>
+      </c>
+      <c r="D179" s="78" t="s">
         <v>169</v>
       </c>
-      <c r="E179" s="21" t="s">
+      <c r="E179" s="78" t="s">
         <v>169</v>
       </c>
-      <c r="F179" s="21">
-        <v>7.9</v>
+      <c r="F179" s="80">
+        <v>64</v>
       </c>
       <c r="G179" s="80" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="H179" s="11"/>
     </row>
     <row r="180" spans="1:8">
       <c r="A180" s="81">
-        <v>33</v>
-      </c>
-      <c r="B180" s="90" t="s">
-        <v>10</v>
-      </c>
-      <c r="C180" s="21" t="s">
-        <v>220</v>
+        <v>32</v>
+      </c>
+      <c r="B180" s="104"/>
+      <c r="C180" s="80" t="s">
+        <v>333</v>
       </c>
       <c r="D180" s="21" t="s">
         <v>169</v>
@@ -8326,117 +8381,119 @@
       <c r="E180" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="F180" s="21" t="s">
+      <c r="F180" s="21">
+        <v>7.9</v>
+      </c>
+      <c r="G180" s="80" t="s">
+        <v>337</v>
+      </c>
+      <c r="H180" s="11"/>
+    </row>
+    <row r="181" spans="1:8">
+      <c r="A181" s="81">
+        <v>33</v>
+      </c>
+      <c r="B181" s="122" t="s">
+        <v>10</v>
+      </c>
+      <c r="C181" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="D181" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E181" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F181" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="G180" s="21" t="s">
+      <c r="G181" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="H180" s="11" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="181" spans="1:8">
-      <c r="A181" s="22">
-        <v>34</v>
-      </c>
-      <c r="B181" s="100"/>
-      <c r="C181" s="84" t="s">
-        <v>223</v>
-      </c>
-      <c r="D181" s="84" t="s">
-        <v>169</v>
-      </c>
-      <c r="E181" s="84" t="s">
-        <v>169</v>
-      </c>
-      <c r="F181" s="84" t="s">
-        <v>224</v>
-      </c>
-      <c r="G181" s="84" t="s">
-        <v>171</v>
-      </c>
-      <c r="H181" s="25" t="s">
+      <c r="H181" s="11" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="182" spans="1:8">
       <c r="A182" s="22">
+        <v>34</v>
+      </c>
+      <c r="B182" s="124"/>
+      <c r="C182" s="84" t="s">
+        <v>223</v>
+      </c>
+      <c r="D182" s="84" t="s">
+        <v>169</v>
+      </c>
+      <c r="E182" s="84" t="s">
+        <v>169</v>
+      </c>
+      <c r="F182" s="84" t="s">
+        <v>224</v>
+      </c>
+      <c r="G182" s="84" t="s">
+        <v>171</v>
+      </c>
+      <c r="H182" s="25" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8">
+      <c r="A183" s="22">
         <v>35</v>
       </c>
-      <c r="B182" s="91"/>
-      <c r="C182" s="83" t="s">
-        <v>340</v>
-      </c>
-      <c r="D182" s="20" t="s">
+      <c r="B183" s="123"/>
+      <c r="C183" s="83" t="s">
+        <v>338</v>
+      </c>
+      <c r="D183" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="E182" s="20" t="s">
+      <c r="E183" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="F182" s="83" t="s">
-        <v>341</v>
-      </c>
-      <c r="G182" s="20" t="s">
+      <c r="F183" s="83" t="s">
+        <v>339</v>
+      </c>
+      <c r="G183" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="H182" s="23" t="s">
+      <c r="H183" s="23" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="183" spans="1:8">
-      <c r="A183" s="16">
+    <row r="184" spans="1:8">
+      <c r="A184" s="16">
         <v>36</v>
       </c>
-      <c r="B183" s="92" t="s">
+      <c r="B184" s="125" t="s">
+        <v>156</v>
+      </c>
+      <c r="C184" s="64" t="s">
         <v>225</v>
       </c>
-      <c r="C183" s="64" t="s">
+      <c r="D184" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="E184" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="F184" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="D183" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="E183" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="F183" s="17" t="s">
+      <c r="G184" s="64" t="s">
         <v>227</v>
       </c>
-      <c r="G183" s="64" t="s">
+      <c r="H184" s="10"/>
+    </row>
+    <row r="185" spans="1:8">
+      <c r="A185" s="19">
+        <v>37</v>
+      </c>
+      <c r="B185" s="126"/>
+      <c r="C185" s="63" t="s">
         <v>228</v>
-      </c>
-      <c r="H183" s="10"/>
-    </row>
-    <row r="184" spans="1:8">
-      <c r="A184" s="19">
-        <v>37</v>
-      </c>
-      <c r="B184" s="93"/>
-      <c r="C184" s="63" t="s">
-        <v>229</v>
-      </c>
-      <c r="D184" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E184" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F184" s="21" t="s">
-        <v>230</v>
-      </c>
-      <c r="G184" s="65" t="s">
-        <v>231</v>
-      </c>
-      <c r="H184" s="11"/>
-    </row>
-    <row r="185" spans="1:8">
-      <c r="A185" s="82">
-        <v>38</v>
-      </c>
-      <c r="B185" s="94"/>
-      <c r="C185" s="65" t="s">
-        <v>232</v>
       </c>
       <c r="D185" s="21" t="s">
         <v>169</v>
@@ -8445,419 +8502,436 @@
         <v>169</v>
       </c>
       <c r="F185" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="G185" s="65" t="s">
         <v>230</v>
       </c>
-      <c r="G185" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="H185" s="23"/>
+      <c r="H185" s="11"/>
     </row>
     <row r="186" spans="1:8">
       <c r="A186" s="82">
-        <v>39</v>
-      </c>
-      <c r="B186" s="94"/>
+        <v>38</v>
+      </c>
+      <c r="B186" s="127"/>
       <c r="C186" s="65" t="s">
-        <v>233</v>
-      </c>
-      <c r="D186" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="D186" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="E186" s="24" t="s">
+      <c r="E186" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="F186" s="24" t="s">
-        <v>234</v>
-      </c>
-      <c r="G186" s="65" t="s">
-        <v>235</v>
-      </c>
-      <c r="H186" s="25"/>
+      <c r="F186" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="G186" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="H186" s="23"/>
     </row>
     <row r="187" spans="1:8">
       <c r="A187" s="82">
-        <v>40</v>
-      </c>
-      <c r="B187" s="94"/>
-      <c r="C187" s="72" t="s">
-        <v>236</v>
-      </c>
-      <c r="D187" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="B187" s="127"/>
+      <c r="C187" s="65" t="s">
+        <v>232</v>
+      </c>
+      <c r="D187" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="E187" s="73" t="s">
+      <c r="E187" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="F187" s="73"/>
-      <c r="G187" s="74" t="s">
-        <v>320</v>
+      <c r="F187" s="24" t="s">
+        <v>233</v>
+      </c>
+      <c r="G187" s="65" t="s">
+        <v>234</v>
       </c>
       <c r="H187" s="25"/>
     </row>
     <row r="188" spans="1:8">
       <c r="A188" s="82">
-        <v>41</v>
-      </c>
-      <c r="B188" s="94"/>
+        <v>40</v>
+      </c>
+      <c r="B188" s="127"/>
       <c r="C188" s="72" t="s">
-        <v>314</v>
+        <v>235</v>
       </c>
       <c r="D188" s="73" t="s">
         <v>169</v>
       </c>
-      <c r="E188" s="73"/>
-      <c r="F188" s="73" t="s">
+      <c r="E188" s="73" t="s">
+        <v>169</v>
+      </c>
+      <c r="F188" s="73"/>
+      <c r="G188" s="74" t="s">
+        <v>318</v>
+      </c>
+      <c r="H188" s="25"/>
+    </row>
+    <row r="189" spans="1:8">
+      <c r="A189" s="82">
+        <v>41</v>
+      </c>
+      <c r="B189" s="127"/>
+      <c r="C189" s="72" t="s">
+        <v>312</v>
+      </c>
+      <c r="D189" s="73" t="s">
+        <v>169</v>
+      </c>
+      <c r="E189" s="73"/>
+      <c r="F189" s="73" t="s">
+        <v>313</v>
+      </c>
+      <c r="G189" s="72" t="s">
+        <v>314</v>
+      </c>
+      <c r="H189" s="25" t="s">
         <v>315</v>
       </c>
-      <c r="G188" s="72" t="s">
+    </row>
+    <row r="190" spans="1:8">
+      <c r="A190" s="26">
+        <v>42</v>
+      </c>
+      <c r="B190" s="112"/>
+      <c r="C190" s="27" t="s">
         <v>316</v>
       </c>
-      <c r="H188" s="25" t="s">
+      <c r="D190" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="E190" s="27"/>
+      <c r="F190" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="G190" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="H190" s="28" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="189" spans="1:8">
-      <c r="A189" s="26">
-        <v>42</v>
-      </c>
-      <c r="B189" s="95"/>
-      <c r="C189" s="27" t="s">
-        <v>318</v>
-      </c>
-      <c r="D189" s="27" t="s">
-        <v>169</v>
-      </c>
-      <c r="E189" s="27"/>
-      <c r="F189" s="27" t="s">
-        <v>230</v>
-      </c>
-      <c r="G189" s="27" t="s">
-        <v>231</v>
-      </c>
-      <c r="H189" s="28" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="190" spans="1:8">
-      <c r="A190" s="1" t="s">
+    <row r="191" spans="1:8">
+      <c r="A191" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B191" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B190" s="1" t="s">
+    </row>
+    <row r="192" spans="1:8">
+      <c r="B192" s="29" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="191" spans="1:8">
-      <c r="B191" s="29" t="s">
+    <row r="193" spans="1:7">
+      <c r="B193" s="129" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7">
+      <c r="A203" s="1" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="192" spans="1:8">
-      <c r="B192" s="1" t="s">
+      <c r="B203" s="1" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="202" spans="1:7">
-      <c r="A202" s="1" t="s">
+    <row r="204" spans="1:7">
+      <c r="A204" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="B202" s="1" t="s">
+      <c r="B204" s="30" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="203" spans="1:7">
-      <c r="A203" s="4" t="s">
+      <c r="C204" s="94" t="s">
         <v>243</v>
       </c>
-      <c r="B203" s="30" t="s">
+      <c r="D204" s="94"/>
+      <c r="E204" s="94"/>
+      <c r="F204" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="C203" s="124" t="s">
+      <c r="G204" s="32" t="s">
         <v>245</v>
       </c>
-      <c r="D203" s="124"/>
-      <c r="E203" s="124"/>
-      <c r="F203" s="31" t="s">
+    </row>
+    <row r="205" spans="1:7">
+      <c r="A205" s="120" t="s">
         <v>246</v>
       </c>
-      <c r="G203" s="32" t="s">
+      <c r="B205" s="104" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="204" spans="1:7">
-      <c r="A204" s="106" t="s">
+      <c r="C205" s="95" t="s">
         <v>248</v>
       </c>
-      <c r="B204" s="96" t="s">
+      <c r="D205" s="96"/>
+      <c r="E205" s="96"/>
+      <c r="F205" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="C204" s="125" t="s">
+      <c r="G205" s="33" t="s">
         <v>250</v>
       </c>
-      <c r="D204" s="126"/>
-      <c r="E204" s="126"/>
-      <c r="F204" s="21" t="s">
+    </row>
+    <row r="206" spans="1:7">
+      <c r="A206" s="120"/>
+      <c r="B206" s="128"/>
+      <c r="C206" s="97" t="s">
+        <v>248</v>
+      </c>
+      <c r="D206" s="98"/>
+      <c r="E206" s="98"/>
+      <c r="F206" s="20" t="s">
         <v>251</v>
       </c>
-      <c r="G204" s="33" t="s">
+      <c r="G206" s="34" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7">
+      <c r="A207" s="120"/>
+      <c r="B207" s="104" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="205" spans="1:7">
-      <c r="A205" s="106"/>
-      <c r="B205" s="97"/>
-      <c r="C205" s="116" t="s">
+      <c r="C207" s="99" t="s">
+        <v>253</v>
+      </c>
+      <c r="D207" s="99"/>
+      <c r="E207" s="99"/>
+      <c r="F207" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="G207" s="33" t="s">
         <v>250</v>
       </c>
-      <c r="D205" s="127"/>
-      <c r="E205" s="127"/>
-      <c r="F205" s="20" t="s">
+    </row>
+    <row r="208" spans="1:7">
+      <c r="A208" s="120"/>
+      <c r="B208" s="104"/>
+      <c r="C208" s="97" t="s">
         <v>253</v>
       </c>
-      <c r="G205" s="34" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="206" spans="1:7">
-      <c r="A206" s="106"/>
-      <c r="B206" s="96" t="s">
-        <v>254</v>
-      </c>
-      <c r="C206" s="120" t="s">
-        <v>255</v>
-      </c>
-      <c r="D206" s="120"/>
-      <c r="E206" s="120"/>
-      <c r="F206" s="21" t="s">
-        <v>251</v>
-      </c>
-      <c r="G206" s="33" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="207" spans="1:7">
-      <c r="A207" s="106"/>
-      <c r="B207" s="96"/>
-      <c r="C207" s="116" t="s">
-        <v>255</v>
-      </c>
-      <c r="D207" s="116"/>
-      <c r="E207" s="116"/>
-      <c r="F207" s="21" t="s">
-        <v>253</v>
-      </c>
-      <c r="G207" s="33" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="208" spans="1:7">
-      <c r="A208" s="106"/>
-      <c r="B208" s="97" t="s">
-        <v>256</v>
-      </c>
-      <c r="C208" s="117" t="s">
-        <v>250</v>
-      </c>
-      <c r="D208" s="118"/>
-      <c r="E208" s="119"/>
+      <c r="D208" s="97"/>
+      <c r="E208" s="97"/>
       <c r="F208" s="21" t="s">
         <v>251</v>
       </c>
       <c r="G208" s="33" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="209" spans="1:7">
-      <c r="A209" s="106"/>
-      <c r="B209" s="98"/>
-      <c r="C209" s="117" t="s">
+      <c r="A209" s="120"/>
+      <c r="B209" s="128" t="s">
+        <v>254</v>
+      </c>
+      <c r="C209" s="100" t="s">
+        <v>248</v>
+      </c>
+      <c r="D209" s="101"/>
+      <c r="E209" s="102"/>
+      <c r="F209" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="G209" s="33" t="s">
         <v>250</v>
       </c>
-      <c r="D209" s="118"/>
-      <c r="E209" s="119"/>
-      <c r="F209" s="21" t="s">
-        <v>253</v>
-      </c>
-      <c r="G209" s="33" t="s">
-        <v>252</v>
-      </c>
     </row>
     <row r="210" spans="1:7">
-      <c r="A210" s="106"/>
-      <c r="B210" s="96" t="s">
-        <v>257</v>
-      </c>
-      <c r="C210" s="120" t="s">
-        <v>258</v>
-      </c>
-      <c r="D210" s="120"/>
-      <c r="E210" s="120"/>
+      <c r="A210" s="120"/>
+      <c r="B210" s="108"/>
+      <c r="C210" s="100" t="s">
+        <v>248</v>
+      </c>
+      <c r="D210" s="101"/>
+      <c r="E210" s="102"/>
       <c r="F210" s="21" t="s">
         <v>251</v>
       </c>
       <c r="G210" s="33" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="211" spans="1:7">
-      <c r="A211" s="106"/>
-      <c r="B211" s="96"/>
-      <c r="C211" s="120" t="s">
-        <v>258</v>
-      </c>
-      <c r="D211" s="120"/>
-      <c r="E211" s="120"/>
+      <c r="A211" s="120"/>
+      <c r="B211" s="104" t="s">
+        <v>255</v>
+      </c>
+      <c r="C211" s="99" t="s">
+        <v>256</v>
+      </c>
+      <c r="D211" s="99"/>
+      <c r="E211" s="99"/>
       <c r="F211" s="21" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="G211" s="33" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="212" spans="1:7">
-      <c r="A212" s="106" t="s">
-        <v>259</v>
-      </c>
-      <c r="B212" s="96" t="s">
-        <v>260</v>
-      </c>
+      <c r="A212" s="120"/>
+      <c r="B212" s="104"/>
       <c r="C212" s="99" t="s">
-        <v>261</v>
-      </c>
-      <c r="D212" s="96"/>
-      <c r="E212" s="96"/>
+        <v>256</v>
+      </c>
+      <c r="D212" s="99"/>
+      <c r="E212" s="99"/>
       <c r="F212" s="21" t="s">
         <v>251</v>
       </c>
       <c r="G212" s="33" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="213" spans="1:7">
-      <c r="A213" s="106"/>
-      <c r="B213" s="96"/>
-      <c r="C213" s="96" t="s">
-        <v>262</v>
-      </c>
-      <c r="D213" s="96"/>
-      <c r="E213" s="96"/>
+      <c r="A213" s="120" t="s">
+        <v>257</v>
+      </c>
+      <c r="B213" s="104" t="s">
+        <v>258</v>
+      </c>
+      <c r="C213" s="103" t="s">
+        <v>259</v>
+      </c>
+      <c r="D213" s="104"/>
+      <c r="E213" s="104"/>
       <c r="F213" s="21" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="G213" s="33" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
     </row>
     <row r="214" spans="1:7">
-      <c r="A214" s="106"/>
-      <c r="B214" s="96" t="s">
-        <v>264</v>
-      </c>
-      <c r="C214" s="96" t="s">
-        <v>265</v>
-      </c>
-      <c r="D214" s="96"/>
-      <c r="E214" s="96"/>
+      <c r="A214" s="120"/>
+      <c r="B214" s="104"/>
+      <c r="C214" s="104" t="s">
+        <v>260</v>
+      </c>
+      <c r="D214" s="104"/>
+      <c r="E214" s="104"/>
       <c r="F214" s="21" t="s">
         <v>251</v>
       </c>
       <c r="G214" s="33" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
     </row>
     <row r="215" spans="1:7">
-      <c r="A215" s="106"/>
-      <c r="B215" s="96"/>
-      <c r="C215" s="96" t="s">
-        <v>266</v>
-      </c>
-      <c r="D215" s="96"/>
-      <c r="E215" s="96"/>
+      <c r="A215" s="120"/>
+      <c r="B215" s="104" t="s">
+        <v>262</v>
+      </c>
+      <c r="C215" s="104" t="s">
+        <v>263</v>
+      </c>
+      <c r="D215" s="104"/>
+      <c r="E215" s="104"/>
       <c r="F215" s="21" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="G215" s="33" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="216" spans="1:7">
-      <c r="A216" s="106" t="s">
-        <v>267</v>
-      </c>
-      <c r="B216" s="96" t="s">
-        <v>268</v>
-      </c>
-      <c r="C216" s="99" t="s">
-        <v>269</v>
-      </c>
-      <c r="D216" s="96"/>
-      <c r="E216" s="96"/>
+      <c r="A216" s="120"/>
+      <c r="B216" s="104"/>
+      <c r="C216" s="104" t="s">
+        <v>264</v>
+      </c>
+      <c r="D216" s="104"/>
+      <c r="E216" s="104"/>
       <c r="F216" s="21" t="s">
         <v>251</v>
       </c>
       <c r="G216" s="33" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="217" spans="1:7">
-      <c r="A217" s="106"/>
-      <c r="B217" s="96"/>
-      <c r="C217" s="96" t="s">
-        <v>270</v>
-      </c>
-      <c r="D217" s="96"/>
-      <c r="E217" s="96"/>
+      <c r="A217" s="120" t="s">
+        <v>265</v>
+      </c>
+      <c r="B217" s="104" t="s">
+        <v>266</v>
+      </c>
+      <c r="C217" s="103" t="s">
+        <v>267</v>
+      </c>
+      <c r="D217" s="104"/>
+      <c r="E217" s="104"/>
       <c r="F217" s="21" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="G217" s="33" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="218" spans="1:7">
-      <c r="A218" s="106"/>
-      <c r="B218" s="96" t="s">
-        <v>271</v>
-      </c>
-      <c r="C218" s="99" t="s">
-        <v>272</v>
-      </c>
-      <c r="D218" s="96"/>
-      <c r="E218" s="96"/>
+      <c r="A218" s="120"/>
+      <c r="B218" s="104"/>
+      <c r="C218" s="104" t="s">
+        <v>268</v>
+      </c>
+      <c r="D218" s="104"/>
+      <c r="E218" s="104"/>
       <c r="F218" s="21" t="s">
         <v>251</v>
       </c>
       <c r="G218" s="33" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="219" spans="1:7">
-      <c r="A219" s="107"/>
-      <c r="B219" s="108"/>
-      <c r="C219" s="108" t="s">
-        <v>273</v>
-      </c>
-      <c r="D219" s="108"/>
-      <c r="E219" s="108"/>
-      <c r="F219" s="27" t="s">
-        <v>253</v>
-      </c>
-      <c r="G219" s="35" t="s">
-        <v>252</v>
+      <c r="A219" s="120"/>
+      <c r="B219" s="104" t="s">
+        <v>269</v>
+      </c>
+      <c r="C219" s="103" t="s">
+        <v>270</v>
+      </c>
+      <c r="D219" s="104"/>
+      <c r="E219" s="104"/>
+      <c r="F219" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="G219" s="33" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="220" spans="1:7">
-      <c r="A220" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="C220" s="29"/>
-      <c r="D220" s="29"/>
-      <c r="E220" s="29"/>
-      <c r="F220" s="29"/>
+      <c r="A220" s="121"/>
+      <c r="B220" s="105"/>
+      <c r="C220" s="105" t="s">
+        <v>271</v>
+      </c>
+      <c r="D220" s="105"/>
+      <c r="E220" s="105"/>
+      <c r="F220" s="27" t="s">
+        <v>251</v>
+      </c>
+      <c r="G220" s="35" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="221" spans="1:7">
+      <c r="A221" s="1" t="s">
+        <v>272</v>
+      </c>
       <c r="C221" s="29"/>
       <c r="D221" s="29"/>
       <c r="E221" s="29"/>
+      <c r="F221" s="29"/>
     </row>
     <row r="222" spans="1:7">
       <c r="C222" s="29"/>
@@ -8865,307 +8939,295 @@
       <c r="E222" s="29"/>
     </row>
     <row r="223" spans="1:7">
-      <c r="A223" s="1" t="s">
-        <v>275</v>
-      </c>
       <c r="C223" s="29"/>
       <c r="D223" s="29"/>
       <c r="E223" s="29"/>
     </row>
     <row r="224" spans="1:7">
-      <c r="A224" s="36" t="s">
+      <c r="A224" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C224" s="29"/>
+      <c r="D224" s="29"/>
+      <c r="E224" s="29"/>
+    </row>
+    <row r="225" spans="1:7">
+      <c r="A225" s="36" t="s">
+        <v>274</v>
+      </c>
+      <c r="B225" s="106" t="s">
+        <v>275</v>
+      </c>
+      <c r="C225" s="106"/>
+      <c r="D225" s="106"/>
+      <c r="E225" s="106"/>
+      <c r="F225" s="37" t="s">
         <v>276</v>
       </c>
-      <c r="B224" s="114" t="s">
+      <c r="G225" s="38" t="s">
         <v>277</v>
       </c>
-      <c r="C224" s="114"/>
-      <c r="D224" s="114"/>
-      <c r="E224" s="114"/>
-      <c r="F224" s="37" t="s">
+    </row>
+    <row r="226" spans="1:7" ht="93" customHeight="1">
+      <c r="A226" s="39" t="s">
         <v>278</v>
       </c>
-      <c r="G224" s="38" t="s">
+      <c r="B226" s="107" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="225" spans="1:7" ht="93" customHeight="1">
-      <c r="A225" s="39" t="s">
+      <c r="C226" s="108"/>
+      <c r="D226" s="108"/>
+      <c r="E226" s="108"/>
+      <c r="F226" s="40" t="s">
+        <v>154</v>
+      </c>
+      <c r="G226" s="41" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" ht="57" customHeight="1">
+      <c r="A227" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="B225" s="115" t="s">
+      <c r="B227" s="109" t="s">
         <v>281</v>
       </c>
-      <c r="C225" s="98"/>
-      <c r="D225" s="98"/>
-      <c r="E225" s="98"/>
-      <c r="F225" s="40" t="s">
-        <v>154</v>
-      </c>
-      <c r="G225" s="41" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="226" spans="1:7" ht="57" customHeight="1">
-      <c r="A226" s="8" t="s">
+      <c r="C227" s="110"/>
+      <c r="D227" s="110"/>
+      <c r="E227" s="111"/>
+      <c r="F227" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="G227" s="11" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7" ht="57" customHeight="1">
+      <c r="A228" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="B226" s="110" t="s">
+      <c r="B228" s="109" t="s">
         <v>283</v>
       </c>
-      <c r="C226" s="111"/>
-      <c r="D226" s="111"/>
-      <c r="E226" s="112"/>
-      <c r="F226" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="G226" s="11" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="227" spans="1:7" ht="57" customHeight="1">
-      <c r="A227" s="12" t="s">
+      <c r="C228" s="110"/>
+      <c r="D228" s="110"/>
+      <c r="E228" s="111"/>
+      <c r="F228" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="G228" s="23" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" ht="69" customHeight="1">
+      <c r="A229" s="14" t="s">
         <v>284</v>
       </c>
-      <c r="B227" s="110" t="s">
+      <c r="B229" s="112" t="s">
         <v>285</v>
       </c>
-      <c r="C227" s="111"/>
-      <c r="D227" s="111"/>
-      <c r="E227" s="112"/>
-      <c r="F227" s="13" t="s">
-        <v>252</v>
-      </c>
-      <c r="G227" s="23" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="228" spans="1:7" ht="69" customHeight="1">
-      <c r="A228" s="14" t="s">
+      <c r="C229" s="105"/>
+      <c r="D229" s="105"/>
+      <c r="E229" s="105"/>
+      <c r="F229" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="G229" s="28" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7">
+      <c r="C230" s="42"/>
+    </row>
+    <row r="232" spans="1:7">
+      <c r="A232" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="B228" s="95" t="s">
+    </row>
+    <row r="233" spans="1:7">
+      <c r="A233" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="C228" s="108"/>
-      <c r="D228" s="108"/>
-      <c r="E228" s="108"/>
-      <c r="F228" s="15" t="s">
-        <v>252</v>
-      </c>
-      <c r="G228" s="28" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="229" spans="1:7">
-      <c r="C229" s="42"/>
-    </row>
-    <row r="231" spans="1:7">
-      <c r="A231" s="1" t="s">
+      <c r="B233" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="C233" s="43" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="232" spans="1:7">
-      <c r="A232" s="4" t="s">
+      <c r="D233" s="44" t="s">
+        <v>275</v>
+      </c>
+      <c r="E233" s="44"/>
+      <c r="F233" s="45"/>
+      <c r="G233" s="32" t="s">
         <v>289</v>
       </c>
-      <c r="B232" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="C232" s="43" t="s">
+    </row>
+    <row r="234" spans="1:7">
+      <c r="A234" s="46">
+        <v>42682</v>
+      </c>
+      <c r="B234" s="47">
+        <v>1.04</v>
+      </c>
+      <c r="C234" s="17" t="s">
         <v>290</v>
       </c>
-      <c r="D232" s="44" t="s">
-        <v>277</v>
-      </c>
-      <c r="E232" s="44"/>
-      <c r="F232" s="45"/>
-      <c r="G232" s="32" t="s">
+      <c r="D234" s="113" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="233" spans="1:7">
-      <c r="A233" s="46">
-        <v>42682</v>
-      </c>
-      <c r="B233" s="47">
-        <v>1.04</v>
-      </c>
-      <c r="C233" s="17" t="s">
-        <v>292</v>
-      </c>
-      <c r="D233" s="113" t="s">
-        <v>293</v>
-      </c>
-      <c r="E233" s="113"/>
-      <c r="F233" s="113"/>
-      <c r="G233" s="48"/>
-    </row>
-    <row r="234" spans="1:7">
-      <c r="A234" s="49">
-        <v>42692</v>
-      </c>
-      <c r="B234" s="50">
-        <v>1.05</v>
-      </c>
-      <c r="C234" s="21" t="s">
-        <v>292</v>
-      </c>
-      <c r="D234" s="109" t="s">
-        <v>294</v>
-      </c>
-      <c r="E234" s="109"/>
-      <c r="F234" s="109"/>
-      <c r="G234" s="33"/>
+      <c r="E234" s="113"/>
+      <c r="F234" s="113"/>
+      <c r="G234" s="48"/>
     </row>
     <row r="235" spans="1:7">
       <c r="A235" s="49">
-        <v>42955</v>
+        <v>42692</v>
       </c>
       <c r="B235" s="50">
-        <v>1.06</v>
+        <v>1.05</v>
       </c>
       <c r="C235" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="D235" s="114" t="s">
         <v>292</v>
       </c>
-      <c r="D235" s="109" t="s">
-        <v>295</v>
-      </c>
-      <c r="E235" s="109"/>
-      <c r="F235" s="109"/>
+      <c r="E235" s="114"/>
+      <c r="F235" s="114"/>
       <c r="G235" s="33"/>
     </row>
     <row r="236" spans="1:7">
       <c r="A236" s="49">
-        <v>42991</v>
+        <v>42955</v>
       </c>
       <c r="B236" s="50">
-        <v>1.07</v>
+        <v>1.06</v>
       </c>
       <c r="C236" s="21" t="s">
-        <v>292</v>
-      </c>
-      <c r="D236" s="109" t="s">
-        <v>296</v>
-      </c>
-      <c r="E236" s="109"/>
-      <c r="F236" s="109"/>
+        <v>290</v>
+      </c>
+      <c r="D236" s="114" t="s">
+        <v>293</v>
+      </c>
+      <c r="E236" s="114"/>
+      <c r="F236" s="114"/>
       <c r="G236" s="33"/>
     </row>
     <row r="237" spans="1:7">
       <c r="A237" s="49">
-        <v>43026</v>
+        <v>42991</v>
       </c>
       <c r="B237" s="50">
-        <v>1.08</v>
+        <v>1.07</v>
       </c>
       <c r="C237" s="21" t="s">
-        <v>292</v>
-      </c>
-      <c r="D237" s="109" t="s">
-        <v>297</v>
-      </c>
-      <c r="E237" s="109"/>
-      <c r="F237" s="109"/>
+        <v>290</v>
+      </c>
+      <c r="D237" s="114" t="s">
+        <v>294</v>
+      </c>
+      <c r="E237" s="114"/>
+      <c r="F237" s="114"/>
       <c r="G237" s="33"/>
     </row>
     <row r="238" spans="1:7">
       <c r="A238" s="49">
+        <v>43026</v>
+      </c>
+      <c r="B238" s="50">
+        <v>1.08</v>
+      </c>
+      <c r="C238" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="D238" s="114" t="s">
+        <v>295</v>
+      </c>
+      <c r="E238" s="114"/>
+      <c r="F238" s="114"/>
+      <c r="G238" s="33"/>
+    </row>
+    <row r="239" spans="1:7">
+      <c r="A239" s="49">
         <v>43069</v>
       </c>
-      <c r="B238" s="50">
+      <c r="B239" s="50">
         <v>1.0900000000000001</v>
       </c>
-      <c r="C238" s="21" t="s">
-        <v>292</v>
-      </c>
-      <c r="D238" s="109" t="s">
-        <v>298</v>
-      </c>
-      <c r="E238" s="109"/>
-      <c r="F238" s="109"/>
-      <c r="G238" s="33"/>
-    </row>
-    <row r="239" spans="1:7">
-      <c r="A239" s="51">
-        <v>43248</v>
-      </c>
-      <c r="B239" s="52">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C239" s="20" t="s">
-        <v>292</v>
-      </c>
-      <c r="D239" s="101" t="s">
-        <v>299</v>
-      </c>
-      <c r="E239" s="102"/>
-      <c r="F239" s="103"/>
-      <c r="G239" s="34"/>
+      <c r="C239" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="D239" s="114" t="s">
+        <v>296</v>
+      </c>
+      <c r="E239" s="114"/>
+      <c r="F239" s="114"/>
+      <c r="G239" s="33"/>
     </row>
     <row r="240" spans="1:7">
       <c r="A240" s="51">
-        <v>43339</v>
+        <v>43248</v>
       </c>
       <c r="B240" s="52">
-        <v>1.1100000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C240" s="20" t="s">
-        <v>292</v>
-      </c>
-      <c r="D240" s="101" t="s">
-        <v>300</v>
-      </c>
-      <c r="E240" s="102"/>
-      <c r="F240" s="103"/>
+        <v>290</v>
+      </c>
+      <c r="D240" s="115" t="s">
+        <v>297</v>
+      </c>
+      <c r="E240" s="116"/>
+      <c r="F240" s="117"/>
       <c r="G240" s="34"/>
     </row>
     <row r="241" spans="1:7">
       <c r="A241" s="51">
-        <v>43542</v>
+        <v>43339</v>
       </c>
       <c r="B241" s="52">
-        <v>1.1200000000000001</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="C241" s="20" t="s">
-        <v>292</v>
-      </c>
-      <c r="D241" s="101" t="s">
-        <v>301</v>
-      </c>
-      <c r="E241" s="102"/>
-      <c r="F241" s="103"/>
+        <v>290</v>
+      </c>
+      <c r="D241" s="115" t="s">
+        <v>298</v>
+      </c>
+      <c r="E241" s="116"/>
+      <c r="F241" s="117"/>
       <c r="G241" s="34"/>
     </row>
     <row r="242" spans="1:7">
       <c r="A242" s="51">
-        <v>43599</v>
+        <v>43542</v>
       </c>
       <c r="B242" s="52">
-        <v>1.1299999999999999</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="C242" s="20" t="s">
-        <v>292</v>
-      </c>
-      <c r="D242" s="53" t="s">
-        <v>302</v>
-      </c>
-      <c r="E242" s="54"/>
-      <c r="F242" s="55"/>
+        <v>290</v>
+      </c>
+      <c r="D242" s="115" t="s">
+        <v>299</v>
+      </c>
+      <c r="E242" s="116"/>
+      <c r="F242" s="117"/>
       <c r="G242" s="34"/>
     </row>
     <row r="243" spans="1:7">
       <c r="A243" s="51">
-        <v>43643</v>
+        <v>43599</v>
       </c>
       <c r="B243" s="52">
-        <v>1.1399999999999999</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="C243" s="20" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D243" s="53" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="E243" s="54"/>
       <c r="F243" s="55"/>
@@ -9173,16 +9235,16 @@
     </row>
     <row r="244" spans="1:7">
       <c r="A244" s="51">
-        <v>43894</v>
+        <v>43643</v>
       </c>
       <c r="B244" s="52">
-        <v>1.1499999999999999</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="C244" s="20" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D244" s="53" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E244" s="54"/>
       <c r="F244" s="55"/>
@@ -9190,16 +9252,16 @@
     </row>
     <row r="245" spans="1:7">
       <c r="A245" s="51">
-        <v>44017</v>
+        <v>43894</v>
       </c>
       <c r="B245" s="52">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="C245" s="73" t="s">
-        <v>292</v>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C245" s="20" t="s">
+        <v>290</v>
       </c>
       <c r="D245" s="53" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="E245" s="54"/>
       <c r="F245" s="55"/>
@@ -9207,16 +9269,16 @@
     </row>
     <row r="246" spans="1:7">
       <c r="A246" s="51">
-        <v>44118</v>
+        <v>44017</v>
       </c>
       <c r="B246" s="52">
-        <v>1.17</v>
-      </c>
-      <c r="C246" s="75" t="s">
-        <v>292</v>
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="C246" s="73" t="s">
+        <v>290</v>
       </c>
       <c r="D246" s="53" t="s">
-        <v>321</v>
+        <v>303</v>
       </c>
       <c r="E246" s="54"/>
       <c r="F246" s="55"/>
@@ -9224,16 +9286,16 @@
     </row>
     <row r="247" spans="1:7">
       <c r="A247" s="51">
-        <v>44209</v>
+        <v>44118</v>
       </c>
       <c r="B247" s="52">
-        <v>1.18</v>
-      </c>
-      <c r="C247" s="79" t="s">
-        <v>292</v>
+        <v>1.17</v>
+      </c>
+      <c r="C247" s="75" t="s">
+        <v>290</v>
       </c>
       <c r="D247" s="53" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="E247" s="54"/>
       <c r="F247" s="55"/>
@@ -9241,99 +9303,133 @@
     </row>
     <row r="248" spans="1:7">
       <c r="A248" s="51">
-        <v>44258</v>
+        <v>44209</v>
       </c>
       <c r="B248" s="52">
-        <v>1.19</v>
-      </c>
-      <c r="C248" s="84" t="s">
-        <v>292</v>
-      </c>
-      <c r="D248" s="53" t="s">
-        <v>330</v>
+        <v>1.18</v>
+      </c>
+      <c r="C248" s="79" t="s">
+        <v>290</v>
+      </c>
+      <c r="D248" s="130" t="s">
+        <v>322</v>
       </c>
       <c r="E248" s="54"/>
       <c r="F248" s="55"/>
       <c r="G248" s="34"/>
     </row>
     <row r="249" spans="1:7">
-      <c r="A249" s="56">
+      <c r="A249" s="51">
+        <v>44258</v>
+      </c>
+      <c r="B249" s="52">
+        <v>1.19</v>
+      </c>
+      <c r="C249" s="84" t="s">
+        <v>290</v>
+      </c>
+      <c r="D249" s="53" t="s">
+        <v>328</v>
+      </c>
+      <c r="E249" s="54"/>
+      <c r="F249" s="55"/>
+      <c r="G249" s="34"/>
+    </row>
+    <row r="250" spans="1:7">
+      <c r="A250" s="51">
         <v>44357</v>
       </c>
-      <c r="B249" s="57">
+      <c r="B250" s="52">
         <v>1.2</v>
       </c>
-      <c r="C249" s="27" t="s">
-        <v>292</v>
-      </c>
-      <c r="D249" s="104" t="s">
-        <v>342</v>
-      </c>
-      <c r="E249" s="105"/>
-      <c r="F249" s="105"/>
-      <c r="G249" s="35"/>
+      <c r="C250" s="86" t="s">
+        <v>290</v>
+      </c>
+      <c r="D250" s="53" t="s">
+        <v>340</v>
+      </c>
+      <c r="E250" s="54"/>
+      <c r="F250" s="55"/>
+      <c r="G250" s="34"/>
+    </row>
+    <row r="251" spans="1:7">
+      <c r="A251" s="56">
+        <v>44487</v>
+      </c>
+      <c r="B251" s="57">
+        <v>1.21</v>
+      </c>
+      <c r="C251" s="27" t="s">
+        <v>290</v>
+      </c>
+      <c r="D251" s="118" t="s">
+        <v>343</v>
+      </c>
+      <c r="E251" s="119"/>
+      <c r="F251" s="119"/>
+      <c r="G251" s="35"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="GSXR3i1/FGR/XuzYi0Mi+qZ0dyL0lbIdypAv+Ro8+vnrK7ecZIvn+JEYuHdVIOyzmoge4uznelYSNioXrXzvjQ==" saltValue="jv9Vc6Hz4FI7+FTdy8JCVQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Y3CbQBUOESlDRywGeoG/3StrDbFnCkeqkNskZfEB2tOROsi5KmkcJgzaGARx/t71p+8XW8S30YXLCnas8V4vyw==" saltValue="Hjy+0Aja5MmvK1SBdUhEOA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
-      <selection activeCell="B3" sqref="B3"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115" topLeftCell="A210">
+      <selection activeCell="C263" sqref="C263"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="51">
-    <mergeCell ref="F111:N111"/>
-    <mergeCell ref="C203:E203"/>
-    <mergeCell ref="C204:E204"/>
-    <mergeCell ref="C205:E205"/>
-    <mergeCell ref="C206:E206"/>
-    <mergeCell ref="C207:E207"/>
+    <mergeCell ref="B181:B183"/>
+    <mergeCell ref="B184:B190"/>
+    <mergeCell ref="B205:B206"/>
+    <mergeCell ref="B207:B208"/>
+    <mergeCell ref="B209:B210"/>
+    <mergeCell ref="B149:B161"/>
+    <mergeCell ref="B162:B163"/>
+    <mergeCell ref="B164:B166"/>
+    <mergeCell ref="B167:B174"/>
+    <mergeCell ref="B175:B180"/>
+    <mergeCell ref="D241:F241"/>
+    <mergeCell ref="D242:F242"/>
+    <mergeCell ref="D251:F251"/>
+    <mergeCell ref="A205:A212"/>
+    <mergeCell ref="A213:A216"/>
+    <mergeCell ref="A217:A220"/>
+    <mergeCell ref="B211:B212"/>
+    <mergeCell ref="B213:B214"/>
+    <mergeCell ref="B215:B216"/>
+    <mergeCell ref="B217:B218"/>
+    <mergeCell ref="B219:B220"/>
+    <mergeCell ref="D236:F236"/>
+    <mergeCell ref="D237:F237"/>
+    <mergeCell ref="D238:F238"/>
+    <mergeCell ref="D239:F239"/>
+    <mergeCell ref="D240:F240"/>
+    <mergeCell ref="B227:E227"/>
+    <mergeCell ref="B228:E228"/>
+    <mergeCell ref="B229:E229"/>
+    <mergeCell ref="D234:F234"/>
+    <mergeCell ref="D235:F235"/>
+    <mergeCell ref="C218:E218"/>
+    <mergeCell ref="C219:E219"/>
+    <mergeCell ref="C220:E220"/>
+    <mergeCell ref="B225:E225"/>
+    <mergeCell ref="B226:E226"/>
+    <mergeCell ref="C213:E213"/>
+    <mergeCell ref="C214:E214"/>
+    <mergeCell ref="C215:E215"/>
+    <mergeCell ref="C216:E216"/>
+    <mergeCell ref="C217:E217"/>
     <mergeCell ref="C208:E208"/>
     <mergeCell ref="C209:E209"/>
     <mergeCell ref="C210:E210"/>
     <mergeCell ref="C211:E211"/>
     <mergeCell ref="C212:E212"/>
-    <mergeCell ref="C213:E213"/>
-    <mergeCell ref="C214:E214"/>
-    <mergeCell ref="C215:E215"/>
-    <mergeCell ref="C216:E216"/>
-    <mergeCell ref="C217:E217"/>
-    <mergeCell ref="C218:E218"/>
-    <mergeCell ref="C219:E219"/>
-    <mergeCell ref="B224:E224"/>
-    <mergeCell ref="B225:E225"/>
-    <mergeCell ref="B226:E226"/>
-    <mergeCell ref="B227:E227"/>
-    <mergeCell ref="B228:E228"/>
-    <mergeCell ref="D233:F233"/>
-    <mergeCell ref="D234:F234"/>
-    <mergeCell ref="D240:F240"/>
-    <mergeCell ref="D241:F241"/>
-    <mergeCell ref="D249:F249"/>
-    <mergeCell ref="A204:A211"/>
-    <mergeCell ref="A212:A215"/>
-    <mergeCell ref="A216:A219"/>
-    <mergeCell ref="B210:B211"/>
-    <mergeCell ref="B212:B213"/>
-    <mergeCell ref="B214:B215"/>
-    <mergeCell ref="B216:B217"/>
-    <mergeCell ref="B218:B219"/>
-    <mergeCell ref="D235:F235"/>
-    <mergeCell ref="D236:F236"/>
-    <mergeCell ref="D237:F237"/>
-    <mergeCell ref="D238:F238"/>
-    <mergeCell ref="D239:F239"/>
-    <mergeCell ref="B148:B160"/>
-    <mergeCell ref="B161:B162"/>
-    <mergeCell ref="B163:B165"/>
-    <mergeCell ref="B166:B173"/>
-    <mergeCell ref="B174:B179"/>
-    <mergeCell ref="B180:B182"/>
-    <mergeCell ref="B183:B189"/>
-    <mergeCell ref="B204:B205"/>
-    <mergeCell ref="B206:B207"/>
-    <mergeCell ref="B208:B209"/>
+    <mergeCell ref="F111:N111"/>
+    <mergeCell ref="C204:E204"/>
+    <mergeCell ref="C205:E205"/>
+    <mergeCell ref="C206:E206"/>
+    <mergeCell ref="C207:E207"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -9354,7 +9450,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -9363,11 +9459,11 @@
       <selection activeCell="D24" sqref="D24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>

</xml_diff>

<commit_message>
i379--Multiple commands support for a single task
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_example/standard_suite/diamond_regression.xlsx
+++ b/tmp_client/doc/TMP_example/standard_suite/diamond_regression.xlsx
@@ -24,17 +24,17 @@
     <definedName name="Z_179F0E1F_F6F7_410E_B883_54B8A90BA550_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AF$2</definedName>
     <definedName name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AF$46</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="3" showComments="commIndAndComment"/>
+    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="3" showComments="commIndAndComment"/>
+    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
     <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
-    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="373">
   <si>
     <t>[suite_info]</t>
   </si>
@@ -664,9 +664,6 @@
   </si>
   <si>
     <t>icecube</t>
-  </si>
-  <si>
-    <t>classic</t>
   </si>
   <si>
     <t>modelsim</t>
@@ -960,9 +957,6 @@
     <t>dir</t>
   </si>
   <si>
-    <t>user prefer launch path setting</t>
-  </si>
-  <si>
     <t>no,sevenz,bz2,bzip2,tbz2,tbz,gz,gzip,tgz,tar,zip,targz,tarbz,tarbz2</t>
   </si>
   <si>
@@ -1044,9 +1038,6 @@
     <t>os_version</t>
   </si>
   <si>
-    <t>windows10, windows7, ubuntu16.04,ubuntu20.04,centos7.9,centos8.2,redhat7.9</t>
-  </si>
-  <si>
     <t>os_family</t>
   </si>
   <si>
@@ -1072,6 +1063,115 @@
   </si>
   <si>
     <t>Reusable column added</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>2@cmd_1</t>
+  </si>
+  <si>
+    <t>3@cmd_2</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>This Environment target for cmd_2 only</t>
+  </si>
+  <si>
+    <t>This Environment target for cmd_1 only</t>
+  </si>
+  <si>
+    <t>cmd_1</t>
+  </si>
+  <si>
+    <t>cmd_2</t>
+  </si>
+  <si>
+    <t>python ***.py --run-par</t>
+  </si>
+  <si>
+    <t>python ***.py --run-par-trce</t>
+  </si>
+  <si>
+    <t>For multiple command mode</t>
+  </si>
+  <si>
+    <t>4. Single command mode: A task case has one single run command line</t>
+  </si>
+  <si>
+    <t>For single command mode</t>
+  </si>
+  <si>
+    <t>radiant</t>
+  </si>
+  <si>
+    <t>ng3_1p.1</t>
+  </si>
+  <si>
+    <t>ng3_1p.1@cmd_2, ng3_1p.2@cmd_1</t>
+  </si>
+  <si>
+    <t>ng3_1p.1 for cmd_2, ng3_1p.2 for cmd_1</t>
+  </si>
+  <si>
+    <t>3.11.0.2, 3.11.0.24@cmd_2</t>
+  </si>
+  <si>
+    <t>3.11.0.2 for cmd_1(by location), 3.11.0.24 for cmd_2</t>
+  </si>
+  <si>
+    <t>20.03 for all commands</t>
+  </si>
+  <si>
+    <t>multiple command line support</t>
+  </si>
+  <si>
+    <t>6. Software: software with @ mark will be used for specific command line</t>
+  </si>
+  <si>
+    <t>windows10, windows7, ubuntu16.04,ubuntu20.04,centos7.9,centos8.2,redhat7.9,redhat8.2</t>
+  </si>
+  <si>
+    <t>parallel</t>
+  </si>
+  <si>
+    <t>If 'true', run all commands in parallel</t>
+  </si>
+  <si>
+    <t>cmd_all</t>
+  </si>
+  <si>
+    <t>cmd_all = --devkit=iCE40UP5K-CM225I</t>
+  </si>
+  <si>
+    <t>Don't apply both single and multiple command modes</t>
+  </si>
+  <si>
+    <t>cmd_n</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5. Multiple command mode: A task case have two or more command lines, all command exit code will be considered and the final result priority will be: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>passed &lt; failed &lt; timeout &lt; caseissue &lt; swissue</t>
+    </r>
+  </si>
+  <si>
+    <t>Only for Case level, used to merge/override globle 'cmd', 'cmd_1'…</t>
+  </si>
+  <si>
+    <t>User prefer launch path setting</t>
   </si>
 </sst>
 </file>
@@ -1082,12 +1182,19 @@
     <numFmt numFmtId="164" formatCode="0.00_);[Red]\(0.00\)"/>
     <numFmt numFmtId="165" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1111,6 +1218,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1630,192 +1745,192 @@
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="37" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="37" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="5" applyNumberFormat="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="5" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="5" applyNumberFormat="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="5" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="5" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="7" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="12" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="12" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="13" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="14" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="14" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="15" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
@@ -1827,10 +1942,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1842,15 +1957,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1863,11 +1975,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
@@ -1876,154 +1988,194 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="33" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="5" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="33" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="34" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="34" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="36" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="36" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -4353,13 +4505,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>193</xdr:row>
+      <xdr:row>203</xdr:row>
       <xdr:rowOff>140970</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>904875</xdr:colOff>
-      <xdr:row>201</xdr:row>
+      <xdr:row>211</xdr:row>
       <xdr:rowOff>102870</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4566,8 +4718,8 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{A5694B8A-CCC3-4ACD-8EF2-0CB46AEC2CBD}">
-  <header guid="{A5694B8A-CCC3-4ACD-8EF2-0CB46AEC2CBD}" dateTime="2021-10-18T15:36:01" maxSheetId="5" userName="Jason Wang" r:id="rId1">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{F1554B03-5648-4025-8796-84263C815341}">
+  <header guid="{F1554B03-5648-4025-8796-84263C815341}" dateTime="2021-11-18T17:44:59" maxSheetId="5" userName="Jason Wang" r:id="rId1">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -4876,7 +5028,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B14:B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -4890,7 +5044,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="59" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4898,7 +5052,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4914,12 +5068,12 @@
         <v>4</v>
       </c>
       <c r="B4" s="59" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="B5" s="59" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4940,7 +5094,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="59" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4966,13 +5120,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
-      <selection activeCell="B35" sqref="B35"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="B4" sqref="B4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="B4" sqref="B4"/>
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+      <selection activeCell="B35" sqref="B35"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -5025,42 +5179,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" s="58" customFormat="1">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="88"/>
-      <c r="N1" s="88"/>
-      <c r="O1" s="88"/>
-      <c r="P1" s="88"/>
-      <c r="Q1" s="88"/>
-      <c r="R1" s="88"/>
-      <c r="S1" s="88"/>
-      <c r="T1" s="88"/>
-      <c r="U1" s="88"/>
-      <c r="V1" s="88"/>
-      <c r="W1" s="88"/>
-      <c r="X1" s="89"/>
-      <c r="Y1" s="90" t="s">
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="103"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="103"/>
+      <c r="N1" s="103"/>
+      <c r="O1" s="103"/>
+      <c r="P1" s="103"/>
+      <c r="Q1" s="103"/>
+      <c r="R1" s="103"/>
+      <c r="S1" s="103"/>
+      <c r="T1" s="103"/>
+      <c r="U1" s="103"/>
+      <c r="V1" s="103"/>
+      <c r="W1" s="103"/>
+      <c r="X1" s="104"/>
+      <c r="Y1" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="Z1" s="90"/>
-      <c r="AA1" s="90"/>
-      <c r="AB1" s="90"/>
-      <c r="AC1" s="90"/>
-      <c r="AD1" s="90"/>
-      <c r="AE1" s="90"/>
-      <c r="AF1" s="90"/>
+      <c r="Z1" s="105"/>
+      <c r="AA1" s="105"/>
+      <c r="AB1" s="105"/>
+      <c r="AC1" s="105"/>
+      <c r="AD1" s="105"/>
+      <c r="AE1" s="105"/>
+      <c r="AF1" s="105"/>
     </row>
     <row r="2" spans="1:32" s="58" customFormat="1">
       <c r="A2" s="61" t="s">
@@ -5100,7 +5254,7 @@
         <v>25</v>
       </c>
       <c r="M2" s="62" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="N2" s="61" t="s">
         <v>4</v>
@@ -5124,7 +5278,7 @@
         <v>26</v>
       </c>
       <c r="U2" s="61" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="V2" s="61" t="s">
         <v>27</v>
@@ -6583,21 +6737,21 @@
   <customSheetViews>
     <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="N7" sqref="N7"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
       <autoFilter ref="A2:AF46"/>
     </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen"/>
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="H23" sqref="H23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
       <autoFilter ref="A2:Y2"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen"/>
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="C23" sqref="C23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
       <autoFilter ref="A2:Y2"/>
@@ -6683,9 +6837,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:N251"/>
+  <dimension ref="A1:N262"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView topLeftCell="A160" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E178" sqref="E178"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -6695,7 +6851,7 @@
     <col min="4" max="4" width="15" style="1" customWidth="1"/>
     <col min="5" max="5" width="24.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="32" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="33.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="28.140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="13.140625" style="1" customWidth="1"/>
     <col min="10" max="10" width="11.7109375" style="1" customWidth="1"/>
@@ -6707,7 +6863,7 @@
         <v>133</v>
       </c>
       <c r="B1" s="2">
-        <v>1.21</v>
+        <v>1.22</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -6715,7 +6871,7 @@
         <v>29</v>
       </c>
       <c r="B2" s="3">
-        <v>44487</v>
+        <v>44518</v>
       </c>
     </row>
     <row r="107" spans="1:14" ht="12.75" customHeight="1"/>
@@ -6745,17 +6901,17 @@
       <c r="E111" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="F111" s="91" t="s">
+      <c r="F111" s="137" t="s">
         <v>140</v>
       </c>
-      <c r="G111" s="92"/>
-      <c r="H111" s="92"/>
-      <c r="I111" s="92"/>
-      <c r="J111" s="92"/>
-      <c r="K111" s="92"/>
-      <c r="L111" s="92"/>
-      <c r="M111" s="92"/>
-      <c r="N111" s="93"/>
+      <c r="G111" s="138"/>
+      <c r="H111" s="138"/>
+      <c r="I111" s="138"/>
+      <c r="J111" s="138"/>
+      <c r="K111" s="138"/>
+      <c r="L111" s="138"/>
+      <c r="M111" s="138"/>
+      <c r="N111" s="139"/>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="6" t="s">
@@ -7097,7 +7253,7 @@
     </row>
     <row r="124" spans="1:14">
       <c r="A124" s="8" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B124" s="9" t="s">
         <v>143</v>
@@ -7332,8 +7488,8 @@
       <c r="N132" s="11"/>
     </row>
     <row r="133" spans="1:14">
-      <c r="A133" s="76" t="s">
-        <v>320</v>
+      <c r="A133" s="75" t="s">
+        <v>318</v>
       </c>
       <c r="B133" s="9" t="s">
         <v>143</v>
@@ -7344,8 +7500,8 @@
       <c r="D133" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="E133" s="77" t="s">
-        <v>321</v>
+      <c r="E133" s="76" t="s">
+        <v>319</v>
       </c>
       <c r="F133" s="9"/>
       <c r="G133" s="9"/>
@@ -7675,7 +7831,7 @@
       <c r="A149" s="19">
         <v>1</v>
       </c>
-      <c r="B149" s="122" t="s">
+      <c r="B149" s="106" t="s">
         <v>4</v>
       </c>
       <c r="C149" s="63" t="s">
@@ -7701,7 +7857,7 @@
       <c r="A150" s="19">
         <v>2</v>
       </c>
-      <c r="B150" s="123"/>
+      <c r="B150" s="108"/>
       <c r="C150" s="21" t="s">
         <v>173</v>
       </c>
@@ -7723,7 +7879,7 @@
       <c r="A151" s="19">
         <v>3</v>
       </c>
-      <c r="B151" s="123"/>
+      <c r="B151" s="108"/>
       <c r="C151" s="21" t="s">
         <v>18</v>
       </c>
@@ -7732,7 +7888,7 @@
         <v>169</v>
       </c>
       <c r="F151" s="21" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G151" s="21" t="s">
         <v>171</v>
@@ -7743,7 +7899,7 @@
       <c r="A152" s="19">
         <v>4</v>
       </c>
-      <c r="B152" s="123"/>
+      <c r="B152" s="108"/>
       <c r="C152" s="21" t="s">
         <v>175</v>
       </c>
@@ -7754,7 +7910,7 @@
         <v>169</v>
       </c>
       <c r="F152" s="21" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G152" s="21" t="s">
         <v>171</v>
@@ -7767,7 +7923,7 @@
       <c r="A153" s="19">
         <v>5</v>
       </c>
-      <c r="B153" s="123"/>
+      <c r="B153" s="108"/>
       <c r="C153" s="63" t="s">
         <v>177</v>
       </c>
@@ -7791,7 +7947,7 @@
       <c r="A154" s="19">
         <v>6</v>
       </c>
-      <c r="B154" s="123"/>
+      <c r="B154" s="108"/>
       <c r="C154" s="63" t="s">
         <v>181</v>
       </c>
@@ -7804,8 +7960,8 @@
       <c r="F154" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="G154" s="71" t="s">
-        <v>307</v>
+      <c r="G154" s="70" t="s">
+        <v>305</v>
       </c>
       <c r="H154" s="11" t="s">
         <v>180</v>
@@ -7815,7 +7971,7 @@
       <c r="A155" s="19">
         <v>7</v>
       </c>
-      <c r="B155" s="123"/>
+      <c r="B155" s="108"/>
       <c r="C155" s="21" t="s">
         <v>183</v>
       </c>
@@ -7826,7 +7982,7 @@
         <v>169</v>
       </c>
       <c r="F155" s="21" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G155" s="21" t="s">
         <v>171</v>
@@ -7837,7 +7993,7 @@
       <c r="A156" s="19">
         <v>8</v>
       </c>
-      <c r="B156" s="123"/>
+      <c r="B156" s="108"/>
       <c r="C156" s="63" t="s">
         <v>184</v>
       </c>
@@ -7861,7 +8017,7 @@
       <c r="A157" s="19">
         <v>9</v>
       </c>
-      <c r="B157" s="123"/>
+      <c r="B157" s="108"/>
       <c r="C157" s="63" t="s">
         <v>185</v>
       </c>
@@ -7885,7 +8041,7 @@
       <c r="A158" s="19">
         <v>10</v>
       </c>
-      <c r="B158" s="123"/>
+      <c r="B158" s="108"/>
       <c r="C158" s="21" t="s">
         <v>186</v>
       </c>
@@ -7898,8 +8054,8 @@
       <c r="F158" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="G158" s="71" t="s">
-        <v>307</v>
+      <c r="G158" s="70" t="s">
+        <v>305</v>
       </c>
       <c r="H158" s="11" t="s">
         <v>180</v>
@@ -7909,7 +8065,7 @@
       <c r="A159" s="19">
         <v>11</v>
       </c>
-      <c r="B159" s="123"/>
+      <c r="B159" s="108"/>
       <c r="C159" s="21" t="s">
         <v>187</v>
       </c>
@@ -7920,7 +8076,7 @@
         <v>169</v>
       </c>
       <c r="F159" s="21" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="G159" s="21" t="s">
         <v>171</v>
@@ -7930,10 +8086,10 @@
       </c>
     </row>
     <row r="160" spans="1:8">
-      <c r="A160" s="19">
+      <c r="A160" s="91">
         <v>12</v>
       </c>
-      <c r="B160" s="123"/>
+      <c r="B160" s="108"/>
       <c r="C160" s="21" t="s">
         <v>189</v>
       </c>
@@ -7951,11 +8107,11 @@
         <v>192</v>
       </c>
     </row>
-    <row r="161" spans="1:8">
-      <c r="A161" s="19">
+    <row r="161" spans="1:9">
+      <c r="A161" s="91">
         <v>13</v>
       </c>
-      <c r="B161" s="108"/>
+      <c r="B161" s="115"/>
       <c r="C161" s="21" t="s">
         <v>193</v>
       </c>
@@ -7975,11 +8131,11 @@
         <v>196</v>
       </c>
     </row>
-    <row r="162" spans="1:8">
-      <c r="A162" s="19">
+    <row r="162" spans="1:9">
+      <c r="A162" s="91">
         <v>14</v>
       </c>
-      <c r="B162" s="103" t="s">
+      <c r="B162" s="116" t="s">
         <v>5</v>
       </c>
       <c r="C162" s="21" t="s">
@@ -7997,87 +8153,91 @@
       <c r="G162" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="H162" s="11" t="s">
+      <c r="H162" s="69" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="163" spans="1:8">
-      <c r="A163" s="19">
+      <c r="I162" s="86"/>
+    </row>
+    <row r="163" spans="1:9">
+      <c r="A163" s="91">
         <v>15</v>
       </c>
-      <c r="B163" s="104"/>
-      <c r="C163" s="21" t="s">
+      <c r="B163" s="116"/>
+      <c r="C163" s="90" t="s">
+        <v>341</v>
+      </c>
+      <c r="D163" s="85" t="s">
+        <v>169</v>
+      </c>
+      <c r="E163" s="88" t="s">
+        <v>169</v>
+      </c>
+      <c r="F163" s="92" t="s">
+        <v>342</v>
+      </c>
+      <c r="G163" s="90" t="s">
+        <v>171</v>
+      </c>
+      <c r="H163" s="69" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9">
+      <c r="A164" s="91">
+        <v>16</v>
+      </c>
+      <c r="B164" s="116"/>
+      <c r="C164" s="90" t="s">
+        <v>344</v>
+      </c>
+      <c r="D164" s="88" t="s">
+        <v>169</v>
+      </c>
+      <c r="E164" s="88" t="s">
+        <v>169</v>
+      </c>
+      <c r="F164" s="92" t="s">
+        <v>343</v>
+      </c>
+      <c r="G164" s="90" t="s">
+        <v>171</v>
+      </c>
+      <c r="H164" s="69" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9">
+      <c r="A165" s="91">
+        <v>17</v>
+      </c>
+      <c r="B165" s="113"/>
+      <c r="C165" s="84" t="s">
         <v>200</v>
       </c>
-      <c r="D163" s="21" t="s">
+      <c r="D165" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="E163" s="21" t="s">
+      <c r="E165" s="88" t="s">
         <v>169</v>
       </c>
-      <c r="F163" s="21" t="s">
-        <v>200</v>
-      </c>
-      <c r="G163" s="21" t="s">
+      <c r="F165" s="92"/>
+      <c r="G165" s="90" t="s">
         <v>171</v>
       </c>
-      <c r="H163" s="11" t="s">
+      <c r="H165" s="69" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="164" spans="1:8">
-      <c r="A164" s="68">
-        <v>16</v>
-      </c>
-      <c r="B164" s="122" t="s">
+      <c r="I165" s="86"/>
+    </row>
+    <row r="166" spans="1:9">
+      <c r="A166" s="98">
+        <v>18</v>
+      </c>
+      <c r="B166" s="106" t="s">
         <v>6</v>
       </c>
-      <c r="C164" s="21" t="s">
+      <c r="C166" s="90" t="s">
         <v>202</v>
-      </c>
-      <c r="D164" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E164" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F164" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="G164" s="67" t="s">
-        <v>171</v>
-      </c>
-      <c r="H164" s="11"/>
-    </row>
-    <row r="165" spans="1:8">
-      <c r="A165" s="68">
-        <v>17</v>
-      </c>
-      <c r="B165" s="124"/>
-      <c r="C165" s="67" t="s">
-        <v>305</v>
-      </c>
-      <c r="D165" s="66" t="s">
-        <v>169</v>
-      </c>
-      <c r="E165" s="66" t="s">
-        <v>169</v>
-      </c>
-      <c r="F165" s="66"/>
-      <c r="G165" s="67" t="s">
-        <v>171</v>
-      </c>
-      <c r="H165" s="70" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="166" spans="1:8">
-      <c r="A166" s="68">
-        <v>18</v>
-      </c>
-      <c r="B166" s="108"/>
-      <c r="C166" s="63" t="s">
-        <v>204</v>
       </c>
       <c r="D166" s="21" t="s">
         <v>169</v>
@@ -8085,143 +8245,160 @@
       <c r="E166" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="F166" s="21"/>
-      <c r="G166" s="21" t="s">
-        <v>205</v>
-      </c>
-      <c r="H166" s="11"/>
-    </row>
-    <row r="167" spans="1:8">
-      <c r="A167" s="68">
+      <c r="F166" s="90" t="s">
+        <v>203</v>
+      </c>
+      <c r="G166" s="67" t="s">
+        <v>171</v>
+      </c>
+      <c r="H166" s="69" t="s">
+        <v>353</v>
+      </c>
+      <c r="I166" s="86"/>
+    </row>
+    <row r="167" spans="1:9">
+      <c r="A167" s="98">
         <v>19</v>
       </c>
-      <c r="B167" s="103" t="s">
-        <v>8</v>
-      </c>
-      <c r="C167" s="21" t="s">
-        <v>206</v>
-      </c>
-      <c r="D167" s="21" t="s">
+      <c r="B167" s="107"/>
+      <c r="C167" s="90" t="s">
+        <v>347</v>
+      </c>
+      <c r="D167" s="88" t="s">
         <v>169</v>
       </c>
-      <c r="E167" s="21" t="s">
+      <c r="E167" s="88" t="s">
         <v>169</v>
       </c>
-      <c r="F167" s="21" t="s">
-        <v>207</v>
-      </c>
-      <c r="G167" s="21" t="s">
-        <v>208</v>
-      </c>
-      <c r="H167" s="11"/>
-    </row>
-    <row r="168" spans="1:8">
-      <c r="A168" s="68">
+      <c r="F167" s="90" t="s">
+        <v>349</v>
+      </c>
+      <c r="G167" s="90" t="s">
+        <v>171</v>
+      </c>
+      <c r="H167" s="69" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9">
+      <c r="A168" s="98">
         <v>20</v>
       </c>
-      <c r="B168" s="104"/>
-      <c r="C168" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D168" s="21" t="s">
+      <c r="B168" s="107"/>
+      <c r="C168" s="90" t="s">
+        <v>348</v>
+      </c>
+      <c r="D168" s="88" t="s">
         <v>169</v>
       </c>
-      <c r="E168" s="21" t="s">
+      <c r="E168" s="88" t="s">
         <v>169</v>
       </c>
-      <c r="F168" s="21"/>
-      <c r="G168" s="21" t="s">
-        <v>208</v>
-      </c>
-      <c r="H168" s="11"/>
-    </row>
-    <row r="169" spans="1:8">
-      <c r="A169" s="68">
+      <c r="F168" s="90" t="s">
+        <v>350</v>
+      </c>
+      <c r="G168" s="90" t="s">
+        <v>171</v>
+      </c>
+      <c r="H168" s="101" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9">
+      <c r="A169" s="98">
         <v>21</v>
       </c>
-      <c r="B169" s="104"/>
-      <c r="C169" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="D169" s="21" t="s">
+      <c r="B169" s="107"/>
+      <c r="C169" s="90" t="s">
+        <v>369</v>
+      </c>
+      <c r="D169" s="88" t="s">
         <v>169</v>
       </c>
-      <c r="E169" s="21" t="s">
+      <c r="E169" s="88" t="s">
         <v>169</v>
       </c>
-      <c r="F169" s="21"/>
-      <c r="G169" s="21" t="s">
-        <v>208</v>
-      </c>
-      <c r="H169" s="11"/>
-    </row>
-    <row r="170" spans="1:8">
-      <c r="A170" s="68">
+      <c r="F169" s="90" t="s">
+        <v>350</v>
+      </c>
+      <c r="G169" s="90" t="s">
+        <v>171</v>
+      </c>
+      <c r="H169" s="69"/>
+    </row>
+    <row r="170" spans="1:9">
+      <c r="A170" s="98">
         <v>22</v>
       </c>
-      <c r="B170" s="104"/>
-      <c r="C170" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="D170" s="21" t="s">
+      <c r="B170" s="107"/>
+      <c r="C170" s="97" t="s">
+        <v>366</v>
+      </c>
+      <c r="D170" s="96"/>
+      <c r="E170" s="96" t="s">
         <v>169</v>
       </c>
-      <c r="E170" s="21" t="s">
+      <c r="F170" s="97" t="s">
+        <v>367</v>
+      </c>
+      <c r="G170" s="97" t="s">
+        <v>171</v>
+      </c>
+      <c r="H170" s="101" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9">
+      <c r="A171" s="98">
+        <v>23</v>
+      </c>
+      <c r="B171" s="107"/>
+      <c r="C171" s="93" t="s">
+        <v>364</v>
+      </c>
+      <c r="D171" s="94" t="s">
         <v>169</v>
       </c>
-      <c r="F170" s="21"/>
-      <c r="G170" s="21" t="s">
-        <v>208</v>
-      </c>
-      <c r="H170" s="11"/>
-    </row>
-    <row r="171" spans="1:8">
-      <c r="A171" s="68">
-        <v>23</v>
-      </c>
-      <c r="B171" s="104"/>
-      <c r="C171" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="D171" s="21" t="s">
+      <c r="E171" s="99"/>
+      <c r="F171" s="93" t="s">
+        <v>228</v>
+      </c>
+      <c r="G171" s="93" t="s">
+        <v>229</v>
+      </c>
+      <c r="H171" s="69" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9">
+      <c r="A172" s="98">
+        <v>24</v>
+      </c>
+      <c r="B172" s="107"/>
+      <c r="C172" s="67" t="s">
+        <v>304</v>
+      </c>
+      <c r="D172" s="66" t="s">
         <v>169</v>
       </c>
-      <c r="E171" s="21" t="s">
+      <c r="E172" s="66" t="s">
         <v>169</v>
       </c>
-      <c r="F171" s="21"/>
-      <c r="G171" s="21" t="s">
-        <v>208</v>
-      </c>
-      <c r="H171" s="11"/>
-    </row>
-    <row r="172" spans="1:8">
-      <c r="A172" s="68">
-        <v>24</v>
-      </c>
-      <c r="B172" s="104"/>
-      <c r="C172" s="21" t="s">
-        <v>213</v>
-      </c>
-      <c r="D172" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E172" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F172" s="21"/>
-      <c r="G172" s="21" t="s">
-        <v>208</v>
-      </c>
-      <c r="H172" s="11"/>
-    </row>
-    <row r="173" spans="1:8">
-      <c r="A173" s="68">
+      <c r="F172" s="66"/>
+      <c r="G172" s="67" t="s">
+        <v>171</v>
+      </c>
+      <c r="H172" s="69" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9">
+      <c r="A173" s="98">
         <v>25</v>
       </c>
-      <c r="B173" s="104"/>
-      <c r="C173" s="21" t="s">
-        <v>214</v>
+      <c r="B173" s="115"/>
+      <c r="C173" s="63" t="s">
+        <v>204</v>
       </c>
       <c r="D173" s="21" t="s">
         <v>169</v>
@@ -8231,17 +8408,19 @@
       </c>
       <c r="F173" s="21"/>
       <c r="G173" s="21" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H173" s="11"/>
     </row>
-    <row r="174" spans="1:8">
-      <c r="A174" s="81">
+    <row r="174" spans="1:9">
+      <c r="A174" s="98">
         <v>26</v>
       </c>
-      <c r="B174" s="104"/>
+      <c r="B174" s="116" t="s">
+        <v>8</v>
+      </c>
       <c r="C174" s="21" t="s">
-        <v>47</v>
+        <v>206</v>
       </c>
       <c r="D174" s="21" t="s">
         <v>169</v>
@@ -8249,21 +8428,23 @@
       <c r="E174" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="F174" s="21"/>
-      <c r="G174" s="21" t="s">
-        <v>208</v>
-      </c>
-      <c r="H174" s="11"/>
-    </row>
-    <row r="175" spans="1:8" ht="45">
-      <c r="A175" s="81">
+      <c r="F174" s="90" t="s">
+        <v>207</v>
+      </c>
+      <c r="G174" s="90" t="s">
+        <v>358</v>
+      </c>
+      <c r="H174" s="69" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9">
+      <c r="A175" s="98">
         <v>27</v>
       </c>
-      <c r="B175" s="103" t="s">
-        <v>9</v>
-      </c>
-      <c r="C175" s="21" t="s">
-        <v>215</v>
+      <c r="B175" s="113"/>
+      <c r="C175" s="90" t="s">
+        <v>354</v>
       </c>
       <c r="D175" s="21" t="s">
         <v>169</v>
@@ -8271,21 +8452,23 @@
       <c r="E175" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="F175" s="69" t="s">
-        <v>329</v>
-      </c>
-      <c r="G175" s="85" t="s">
-        <v>334</v>
-      </c>
-      <c r="H175" s="11"/>
-    </row>
-    <row r="176" spans="1:8">
-      <c r="A176" s="81">
+      <c r="F175" s="90" t="s">
+        <v>355</v>
+      </c>
+      <c r="G175" s="90" t="s">
+        <v>356</v>
+      </c>
+      <c r="H175" s="69" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9">
+      <c r="A176" s="98">
         <v>28</v>
       </c>
-      <c r="B176" s="104"/>
-      <c r="C176" s="63" t="s">
-        <v>216</v>
+      <c r="B176" s="113"/>
+      <c r="C176" s="90" t="s">
+        <v>209</v>
       </c>
       <c r="D176" s="21" t="s">
         <v>169</v>
@@ -8293,87 +8476,85 @@
       <c r="E176" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="F176" s="63" t="s">
-        <v>217</v>
-      </c>
-      <c r="G176" s="63" t="s">
-        <v>218</v>
+      <c r="F176" s="21"/>
+      <c r="G176" s="21" t="s">
+        <v>208</v>
       </c>
       <c r="H176" s="11"/>
     </row>
     <row r="177" spans="1:8">
-      <c r="A177" s="81">
+      <c r="A177" s="98">
         <v>29</v>
       </c>
-      <c r="B177" s="104"/>
-      <c r="C177" s="80" t="s">
-        <v>335</v>
-      </c>
-      <c r="D177" s="78" t="s">
+      <c r="B177" s="113"/>
+      <c r="C177" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="D177" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="E177" s="78" t="s">
+      <c r="E177" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="F177" s="80" t="s">
-        <v>217</v>
-      </c>
-      <c r="G177" s="80" t="s">
-        <v>336</v>
-      </c>
-      <c r="H177" s="11"/>
+      <c r="F177" s="21">
+        <v>20.03</v>
+      </c>
+      <c r="G177" s="90">
+        <v>20.03</v>
+      </c>
+      <c r="H177" s="69" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="178" spans="1:8">
-      <c r="A178" s="81">
+      <c r="A178" s="98">
         <v>30</v>
       </c>
-      <c r="B178" s="104"/>
-      <c r="C178" s="80" t="s">
-        <v>219</v>
-      </c>
-      <c r="D178" s="78" t="s">
+      <c r="B178" s="113"/>
+      <c r="C178" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="D178" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="E178" s="78" t="s">
+      <c r="E178" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="F178" s="80" t="s">
-        <v>330</v>
-      </c>
-      <c r="G178" s="80" t="s">
-        <v>330</v>
+      <c r="F178" s="21">
+        <v>20.04</v>
+      </c>
+      <c r="G178" s="21" t="s">
+        <v>208</v>
       </c>
       <c r="H178" s="11"/>
     </row>
     <row r="179" spans="1:8">
-      <c r="A179" s="81">
+      <c r="A179" s="98">
         <v>31</v>
       </c>
-      <c r="B179" s="104"/>
-      <c r="C179" s="80" t="s">
-        <v>332</v>
-      </c>
-      <c r="D179" s="78" t="s">
+      <c r="B179" s="113"/>
+      <c r="C179" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="D179" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="E179" s="78" t="s">
+      <c r="E179" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="F179" s="80">
-        <v>64</v>
-      </c>
-      <c r="G179" s="80" t="s">
-        <v>331</v>
+      <c r="F179" s="21"/>
+      <c r="G179" s="21" t="s">
+        <v>208</v>
       </c>
       <c r="H179" s="11"/>
     </row>
     <row r="180" spans="1:8">
-      <c r="A180" s="81">
+      <c r="A180" s="98">
         <v>32</v>
       </c>
-      <c r="B180" s="104"/>
-      <c r="C180" s="80" t="s">
-        <v>333</v>
+      <c r="B180" s="113"/>
+      <c r="C180" s="21" t="s">
+        <v>213</v>
       </c>
       <c r="D180" s="21" t="s">
         <v>169</v>
@@ -8381,23 +8562,19 @@
       <c r="E180" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="F180" s="21">
-        <v>7.9</v>
-      </c>
-      <c r="G180" s="80" t="s">
-        <v>337</v>
+      <c r="F180" s="21"/>
+      <c r="G180" s="21" t="s">
+        <v>208</v>
       </c>
       <c r="H180" s="11"/>
     </row>
     <row r="181" spans="1:8">
-      <c r="A181" s="81">
+      <c r="A181" s="98">
         <v>33</v>
       </c>
-      <c r="B181" s="122" t="s">
-        <v>10</v>
-      </c>
+      <c r="B181" s="113"/>
       <c r="C181" s="21" t="s">
-        <v>220</v>
+        <v>47</v>
       </c>
       <c r="D181" s="21" t="s">
         <v>169</v>
@@ -8405,1035 +8582,1223 @@
       <c r="E181" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="F181" s="21" t="s">
+      <c r="F181" s="21"/>
+      <c r="G181" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="H181" s="11"/>
+    </row>
+    <row r="182" spans="1:8" ht="45">
+      <c r="A182" s="98">
+        <v>34</v>
+      </c>
+      <c r="B182" s="116" t="s">
+        <v>9</v>
+      </c>
+      <c r="C182" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="D182" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E182" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F182" s="68" t="s">
+        <v>327</v>
+      </c>
+      <c r="G182" s="82" t="s">
+        <v>363</v>
+      </c>
+      <c r="H182" s="11"/>
+    </row>
+    <row r="183" spans="1:8">
+      <c r="A183" s="98">
+        <v>35</v>
+      </c>
+      <c r="B183" s="113"/>
+      <c r="C183" s="63" t="s">
+        <v>215</v>
+      </c>
+      <c r="D183" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E183" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F183" s="63" t="s">
+        <v>216</v>
+      </c>
+      <c r="G183" s="63" t="s">
+        <v>217</v>
+      </c>
+      <c r="H183" s="11"/>
+    </row>
+    <row r="184" spans="1:8">
+      <c r="A184" s="98">
+        <v>36</v>
+      </c>
+      <c r="B184" s="113"/>
+      <c r="C184" s="79" t="s">
+        <v>332</v>
+      </c>
+      <c r="D184" s="77" t="s">
+        <v>169</v>
+      </c>
+      <c r="E184" s="77" t="s">
+        <v>169</v>
+      </c>
+      <c r="F184" s="79" t="s">
+        <v>216</v>
+      </c>
+      <c r="G184" s="79" t="s">
+        <v>333</v>
+      </c>
+      <c r="H184" s="11"/>
+    </row>
+    <row r="185" spans="1:8">
+      <c r="A185" s="98">
+        <v>37</v>
+      </c>
+      <c r="B185" s="113"/>
+      <c r="C185" s="79" t="s">
+        <v>218</v>
+      </c>
+      <c r="D185" s="77" t="s">
+        <v>169</v>
+      </c>
+      <c r="E185" s="77" t="s">
+        <v>169</v>
+      </c>
+      <c r="F185" s="79" t="s">
+        <v>328</v>
+      </c>
+      <c r="G185" s="79" t="s">
+        <v>328</v>
+      </c>
+      <c r="H185" s="11"/>
+    </row>
+    <row r="186" spans="1:8">
+      <c r="A186" s="98">
+        <v>38</v>
+      </c>
+      <c r="B186" s="113"/>
+      <c r="C186" s="79" t="s">
+        <v>330</v>
+      </c>
+      <c r="D186" s="77" t="s">
+        <v>169</v>
+      </c>
+      <c r="E186" s="77" t="s">
+        <v>169</v>
+      </c>
+      <c r="F186" s="79">
+        <v>64</v>
+      </c>
+      <c r="G186" s="79" t="s">
+        <v>329</v>
+      </c>
+      <c r="H186" s="11"/>
+    </row>
+    <row r="187" spans="1:8">
+      <c r="A187" s="98">
+        <v>39</v>
+      </c>
+      <c r="B187" s="113"/>
+      <c r="C187" s="79" t="s">
+        <v>331</v>
+      </c>
+      <c r="D187" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E187" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F187" s="21">
+        <v>7.9</v>
+      </c>
+      <c r="G187" s="79" t="s">
+        <v>334</v>
+      </c>
+      <c r="H187" s="11"/>
+    </row>
+    <row r="188" spans="1:8">
+      <c r="A188" s="98">
+        <v>40</v>
+      </c>
+      <c r="B188" s="106" t="s">
+        <v>10</v>
+      </c>
+      <c r="C188" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="D188" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E188" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F188" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="G188" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="H188" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="G181" s="21" t="s">
+    </row>
+    <row r="189" spans="1:8">
+      <c r="A189" s="98">
+        <v>41</v>
+      </c>
+      <c r="B189" s="107"/>
+      <c r="C189" s="81" t="s">
+        <v>222</v>
+      </c>
+      <c r="D189" s="81" t="s">
+        <v>169</v>
+      </c>
+      <c r="E189" s="81" t="s">
+        <v>169</v>
+      </c>
+      <c r="F189" s="81" t="s">
+        <v>223</v>
+      </c>
+      <c r="G189" s="81" t="s">
         <v>171</v>
       </c>
-      <c r="H181" s="11" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="182" spans="1:8">
-      <c r="A182" s="22">
-        <v>34</v>
-      </c>
-      <c r="B182" s="124"/>
-      <c r="C182" s="84" t="s">
-        <v>223</v>
-      </c>
-      <c r="D182" s="84" t="s">
+      <c r="H189" s="25" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8">
+      <c r="A190" s="22">
+        <v>42</v>
+      </c>
+      <c r="B190" s="108"/>
+      <c r="C190" s="80" t="s">
+        <v>335</v>
+      </c>
+      <c r="D190" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="E182" s="84" t="s">
+      <c r="E190" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="F182" s="84" t="s">
+      <c r="F190" s="80" t="s">
+        <v>336</v>
+      </c>
+      <c r="G190" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="H190" s="23" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8">
+      <c r="A191" s="16">
+        <v>43</v>
+      </c>
+      <c r="B191" s="109" t="s">
+        <v>156</v>
+      </c>
+      <c r="C191" s="64" t="s">
         <v>224</v>
       </c>
-      <c r="G182" s="84" t="s">
-        <v>171</v>
-      </c>
-      <c r="H182" s="25" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="183" spans="1:8">
-      <c r="A183" s="22">
-        <v>35</v>
-      </c>
-      <c r="B183" s="123"/>
-      <c r="C183" s="83" t="s">
-        <v>338</v>
-      </c>
-      <c r="D183" s="20" t="s">
+      <c r="D191" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="E183" s="20" t="s">
+      <c r="E191" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="F183" s="83" t="s">
+      <c r="F191" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="G191" s="64" t="s">
+        <v>226</v>
+      </c>
+      <c r="H191" s="10"/>
+    </row>
+    <row r="192" spans="1:8">
+      <c r="A192" s="19">
+        <v>44</v>
+      </c>
+      <c r="B192" s="110"/>
+      <c r="C192" s="63" t="s">
+        <v>227</v>
+      </c>
+      <c r="D192" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E192" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F192" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="G192" s="65" t="s">
+        <v>229</v>
+      </c>
+      <c r="H192" s="11"/>
+    </row>
+    <row r="193" spans="1:8">
+      <c r="A193" s="95">
+        <v>45</v>
+      </c>
+      <c r="B193" s="111"/>
+      <c r="C193" s="65" t="s">
+        <v>230</v>
+      </c>
+      <c r="D193" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E193" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F193" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="G193" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="H193" s="23"/>
+    </row>
+    <row r="194" spans="1:8">
+      <c r="A194" s="98">
+        <v>46</v>
+      </c>
+      <c r="B194" s="111"/>
+      <c r="C194" s="65" t="s">
+        <v>231</v>
+      </c>
+      <c r="D194" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="E194" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="F194" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="G194" s="65" t="s">
+        <v>233</v>
+      </c>
+      <c r="H194" s="25"/>
+    </row>
+    <row r="195" spans="1:8">
+      <c r="A195" s="98">
+        <v>47</v>
+      </c>
+      <c r="B195" s="111"/>
+      <c r="C195" s="71" t="s">
+        <v>234</v>
+      </c>
+      <c r="D195" s="72" t="s">
+        <v>169</v>
+      </c>
+      <c r="E195" s="72" t="s">
+        <v>169</v>
+      </c>
+      <c r="F195" s="72"/>
+      <c r="G195" s="73" t="s">
+        <v>316</v>
+      </c>
+      <c r="H195" s="25"/>
+    </row>
+    <row r="196" spans="1:8">
+      <c r="A196" s="98">
+        <v>48</v>
+      </c>
+      <c r="B196" s="111"/>
+      <c r="C196" s="71" t="s">
+        <v>310</v>
+      </c>
+      <c r="D196" s="72" t="s">
+        <v>169</v>
+      </c>
+      <c r="E196" s="72"/>
+      <c r="F196" s="72" t="s">
+        <v>311</v>
+      </c>
+      <c r="G196" s="71" t="s">
+        <v>312</v>
+      </c>
+      <c r="H196" s="25" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8">
+      <c r="A197" s="26">
+        <v>49</v>
+      </c>
+      <c r="B197" s="112"/>
+      <c r="C197" s="27" t="s">
+        <v>314</v>
+      </c>
+      <c r="D197" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="E197" s="27"/>
+      <c r="F197" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="G197" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="H197" s="28" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8">
+      <c r="A198" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8">
+      <c r="B199" s="29" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8">
+      <c r="B200" s="86" t="s">
         <v>339</v>
       </c>
-      <c r="G183" s="20" t="s">
-        <v>171</v>
-      </c>
-      <c r="H183" s="23" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="184" spans="1:8">
-      <c r="A184" s="16">
-        <v>36</v>
-      </c>
-      <c r="B184" s="125" t="s">
-        <v>156</v>
-      </c>
-      <c r="C184" s="64" t="s">
-        <v>225</v>
-      </c>
-      <c r="D184" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="E184" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="F184" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="G184" s="64" t="s">
-        <v>227</v>
-      </c>
-      <c r="H184" s="10"/>
-    </row>
-    <row r="185" spans="1:8">
-      <c r="A185" s="19">
-        <v>37</v>
-      </c>
-      <c r="B185" s="126"/>
-      <c r="C185" s="63" t="s">
-        <v>228</v>
-      </c>
-      <c r="D185" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E185" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F185" s="21" t="s">
-        <v>229</v>
-      </c>
-      <c r="G185" s="65" t="s">
-        <v>230</v>
-      </c>
-      <c r="H185" s="11"/>
-    </row>
-    <row r="186" spans="1:8">
-      <c r="A186" s="82">
-        <v>38</v>
-      </c>
-      <c r="B186" s="127"/>
-      <c r="C186" s="65" t="s">
-        <v>231</v>
-      </c>
-      <c r="D186" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E186" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F186" s="21" t="s">
-        <v>229</v>
-      </c>
-      <c r="G186" s="20" t="s">
-        <v>230</v>
-      </c>
-      <c r="H186" s="23"/>
-    </row>
-    <row r="187" spans="1:8">
-      <c r="A187" s="82">
-        <v>39</v>
-      </c>
-      <c r="B187" s="127"/>
-      <c r="C187" s="65" t="s">
-        <v>232</v>
-      </c>
-      <c r="D187" s="24" t="s">
-        <v>169</v>
-      </c>
-      <c r="E187" s="24" t="s">
-        <v>169</v>
-      </c>
-      <c r="F187" s="24" t="s">
-        <v>233</v>
-      </c>
-      <c r="G187" s="65" t="s">
-        <v>234</v>
-      </c>
-      <c r="H187" s="25"/>
-    </row>
-    <row r="188" spans="1:8">
-      <c r="A188" s="82">
-        <v>40</v>
-      </c>
-      <c r="B188" s="127"/>
-      <c r="C188" s="72" t="s">
-        <v>235</v>
-      </c>
-      <c r="D188" s="73" t="s">
-        <v>169</v>
-      </c>
-      <c r="E188" s="73" t="s">
-        <v>169</v>
-      </c>
-      <c r="F188" s="73"/>
-      <c r="G188" s="74" t="s">
-        <v>318</v>
-      </c>
-      <c r="H188" s="25"/>
-    </row>
-    <row r="189" spans="1:8">
-      <c r="A189" s="82">
-        <v>41</v>
-      </c>
-      <c r="B189" s="127"/>
-      <c r="C189" s="72" t="s">
-        <v>312</v>
-      </c>
-      <c r="D189" s="73" t="s">
-        <v>169</v>
-      </c>
-      <c r="E189" s="73"/>
-      <c r="F189" s="73" t="s">
-        <v>313</v>
-      </c>
-      <c r="G189" s="72" t="s">
-        <v>314</v>
-      </c>
-      <c r="H189" s="25" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="190" spans="1:8">
-      <c r="A190" s="26">
-        <v>42</v>
-      </c>
-      <c r="B190" s="112"/>
-      <c r="C190" s="27" t="s">
-        <v>316</v>
-      </c>
-      <c r="D190" s="27" t="s">
-        <v>169</v>
-      </c>
-      <c r="E190" s="27"/>
-      <c r="F190" s="27" t="s">
-        <v>229</v>
-      </c>
-      <c r="G190" s="27" t="s">
-        <v>230</v>
-      </c>
-      <c r="H190" s="28" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="191" spans="1:8">
-      <c r="A191" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B191" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="192" spans="1:8">
-      <c r="B192" s="29" t="s">
+    </row>
+    <row r="201" spans="1:8">
+      <c r="B201" s="86" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8">
+      <c r="B202" s="100" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8">
+      <c r="B203" s="86" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7">
+      <c r="A213" s="1" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="193" spans="1:7">
-      <c r="B193" s="129" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="203" spans="1:7">
-      <c r="A203" s="1" t="s">
+      <c r="B213" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B203" s="1" t="s">
+    </row>
+    <row r="214" spans="1:7">
+      <c r="A214" s="4" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="204" spans="1:7">
-      <c r="A204" s="4" t="s">
+      <c r="B214" s="30" t="s">
         <v>241</v>
       </c>
-      <c r="B204" s="30" t="s">
+      <c r="C214" s="140" t="s">
         <v>242</v>
       </c>
-      <c r="C204" s="94" t="s">
+      <c r="D214" s="140"/>
+      <c r="E214" s="140"/>
+      <c r="F214" s="31" t="s">
         <v>243</v>
       </c>
-      <c r="D204" s="94"/>
-      <c r="E204" s="94"/>
-      <c r="F204" s="31" t="s">
+      <c r="G214" s="32" t="s">
         <v>244</v>
       </c>
-      <c r="G204" s="32" t="s">
+    </row>
+    <row r="215" spans="1:7">
+      <c r="A215" s="122" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="205" spans="1:7">
-      <c r="A205" s="120" t="s">
+      <c r="B215" s="113" t="s">
         <v>246</v>
       </c>
-      <c r="B205" s="104" t="s">
+      <c r="C215" s="141" t="s">
         <v>247</v>
       </c>
-      <c r="C205" s="95" t="s">
+      <c r="D215" s="142"/>
+      <c r="E215" s="142"/>
+      <c r="F215" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="D205" s="96"/>
-      <c r="E205" s="96"/>
-      <c r="F205" s="21" t="s">
+      <c r="G215" s="33" t="s">
         <v>249</v>
       </c>
-      <c r="G205" s="33" t="s">
+    </row>
+    <row r="216" spans="1:7">
+      <c r="A216" s="122"/>
+      <c r="B216" s="114"/>
+      <c r="C216" s="132" t="s">
+        <v>247</v>
+      </c>
+      <c r="D216" s="143"/>
+      <c r="E216" s="143"/>
+      <c r="F216" s="20" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="206" spans="1:7">
-      <c r="A206" s="120"/>
-      <c r="B206" s="128"/>
-      <c r="C206" s="97" t="s">
+      <c r="G216" s="34" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7">
+      <c r="A217" s="122"/>
+      <c r="B217" s="113" t="s">
+        <v>251</v>
+      </c>
+      <c r="C217" s="136" t="s">
+        <v>252</v>
+      </c>
+      <c r="D217" s="136"/>
+      <c r="E217" s="136"/>
+      <c r="F217" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="D206" s="98"/>
-      <c r="E206" s="98"/>
-      <c r="F206" s="20" t="s">
-        <v>251</v>
-      </c>
-      <c r="G206" s="34" t="s">
+      <c r="G217" s="33" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7">
+      <c r="A218" s="122"/>
+      <c r="B218" s="113"/>
+      <c r="C218" s="132" t="s">
+        <v>252</v>
+      </c>
+      <c r="D218" s="132"/>
+      <c r="E218" s="132"/>
+      <c r="F218" s="21" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="207" spans="1:7">
-      <c r="A207" s="120"/>
-      <c r="B207" s="104" t="s">
-        <v>252</v>
-      </c>
-      <c r="C207" s="99" t="s">
+      <c r="G218" s="33" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7">
+      <c r="A219" s="122"/>
+      <c r="B219" s="114" t="s">
         <v>253</v>
       </c>
-      <c r="D207" s="99"/>
-      <c r="E207" s="99"/>
-      <c r="F207" s="21" t="s">
+      <c r="C219" s="133" t="s">
+        <v>247</v>
+      </c>
+      <c r="D219" s="134"/>
+      <c r="E219" s="135"/>
+      <c r="F219" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="G219" s="33" t="s">
         <v>249</v>
       </c>
-      <c r="G207" s="33" t="s">
+    </row>
+    <row r="220" spans="1:7">
+      <c r="A220" s="122"/>
+      <c r="B220" s="115"/>
+      <c r="C220" s="133" t="s">
+        <v>247</v>
+      </c>
+      <c r="D220" s="134"/>
+      <c r="E220" s="135"/>
+      <c r="F220" s="21" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="208" spans="1:7">
-      <c r="A208" s="120"/>
-      <c r="B208" s="104"/>
-      <c r="C208" s="97" t="s">
-        <v>253</v>
-      </c>
-      <c r="D208" s="97"/>
-      <c r="E208" s="97"/>
-      <c r="F208" s="21" t="s">
-        <v>251</v>
-      </c>
-      <c r="G208" s="33" t="s">
+      <c r="G220" s="33" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7">
+      <c r="A221" s="122"/>
+      <c r="B221" s="113" t="s">
+        <v>254</v>
+      </c>
+      <c r="C221" s="136" t="s">
+        <v>255</v>
+      </c>
+      <c r="D221" s="136"/>
+      <c r="E221" s="136"/>
+      <c r="F221" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="G221" s="33" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7">
+      <c r="A222" s="122"/>
+      <c r="B222" s="113"/>
+      <c r="C222" s="136" t="s">
+        <v>255</v>
+      </c>
+      <c r="D222" s="136"/>
+      <c r="E222" s="136"/>
+      <c r="F222" s="21" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="209" spans="1:7">
-      <c r="A209" s="120"/>
-      <c r="B209" s="128" t="s">
-        <v>254</v>
-      </c>
-      <c r="C209" s="100" t="s">
+      <c r="G222" s="33" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7">
+      <c r="A223" s="122" t="s">
+        <v>256</v>
+      </c>
+      <c r="B223" s="113" t="s">
+        <v>257</v>
+      </c>
+      <c r="C223" s="116" t="s">
+        <v>258</v>
+      </c>
+      <c r="D223" s="113"/>
+      <c r="E223" s="113"/>
+      <c r="F223" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="D209" s="101"/>
-      <c r="E209" s="102"/>
-      <c r="F209" s="21" t="s">
+      <c r="G223" s="33" t="s">
         <v>249</v>
       </c>
-      <c r="G209" s="33" t="s">
+    </row>
+    <row r="224" spans="1:7">
+      <c r="A224" s="122"/>
+      <c r="B224" s="113"/>
+      <c r="C224" s="113" t="s">
+        <v>259</v>
+      </c>
+      <c r="D224" s="113"/>
+      <c r="E224" s="113"/>
+      <c r="F224" s="21" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="210" spans="1:7">
-      <c r="A210" s="120"/>
-      <c r="B210" s="108"/>
-      <c r="C210" s="100" t="s">
+      <c r="G224" s="33" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7">
+      <c r="A225" s="122"/>
+      <c r="B225" s="113" t="s">
+        <v>261</v>
+      </c>
+      <c r="C225" s="113" t="s">
+        <v>262</v>
+      </c>
+      <c r="D225" s="113"/>
+      <c r="E225" s="113"/>
+      <c r="F225" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="D210" s="101"/>
-      <c r="E210" s="102"/>
-      <c r="F210" s="21" t="s">
-        <v>251</v>
-      </c>
-      <c r="G210" s="33" t="s">
+      <c r="G225" s="33" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7">
+      <c r="A226" s="122"/>
+      <c r="B226" s="113"/>
+      <c r="C226" s="113" t="s">
+        <v>263</v>
+      </c>
+      <c r="D226" s="113"/>
+      <c r="E226" s="113"/>
+      <c r="F226" s="21" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="211" spans="1:7">
-      <c r="A211" s="120"/>
-      <c r="B211" s="104" t="s">
-        <v>255</v>
-      </c>
-      <c r="C211" s="99" t="s">
-        <v>256</v>
-      </c>
-      <c r="D211" s="99"/>
-      <c r="E211" s="99"/>
-      <c r="F211" s="21" t="s">
+      <c r="G226" s="33" t="s">
         <v>249</v>
       </c>
-      <c r="G211" s="33" t="s">
+    </row>
+    <row r="227" spans="1:7">
+      <c r="A227" s="122" t="s">
+        <v>264</v>
+      </c>
+      <c r="B227" s="113" t="s">
+        <v>265</v>
+      </c>
+      <c r="C227" s="116" t="s">
+        <v>266</v>
+      </c>
+      <c r="D227" s="113"/>
+      <c r="E227" s="113"/>
+      <c r="F227" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="G227" s="33" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7">
+      <c r="A228" s="122"/>
+      <c r="B228" s="113"/>
+      <c r="C228" s="113" t="s">
+        <v>267</v>
+      </c>
+      <c r="D228" s="113"/>
+      <c r="E228" s="113"/>
+      <c r="F228" s="21" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="212" spans="1:7">
-      <c r="A212" s="120"/>
-      <c r="B212" s="104"/>
-      <c r="C212" s="99" t="s">
-        <v>256</v>
-      </c>
-      <c r="D212" s="99"/>
-      <c r="E212" s="99"/>
-      <c r="F212" s="21" t="s">
-        <v>251</v>
-      </c>
-      <c r="G212" s="33" t="s">
+      <c r="G228" s="33" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7">
+      <c r="A229" s="122"/>
+      <c r="B229" s="113" t="s">
+        <v>268</v>
+      </c>
+      <c r="C229" s="116" t="s">
+        <v>269</v>
+      </c>
+      <c r="D229" s="113"/>
+      <c r="E229" s="113"/>
+      <c r="F229" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="G229" s="33" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7">
+      <c r="A230" s="123"/>
+      <c r="B230" s="124"/>
+      <c r="C230" s="124" t="s">
+        <v>270</v>
+      </c>
+      <c r="D230" s="124"/>
+      <c r="E230" s="124"/>
+      <c r="F230" s="27" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="213" spans="1:7">
-      <c r="A213" s="120" t="s">
-        <v>257</v>
-      </c>
-      <c r="B213" s="104" t="s">
-        <v>258</v>
-      </c>
-      <c r="C213" s="103" t="s">
-        <v>259</v>
-      </c>
-      <c r="D213" s="104"/>
-      <c r="E213" s="104"/>
-      <c r="F213" s="21" t="s">
+      <c r="G230" s="35" t="s">
         <v>249</v>
       </c>
-      <c r="G213" s="33" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="214" spans="1:7">
-      <c r="A214" s="120"/>
-      <c r="B214" s="104"/>
-      <c r="C214" s="104" t="s">
-        <v>260</v>
-      </c>
-      <c r="D214" s="104"/>
-      <c r="E214" s="104"/>
-      <c r="F214" s="21" t="s">
-        <v>251</v>
-      </c>
-      <c r="G214" s="33" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="215" spans="1:7">
-      <c r="A215" s="120"/>
-      <c r="B215" s="104" t="s">
-        <v>262</v>
-      </c>
-      <c r="C215" s="104" t="s">
-        <v>263</v>
-      </c>
-      <c r="D215" s="104"/>
-      <c r="E215" s="104"/>
-      <c r="F215" s="21" t="s">
+    </row>
+    <row r="231" spans="1:7">
+      <c r="A231" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C231" s="29"/>
+      <c r="D231" s="29"/>
+      <c r="E231" s="29"/>
+      <c r="F231" s="29"/>
+    </row>
+    <row r="232" spans="1:7">
+      <c r="C232" s="29"/>
+      <c r="D232" s="29"/>
+      <c r="E232" s="29"/>
+    </row>
+    <row r="233" spans="1:7">
+      <c r="C233" s="29"/>
+      <c r="D233" s="29"/>
+      <c r="E233" s="29"/>
+    </row>
+    <row r="234" spans="1:7">
+      <c r="A234" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C234" s="29"/>
+      <c r="D234" s="29"/>
+      <c r="E234" s="29"/>
+    </row>
+    <row r="235" spans="1:7">
+      <c r="A235" s="36" t="s">
+        <v>273</v>
+      </c>
+      <c r="B235" s="130" t="s">
+        <v>274</v>
+      </c>
+      <c r="C235" s="130"/>
+      <c r="D235" s="130"/>
+      <c r="E235" s="130"/>
+      <c r="F235" s="37" t="s">
+        <v>275</v>
+      </c>
+      <c r="G235" s="38" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7" ht="93" customHeight="1">
+      <c r="A236" s="39" t="s">
+        <v>277</v>
+      </c>
+      <c r="B236" s="131" t="s">
+        <v>278</v>
+      </c>
+      <c r="C236" s="115"/>
+      <c r="D236" s="115"/>
+      <c r="E236" s="115"/>
+      <c r="F236" s="40" t="s">
+        <v>154</v>
+      </c>
+      <c r="G236" s="41" t="s">
         <v>249</v>
       </c>
-      <c r="G215" s="33" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="216" spans="1:7">
-      <c r="A216" s="120"/>
-      <c r="B216" s="104"/>
-      <c r="C216" s="104" t="s">
-        <v>264</v>
-      </c>
-      <c r="D216" s="104"/>
-      <c r="E216" s="104"/>
-      <c r="F216" s="21" t="s">
-        <v>251</v>
-      </c>
-      <c r="G216" s="33" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="217" spans="1:7">
-      <c r="A217" s="120" t="s">
-        <v>265</v>
-      </c>
-      <c r="B217" s="104" t="s">
-        <v>266</v>
-      </c>
-      <c r="C217" s="103" t="s">
-        <v>267</v>
-      </c>
-      <c r="D217" s="104"/>
-      <c r="E217" s="104"/>
-      <c r="F217" s="21" t="s">
+    </row>
+    <row r="237" spans="1:7" ht="57" customHeight="1">
+      <c r="A237" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="B237" s="126" t="s">
+        <v>280</v>
+      </c>
+      <c r="C237" s="127"/>
+      <c r="D237" s="127"/>
+      <c r="E237" s="128"/>
+      <c r="F237" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="G217" s="33" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="218" spans="1:7">
-      <c r="A218" s="120"/>
-      <c r="B218" s="104"/>
-      <c r="C218" s="104" t="s">
-        <v>268</v>
-      </c>
-      <c r="D218" s="104"/>
-      <c r="E218" s="104"/>
-      <c r="F218" s="21" t="s">
-        <v>251</v>
-      </c>
-      <c r="G218" s="33" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="219" spans="1:7">
-      <c r="A219" s="120"/>
-      <c r="B219" s="104" t="s">
-        <v>269</v>
-      </c>
-      <c r="C219" s="103" t="s">
-        <v>270</v>
-      </c>
-      <c r="D219" s="104"/>
-      <c r="E219" s="104"/>
-      <c r="F219" s="21" t="s">
+      <c r="G237" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="G219" s="33" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="220" spans="1:7">
-      <c r="A220" s="121"/>
-      <c r="B220" s="105"/>
-      <c r="C220" s="105" t="s">
-        <v>271</v>
-      </c>
-      <c r="D220" s="105"/>
-      <c r="E220" s="105"/>
-      <c r="F220" s="27" t="s">
-        <v>251</v>
-      </c>
-      <c r="G220" s="35" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="221" spans="1:7">
-      <c r="A221" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="C221" s="29"/>
-      <c r="D221" s="29"/>
-      <c r="E221" s="29"/>
-      <c r="F221" s="29"/>
-    </row>
-    <row r="222" spans="1:7">
-      <c r="C222" s="29"/>
-      <c r="D222" s="29"/>
-      <c r="E222" s="29"/>
-    </row>
-    <row r="223" spans="1:7">
-      <c r="C223" s="29"/>
-      <c r="D223" s="29"/>
-      <c r="E223" s="29"/>
-    </row>
-    <row r="224" spans="1:7">
-      <c r="A224" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="C224" s="29"/>
-      <c r="D224" s="29"/>
-      <c r="E224" s="29"/>
-    </row>
-    <row r="225" spans="1:7">
-      <c r="A225" s="36" t="s">
+    </row>
+    <row r="238" spans="1:7" ht="57" customHeight="1">
+      <c r="A238" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="B238" s="126" t="s">
+        <v>282</v>
+      </c>
+      <c r="C238" s="127"/>
+      <c r="D238" s="127"/>
+      <c r="E238" s="128"/>
+      <c r="F238" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="G238" s="23" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" ht="69" customHeight="1">
+      <c r="A239" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="B239" s="112" t="s">
+        <v>284</v>
+      </c>
+      <c r="C239" s="124"/>
+      <c r="D239" s="124"/>
+      <c r="E239" s="124"/>
+      <c r="F239" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="G239" s="28" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7">
+      <c r="C240" s="42"/>
+    </row>
+    <row r="242" spans="1:7">
+      <c r="A242" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7">
+      <c r="A243" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B243" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="C243" s="43" t="s">
+        <v>287</v>
+      </c>
+      <c r="D243" s="44" t="s">
         <v>274</v>
       </c>
-      <c r="B225" s="106" t="s">
-        <v>275</v>
-      </c>
-      <c r="C225" s="106"/>
-      <c r="D225" s="106"/>
-      <c r="E225" s="106"/>
-      <c r="F225" s="37" t="s">
-        <v>276</v>
-      </c>
-      <c r="G225" s="38" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="226" spans="1:7" ht="93" customHeight="1">
-      <c r="A226" s="39" t="s">
-        <v>278</v>
-      </c>
-      <c r="B226" s="107" t="s">
-        <v>279</v>
-      </c>
-      <c r="C226" s="108"/>
-      <c r="D226" s="108"/>
-      <c r="E226" s="108"/>
-      <c r="F226" s="40" t="s">
-        <v>154</v>
-      </c>
-      <c r="G226" s="41" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="227" spans="1:7" ht="57" customHeight="1">
-      <c r="A227" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="B227" s="109" t="s">
-        <v>281</v>
-      </c>
-      <c r="C227" s="110"/>
-      <c r="D227" s="110"/>
-      <c r="E227" s="111"/>
-      <c r="F227" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="G227" s="11" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="228" spans="1:7" ht="57" customHeight="1">
-      <c r="A228" s="12" t="s">
-        <v>282</v>
-      </c>
-      <c r="B228" s="109" t="s">
-        <v>283</v>
-      </c>
-      <c r="C228" s="110"/>
-      <c r="D228" s="110"/>
-      <c r="E228" s="111"/>
-      <c r="F228" s="13" t="s">
-        <v>250</v>
-      </c>
-      <c r="G228" s="23" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="229" spans="1:7" ht="69" customHeight="1">
-      <c r="A229" s="14" t="s">
-        <v>284</v>
-      </c>
-      <c r="B229" s="112" t="s">
-        <v>285</v>
-      </c>
-      <c r="C229" s="105"/>
-      <c r="D229" s="105"/>
-      <c r="E229" s="105"/>
-      <c r="F229" s="15" t="s">
-        <v>250</v>
-      </c>
-      <c r="G229" s="28" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="230" spans="1:7">
-      <c r="C230" s="42"/>
-    </row>
-    <row r="232" spans="1:7">
-      <c r="A232" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="233" spans="1:7">
-      <c r="A233" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="B233" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="C233" s="43" t="s">
+      <c r="E243" s="44"/>
+      <c r="F243" s="45"/>
+      <c r="G243" s="32" t="s">
         <v>288</v>
       </c>
-      <c r="D233" s="44" t="s">
-        <v>275</v>
-      </c>
-      <c r="E233" s="44"/>
-      <c r="F233" s="45"/>
-      <c r="G233" s="32" t="s">
+    </row>
+    <row r="244" spans="1:7">
+      <c r="A244" s="46">
+        <v>42682</v>
+      </c>
+      <c r="B244" s="47">
+        <v>1.04</v>
+      </c>
+      <c r="C244" s="17" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="234" spans="1:7">
-      <c r="A234" s="46">
-        <v>42682</v>
-      </c>
-      <c r="B234" s="47">
-        <v>1.04</v>
-      </c>
-      <c r="C234" s="17" t="s">
+      <c r="D244" s="129" t="s">
         <v>290</v>
       </c>
-      <c r="D234" s="113" t="s">
+      <c r="E244" s="129"/>
+      <c r="F244" s="129"/>
+      <c r="G244" s="48"/>
+    </row>
+    <row r="245" spans="1:7">
+      <c r="A245" s="49">
+        <v>42692</v>
+      </c>
+      <c r="B245" s="50">
+        <v>1.05</v>
+      </c>
+      <c r="C245" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="D245" s="125" t="s">
         <v>291</v>
       </c>
-      <c r="E234" s="113"/>
-      <c r="F234" s="113"/>
-      <c r="G234" s="48"/>
-    </row>
-    <row r="235" spans="1:7">
-      <c r="A235" s="49">
-        <v>42692</v>
-      </c>
-      <c r="B235" s="50">
-        <v>1.05</v>
-      </c>
-      <c r="C235" s="21" t="s">
-        <v>290</v>
-      </c>
-      <c r="D235" s="114" t="s">
+      <c r="E245" s="125"/>
+      <c r="F245" s="125"/>
+      <c r="G245" s="33"/>
+    </row>
+    <row r="246" spans="1:7">
+      <c r="A246" s="49">
+        <v>42955</v>
+      </c>
+      <c r="B246" s="50">
+        <v>1.06</v>
+      </c>
+      <c r="C246" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="D246" s="125" t="s">
         <v>292</v>
       </c>
-      <c r="E235" s="114"/>
-      <c r="F235" s="114"/>
-      <c r="G235" s="33"/>
-    </row>
-    <row r="236" spans="1:7">
-      <c r="A236" s="49">
-        <v>42955</v>
-      </c>
-      <c r="B236" s="50">
-        <v>1.06</v>
-      </c>
-      <c r="C236" s="21" t="s">
-        <v>290</v>
-      </c>
-      <c r="D236" s="114" t="s">
+      <c r="E246" s="125"/>
+      <c r="F246" s="125"/>
+      <c r="G246" s="33"/>
+    </row>
+    <row r="247" spans="1:7">
+      <c r="A247" s="49">
+        <v>42991</v>
+      </c>
+      <c r="B247" s="50">
+        <v>1.07</v>
+      </c>
+      <c r="C247" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="D247" s="125" t="s">
         <v>293</v>
       </c>
-      <c r="E236" s="114"/>
-      <c r="F236" s="114"/>
-      <c r="G236" s="33"/>
-    </row>
-    <row r="237" spans="1:7">
-      <c r="A237" s="49">
-        <v>42991</v>
-      </c>
-      <c r="B237" s="50">
-        <v>1.07</v>
-      </c>
-      <c r="C237" s="21" t="s">
-        <v>290</v>
-      </c>
-      <c r="D237" s="114" t="s">
+      <c r="E247" s="125"/>
+      <c r="F247" s="125"/>
+      <c r="G247" s="33"/>
+    </row>
+    <row r="248" spans="1:7">
+      <c r="A248" s="49">
+        <v>43026</v>
+      </c>
+      <c r="B248" s="50">
+        <v>1.08</v>
+      </c>
+      <c r="C248" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="D248" s="125" t="s">
         <v>294</v>
       </c>
-      <c r="E237" s="114"/>
-      <c r="F237" s="114"/>
-      <c r="G237" s="33"/>
-    </row>
-    <row r="238" spans="1:7">
-      <c r="A238" s="49">
-        <v>43026</v>
-      </c>
-      <c r="B238" s="50">
-        <v>1.08</v>
-      </c>
-      <c r="C238" s="21" t="s">
-        <v>290</v>
-      </c>
-      <c r="D238" s="114" t="s">
+      <c r="E248" s="125"/>
+      <c r="F248" s="125"/>
+      <c r="G248" s="33"/>
+    </row>
+    <row r="249" spans="1:7">
+      <c r="A249" s="49">
+        <v>43069</v>
+      </c>
+      <c r="B249" s="50">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="C249" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="D249" s="125" t="s">
         <v>295</v>
       </c>
-      <c r="E238" s="114"/>
-      <c r="F238" s="114"/>
-      <c r="G238" s="33"/>
-    </row>
-    <row r="239" spans="1:7">
-      <c r="A239" s="49">
-        <v>43069</v>
-      </c>
-      <c r="B239" s="50">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="C239" s="21" t="s">
-        <v>290</v>
-      </c>
-      <c r="D239" s="114" t="s">
-        <v>296</v>
-      </c>
-      <c r="E239" s="114"/>
-      <c r="F239" s="114"/>
-      <c r="G239" s="33"/>
-    </row>
-    <row r="240" spans="1:7">
-      <c r="A240" s="51">
-        <v>43248</v>
-      </c>
-      <c r="B240" s="52">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C240" s="20" t="s">
-        <v>290</v>
-      </c>
-      <c r="D240" s="115" t="s">
-        <v>297</v>
-      </c>
-      <c r="E240" s="116"/>
-      <c r="F240" s="117"/>
-      <c r="G240" s="34"/>
-    </row>
-    <row r="241" spans="1:7">
-      <c r="A241" s="51">
-        <v>43339</v>
-      </c>
-      <c r="B241" s="52">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="C241" s="20" t="s">
-        <v>290</v>
-      </c>
-      <c r="D241" s="115" t="s">
-        <v>298</v>
-      </c>
-      <c r="E241" s="116"/>
-      <c r="F241" s="117"/>
-      <c r="G241" s="34"/>
-    </row>
-    <row r="242" spans="1:7">
-      <c r="A242" s="51">
-        <v>43542</v>
-      </c>
-      <c r="B242" s="52">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="C242" s="20" t="s">
-        <v>290</v>
-      </c>
-      <c r="D242" s="115" t="s">
-        <v>299</v>
-      </c>
-      <c r="E242" s="116"/>
-      <c r="F242" s="117"/>
-      <c r="G242" s="34"/>
-    </row>
-    <row r="243" spans="1:7">
-      <c r="A243" s="51">
-        <v>43599</v>
-      </c>
-      <c r="B243" s="52">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="C243" s="20" t="s">
-        <v>290</v>
-      </c>
-      <c r="D243" s="53" t="s">
-        <v>300</v>
-      </c>
-      <c r="E243" s="54"/>
-      <c r="F243" s="55"/>
-      <c r="G243" s="34"/>
-    </row>
-    <row r="244" spans="1:7">
-      <c r="A244" s="51">
-        <v>43643</v>
-      </c>
-      <c r="B244" s="52">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="C244" s="20" t="s">
-        <v>290</v>
-      </c>
-      <c r="D244" s="53" t="s">
-        <v>301</v>
-      </c>
-      <c r="E244" s="54"/>
-      <c r="F244" s="55"/>
-      <c r="G244" s="34"/>
-    </row>
-    <row r="245" spans="1:7">
-      <c r="A245" s="51">
-        <v>43894</v>
-      </c>
-      <c r="B245" s="52">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="C245" s="20" t="s">
-        <v>290</v>
-      </c>
-      <c r="D245" s="53" t="s">
-        <v>302</v>
-      </c>
-      <c r="E245" s="54"/>
-      <c r="F245" s="55"/>
-      <c r="G245" s="34"/>
-    </row>
-    <row r="246" spans="1:7">
-      <c r="A246" s="51">
-        <v>44017</v>
-      </c>
-      <c r="B246" s="52">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="C246" s="73" t="s">
-        <v>290</v>
-      </c>
-      <c r="D246" s="53" t="s">
-        <v>303</v>
-      </c>
-      <c r="E246" s="54"/>
-      <c r="F246" s="55"/>
-      <c r="G246" s="34"/>
-    </row>
-    <row r="247" spans="1:7">
-      <c r="A247" s="51">
-        <v>44118</v>
-      </c>
-      <c r="B247" s="52">
-        <v>1.17</v>
-      </c>
-      <c r="C247" s="75" t="s">
-        <v>290</v>
-      </c>
-      <c r="D247" s="53" t="s">
-        <v>319</v>
-      </c>
-      <c r="E247" s="54"/>
-      <c r="F247" s="55"/>
-      <c r="G247" s="34"/>
-    </row>
-    <row r="248" spans="1:7">
-      <c r="A248" s="51">
-        <v>44209</v>
-      </c>
-      <c r="B248" s="52">
-        <v>1.18</v>
-      </c>
-      <c r="C248" s="79" t="s">
-        <v>290</v>
-      </c>
-      <c r="D248" s="130" t="s">
-        <v>322</v>
-      </c>
-      <c r="E248" s="54"/>
-      <c r="F248" s="55"/>
-      <c r="G248" s="34"/>
-    </row>
-    <row r="249" spans="1:7">
-      <c r="A249" s="51">
-        <v>44258</v>
-      </c>
-      <c r="B249" s="52">
-        <v>1.19</v>
-      </c>
-      <c r="C249" s="84" t="s">
-        <v>290</v>
-      </c>
-      <c r="D249" s="53" t="s">
-        <v>328</v>
-      </c>
-      <c r="E249" s="54"/>
-      <c r="F249" s="55"/>
-      <c r="G249" s="34"/>
+      <c r="E249" s="125"/>
+      <c r="F249" s="125"/>
+      <c r="G249" s="33"/>
     </row>
     <row r="250" spans="1:7">
       <c r="A250" s="51">
+        <v>43248</v>
+      </c>
+      <c r="B250" s="52">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C250" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="D250" s="117" t="s">
+        <v>296</v>
+      </c>
+      <c r="E250" s="118"/>
+      <c r="F250" s="119"/>
+      <c r="G250" s="34"/>
+    </row>
+    <row r="251" spans="1:7">
+      <c r="A251" s="51">
+        <v>43339</v>
+      </c>
+      <c r="B251" s="52">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="C251" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="D251" s="117" t="s">
+        <v>297</v>
+      </c>
+      <c r="E251" s="118"/>
+      <c r="F251" s="119"/>
+      <c r="G251" s="34"/>
+    </row>
+    <row r="252" spans="1:7">
+      <c r="A252" s="51">
+        <v>43542</v>
+      </c>
+      <c r="B252" s="52">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="C252" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="D252" s="117" t="s">
+        <v>298</v>
+      </c>
+      <c r="E252" s="118"/>
+      <c r="F252" s="119"/>
+      <c r="G252" s="34"/>
+    </row>
+    <row r="253" spans="1:7">
+      <c r="A253" s="51">
+        <v>43599</v>
+      </c>
+      <c r="B253" s="52">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="C253" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="D253" s="53" t="s">
+        <v>299</v>
+      </c>
+      <c r="E253" s="54"/>
+      <c r="F253" s="55"/>
+      <c r="G253" s="34"/>
+    </row>
+    <row r="254" spans="1:7">
+      <c r="A254" s="51">
+        <v>43643</v>
+      </c>
+      <c r="B254" s="52">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="C254" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="D254" s="53" t="s">
+        <v>300</v>
+      </c>
+      <c r="E254" s="54"/>
+      <c r="F254" s="55"/>
+      <c r="G254" s="34"/>
+    </row>
+    <row r="255" spans="1:7">
+      <c r="A255" s="51">
+        <v>43894</v>
+      </c>
+      <c r="B255" s="52">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C255" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="D255" s="53" t="s">
+        <v>301</v>
+      </c>
+      <c r="E255" s="54"/>
+      <c r="F255" s="55"/>
+      <c r="G255" s="34"/>
+    </row>
+    <row r="256" spans="1:7">
+      <c r="A256" s="51">
+        <v>44017</v>
+      </c>
+      <c r="B256" s="52">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="C256" s="72" t="s">
+        <v>289</v>
+      </c>
+      <c r="D256" s="53" t="s">
+        <v>302</v>
+      </c>
+      <c r="E256" s="54"/>
+      <c r="F256" s="55"/>
+      <c r="G256" s="34"/>
+    </row>
+    <row r="257" spans="1:7">
+      <c r="A257" s="51">
+        <v>44118</v>
+      </c>
+      <c r="B257" s="52">
+        <v>1.17</v>
+      </c>
+      <c r="C257" s="74" t="s">
+        <v>289</v>
+      </c>
+      <c r="D257" s="53" t="s">
+        <v>317</v>
+      </c>
+      <c r="E257" s="54"/>
+      <c r="F257" s="55"/>
+      <c r="G257" s="34"/>
+    </row>
+    <row r="258" spans="1:7">
+      <c r="A258" s="51">
+        <v>44209</v>
+      </c>
+      <c r="B258" s="52">
+        <v>1.18</v>
+      </c>
+      <c r="C258" s="78" t="s">
+        <v>289</v>
+      </c>
+      <c r="D258" s="87" t="s">
+        <v>320</v>
+      </c>
+      <c r="E258" s="54"/>
+      <c r="F258" s="55"/>
+      <c r="G258" s="34"/>
+    </row>
+    <row r="259" spans="1:7">
+      <c r="A259" s="51">
+        <v>44258</v>
+      </c>
+      <c r="B259" s="52">
+        <v>1.19</v>
+      </c>
+      <c r="C259" s="81" t="s">
+        <v>289</v>
+      </c>
+      <c r="D259" s="53" t="s">
+        <v>326</v>
+      </c>
+      <c r="E259" s="54"/>
+      <c r="F259" s="55"/>
+      <c r="G259" s="34"/>
+    </row>
+    <row r="260" spans="1:7">
+      <c r="A260" s="51">
         <v>44357</v>
       </c>
-      <c r="B250" s="52">
+      <c r="B260" s="52">
         <v>1.2</v>
       </c>
-      <c r="C250" s="86" t="s">
-        <v>290</v>
-      </c>
-      <c r="D250" s="53" t="s">
+      <c r="C260" s="83" t="s">
+        <v>289</v>
+      </c>
+      <c r="D260" s="53" t="s">
+        <v>337</v>
+      </c>
+      <c r="E260" s="54"/>
+      <c r="F260" s="55"/>
+      <c r="G260" s="34"/>
+    </row>
+    <row r="261" spans="1:7">
+      <c r="A261" s="51">
+        <v>44487</v>
+      </c>
+      <c r="B261" s="52">
+        <v>1.21</v>
+      </c>
+      <c r="C261" s="89" t="s">
+        <v>289</v>
+      </c>
+      <c r="D261" s="53" t="s">
         <v>340</v>
       </c>
-      <c r="E250" s="54"/>
-      <c r="F250" s="55"/>
-      <c r="G250" s="34"/>
-    </row>
-    <row r="251" spans="1:7">
-      <c r="A251" s="56">
-        <v>44487</v>
-      </c>
-      <c r="B251" s="57">
-        <v>1.21</v>
-      </c>
-      <c r="C251" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="D251" s="118" t="s">
-        <v>343</v>
-      </c>
-      <c r="E251" s="119"/>
-      <c r="F251" s="119"/>
-      <c r="G251" s="35"/>
+      <c r="E261" s="54"/>
+      <c r="F261" s="55"/>
+      <c r="G261" s="34"/>
+    </row>
+    <row r="262" spans="1:7">
+      <c r="A262" s="56">
+        <v>44518</v>
+      </c>
+      <c r="B262" s="57">
+        <v>1.22</v>
+      </c>
+      <c r="C262" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="D262" s="120" t="s">
+        <v>361</v>
+      </c>
+      <c r="E262" s="121"/>
+      <c r="F262" s="121"/>
+      <c r="G262" s="35"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Y3CbQBUOESlDRywGeoG/3StrDbFnCkeqkNskZfEB2tOROsi5KmkcJgzaGARx/t71p+8XW8S30YXLCnas8V4vyw==" saltValue="Hjy+0Aja5MmvK1SBdUhEOA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="AvmlTycRJrHI13fCd7cIQ/Dn+gmrYpQp4XPuUL3WpjohH7V9juXOiFmcKPrSJmyrMBSvNI2gugBPkwXzH29RUQ==" saltValue="j8Is4R47FiVfYfWEOMDE5w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115" topLeftCell="A210">
-      <selection activeCell="C263" sqref="C263"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115" topLeftCell="A160">
+      <selection activeCell="E171" sqref="E171"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="51">
-    <mergeCell ref="B181:B183"/>
-    <mergeCell ref="B184:B190"/>
-    <mergeCell ref="B205:B206"/>
-    <mergeCell ref="B207:B208"/>
-    <mergeCell ref="B209:B210"/>
-    <mergeCell ref="B149:B161"/>
-    <mergeCell ref="B162:B163"/>
-    <mergeCell ref="B164:B166"/>
-    <mergeCell ref="B167:B174"/>
-    <mergeCell ref="B175:B180"/>
-    <mergeCell ref="D241:F241"/>
-    <mergeCell ref="D242:F242"/>
-    <mergeCell ref="D251:F251"/>
-    <mergeCell ref="A205:A212"/>
-    <mergeCell ref="A213:A216"/>
-    <mergeCell ref="A217:A220"/>
-    <mergeCell ref="B211:B212"/>
-    <mergeCell ref="B213:B214"/>
-    <mergeCell ref="B215:B216"/>
-    <mergeCell ref="B217:B218"/>
-    <mergeCell ref="B219:B220"/>
-    <mergeCell ref="D236:F236"/>
-    <mergeCell ref="D237:F237"/>
-    <mergeCell ref="D238:F238"/>
-    <mergeCell ref="D239:F239"/>
-    <mergeCell ref="D240:F240"/>
-    <mergeCell ref="B227:E227"/>
-    <mergeCell ref="B228:E228"/>
-    <mergeCell ref="B229:E229"/>
-    <mergeCell ref="D234:F234"/>
-    <mergeCell ref="D235:F235"/>
-    <mergeCell ref="C218:E218"/>
-    <mergeCell ref="C219:E219"/>
-    <mergeCell ref="C220:E220"/>
-    <mergeCell ref="B225:E225"/>
-    <mergeCell ref="B226:E226"/>
-    <mergeCell ref="C213:E213"/>
+    <mergeCell ref="F111:N111"/>
     <mergeCell ref="C214:E214"/>
     <mergeCell ref="C215:E215"/>
     <mergeCell ref="C216:E216"/>
     <mergeCell ref="C217:E217"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C209:E209"/>
-    <mergeCell ref="C210:E210"/>
-    <mergeCell ref="C211:E211"/>
-    <mergeCell ref="C212:E212"/>
-    <mergeCell ref="F111:N111"/>
-    <mergeCell ref="C204:E204"/>
-    <mergeCell ref="C205:E205"/>
-    <mergeCell ref="C206:E206"/>
-    <mergeCell ref="C207:E207"/>
+    <mergeCell ref="C218:E218"/>
+    <mergeCell ref="C219:E219"/>
+    <mergeCell ref="C220:E220"/>
+    <mergeCell ref="C221:E221"/>
+    <mergeCell ref="C222:E222"/>
+    <mergeCell ref="C223:E223"/>
+    <mergeCell ref="C224:E224"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C226:E226"/>
+    <mergeCell ref="C227:E227"/>
+    <mergeCell ref="C228:E228"/>
+    <mergeCell ref="C229:E229"/>
+    <mergeCell ref="C230:E230"/>
+    <mergeCell ref="B235:E235"/>
+    <mergeCell ref="B236:E236"/>
+    <mergeCell ref="B237:E237"/>
+    <mergeCell ref="B238:E238"/>
+    <mergeCell ref="B239:E239"/>
+    <mergeCell ref="D244:F244"/>
+    <mergeCell ref="D245:F245"/>
+    <mergeCell ref="D251:F251"/>
+    <mergeCell ref="D252:F252"/>
+    <mergeCell ref="D262:F262"/>
+    <mergeCell ref="A215:A222"/>
+    <mergeCell ref="A223:A226"/>
+    <mergeCell ref="A227:A230"/>
+    <mergeCell ref="B221:B222"/>
+    <mergeCell ref="B223:B224"/>
+    <mergeCell ref="B225:B226"/>
+    <mergeCell ref="B227:B228"/>
+    <mergeCell ref="B229:B230"/>
+    <mergeCell ref="D246:F246"/>
+    <mergeCell ref="D247:F247"/>
+    <mergeCell ref="D248:F248"/>
+    <mergeCell ref="D249:F249"/>
+    <mergeCell ref="D250:F250"/>
+    <mergeCell ref="B149:B161"/>
+    <mergeCell ref="B162:B165"/>
+    <mergeCell ref="B166:B173"/>
+    <mergeCell ref="B174:B181"/>
+    <mergeCell ref="B182:B187"/>
+    <mergeCell ref="B188:B190"/>
+    <mergeCell ref="B191:B197"/>
+    <mergeCell ref="B215:B216"/>
+    <mergeCell ref="B217:B218"/>
+    <mergeCell ref="B219:B220"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -9450,7 +9815,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -9459,11 +9824,11 @@
       <selection activeCell="D24" sqref="D24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>

</xml_diff>

<commit_message>
i397--estimate memory involved for task launch,2
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_example/standard_suite/diamond_regression.xlsx
+++ b/tmp_client/doc/TMP_example/standard_suite/diamond_regression.xlsx
@@ -5,12 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\repository\tmp_client\doc\TMP_example\standard_suite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="sXipEUe4ofmbJ/VNsEp+rzubWcfs6D2Dd011fah7XjWPwWDEMNPI+WgbTdHC9ocktcX0RezfEDwP38HjohLwAA==" workbookSaltValue="V2+JL2w8HFZBCHZgrfWRgg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13740" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
   </bookViews>
   <sheets>
     <sheet name="suite" sheetId="1" r:id="rId1"/>
@@ -26,15 +25,15 @@
   </definedNames>
   <calcPr calcId="144525"/>
   <customWorkbookViews>
-    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="3" showComments="commIndAndComment"/>
+    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="2391" yWindow="-9" windowWidth="2418" windowHeight="1318" activeSheetId="3" showComments="commIndAndComment"/>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
     <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="401">
   <si>
     <t>[suite_info]</t>
   </si>
@@ -1254,6 +1253,21 @@
   </si>
   <si>
     <t>System dynamic status(CPU, MEM, space) attribute update</t>
+  </si>
+  <si>
+    <t>1~16</t>
+  </si>
+  <si>
+    <t>1(G, default)</t>
+  </si>
+  <si>
+    <t>estimated memory usage for task case run</t>
+  </si>
+  <si>
+    <t>estimated memory usage info added for a test suite/case</t>
+  </si>
+  <si>
+    <t>est_mem</t>
   </si>
 </sst>
 </file>
@@ -1863,7 +1877,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5">
       <alignment vertical="center"/>
@@ -2130,16 +2144,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2159,9 +2167,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -2192,6 +2197,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="33" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2204,109 +2221,109 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -4636,13 +4653,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>212</xdr:row>
+      <xdr:row>213</xdr:row>
       <xdr:rowOff>140970</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>904875</xdr:colOff>
-      <xdr:row>220</xdr:row>
+      <xdr:row>221</xdr:row>
       <xdr:rowOff>102870</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4849,8 +4866,8 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{B3C8CCF3-8B87-4AA5-AD1F-3AFB2F27ABAD}">
-  <header guid="{B3C8CCF3-8B87-4AA5-AD1F-3AFB2F27ABAD}" dateTime="2021-11-29T17:47:55" maxSheetId="5" userName="Jason Wang" r:id="rId1">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{77E4B79D-4F2B-4D50-B486-0C91AC1CF622}">
+  <header guid="{77E4B79D-4F2B-4D50-B486-0C91AC1CF622}" dateTime="2021-12-29T10:58:06" maxSheetId="5" userName="Jason Wang" r:id="rId1">
     <sheetIdMap count="4">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -5159,11 +5176,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15" style="58" customWidth="1"/>
     <col min="2" max="2" width="28" style="58" customWidth="1"/>
@@ -5247,17 +5264,17 @@
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
     <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B41" sqref="B41"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait"/>
+    </customSheetView>
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+      <selection activeCell="B35" sqref="B35"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
     <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
       <selection activeCell="B4" sqref="B4"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait"/>
-    </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
-      <selection activeCell="B35" sqref="B35"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -5279,73 +5296,73 @@
       <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="58" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="58" customWidth="1"/>
     <col min="2" max="2" width="9" style="58" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" style="58" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="58" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" style="58" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="58" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" style="58" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" style="58" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" style="58" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="58" customWidth="1"/>
     <col min="7" max="7" width="24" style="58" customWidth="1"/>
     <col min="8" max="8" width="37" style="58" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="58" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" style="58" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" style="58" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" style="58" customWidth="1"/>
     <col min="11" max="11" width="12" style="58" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" style="59" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" style="59" customWidth="1"/>
+    <col min="12" max="12" width="9.5546875" style="59" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" style="59" customWidth="1"/>
     <col min="14" max="14" width="38" style="58" customWidth="1"/>
-    <col min="15" max="15" width="19.42578125" style="58" customWidth="1"/>
-    <col min="16" max="16" width="30.28515625" style="58" customWidth="1"/>
-    <col min="17" max="17" width="17.28515625" style="58" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" style="58" customWidth="1"/>
+    <col min="15" max="15" width="19.44140625" style="58" customWidth="1"/>
+    <col min="16" max="16" width="30.33203125" style="58" customWidth="1"/>
+    <col min="17" max="17" width="17.33203125" style="58" customWidth="1"/>
+    <col min="18" max="18" width="15.44140625" style="58" customWidth="1"/>
     <col min="19" max="19" width="13" style="58" customWidth="1"/>
-    <col min="20" max="21" width="9.7109375" style="58" customWidth="1"/>
-    <col min="22" max="22" width="9.42578125" style="58" customWidth="1"/>
+    <col min="20" max="21" width="9.6640625" style="58" customWidth="1"/>
+    <col min="22" max="22" width="9.44140625" style="58" customWidth="1"/>
     <col min="23" max="23" width="11" style="58" customWidth="1"/>
-    <col min="24" max="24" width="11.7109375" style="58" customWidth="1"/>
+    <col min="24" max="24" width="11.6640625" style="58" customWidth="1"/>
     <col min="25" max="30" width="9" style="58"/>
-    <col min="31" max="31" width="10.140625" style="58" customWidth="1"/>
+    <col min="31" max="31" width="10.109375" style="58" customWidth="1"/>
     <col min="32" max="16384" width="9" style="58"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" s="57" customFormat="1">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="113" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
-      <c r="M1" s="113"/>
-      <c r="N1" s="113"/>
-      <c r="O1" s="113"/>
-      <c r="P1" s="113"/>
-      <c r="Q1" s="113"/>
-      <c r="R1" s="113"/>
-      <c r="S1" s="113"/>
-      <c r="T1" s="113"/>
-      <c r="U1" s="113"/>
-      <c r="V1" s="113"/>
-      <c r="W1" s="113"/>
-      <c r="X1" s="114"/>
-      <c r="Y1" s="115" t="s">
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
+      <c r="L1" s="114"/>
+      <c r="M1" s="114"/>
+      <c r="N1" s="114"/>
+      <c r="O1" s="114"/>
+      <c r="P1" s="114"/>
+      <c r="Q1" s="114"/>
+      <c r="R1" s="114"/>
+      <c r="S1" s="114"/>
+      <c r="T1" s="114"/>
+      <c r="U1" s="114"/>
+      <c r="V1" s="114"/>
+      <c r="W1" s="114"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="116" t="s">
         <v>13</v>
       </c>
-      <c r="Z1" s="115"/>
-      <c r="AA1" s="115"/>
-      <c r="AB1" s="115"/>
-      <c r="AC1" s="115"/>
-      <c r="AD1" s="115"/>
-      <c r="AE1" s="115"/>
-      <c r="AF1" s="115"/>
+      <c r="Z1" s="116"/>
+      <c r="AA1" s="116"/>
+      <c r="AB1" s="116"/>
+      <c r="AC1" s="116"/>
+      <c r="AD1" s="116"/>
+      <c r="AE1" s="116"/>
+      <c r="AF1" s="116"/>
     </row>
     <row r="2" spans="1:32" s="57" customFormat="1">
       <c r="A2" s="60" t="s">
@@ -6873,16 +6890,16 @@
       <pageSetup paperSize="9" orientation="portrait"/>
       <autoFilter ref="A2:AF46"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen"/>
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="C23" sqref="C23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
       <autoFilter ref="A2:Y2"/>
     </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen"/>
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="H23" sqref="H23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
       <autoFilter ref="A2:Y2"/>
@@ -6968,24 +6985,24 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:N272"/>
+  <dimension ref="A1:N274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E199" sqref="E199"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D173" sqref="D173"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.88671875" style="1" customWidth="1"/>
     <col min="6" max="6" width="32" style="1" customWidth="1"/>
-    <col min="7" max="7" width="33.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="28.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="33.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="28.109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -6994,7 +7011,7 @@
         <v>133</v>
       </c>
       <c r="B1" s="2">
-        <v>1.23</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -7002,7 +7019,7 @@
         <v>29</v>
       </c>
       <c r="B2" s="3">
-        <v>44530</v>
+        <v>44559</v>
       </c>
     </row>
     <row r="107" spans="1:14" ht="12.75" customHeight="1"/>
@@ -7032,17 +7049,17 @@
       <c r="E111" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="F111" s="147" t="s">
+      <c r="F111" s="117" t="s">
         <v>140</v>
       </c>
-      <c r="G111" s="148"/>
-      <c r="H111" s="148"/>
-      <c r="I111" s="148"/>
-      <c r="J111" s="148"/>
-      <c r="K111" s="148"/>
-      <c r="L111" s="148"/>
-      <c r="M111" s="148"/>
-      <c r="N111" s="149"/>
+      <c r="G111" s="118"/>
+      <c r="H111" s="118"/>
+      <c r="I111" s="118"/>
+      <c r="J111" s="118"/>
+      <c r="K111" s="118"/>
+      <c r="L111" s="118"/>
+      <c r="M111" s="118"/>
+      <c r="N111" s="119"/>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="6" t="s">
@@ -7962,7 +7979,7 @@
       <c r="A149" s="19">
         <v>1</v>
       </c>
-      <c r="B149" s="116" t="s">
+      <c r="B149" s="148" t="s">
         <v>4</v>
       </c>
       <c r="C149" s="62" t="s">
@@ -7988,7 +8005,7 @@
       <c r="A150" s="19">
         <v>2</v>
       </c>
-      <c r="B150" s="118"/>
+      <c r="B150" s="149"/>
       <c r="C150" s="21" t="s">
         <v>173</v>
       </c>
@@ -8010,7 +8027,7 @@
       <c r="A151" s="19">
         <v>3</v>
       </c>
-      <c r="B151" s="118"/>
+      <c r="B151" s="149"/>
       <c r="C151" s="21" t="s">
         <v>18</v>
       </c>
@@ -8030,7 +8047,7 @@
       <c r="A152" s="19">
         <v>4</v>
       </c>
-      <c r="B152" s="118"/>
+      <c r="B152" s="149"/>
       <c r="C152" s="21" t="s">
         <v>175</v>
       </c>
@@ -8054,7 +8071,7 @@
       <c r="A153" s="19">
         <v>5</v>
       </c>
-      <c r="B153" s="118"/>
+      <c r="B153" s="149"/>
       <c r="C153" s="62" t="s">
         <v>177</v>
       </c>
@@ -8078,7 +8095,7 @@
       <c r="A154" s="19">
         <v>6</v>
       </c>
-      <c r="B154" s="118"/>
+      <c r="B154" s="149"/>
       <c r="C154" s="62" t="s">
         <v>181</v>
       </c>
@@ -8102,7 +8119,7 @@
       <c r="A155" s="19">
         <v>7</v>
       </c>
-      <c r="B155" s="118"/>
+      <c r="B155" s="149"/>
       <c r="C155" s="21" t="s">
         <v>183</v>
       </c>
@@ -8124,7 +8141,7 @@
       <c r="A156" s="19">
         <v>8</v>
       </c>
-      <c r="B156" s="118"/>
+      <c r="B156" s="149"/>
       <c r="C156" s="62" t="s">
         <v>184</v>
       </c>
@@ -8148,7 +8165,7 @@
       <c r="A157" s="19">
         <v>9</v>
       </c>
-      <c r="B157" s="118"/>
+      <c r="B157" s="149"/>
       <c r="C157" s="62" t="s">
         <v>185</v>
       </c>
@@ -8172,7 +8189,7 @@
       <c r="A158" s="19">
         <v>10</v>
       </c>
-      <c r="B158" s="118"/>
+      <c r="B158" s="149"/>
       <c r="C158" s="21" t="s">
         <v>186</v>
       </c>
@@ -8193,10 +8210,10 @@
       </c>
     </row>
     <row r="159" spans="1:8">
-      <c r="A159" s="19">
+      <c r="A159" s="112">
         <v>11</v>
       </c>
-      <c r="B159" s="118"/>
+      <c r="B159" s="149"/>
       <c r="C159" s="21" t="s">
         <v>187</v>
       </c>
@@ -8217,10 +8234,10 @@
       </c>
     </row>
     <row r="160" spans="1:8">
-      <c r="A160" s="90">
+      <c r="A160" s="112">
         <v>12</v>
       </c>
-      <c r="B160" s="118"/>
+      <c r="B160" s="149"/>
       <c r="C160" s="21" t="s">
         <v>189</v>
       </c>
@@ -8239,591 +8256,593 @@
       </c>
     </row>
     <row r="161" spans="1:9">
-      <c r="A161" s="90">
+      <c r="A161" s="112">
         <v>13</v>
       </c>
-      <c r="B161" s="125"/>
-      <c r="C161" s="21" t="s">
+      <c r="B161" s="149"/>
+      <c r="C161" s="111" t="s">
+        <v>400</v>
+      </c>
+      <c r="D161" s="109" t="s">
+        <v>169</v>
+      </c>
+      <c r="E161" s="109"/>
+      <c r="F161" s="111" t="s">
+        <v>397</v>
+      </c>
+      <c r="G161" s="111" t="s">
+        <v>396</v>
+      </c>
+      <c r="H161" s="68" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9">
+      <c r="A162" s="112">
+        <v>14</v>
+      </c>
+      <c r="B162" s="134"/>
+      <c r="C162" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="D161" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E161" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F161" s="21" t="s">
+      <c r="D162" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E162" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F162" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="G161" s="21" t="s">
+      <c r="G162" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="H161" s="11" t="s">
+      <c r="H162" s="11" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="162" spans="1:9">
-      <c r="A162" s="90">
-        <v>14</v>
-      </c>
-      <c r="B162" s="126" t="s">
+    <row r="163" spans="1:9">
+      <c r="A163" s="112">
+        <v>15</v>
+      </c>
+      <c r="B163" s="129" t="s">
         <v>5</v>
       </c>
-      <c r="C162" s="21" t="s">
+      <c r="C163" s="21" t="s">
         <v>197</v>
       </c>
-      <c r="D162" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E162" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F162" s="21" t="s">
+      <c r="D163" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E163" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F163" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="G162" s="21" t="s">
+      <c r="G163" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="H162" s="68" t="s">
+      <c r="H163" s="68" t="s">
         <v>199</v>
       </c>
-      <c r="I162" s="85"/>
-    </row>
-    <row r="163" spans="1:9">
-      <c r="A163" s="90">
-        <v>15</v>
-      </c>
-      <c r="B163" s="126"/>
-      <c r="C163" s="89" t="s">
+      <c r="I163" s="85"/>
+    </row>
+    <row r="164" spans="1:9">
+      <c r="A164" s="112">
+        <v>16</v>
+      </c>
+      <c r="B164" s="129"/>
+      <c r="C164" s="89" t="s">
         <v>341</v>
       </c>
-      <c r="D163" s="84" t="s">
-        <v>169</v>
-      </c>
-      <c r="E163" s="87" t="s">
-        <v>169</v>
-      </c>
-      <c r="F163" s="91" t="s">
+      <c r="D164" s="84" t="s">
+        <v>169</v>
+      </c>
+      <c r="E164" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="F164" s="90" t="s">
         <v>342</v>
-      </c>
-      <c r="G163" s="89" t="s">
-        <v>171</v>
-      </c>
-      <c r="H163" s="68" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="164" spans="1:9">
-      <c r="A164" s="90">
-        <v>16</v>
-      </c>
-      <c r="B164" s="126"/>
-      <c r="C164" s="89" t="s">
-        <v>344</v>
-      </c>
-      <c r="D164" s="87" t="s">
-        <v>169</v>
-      </c>
-      <c r="E164" s="87" t="s">
-        <v>169</v>
-      </c>
-      <c r="F164" s="91" t="s">
-        <v>343</v>
       </c>
       <c r="G164" s="89" t="s">
         <v>171</v>
       </c>
       <c r="H164" s="68" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9">
+      <c r="A165" s="112">
+        <v>17</v>
+      </c>
+      <c r="B165" s="129"/>
+      <c r="C165" s="89" t="s">
+        <v>344</v>
+      </c>
+      <c r="D165" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="E165" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="F165" s="90" t="s">
+        <v>343</v>
+      </c>
+      <c r="G165" s="89" t="s">
+        <v>171</v>
+      </c>
+      <c r="H165" s="68" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="165" spans="1:9">
-      <c r="A165" s="101">
-        <v>17</v>
-      </c>
-      <c r="B165" s="126"/>
-      <c r="C165" s="103" t="s">
+    <row r="166" spans="1:9">
+      <c r="A166" s="112">
+        <v>18</v>
+      </c>
+      <c r="B166" s="129"/>
+      <c r="C166" s="100" t="s">
         <v>377</v>
       </c>
-      <c r="D165" s="99" t="s">
-        <v>169</v>
-      </c>
-      <c r="E165" s="99" t="s">
-        <v>169</v>
-      </c>
-      <c r="F165" s="102">
+      <c r="D166" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="E166" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="F166" s="99">
         <v>0</v>
       </c>
-      <c r="G165" s="103" t="s">
+      <c r="G166" s="100" t="s">
         <v>380</v>
       </c>
-      <c r="H165" s="104" t="s">
+      <c r="H166" s="101" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="166" spans="1:9">
-      <c r="A166" s="101">
-        <v>18</v>
-      </c>
-      <c r="B166" s="126"/>
-      <c r="C166" s="103" t="s">
+    <row r="167" spans="1:9">
+      <c r="A167" s="112">
+        <v>19</v>
+      </c>
+      <c r="B167" s="129"/>
+      <c r="C167" s="100" t="s">
         <v>378</v>
       </c>
-      <c r="D166" s="99" t="s">
-        <v>169</v>
-      </c>
-      <c r="E166" s="99" t="s">
-        <v>169</v>
-      </c>
-      <c r="F166" s="102">
+      <c r="D167" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="E167" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="F167" s="99">
         <v>0</v>
       </c>
-      <c r="G166" s="103" t="s">
+      <c r="G167" s="100" t="s">
         <v>380</v>
       </c>
-      <c r="H166" s="104"/>
-    </row>
-    <row r="167" spans="1:9">
-      <c r="A167" s="101">
-        <v>19</v>
-      </c>
-      <c r="B167" s="126"/>
-      <c r="C167" s="103" t="s">
+      <c r="H167" s="101"/>
+    </row>
+    <row r="168" spans="1:9">
+      <c r="A168" s="112">
+        <v>20</v>
+      </c>
+      <c r="B168" s="129"/>
+      <c r="C168" s="100" t="s">
         <v>379</v>
       </c>
-      <c r="D167" s="99" t="s">
-        <v>169</v>
-      </c>
-      <c r="E167" s="99" t="s">
-        <v>169</v>
-      </c>
-      <c r="F167" s="102">
+      <c r="D168" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="E168" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="F168" s="99">
         <v>1</v>
       </c>
-      <c r="G167" s="103" t="s">
+      <c r="G168" s="100" t="s">
         <v>380</v>
       </c>
-      <c r="H167" s="68"/>
-    </row>
-    <row r="168" spans="1:9">
-      <c r="A168" s="101">
-        <v>20</v>
-      </c>
-      <c r="B168" s="123"/>
-      <c r="C168" s="83" t="s">
+      <c r="H168" s="68"/>
+    </row>
+    <row r="169" spans="1:9">
+      <c r="A169" s="112">
+        <v>21</v>
+      </c>
+      <c r="B169" s="130"/>
+      <c r="C169" s="83" t="s">
         <v>200</v>
       </c>
-      <c r="D168" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E168" s="87" t="s">
-        <v>169</v>
-      </c>
-      <c r="F168" s="91"/>
-      <c r="G168" s="89" t="s">
+      <c r="D169" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E169" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="F169" s="90"/>
+      <c r="G169" s="89" t="s">
         <v>171</v>
       </c>
-      <c r="H168" s="68" t="s">
+      <c r="H169" s="68" t="s">
         <v>201</v>
       </c>
-      <c r="I168" s="85"/>
-    </row>
-    <row r="169" spans="1:9">
-      <c r="A169" s="101">
-        <v>21</v>
-      </c>
-      <c r="B169" s="116" t="s">
+      <c r="I169" s="85"/>
+    </row>
+    <row r="170" spans="1:9">
+      <c r="A170" s="112">
+        <v>22</v>
+      </c>
+      <c r="B170" s="148" t="s">
         <v>6</v>
       </c>
-      <c r="C169" s="89" t="s">
+      <c r="C170" s="89" t="s">
         <v>202</v>
       </c>
-      <c r="D169" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E169" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F169" s="89" t="s">
+      <c r="D170" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E170" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F170" s="89" t="s">
         <v>203</v>
       </c>
-      <c r="G169" s="66" t="s">
+      <c r="G170" s="66" t="s">
         <v>171</v>
       </c>
-      <c r="H169" s="68" t="s">
+      <c r="H170" s="68" t="s">
         <v>353</v>
       </c>
-      <c r="I169" s="85"/>
-    </row>
-    <row r="170" spans="1:9">
-      <c r="A170" s="101">
-        <v>22</v>
-      </c>
-      <c r="B170" s="117"/>
-      <c r="C170" s="103" t="s">
+      <c r="I170" s="85"/>
+    </row>
+    <row r="171" spans="1:9">
+      <c r="A171" s="112">
+        <v>23</v>
+      </c>
+      <c r="B171" s="150"/>
+      <c r="C171" s="100" t="s">
         <v>347</v>
       </c>
-      <c r="D170" s="87" t="s">
-        <v>169</v>
-      </c>
-      <c r="E170" s="87" t="s">
-        <v>169</v>
-      </c>
-      <c r="F170" s="89" t="s">
+      <c r="D171" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="E171" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="F171" s="89" t="s">
         <v>349</v>
-      </c>
-      <c r="G170" s="89" t="s">
-        <v>171</v>
-      </c>
-      <c r="H170" s="68" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="171" spans="1:9">
-      <c r="A171" s="101">
-        <v>23</v>
-      </c>
-      <c r="B171" s="117"/>
-      <c r="C171" s="103" t="s">
-        <v>348</v>
-      </c>
-      <c r="D171" s="87" t="s">
-        <v>169</v>
-      </c>
-      <c r="E171" s="87" t="s">
-        <v>169</v>
-      </c>
-      <c r="F171" s="89" t="s">
-        <v>350</v>
       </c>
       <c r="G171" s="89" t="s">
         <v>171</v>
       </c>
-      <c r="H171" s="98" t="s">
+      <c r="H171" s="68" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9">
+      <c r="A172" s="112">
+        <v>24</v>
+      </c>
+      <c r="B172" s="150"/>
+      <c r="C172" s="100" t="s">
+        <v>348</v>
+      </c>
+      <c r="D172" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="E172" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="F172" s="89" t="s">
+        <v>350</v>
+      </c>
+      <c r="G172" s="89" t="s">
+        <v>171</v>
+      </c>
+      <c r="H172" s="96" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="172" spans="1:9">
-      <c r="A172" s="101">
-        <v>24</v>
-      </c>
-      <c r="B172" s="117"/>
-      <c r="C172" s="103" t="s">
+    <row r="173" spans="1:9">
+      <c r="A173" s="112">
+        <v>25</v>
+      </c>
+      <c r="B173" s="150"/>
+      <c r="C173" s="100" t="s">
         <v>382</v>
       </c>
-      <c r="D172" s="99" t="s">
-        <v>169</v>
-      </c>
-      <c r="E172" s="99" t="s">
-        <v>169</v>
-      </c>
-      <c r="F172" s="100" t="s">
+      <c r="D173" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="E173" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="F173" s="98" t="s">
         <v>350</v>
       </c>
-      <c r="G172" s="100" t="s">
+      <c r="G173" s="98" t="s">
         <v>171</v>
       </c>
-      <c r="H172" s="98"/>
-    </row>
-    <row r="173" spans="1:9">
-      <c r="A173" s="101">
-        <v>25</v>
-      </c>
-      <c r="B173" s="117"/>
-      <c r="C173" s="103" t="s">
+      <c r="H173" s="96"/>
+    </row>
+    <row r="174" spans="1:9">
+      <c r="A174" s="112">
+        <v>26</v>
+      </c>
+      <c r="B174" s="150"/>
+      <c r="C174" s="100" t="s">
         <v>369</v>
       </c>
-      <c r="D173" s="87" t="s">
-        <v>169</v>
-      </c>
-      <c r="E173" s="87" t="s">
-        <v>169</v>
-      </c>
-      <c r="F173" s="89" t="s">
+      <c r="D174" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="E174" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="F174" s="89" t="s">
         <v>350</v>
       </c>
-      <c r="G173" s="89" t="s">
+      <c r="G174" s="89" t="s">
         <v>171</v>
       </c>
-      <c r="H173" s="68"/>
-    </row>
-    <row r="174" spans="1:9">
-      <c r="A174" s="101">
-        <v>26</v>
-      </c>
-      <c r="B174" s="117"/>
-      <c r="C174" s="95" t="s">
+      <c r="H174" s="68"/>
+    </row>
+    <row r="175" spans="1:9">
+      <c r="A175" s="112">
+        <v>27</v>
+      </c>
+      <c r="B175" s="150"/>
+      <c r="C175" s="93" t="s">
         <v>366</v>
       </c>
-      <c r="D174" s="94"/>
-      <c r="E174" s="94" t="s">
-        <v>169</v>
-      </c>
-      <c r="F174" s="95" t="s">
+      <c r="D175" s="92"/>
+      <c r="E175" s="92" t="s">
+        <v>169</v>
+      </c>
+      <c r="F175" s="93" t="s">
         <v>367</v>
       </c>
-      <c r="G174" s="95" t="s">
+      <c r="G175" s="93" t="s">
         <v>171</v>
       </c>
-      <c r="H174" s="98" t="s">
+      <c r="H175" s="96" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="175" spans="1:9">
-      <c r="A175" s="101">
-        <v>27</v>
-      </c>
-      <c r="B175" s="117"/>
-      <c r="C175" s="105" t="s">
+    <row r="176" spans="1:9">
+      <c r="A176" s="112">
+        <v>28</v>
+      </c>
+      <c r="B176" s="150"/>
+      <c r="C176" s="102" t="s">
         <v>376</v>
       </c>
-      <c r="D175" s="99" t="s">
-        <v>169</v>
-      </c>
-      <c r="E175" s="99" t="s">
-        <v>169</v>
-      </c>
-      <c r="F175" s="105" t="s">
+      <c r="D176" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="E176" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="F176" s="102" t="s">
         <v>373</v>
       </c>
-      <c r="G175" s="111" t="s">
+      <c r="G176" s="108" t="s">
         <v>386</v>
       </c>
-      <c r="H175" s="98" t="s">
+      <c r="H176" s="96" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="176" spans="1:9">
-      <c r="A176" s="101">
-        <v>28</v>
-      </c>
-      <c r="B176" s="117"/>
-      <c r="C176" s="92" t="s">
+    <row r="177" spans="1:8">
+      <c r="A177" s="112">
+        <v>29</v>
+      </c>
+      <c r="B177" s="150"/>
+      <c r="C177" s="91" t="s">
         <v>364</v>
       </c>
-      <c r="D176" s="103" t="s">
-        <v>169</v>
-      </c>
-      <c r="E176" s="96"/>
-      <c r="F176" s="92" t="s">
+      <c r="D177" s="100" t="s">
+        <v>169</v>
+      </c>
+      <c r="E177" s="94"/>
+      <c r="F177" s="91" t="s">
         <v>228</v>
       </c>
-      <c r="G176" s="92" t="s">
+      <c r="G177" s="91" t="s">
         <v>229</v>
       </c>
-      <c r="H176" s="68" t="s">
+      <c r="H177" s="68" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="177" spans="1:8">
-      <c r="A177" s="101">
-        <v>29</v>
-      </c>
-      <c r="B177" s="117"/>
-      <c r="C177" s="103" t="s">
+    <row r="178" spans="1:8">
+      <c r="A178" s="112">
+        <v>30</v>
+      </c>
+      <c r="B178" s="150"/>
+      <c r="C178" s="100" t="s">
         <v>372</v>
       </c>
-      <c r="D177" s="103" t="s">
-        <v>169</v>
-      </c>
-      <c r="E177" s="103" t="s">
-        <v>169</v>
-      </c>
-      <c r="F177" s="105" t="s">
+      <c r="D178" s="100" t="s">
+        <v>169</v>
+      </c>
+      <c r="E178" s="100" t="s">
+        <v>169</v>
+      </c>
+      <c r="F178" s="102" t="s">
         <v>385</v>
       </c>
-      <c r="G177" s="105" t="s">
+      <c r="G178" s="102" t="s">
         <v>383</v>
       </c>
-      <c r="H177" s="106" t="s">
+      <c r="H178" s="103" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="178" spans="1:8">
-      <c r="A178" s="101">
-        <v>30</v>
-      </c>
-      <c r="B178" s="117"/>
-      <c r="C178" s="66" t="s">
+    <row r="179" spans="1:8">
+      <c r="A179" s="112">
+        <v>31</v>
+      </c>
+      <c r="B179" s="150"/>
+      <c r="C179" s="66" t="s">
         <v>304</v>
       </c>
-      <c r="D178" s="65" t="s">
-        <v>169</v>
-      </c>
-      <c r="E178" s="65" t="s">
-        <v>169</v>
-      </c>
-      <c r="F178" s="65"/>
-      <c r="G178" s="66" t="s">
+      <c r="D179" s="65" t="s">
+        <v>169</v>
+      </c>
+      <c r="E179" s="65" t="s">
+        <v>169</v>
+      </c>
+      <c r="F179" s="65"/>
+      <c r="G179" s="66" t="s">
         <v>171</v>
       </c>
-      <c r="H178" s="68" t="s">
+      <c r="H179" s="68" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="179" spans="1:8">
-      <c r="A179" s="101">
-        <v>31</v>
-      </c>
-      <c r="B179" s="125"/>
-      <c r="C179" s="62" t="s">
+    <row r="180" spans="1:8">
+      <c r="A180" s="112">
+        <v>32</v>
+      </c>
+      <c r="B180" s="134"/>
+      <c r="C180" s="62" t="s">
         <v>204</v>
       </c>
-      <c r="D179" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E179" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F179" s="21"/>
-      <c r="G179" s="21" t="s">
+      <c r="D180" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E180" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F180" s="21"/>
+      <c r="G180" s="21" t="s">
         <v>205</v>
       </c>
-      <c r="H179" s="11"/>
-    </row>
-    <row r="180" spans="1:8">
-      <c r="A180" s="101">
-        <v>32</v>
-      </c>
-      <c r="B180" s="126" t="s">
+      <c r="H180" s="11"/>
+    </row>
+    <row r="181" spans="1:8">
+      <c r="A181" s="112">
+        <v>33</v>
+      </c>
+      <c r="B181" s="129" t="s">
         <v>8</v>
       </c>
-      <c r="C180" s="21" t="s">
+      <c r="C181" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="D180" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E180" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F180" s="89" t="s">
+      <c r="D181" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E181" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F181" s="89" t="s">
         <v>207</v>
       </c>
-      <c r="G180" s="89" t="s">
+      <c r="G181" s="89" t="s">
         <v>358</v>
       </c>
-      <c r="H180" s="68" t="s">
+      <c r="H181" s="68" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="181" spans="1:8">
-      <c r="A181" s="101">
-        <v>33</v>
-      </c>
-      <c r="B181" s="123"/>
-      <c r="C181" s="89" t="s">
+    <row r="182" spans="1:8">
+      <c r="A182" s="112">
+        <v>34</v>
+      </c>
+      <c r="B182" s="130"/>
+      <c r="C182" s="89" t="s">
         <v>354</v>
       </c>
-      <c r="D181" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E181" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F181" s="89" t="s">
+      <c r="D182" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E182" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F182" s="89" t="s">
         <v>355</v>
       </c>
-      <c r="G181" s="103" t="s">
+      <c r="G182" s="100" t="s">
         <v>356</v>
       </c>
-      <c r="H181" s="68" t="s">
+      <c r="H182" s="68" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="182" spans="1:8">
-      <c r="A182" s="101">
-        <v>34</v>
-      </c>
-      <c r="B182" s="123"/>
-      <c r="C182" s="89" t="s">
+    <row r="183" spans="1:8">
+      <c r="A183" s="112">
+        <v>35</v>
+      </c>
+      <c r="B183" s="130"/>
+      <c r="C183" s="89" t="s">
         <v>209</v>
       </c>
-      <c r="D182" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E182" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F182" s="21"/>
-      <c r="G182" s="21" t="s">
+      <c r="D183" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E183" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F183" s="21"/>
+      <c r="G183" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="H182" s="11"/>
-    </row>
-    <row r="183" spans="1:8">
-      <c r="A183" s="101">
-        <v>35</v>
-      </c>
-      <c r="B183" s="123"/>
-      <c r="C183" s="21" t="s">
+      <c r="H183" s="11"/>
+    </row>
+    <row r="184" spans="1:8">
+      <c r="A184" s="112">
+        <v>36</v>
+      </c>
+      <c r="B184" s="130"/>
+      <c r="C184" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="D183" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E183" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F183" s="21">
+      <c r="D184" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E184" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F184" s="21">
         <v>20.03</v>
       </c>
-      <c r="G183" s="89">
+      <c r="G184" s="89">
         <v>20.03</v>
       </c>
-      <c r="H183" s="68" t="s">
+      <c r="H184" s="68" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="184" spans="1:8">
-      <c r="A184" s="101">
-        <v>36</v>
-      </c>
-      <c r="B184" s="123"/>
-      <c r="C184" s="21" t="s">
+    <row r="185" spans="1:8">
+      <c r="A185" s="112">
+        <v>37</v>
+      </c>
+      <c r="B185" s="130"/>
+      <c r="C185" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="D184" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E184" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F184" s="21">
+      <c r="D185" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E185" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F185" s="21">
         <v>20.04</v>
       </c>
-      <c r="G184" s="21" t="s">
-        <v>208</v>
-      </c>
-      <c r="H184" s="11"/>
-    </row>
-    <row r="185" spans="1:8">
-      <c r="A185" s="101">
-        <v>37</v>
-      </c>
-      <c r="B185" s="123"/>
-      <c r="C185" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="D185" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E185" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F185" s="21"/>
       <c r="G185" s="21" t="s">
         <v>208</v>
       </c>
       <c r="H185" s="11"/>
     </row>
     <row r="186" spans="1:8">
-      <c r="A186" s="101">
+      <c r="A186" s="112">
         <v>38</v>
       </c>
-      <c r="B186" s="123"/>
+      <c r="B186" s="130"/>
       <c r="C186" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D186" s="21" t="s">
         <v>169</v>
@@ -8838,12 +8857,12 @@
       <c r="H186" s="11"/>
     </row>
     <row r="187" spans="1:8">
-      <c r="A187" s="101">
+      <c r="A187" s="112">
         <v>39</v>
       </c>
-      <c r="B187" s="123"/>
+      <c r="B187" s="130"/>
       <c r="C187" s="21" t="s">
-        <v>47</v>
+        <v>213</v>
       </c>
       <c r="D187" s="21" t="s">
         <v>169</v>
@@ -8857,333 +8876,331 @@
       </c>
       <c r="H187" s="11"/>
     </row>
-    <row r="188" spans="1:8" ht="45">
-      <c r="A188" s="101">
+    <row r="188" spans="1:8">
+      <c r="A188" s="112">
         <v>40</v>
       </c>
-      <c r="B188" s="126" t="s">
+      <c r="B188" s="130"/>
+      <c r="C188" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D188" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E188" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F188" s="21"/>
+      <c r="G188" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="H188" s="11"/>
+    </row>
+    <row r="189" spans="1:8" ht="43.2">
+      <c r="A189" s="112">
+        <v>41</v>
+      </c>
+      <c r="B189" s="129" t="s">
         <v>9</v>
       </c>
-      <c r="C188" s="21" t="s">
+      <c r="C189" s="21" t="s">
         <v>214</v>
       </c>
-      <c r="D188" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E188" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F188" s="67" t="s">
+      <c r="D189" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E189" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F189" s="67" t="s">
         <v>327</v>
       </c>
-      <c r="G188" s="81" t="s">
+      <c r="G189" s="81" t="s">
         <v>363</v>
       </c>
-      <c r="H188" s="11"/>
-    </row>
-    <row r="189" spans="1:8">
-      <c r="A189" s="101">
-        <v>41</v>
-      </c>
-      <c r="B189" s="123"/>
-      <c r="C189" s="62" t="s">
+      <c r="H189" s="11"/>
+    </row>
+    <row r="190" spans="1:8">
+      <c r="A190" s="112">
+        <v>42</v>
+      </c>
+      <c r="B190" s="130"/>
+      <c r="C190" s="62" t="s">
         <v>215</v>
       </c>
-      <c r="D189" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E189" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F189" s="62" t="s">
+      <c r="D190" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E190" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F190" s="62" t="s">
         <v>216</v>
       </c>
-      <c r="G189" s="62" t="s">
+      <c r="G190" s="62" t="s">
         <v>217</v>
       </c>
-      <c r="H189" s="11"/>
-    </row>
-    <row r="190" spans="1:8">
-      <c r="A190" s="101">
-        <v>42</v>
-      </c>
-      <c r="B190" s="123"/>
-      <c r="C190" s="78" t="s">
+      <c r="H190" s="11"/>
+    </row>
+    <row r="191" spans="1:8">
+      <c r="A191" s="112">
+        <v>43</v>
+      </c>
+      <c r="B191" s="130"/>
+      <c r="C191" s="78" t="s">
         <v>332</v>
       </c>
-      <c r="D190" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="E190" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="F190" s="78" t="s">
+      <c r="D191" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="E191" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="F191" s="78" t="s">
         <v>216</v>
       </c>
-      <c r="G190" s="78" t="s">
+      <c r="G191" s="78" t="s">
         <v>333</v>
       </c>
-      <c r="H190" s="11"/>
-    </row>
-    <row r="191" spans="1:8">
-      <c r="A191" s="101">
-        <v>43</v>
-      </c>
-      <c r="B191" s="123"/>
-      <c r="C191" s="78" t="s">
+      <c r="H191" s="11"/>
+    </row>
+    <row r="192" spans="1:8">
+      <c r="A192" s="112">
+        <v>44</v>
+      </c>
+      <c r="B192" s="130"/>
+      <c r="C192" s="78" t="s">
         <v>218</v>
       </c>
-      <c r="D191" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="E191" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="F191" s="78" t="s">
+      <c r="D192" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="E192" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="F192" s="78" t="s">
         <v>328</v>
       </c>
-      <c r="G191" s="78" t="s">
+      <c r="G192" s="78" t="s">
         <v>328</v>
       </c>
-      <c r="H191" s="11"/>
-    </row>
-    <row r="192" spans="1:8">
-      <c r="A192" s="101">
-        <v>44</v>
-      </c>
-      <c r="B192" s="123"/>
-      <c r="C192" s="78" t="s">
+      <c r="H192" s="11"/>
+    </row>
+    <row r="193" spans="1:8">
+      <c r="A193" s="112">
+        <v>45</v>
+      </c>
+      <c r="B193" s="130"/>
+      <c r="C193" s="78" t="s">
         <v>330</v>
       </c>
-      <c r="D192" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="E192" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="F192" s="78">
+      <c r="D193" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="E193" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="F193" s="78">
         <v>64</v>
       </c>
-      <c r="G192" s="78" t="s">
+      <c r="G193" s="78" t="s">
         <v>329</v>
       </c>
-      <c r="H192" s="11"/>
-    </row>
-    <row r="193" spans="1:8">
-      <c r="A193" s="109">
-        <v>45</v>
-      </c>
-      <c r="B193" s="123"/>
-      <c r="C193" s="107" t="s">
+      <c r="H193" s="11"/>
+    </row>
+    <row r="194" spans="1:8">
+      <c r="A194" s="112">
+        <v>46</v>
+      </c>
+      <c r="B194" s="130"/>
+      <c r="C194" s="104" t="s">
         <v>331</v>
       </c>
-      <c r="D193" s="108" t="s">
-        <v>169</v>
-      </c>
-      <c r="E193" s="108" t="s">
-        <v>169</v>
-      </c>
-      <c r="F193" s="107">
+      <c r="D194" s="105" t="s">
+        <v>169</v>
+      </c>
+      <c r="E194" s="105" t="s">
+        <v>169</v>
+      </c>
+      <c r="F194" s="104">
         <v>7.9</v>
       </c>
-      <c r="G193" s="107" t="s">
+      <c r="G194" s="104" t="s">
         <v>334</v>
       </c>
-      <c r="H193" s="11"/>
-    </row>
-    <row r="194" spans="1:8">
-      <c r="A194" s="109">
-        <v>46</v>
-      </c>
-      <c r="B194" s="123"/>
-      <c r="C194" s="107" t="s">
+      <c r="H194" s="11"/>
+    </row>
+    <row r="195" spans="1:8">
+      <c r="A195" s="112">
+        <v>47</v>
+      </c>
+      <c r="B195" s="130"/>
+      <c r="C195" s="104" t="s">
         <v>387</v>
       </c>
-      <c r="D194" s="108" t="s">
-        <v>169</v>
-      </c>
-      <c r="E194" s="108"/>
-      <c r="F194" s="107">
+      <c r="D195" s="105" t="s">
+        <v>169</v>
+      </c>
+      <c r="E195" s="105"/>
+      <c r="F195" s="104">
         <v>50</v>
       </c>
-      <c r="G194" s="107" t="s">
+      <c r="G195" s="104" t="s">
         <v>390</v>
       </c>
-      <c r="H194" s="68" t="s">
+      <c r="H195" s="68" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="195" spans="1:8">
-      <c r="A195" s="109">
-        <v>47</v>
-      </c>
-      <c r="B195" s="123"/>
-      <c r="C195" s="107" t="s">
+    <row r="196" spans="1:8">
+      <c r="A196" s="112">
+        <v>48</v>
+      </c>
+      <c r="B196" s="130"/>
+      <c r="C196" s="104" t="s">
         <v>388</v>
       </c>
-      <c r="D195" s="108" t="s">
-        <v>169</v>
-      </c>
-      <c r="E195" s="108"/>
-      <c r="F195" s="107">
+      <c r="D196" s="105" t="s">
+        <v>169</v>
+      </c>
+      <c r="E196" s="105"/>
+      <c r="F196" s="104">
         <v>50</v>
       </c>
-      <c r="G195" s="107" t="s">
+      <c r="G196" s="104" t="s">
         <v>390</v>
       </c>
-      <c r="H195" s="68" t="s">
+      <c r="H196" s="68" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="196" spans="1:8">
-      <c r="A196" s="109">
-        <v>48</v>
-      </c>
-      <c r="B196" s="123"/>
-      <c r="C196" s="78" t="s">
+    <row r="197" spans="1:8">
+      <c r="A197" s="112">
+        <v>49</v>
+      </c>
+      <c r="B197" s="130"/>
+      <c r="C197" s="78" t="s">
         <v>389</v>
       </c>
-      <c r="D196" s="108" t="s">
-        <v>169</v>
-      </c>
-      <c r="E196" s="108"/>
-      <c r="F196" s="21">
+      <c r="D197" s="105" t="s">
+        <v>169</v>
+      </c>
+      <c r="E197" s="105"/>
+      <c r="F197" s="21">
         <v>10</v>
       </c>
-      <c r="G196" s="78" t="s">
+      <c r="G197" s="78" t="s">
         <v>391</v>
       </c>
-      <c r="H196" s="68" t="s">
+      <c r="H197" s="68" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="197" spans="1:8">
-      <c r="A197" s="109">
-        <v>49</v>
-      </c>
-      <c r="B197" s="116" t="s">
+    <row r="198" spans="1:8">
+      <c r="A198" s="112">
+        <v>50</v>
+      </c>
+      <c r="B198" s="148" t="s">
         <v>10</v>
       </c>
-      <c r="C197" s="21" t="s">
+      <c r="C198" s="21" t="s">
         <v>219</v>
       </c>
-      <c r="D197" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E197" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F197" s="21" t="s">
+      <c r="D198" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E198" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F198" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="G197" s="21" t="s">
+      <c r="G198" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="H197" s="11" t="s">
+      <c r="H198" s="11" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="198" spans="1:8">
-      <c r="A198" s="109">
-        <v>50</v>
-      </c>
-      <c r="B198" s="117"/>
-      <c r="C198" s="80" t="s">
+    <row r="199" spans="1:8">
+      <c r="A199" s="112">
+        <v>51</v>
+      </c>
+      <c r="B199" s="150"/>
+      <c r="C199" s="80" t="s">
         <v>222</v>
       </c>
-      <c r="D198" s="80" t="s">
-        <v>169</v>
-      </c>
-      <c r="E198" s="80" t="s">
-        <v>169</v>
-      </c>
-      <c r="F198" s="80" t="s">
+      <c r="D199" s="80" t="s">
+        <v>169</v>
+      </c>
+      <c r="E199" s="80" t="s">
+        <v>169</v>
+      </c>
+      <c r="F199" s="80" t="s">
         <v>223</v>
       </c>
-      <c r="G198" s="80" t="s">
+      <c r="G199" s="80" t="s">
         <v>171</v>
       </c>
-      <c r="H198" s="24" t="s">
+      <c r="H199" s="24" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="199" spans="1:8">
-      <c r="A199" s="109">
-        <v>51</v>
-      </c>
-      <c r="B199" s="118"/>
-      <c r="C199" s="79" t="s">
+    <row r="200" spans="1:8">
+      <c r="A200" s="106">
+        <v>52</v>
+      </c>
+      <c r="B200" s="149"/>
+      <c r="C200" s="79" t="s">
         <v>335</v>
       </c>
-      <c r="D199" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="E199" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="F199" s="79" t="s">
+      <c r="D200" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="E200" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="F200" s="79" t="s">
         <v>336</v>
       </c>
-      <c r="G199" s="20" t="s">
+      <c r="G200" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="H199" s="22" t="s">
+      <c r="H200" s="22" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="200" spans="1:8">
-      <c r="A200" s="16">
-        <v>52</v>
-      </c>
-      <c r="B200" s="119" t="s">
+    <row r="201" spans="1:8">
+      <c r="A201" s="16">
+        <v>53</v>
+      </c>
+      <c r="B201" s="151" t="s">
         <v>156</v>
       </c>
-      <c r="C200" s="63" t="s">
+      <c r="C201" s="63" t="s">
         <v>224</v>
       </c>
-      <c r="D200" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="E200" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="F200" s="17" t="s">
+      <c r="D201" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="E201" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="F201" s="17" t="s">
         <v>225</v>
       </c>
-      <c r="G200" s="63" t="s">
+      <c r="G201" s="63" t="s">
         <v>226</v>
       </c>
-      <c r="H200" s="10"/>
-    </row>
-    <row r="201" spans="1:8">
-      <c r="A201" s="19">
-        <v>53</v>
-      </c>
-      <c r="B201" s="120"/>
-      <c r="C201" s="62" t="s">
+      <c r="H201" s="10"/>
+    </row>
+    <row r="202" spans="1:8">
+      <c r="A202" s="19">
+        <v>54</v>
+      </c>
+      <c r="B202" s="152"/>
+      <c r="C202" s="62" t="s">
         <v>227</v>
-      </c>
-      <c r="D201" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E201" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F201" s="21" t="s">
-        <v>228</v>
-      </c>
-      <c r="G201" s="64" t="s">
-        <v>229</v>
-      </c>
-      <c r="H201" s="11"/>
-    </row>
-    <row r="202" spans="1:8">
-      <c r="A202" s="93">
-        <v>54</v>
-      </c>
-      <c r="B202" s="121"/>
-      <c r="C202" s="64" t="s">
-        <v>230</v>
       </c>
       <c r="D202" s="21" t="s">
         <v>169</v>
@@ -9194,432 +9211,449 @@
       <c r="F202" s="21" t="s">
         <v>228</v>
       </c>
-      <c r="G202" s="20" t="s">
+      <c r="G202" s="64" t="s">
         <v>229</v>
       </c>
-      <c r="H202" s="22"/>
+      <c r="H202" s="11"/>
     </row>
     <row r="203" spans="1:8">
-      <c r="A203" s="109">
+      <c r="A203" s="112">
         <v>55</v>
       </c>
-      <c r="B203" s="121"/>
+      <c r="B203" s="153"/>
       <c r="C203" s="64" t="s">
+        <v>230</v>
+      </c>
+      <c r="D203" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E203" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F203" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="G203" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="H203" s="22"/>
+    </row>
+    <row r="204" spans="1:8">
+      <c r="A204" s="112">
+        <v>56</v>
+      </c>
+      <c r="B204" s="153"/>
+      <c r="C204" s="64" t="s">
         <v>231</v>
       </c>
-      <c r="D203" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="E203" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="F203" s="23" t="s">
+      <c r="D204" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="E204" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="F204" s="23" t="s">
         <v>232</v>
       </c>
-      <c r="G203" s="64" t="s">
+      <c r="G204" s="64" t="s">
         <v>233</v>
       </c>
-      <c r="H203" s="24"/>
-    </row>
-    <row r="204" spans="1:8">
-      <c r="A204" s="109">
-        <v>56</v>
-      </c>
-      <c r="B204" s="121"/>
-      <c r="C204" s="70" t="s">
+      <c r="H204" s="24"/>
+    </row>
+    <row r="205" spans="1:8">
+      <c r="A205" s="112">
+        <v>57</v>
+      </c>
+      <c r="B205" s="153"/>
+      <c r="C205" s="70" t="s">
         <v>234</v>
       </c>
-      <c r="D204" s="71" t="s">
-        <v>169</v>
-      </c>
-      <c r="E204" s="71" t="s">
-        <v>169</v>
-      </c>
-      <c r="F204" s="71"/>
-      <c r="G204" s="72" t="s">
+      <c r="D205" s="71" t="s">
+        <v>169</v>
+      </c>
+      <c r="E205" s="71" t="s">
+        <v>169</v>
+      </c>
+      <c r="F205" s="71"/>
+      <c r="G205" s="72" t="s">
         <v>316</v>
       </c>
-      <c r="H204" s="24"/>
-    </row>
-    <row r="205" spans="1:8">
-      <c r="A205" s="109">
-        <v>57</v>
-      </c>
-      <c r="B205" s="121"/>
-      <c r="C205" s="70" t="s">
+      <c r="H205" s="24"/>
+    </row>
+    <row r="206" spans="1:8">
+      <c r="A206" s="112">
+        <v>58</v>
+      </c>
+      <c r="B206" s="153"/>
+      <c r="C206" s="70" t="s">
         <v>310</v>
       </c>
-      <c r="D205" s="71" t="s">
-        <v>169</v>
-      </c>
-      <c r="E205" s="71"/>
-      <c r="F205" s="71" t="s">
+      <c r="D206" s="71" t="s">
+        <v>169</v>
+      </c>
+      <c r="E206" s="71"/>
+      <c r="F206" s="71" t="s">
         <v>311</v>
       </c>
-      <c r="G205" s="70" t="s">
+      <c r="G206" s="70" t="s">
         <v>312</v>
       </c>
-      <c r="H205" s="24" t="s">
+      <c r="H206" s="24" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="206" spans="1:8">
-      <c r="A206" s="25">
-        <v>58</v>
-      </c>
-      <c r="B206" s="122"/>
-      <c r="C206" s="26" t="s">
+    <row r="207" spans="1:8">
+      <c r="A207" s="25">
+        <v>59</v>
+      </c>
+      <c r="B207" s="138"/>
+      <c r="C207" s="26" t="s">
         <v>314</v>
       </c>
-      <c r="D206" s="26" t="s">
-        <v>169</v>
-      </c>
-      <c r="E206" s="26"/>
-      <c r="F206" s="26" t="s">
+      <c r="D207" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="E207" s="26"/>
+      <c r="F207" s="26" t="s">
         <v>228</v>
       </c>
-      <c r="G206" s="26" t="s">
+      <c r="G207" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="H206" s="27" t="s">
+      <c r="H207" s="27" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="207" spans="1:8">
-      <c r="A207" s="1" t="s">
+    <row r="208" spans="1:8">
+      <c r="A208" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B207" s="1" t="s">
+      <c r="B208" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="208" spans="1:8">
-      <c r="B208" s="28" t="s">
+    <row r="209" spans="1:7">
+      <c r="B209" s="28" t="s">
         <v>237</v>
-      </c>
-    </row>
-    <row r="209" spans="1:7">
-      <c r="B209" s="85" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="210" spans="1:7">
       <c r="B210" s="85" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7">
+      <c r="B211" s="85" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="211" spans="1:7">
-      <c r="B211" s="97" t="s">
+    <row r="212" spans="1:7">
+      <c r="B212" s="95" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="212" spans="1:7">
-      <c r="B212" s="85" t="s">
+    <row r="213" spans="1:7">
+      <c r="B213" s="85" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="222" spans="1:7">
-      <c r="A222" s="1" t="s">
+    <row r="223" spans="1:7">
+      <c r="A223" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B222" s="1" t="s">
+      <c r="B223" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="223" spans="1:7">
-      <c r="A223" s="4" t="s">
+    <row r="224" spans="1:7">
+      <c r="A224" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="B223" s="29" t="s">
+      <c r="B224" s="29" t="s">
         <v>241</v>
       </c>
-      <c r="C223" s="150" t="s">
+      <c r="C224" s="120" t="s">
         <v>242</v>
       </c>
-      <c r="D223" s="150"/>
-      <c r="E223" s="150"/>
-      <c r="F223" s="30" t="s">
+      <c r="D224" s="120"/>
+      <c r="E224" s="120"/>
+      <c r="F224" s="30" t="s">
         <v>243</v>
       </c>
-      <c r="G223" s="31" t="s">
+      <c r="G224" s="31" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="224" spans="1:7">
-      <c r="A224" s="132" t="s">
+    <row r="225" spans="1:7">
+      <c r="A225" s="146" t="s">
         <v>245</v>
       </c>
-      <c r="B224" s="123" t="s">
+      <c r="B225" s="130" t="s">
         <v>246</v>
       </c>
-      <c r="C224" s="151" t="s">
+      <c r="C225" s="121" t="s">
         <v>247</v>
       </c>
-      <c r="D224" s="152"/>
-      <c r="E224" s="152"/>
-      <c r="F224" s="21" t="s">
+      <c r="D225" s="122"/>
+      <c r="E225" s="122"/>
+      <c r="F225" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="G224" s="32" t="s">
+      <c r="G225" s="32" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="225" spans="1:7">
-      <c r="A225" s="132"/>
-      <c r="B225" s="124"/>
-      <c r="C225" s="142" t="s">
+    <row r="226" spans="1:7">
+      <c r="A226" s="146"/>
+      <c r="B226" s="154"/>
+      <c r="C226" s="123" t="s">
         <v>247</v>
       </c>
-      <c r="D225" s="153"/>
-      <c r="E225" s="153"/>
-      <c r="F225" s="20" t="s">
+      <c r="D226" s="124"/>
+      <c r="E226" s="124"/>
+      <c r="F226" s="20" t="s">
         <v>250</v>
       </c>
-      <c r="G225" s="33" t="s">
+      <c r="G226" s="33" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="226" spans="1:7">
-      <c r="A226" s="132"/>
-      <c r="B226" s="123" t="s">
+    <row r="227" spans="1:7">
+      <c r="A227" s="146"/>
+      <c r="B227" s="130" t="s">
         <v>251</v>
       </c>
-      <c r="C226" s="146" t="s">
+      <c r="C227" s="125" t="s">
         <v>252</v>
       </c>
-      <c r="D226" s="146"/>
-      <c r="E226" s="146"/>
-      <c r="F226" s="21" t="s">
+      <c r="D227" s="125"/>
+      <c r="E227" s="125"/>
+      <c r="F227" s="21" t="s">
         <v>248</v>
-      </c>
-      <c r="G226" s="32" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="227" spans="1:7">
-      <c r="A227" s="132"/>
-      <c r="B227" s="123"/>
-      <c r="C227" s="142" t="s">
-        <v>252</v>
-      </c>
-      <c r="D227" s="142"/>
-      <c r="E227" s="142"/>
-      <c r="F227" s="21" t="s">
-        <v>250</v>
       </c>
       <c r="G227" s="32" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="228" spans="1:7">
-      <c r="A228" s="132"/>
-      <c r="B228" s="124" t="s">
-        <v>253</v>
-      </c>
-      <c r="C228" s="143" t="s">
-        <v>247</v>
-      </c>
-      <c r="D228" s="144"/>
-      <c r="E228" s="145"/>
+      <c r="A228" s="146"/>
+      <c r="B228" s="130"/>
+      <c r="C228" s="123" t="s">
+        <v>252</v>
+      </c>
+      <c r="D228" s="123"/>
+      <c r="E228" s="123"/>
       <c r="F228" s="21" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="G228" s="32" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="229" spans="1:7">
-      <c r="A229" s="132"/>
-      <c r="B229" s="125"/>
-      <c r="C229" s="143" t="s">
+      <c r="A229" s="146"/>
+      <c r="B229" s="154" t="s">
+        <v>253</v>
+      </c>
+      <c r="C229" s="126" t="s">
         <v>247</v>
       </c>
-      <c r="D229" s="144"/>
-      <c r="E229" s="145"/>
+      <c r="D229" s="127"/>
+      <c r="E229" s="128"/>
       <c r="F229" s="21" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G229" s="32" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="230" spans="1:7">
-      <c r="A230" s="132"/>
-      <c r="B230" s="123" t="s">
-        <v>254</v>
-      </c>
-      <c r="C230" s="146" t="s">
-        <v>255</v>
-      </c>
-      <c r="D230" s="146"/>
-      <c r="E230" s="146"/>
+      <c r="A230" s="146"/>
+      <c r="B230" s="134"/>
+      <c r="C230" s="126" t="s">
+        <v>247</v>
+      </c>
+      <c r="D230" s="127"/>
+      <c r="E230" s="128"/>
       <c r="F230" s="21" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="G230" s="32" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="231" spans="1:7">
-      <c r="A231" s="132"/>
-      <c r="B231" s="123"/>
-      <c r="C231" s="146" t="s">
+      <c r="A231" s="146"/>
+      <c r="B231" s="130" t="s">
+        <v>254</v>
+      </c>
+      <c r="C231" s="125" t="s">
         <v>255</v>
       </c>
-      <c r="D231" s="146"/>
-      <c r="E231" s="146"/>
+      <c r="D231" s="125"/>
+      <c r="E231" s="125"/>
       <c r="F231" s="21" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G231" s="32" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="232" spans="1:7">
-      <c r="A232" s="132" t="s">
-        <v>256</v>
-      </c>
-      <c r="B232" s="123" t="s">
-        <v>257</v>
-      </c>
-      <c r="C232" s="126" t="s">
-        <v>258</v>
-      </c>
-      <c r="D232" s="123"/>
-      <c r="E232" s="123"/>
+      <c r="A232" s="146"/>
+      <c r="B232" s="130"/>
+      <c r="C232" s="125" t="s">
+        <v>255</v>
+      </c>
+      <c r="D232" s="125"/>
+      <c r="E232" s="125"/>
       <c r="F232" s="21" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="G232" s="32" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="233" spans="1:7">
-      <c r="A233" s="132"/>
-      <c r="B233" s="123"/>
-      <c r="C233" s="123" t="s">
+      <c r="A233" s="146" t="s">
+        <v>256</v>
+      </c>
+      <c r="B233" s="130" t="s">
+        <v>257</v>
+      </c>
+      <c r="C233" s="129" t="s">
+        <v>258</v>
+      </c>
+      <c r="D233" s="130"/>
+      <c r="E233" s="130"/>
+      <c r="F233" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="G233" s="32" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7">
+      <c r="A234" s="146"/>
+      <c r="B234" s="130"/>
+      <c r="C234" s="130" t="s">
         <v>259</v>
       </c>
-      <c r="D233" s="123"/>
-      <c r="E233" s="123"/>
-      <c r="F233" s="21" t="s">
+      <c r="D234" s="130"/>
+      <c r="E234" s="130"/>
+      <c r="F234" s="21" t="s">
         <v>250</v>
       </c>
-      <c r="G233" s="32" t="s">
+      <c r="G234" s="32" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="234" spans="1:7">
-      <c r="A234" s="132"/>
-      <c r="B234" s="123" t="s">
+    <row r="235" spans="1:7">
+      <c r="A235" s="146"/>
+      <c r="B235" s="130" t="s">
         <v>261</v>
       </c>
-      <c r="C234" s="123" t="s">
+      <c r="C235" s="130" t="s">
         <v>262</v>
       </c>
-      <c r="D234" s="123"/>
-      <c r="E234" s="123"/>
-      <c r="F234" s="21" t="s">
+      <c r="D235" s="130"/>
+      <c r="E235" s="130"/>
+      <c r="F235" s="21" t="s">
         <v>248</v>
-      </c>
-      <c r="G234" s="32" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="235" spans="1:7">
-      <c r="A235" s="132"/>
-      <c r="B235" s="123"/>
-      <c r="C235" s="123" t="s">
-        <v>263</v>
-      </c>
-      <c r="D235" s="123"/>
-      <c r="E235" s="123"/>
-      <c r="F235" s="21" t="s">
-        <v>250</v>
       </c>
       <c r="G235" s="32" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="236" spans="1:7">
-      <c r="A236" s="132" t="s">
-        <v>264</v>
-      </c>
-      <c r="B236" s="123" t="s">
-        <v>265</v>
-      </c>
-      <c r="C236" s="126" t="s">
-        <v>266</v>
-      </c>
-      <c r="D236" s="123"/>
-      <c r="E236" s="123"/>
+      <c r="A236" s="146"/>
+      <c r="B236" s="130"/>
+      <c r="C236" s="130" t="s">
+        <v>263</v>
+      </c>
+      <c r="D236" s="130"/>
+      <c r="E236" s="130"/>
       <c r="F236" s="21" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="G236" s="32" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="237" spans="1:7">
-      <c r="A237" s="132"/>
-      <c r="B237" s="123"/>
-      <c r="C237" s="123" t="s">
-        <v>267</v>
-      </c>
-      <c r="D237" s="123"/>
-      <c r="E237" s="123"/>
+      <c r="A237" s="146" t="s">
+        <v>264</v>
+      </c>
+      <c r="B237" s="130" t="s">
+        <v>265</v>
+      </c>
+      <c r="C237" s="129" t="s">
+        <v>266</v>
+      </c>
+      <c r="D237" s="130"/>
+      <c r="E237" s="130"/>
       <c r="F237" s="21" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G237" s="32" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="238" spans="1:7">
-      <c r="A238" s="132"/>
-      <c r="B238" s="123" t="s">
-        <v>268</v>
-      </c>
-      <c r="C238" s="126" t="s">
-        <v>269</v>
-      </c>
-      <c r="D238" s="123"/>
-      <c r="E238" s="123"/>
+      <c r="A238" s="146"/>
+      <c r="B238" s="130"/>
+      <c r="C238" s="130" t="s">
+        <v>267</v>
+      </c>
+      <c r="D238" s="130"/>
+      <c r="E238" s="130"/>
       <c r="F238" s="21" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="G238" s="32" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="239" spans="1:7">
-      <c r="A239" s="133"/>
-      <c r="B239" s="134"/>
-      <c r="C239" s="134" t="s">
+      <c r="A239" s="146"/>
+      <c r="B239" s="130" t="s">
+        <v>268</v>
+      </c>
+      <c r="C239" s="129" t="s">
+        <v>269</v>
+      </c>
+      <c r="D239" s="130"/>
+      <c r="E239" s="130"/>
+      <c r="F239" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="G239" s="32" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7">
+      <c r="A240" s="147"/>
+      <c r="B240" s="131"/>
+      <c r="C240" s="131" t="s">
         <v>270</v>
       </c>
-      <c r="D239" s="134"/>
-      <c r="E239" s="134"/>
-      <c r="F239" s="26" t="s">
+      <c r="D240" s="131"/>
+      <c r="E240" s="131"/>
+      <c r="F240" s="26" t="s">
         <v>250</v>
       </c>
-      <c r="G239" s="34" t="s">
+      <c r="G240" s="34" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="240" spans="1:7">
-      <c r="A240" s="1" t="s">
+    <row r="241" spans="1:7">
+      <c r="A241" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="C240" s="28"/>
-      <c r="D240" s="28"/>
-      <c r="E240" s="28"/>
-      <c r="F240" s="28"/>
-    </row>
-    <row r="241" spans="1:7">
       <c r="C241" s="28"/>
       <c r="D241" s="28"/>
       <c r="E241" s="28"/>
+      <c r="F241" s="28"/>
     </row>
     <row r="242" spans="1:7">
       <c r="C242" s="28"/>
@@ -9627,307 +9661,295 @@
       <c r="E242" s="28"/>
     </row>
     <row r="243" spans="1:7">
-      <c r="A243" s="1" t="s">
-        <v>272</v>
-      </c>
       <c r="C243" s="28"/>
       <c r="D243" s="28"/>
       <c r="E243" s="28"/>
     </row>
     <row r="244" spans="1:7">
-      <c r="A244" s="35" t="s">
+      <c r="A244" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C244" s="28"/>
+      <c r="D244" s="28"/>
+      <c r="E244" s="28"/>
+    </row>
+    <row r="245" spans="1:7">
+      <c r="A245" s="35" t="s">
         <v>273</v>
       </c>
-      <c r="B244" s="140" t="s">
+      <c r="B245" s="132" t="s">
         <v>274</v>
       </c>
-      <c r="C244" s="140"/>
-      <c r="D244" s="140"/>
-      <c r="E244" s="140"/>
-      <c r="F244" s="36" t="s">
+      <c r="C245" s="132"/>
+      <c r="D245" s="132"/>
+      <c r="E245" s="132"/>
+      <c r="F245" s="36" t="s">
         <v>275</v>
       </c>
-      <c r="G244" s="37" t="s">
+      <c r="G245" s="37" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="245" spans="1:7" ht="93" customHeight="1">
-      <c r="A245" s="38" t="s">
+    <row r="246" spans="1:7" ht="93" customHeight="1">
+      <c r="A246" s="38" t="s">
         <v>277</v>
       </c>
-      <c r="B245" s="141" t="s">
+      <c r="B246" s="133" t="s">
         <v>278</v>
       </c>
-      <c r="C245" s="125"/>
-      <c r="D245" s="125"/>
-      <c r="E245" s="125"/>
-      <c r="F245" s="39" t="s">
+      <c r="C246" s="134"/>
+      <c r="D246" s="134"/>
+      <c r="E246" s="134"/>
+      <c r="F246" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="G245" s="40" t="s">
+      <c r="G246" s="40" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="246" spans="1:7" ht="57" customHeight="1">
-      <c r="A246" s="8" t="s">
+    <row r="247" spans="1:7" ht="57" customHeight="1">
+      <c r="A247" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="B246" s="136" t="s">
+      <c r="B247" s="135" t="s">
         <v>280</v>
       </c>
-      <c r="C246" s="137"/>
-      <c r="D246" s="137"/>
-      <c r="E246" s="138"/>
-      <c r="F246" s="9" t="s">
+      <c r="C247" s="136"/>
+      <c r="D247" s="136"/>
+      <c r="E247" s="137"/>
+      <c r="F247" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="G246" s="11" t="s">
+      <c r="G247" s="11" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="247" spans="1:7" ht="57" customHeight="1">
-      <c r="A247" s="12" t="s">
+    <row r="248" spans="1:7" ht="57" customHeight="1">
+      <c r="A248" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="B247" s="136" t="s">
+      <c r="B248" s="135" t="s">
         <v>282</v>
       </c>
-      <c r="C247" s="137"/>
-      <c r="D247" s="137"/>
-      <c r="E247" s="138"/>
-      <c r="F247" s="13" t="s">
+      <c r="C248" s="136"/>
+      <c r="D248" s="136"/>
+      <c r="E248" s="137"/>
+      <c r="F248" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="G247" s="22" t="s">
+      <c r="G248" s="22" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="248" spans="1:7" ht="69" customHeight="1">
-      <c r="A248" s="14" t="s">
+    <row r="249" spans="1:7" ht="69" customHeight="1">
+      <c r="A249" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="B248" s="122" t="s">
+      <c r="B249" s="138" t="s">
         <v>284</v>
       </c>
-      <c r="C248" s="134"/>
-      <c r="D248" s="134"/>
-      <c r="E248" s="134"/>
-      <c r="F248" s="15" t="s">
+      <c r="C249" s="131"/>
+      <c r="D249" s="131"/>
+      <c r="E249" s="131"/>
+      <c r="F249" s="15" t="s">
         <v>249</v>
       </c>
-      <c r="G248" s="27" t="s">
+      <c r="G249" s="27" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="249" spans="1:7">
-      <c r="C249" s="41"/>
-    </row>
-    <row r="251" spans="1:7">
-      <c r="A251" s="1" t="s">
+    <row r="250" spans="1:7">
+      <c r="C250" s="41"/>
+    </row>
+    <row r="252" spans="1:7">
+      <c r="A252" s="1" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="252" spans="1:7">
-      <c r="A252" s="4" t="s">
+    <row r="253" spans="1:7">
+      <c r="A253" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="B252" s="29" t="s">
+      <c r="B253" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="C252" s="42" t="s">
+      <c r="C253" s="42" t="s">
         <v>287</v>
       </c>
-      <c r="D252" s="43" t="s">
+      <c r="D253" s="43" t="s">
         <v>274</v>
       </c>
-      <c r="E252" s="43"/>
-      <c r="F252" s="44"/>
-      <c r="G252" s="31" t="s">
+      <c r="E253" s="43"/>
+      <c r="F253" s="44"/>
+      <c r="G253" s="31" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="253" spans="1:7">
-      <c r="A253" s="45">
+    <row r="254" spans="1:7">
+      <c r="A254" s="45">
         <v>42682</v>
       </c>
-      <c r="B253" s="46">
+      <c r="B254" s="46">
         <v>1.04</v>
       </c>
-      <c r="C253" s="17" t="s">
+      <c r="C254" s="17" t="s">
         <v>289</v>
       </c>
-      <c r="D253" s="139" t="s">
+      <c r="D254" s="139" t="s">
         <v>290</v>
       </c>
-      <c r="E253" s="139"/>
-      <c r="F253" s="139"/>
-      <c r="G253" s="47"/>
-    </row>
-    <row r="254" spans="1:7">
-      <c r="A254" s="48">
-        <v>42692</v>
-      </c>
-      <c r="B254" s="49">
-        <v>1.05</v>
-      </c>
-      <c r="C254" s="21" t="s">
-        <v>289</v>
-      </c>
-      <c r="D254" s="135" t="s">
-        <v>291</v>
-      </c>
-      <c r="E254" s="135"/>
-      <c r="F254" s="135"/>
-      <c r="G254" s="32"/>
+      <c r="E254" s="139"/>
+      <c r="F254" s="139"/>
+      <c r="G254" s="47"/>
     </row>
     <row r="255" spans="1:7">
       <c r="A255" s="48">
-        <v>42955</v>
+        <v>42692</v>
       </c>
       <c r="B255" s="49">
-        <v>1.06</v>
+        <v>1.05</v>
       </c>
       <c r="C255" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="D255" s="135" t="s">
-        <v>292</v>
-      </c>
-      <c r="E255" s="135"/>
-      <c r="F255" s="135"/>
+      <c r="D255" s="140" t="s">
+        <v>291</v>
+      </c>
+      <c r="E255" s="140"/>
+      <c r="F255" s="140"/>
       <c r="G255" s="32"/>
     </row>
     <row r="256" spans="1:7">
       <c r="A256" s="48">
-        <v>42991</v>
+        <v>42955</v>
       </c>
       <c r="B256" s="49">
-        <v>1.07</v>
+        <v>1.06</v>
       </c>
       <c r="C256" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="D256" s="135" t="s">
-        <v>293</v>
-      </c>
-      <c r="E256" s="135"/>
-      <c r="F256" s="135"/>
+      <c r="D256" s="140" t="s">
+        <v>292</v>
+      </c>
+      <c r="E256" s="140"/>
+      <c r="F256" s="140"/>
       <c r="G256" s="32"/>
     </row>
     <row r="257" spans="1:7">
       <c r="A257" s="48">
-        <v>43026</v>
+        <v>42991</v>
       </c>
       <c r="B257" s="49">
-        <v>1.08</v>
+        <v>1.07</v>
       </c>
       <c r="C257" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="D257" s="135" t="s">
-        <v>294</v>
-      </c>
-      <c r="E257" s="135"/>
-      <c r="F257" s="135"/>
+      <c r="D257" s="140" t="s">
+        <v>293</v>
+      </c>
+      <c r="E257" s="140"/>
+      <c r="F257" s="140"/>
       <c r="G257" s="32"/>
     </row>
     <row r="258" spans="1:7">
       <c r="A258" s="48">
-        <v>43069</v>
+        <v>43026</v>
       </c>
       <c r="B258" s="49">
-        <v>1.0900000000000001</v>
+        <v>1.08</v>
       </c>
       <c r="C258" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="D258" s="135" t="s">
+      <c r="D258" s="140" t="s">
+        <v>294</v>
+      </c>
+      <c r="E258" s="140"/>
+      <c r="F258" s="140"/>
+      <c r="G258" s="32"/>
+    </row>
+    <row r="259" spans="1:7">
+      <c r="A259" s="48">
+        <v>43069</v>
+      </c>
+      <c r="B259" s="49">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="C259" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="D259" s="140" t="s">
         <v>295</v>
       </c>
-      <c r="E258" s="135"/>
-      <c r="F258" s="135"/>
-      <c r="G258" s="32"/>
-    </row>
-    <row r="259" spans="1:7">
-      <c r="A259" s="50">
-        <v>43248</v>
-      </c>
-      <c r="B259" s="51">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C259" s="20" t="s">
-        <v>289</v>
-      </c>
-      <c r="D259" s="127" t="s">
-        <v>296</v>
-      </c>
-      <c r="E259" s="128"/>
-      <c r="F259" s="129"/>
-      <c r="G259" s="33"/>
+      <c r="E259" s="140"/>
+      <c r="F259" s="140"/>
+      <c r="G259" s="32"/>
     </row>
     <row r="260" spans="1:7">
       <c r="A260" s="50">
-        <v>43339</v>
+        <v>43248</v>
       </c>
       <c r="B260" s="51">
-        <v>1.1100000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C260" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="D260" s="127" t="s">
-        <v>297</v>
-      </c>
-      <c r="E260" s="128"/>
-      <c r="F260" s="129"/>
+      <c r="D260" s="141" t="s">
+        <v>296</v>
+      </c>
+      <c r="E260" s="142"/>
+      <c r="F260" s="143"/>
       <c r="G260" s="33"/>
     </row>
     <row r="261" spans="1:7">
       <c r="A261" s="50">
-        <v>43542</v>
+        <v>43339</v>
       </c>
       <c r="B261" s="51">
-        <v>1.1200000000000001</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="C261" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="D261" s="127" t="s">
-        <v>298</v>
-      </c>
-      <c r="E261" s="128"/>
-      <c r="F261" s="129"/>
+      <c r="D261" s="141" t="s">
+        <v>297</v>
+      </c>
+      <c r="E261" s="142"/>
+      <c r="F261" s="143"/>
       <c r="G261" s="33"/>
     </row>
     <row r="262" spans="1:7">
       <c r="A262" s="50">
-        <v>43599</v>
+        <v>43542</v>
       </c>
       <c r="B262" s="51">
-        <v>1.1299999999999999</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="C262" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="D262" s="52" t="s">
-        <v>299</v>
-      </c>
-      <c r="E262" s="53"/>
-      <c r="F262" s="54"/>
+      <c r="D262" s="141" t="s">
+        <v>298</v>
+      </c>
+      <c r="E262" s="142"/>
+      <c r="F262" s="143"/>
       <c r="G262" s="33"/>
     </row>
     <row r="263" spans="1:7">
       <c r="A263" s="50">
-        <v>43643</v>
+        <v>43599</v>
       </c>
       <c r="B263" s="51">
-        <v>1.1399999999999999</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="C263" s="20" t="s">
         <v>289</v>
       </c>
       <c r="D263" s="52" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E263" s="53"/>
       <c r="F263" s="54"/>
@@ -9935,16 +9957,16 @@
     </row>
     <row r="264" spans="1:7">
       <c r="A264" s="50">
-        <v>43894</v>
+        <v>43643</v>
       </c>
       <c r="B264" s="51">
-        <v>1.1499999999999999</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="C264" s="20" t="s">
         <v>289</v>
       </c>
       <c r="D264" s="52" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E264" s="53"/>
       <c r="F264" s="54"/>
@@ -9952,16 +9974,16 @@
     </row>
     <row r="265" spans="1:7">
       <c r="A265" s="50">
-        <v>44017</v>
+        <v>43894</v>
       </c>
       <c r="B265" s="51">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="C265" s="71" t="s">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C265" s="20" t="s">
         <v>289</v>
       </c>
       <c r="D265" s="52" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E265" s="53"/>
       <c r="F265" s="54"/>
@@ -9969,16 +9991,16 @@
     </row>
     <row r="266" spans="1:7">
       <c r="A266" s="50">
-        <v>44118</v>
+        <v>44017</v>
       </c>
       <c r="B266" s="51">
-        <v>1.17</v>
-      </c>
-      <c r="C266" s="73" t="s">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="C266" s="71" t="s">
         <v>289</v>
       </c>
       <c r="D266" s="52" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="E266" s="53"/>
       <c r="F266" s="54"/>
@@ -9986,16 +10008,16 @@
     </row>
     <row r="267" spans="1:7">
       <c r="A267" s="50">
-        <v>44209</v>
+        <v>44118</v>
       </c>
       <c r="B267" s="51">
-        <v>1.18</v>
-      </c>
-      <c r="C267" s="77" t="s">
+        <v>1.17</v>
+      </c>
+      <c r="C267" s="73" t="s">
         <v>289</v>
       </c>
-      <c r="D267" s="86" t="s">
-        <v>320</v>
+      <c r="D267" s="52" t="s">
+        <v>317</v>
       </c>
       <c r="E267" s="53"/>
       <c r="F267" s="54"/>
@@ -10003,16 +10025,16 @@
     </row>
     <row r="268" spans="1:7">
       <c r="A268" s="50">
-        <v>44258</v>
+        <v>44209</v>
       </c>
       <c r="B268" s="51">
-        <v>1.19</v>
-      </c>
-      <c r="C268" s="80" t="s">
+        <v>1.18</v>
+      </c>
+      <c r="C268" s="77" t="s">
         <v>289</v>
       </c>
-      <c r="D268" s="52" t="s">
-        <v>326</v>
+      <c r="D268" s="86" t="s">
+        <v>320</v>
       </c>
       <c r="E268" s="53"/>
       <c r="F268" s="54"/>
@@ -10020,16 +10042,16 @@
     </row>
     <row r="269" spans="1:7">
       <c r="A269" s="50">
-        <v>44357</v>
+        <v>44258</v>
       </c>
       <c r="B269" s="51">
-        <v>1.2</v>
-      </c>
-      <c r="C269" s="82" t="s">
+        <v>1.19</v>
+      </c>
+      <c r="C269" s="80" t="s">
         <v>289</v>
       </c>
       <c r="D269" s="52" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="E269" s="53"/>
       <c r="F269" s="54"/>
@@ -10037,16 +10059,16 @@
     </row>
     <row r="270" spans="1:7">
       <c r="A270" s="50">
-        <v>44487</v>
+        <v>44357</v>
       </c>
       <c r="B270" s="51">
-        <v>1.21</v>
-      </c>
-      <c r="C270" s="88" t="s">
+        <v>1.2</v>
+      </c>
+      <c r="C270" s="82" t="s">
         <v>289</v>
       </c>
       <c r="D270" s="52" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E270" s="53"/>
       <c r="F270" s="54"/>
@@ -10054,99 +10076,133 @@
     </row>
     <row r="271" spans="1:7">
       <c r="A271" s="50">
-        <v>44518</v>
+        <v>44487</v>
       </c>
       <c r="B271" s="51">
-        <v>1.22</v>
-      </c>
-      <c r="C271" s="110" t="s">
+        <v>1.21</v>
+      </c>
+      <c r="C271" s="88" t="s">
         <v>289</v>
       </c>
       <c r="D271" s="52" t="s">
-        <v>361</v>
+        <v>340</v>
       </c>
       <c r="E271" s="53"/>
       <c r="F271" s="54"/>
       <c r="G271" s="33"/>
     </row>
     <row r="272" spans="1:7">
-      <c r="A272" s="55">
+      <c r="A272" s="50">
+        <v>44518</v>
+      </c>
+      <c r="B272" s="51">
+        <v>1.22</v>
+      </c>
+      <c r="C272" s="107" t="s">
+        <v>289</v>
+      </c>
+      <c r="D272" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="E272" s="53"/>
+      <c r="F272" s="54"/>
+      <c r="G272" s="33"/>
+    </row>
+    <row r="273" spans="1:7">
+      <c r="A273" s="50">
         <v>44530</v>
       </c>
-      <c r="B272" s="56">
+      <c r="B273" s="51">
         <v>1.23</v>
       </c>
-      <c r="C272" s="26" t="s">
+      <c r="C273" s="110" t="s">
         <v>289</v>
       </c>
-      <c r="D272" s="130" t="s">
+      <c r="D273" s="52" t="s">
         <v>395</v>
       </c>
-      <c r="E272" s="131"/>
-      <c r="F272" s="131"/>
-      <c r="G272" s="34"/>
+      <c r="E273" s="53"/>
+      <c r="F273" s="54"/>
+      <c r="G273" s="33"/>
+    </row>
+    <row r="274" spans="1:7">
+      <c r="A274" s="55">
+        <v>44559</v>
+      </c>
+      <c r="B274" s="56">
+        <v>1.24</v>
+      </c>
+      <c r="C274" s="26" t="s">
+        <v>289</v>
+      </c>
+      <c r="D274" s="144" t="s">
+        <v>399</v>
+      </c>
+      <c r="E274" s="145"/>
+      <c r="F274" s="145"/>
+      <c r="G274" s="34"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="MPVJvTiHRN320pKoKToVhuwektmJFEJT0+KL2ERT4h53dvLO23ISBj6m2i/Gqig7UZNEkdNfs7XDy4ACEf45Tw==" saltValue="2z5w4jiPEsDkIfJJ6iS06A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="apWuLBIlzSrG8yzhsN6NRNuUMxPsVv6nh9x2ibQ2WTXetoAj2BIKJUf55DVFWNeEvBrjPDVHqwNr8Lr9q27wyQ==" saltValue="38Ewv6vELDf+Pf6Dvr7g9A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115" topLeftCell="A184">
-      <selection activeCell="E194" sqref="E194:E196"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115" topLeftCell="A139">
+      <selection activeCell="D163" sqref="D163"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="51">
-    <mergeCell ref="F111:N111"/>
-    <mergeCell ref="C223:E223"/>
-    <mergeCell ref="C224:E224"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C226:E226"/>
-    <mergeCell ref="C227:E227"/>
+    <mergeCell ref="B198:B200"/>
+    <mergeCell ref="B201:B207"/>
+    <mergeCell ref="B225:B226"/>
+    <mergeCell ref="B227:B228"/>
+    <mergeCell ref="B229:B230"/>
+    <mergeCell ref="B149:B162"/>
+    <mergeCell ref="B163:B169"/>
+    <mergeCell ref="B170:B180"/>
+    <mergeCell ref="B181:B188"/>
+    <mergeCell ref="B189:B197"/>
+    <mergeCell ref="D261:F261"/>
+    <mergeCell ref="D262:F262"/>
+    <mergeCell ref="D274:F274"/>
+    <mergeCell ref="A225:A232"/>
+    <mergeCell ref="A233:A236"/>
+    <mergeCell ref="A237:A240"/>
+    <mergeCell ref="B231:B232"/>
+    <mergeCell ref="B233:B234"/>
+    <mergeCell ref="B235:B236"/>
+    <mergeCell ref="B237:B238"/>
+    <mergeCell ref="B239:B240"/>
+    <mergeCell ref="D256:F256"/>
+    <mergeCell ref="D257:F257"/>
+    <mergeCell ref="D258:F258"/>
+    <mergeCell ref="D259:F259"/>
+    <mergeCell ref="D260:F260"/>
+    <mergeCell ref="B247:E247"/>
+    <mergeCell ref="B248:E248"/>
+    <mergeCell ref="B249:E249"/>
+    <mergeCell ref="D254:F254"/>
+    <mergeCell ref="D255:F255"/>
+    <mergeCell ref="C238:E238"/>
+    <mergeCell ref="C239:E239"/>
+    <mergeCell ref="C240:E240"/>
+    <mergeCell ref="B245:E245"/>
+    <mergeCell ref="B246:E246"/>
+    <mergeCell ref="C233:E233"/>
+    <mergeCell ref="C234:E234"/>
+    <mergeCell ref="C235:E235"/>
+    <mergeCell ref="C236:E236"/>
+    <mergeCell ref="C237:E237"/>
     <mergeCell ref="C228:E228"/>
     <mergeCell ref="C229:E229"/>
     <mergeCell ref="C230:E230"/>
     <mergeCell ref="C231:E231"/>
     <mergeCell ref="C232:E232"/>
-    <mergeCell ref="C233:E233"/>
-    <mergeCell ref="C234:E234"/>
-    <mergeCell ref="C235:E235"/>
-    <mergeCell ref="C236:E236"/>
-    <mergeCell ref="C237:E237"/>
-    <mergeCell ref="C238:E238"/>
-    <mergeCell ref="C239:E239"/>
-    <mergeCell ref="B244:E244"/>
-    <mergeCell ref="B245:E245"/>
-    <mergeCell ref="B246:E246"/>
-    <mergeCell ref="B247:E247"/>
-    <mergeCell ref="B248:E248"/>
-    <mergeCell ref="D253:F253"/>
-    <mergeCell ref="D254:F254"/>
-    <mergeCell ref="D260:F260"/>
-    <mergeCell ref="D261:F261"/>
-    <mergeCell ref="D272:F272"/>
-    <mergeCell ref="A224:A231"/>
-    <mergeCell ref="A232:A235"/>
-    <mergeCell ref="A236:A239"/>
-    <mergeCell ref="B230:B231"/>
-    <mergeCell ref="B232:B233"/>
-    <mergeCell ref="B234:B235"/>
-    <mergeCell ref="B236:B237"/>
-    <mergeCell ref="B238:B239"/>
-    <mergeCell ref="D255:F255"/>
-    <mergeCell ref="D256:F256"/>
-    <mergeCell ref="D257:F257"/>
-    <mergeCell ref="D258:F258"/>
-    <mergeCell ref="D259:F259"/>
-    <mergeCell ref="B149:B161"/>
-    <mergeCell ref="B162:B168"/>
-    <mergeCell ref="B169:B179"/>
-    <mergeCell ref="B180:B187"/>
-    <mergeCell ref="B188:B196"/>
-    <mergeCell ref="B197:B199"/>
-    <mergeCell ref="B200:B206"/>
-    <mergeCell ref="B224:B225"/>
-    <mergeCell ref="B226:B227"/>
-    <mergeCell ref="B228:B229"/>
+    <mergeCell ref="F111:N111"/>
+    <mergeCell ref="C224:E224"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C226:E226"/>
+    <mergeCell ref="C227:E227"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -10163,7 +10219,7 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -10176,11 +10232,11 @@
       <selection activeCell="D24" sqref="D24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>

</xml_diff>

<commit_message>
i400--result delete function added
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_example/standard_suite/diamond_regression.xlsx
+++ b/tmp_client/doc/TMP_example/standard_suite/diamond_regression.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\repository\tmp_client\doc\TMP_example\standard_suite\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="suite" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,9 @@
   </definedNames>
   <calcPr calcId="144525"/>
   <customWorkbookViews>
+    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
     <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="2391" yWindow="-9" windowWidth="2418" windowHeight="1318" activeSheetId="3" showComments="commIndAndComment"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
-    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -2221,109 +2221,109 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -5176,11 +5176,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" style="58" customWidth="1"/>
     <col min="2" max="2" width="28" style="58" customWidth="1"/>
@@ -5263,8 +5261,8 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="B41" sqref="B41"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="B4" sqref="B4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -5273,8 +5271,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="B4" sqref="B4"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="B41" sqref="B41"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -5296,33 +5294,33 @@
       <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="58" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="58" customWidth="1"/>
     <col min="2" max="2" width="9" style="58" customWidth="1"/>
-    <col min="3" max="3" width="33.33203125" style="58" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" style="58" customWidth="1"/>
-    <col min="5" max="5" width="30.33203125" style="58" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="58" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" style="58" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="58" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" style="58" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="58" customWidth="1"/>
     <col min="7" max="7" width="24" style="58" customWidth="1"/>
     <col min="8" max="8" width="37" style="58" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" style="58" customWidth="1"/>
-    <col min="10" max="10" width="9.88671875" style="58" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="58" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" style="58" customWidth="1"/>
     <col min="11" max="11" width="12" style="58" customWidth="1"/>
-    <col min="12" max="12" width="9.5546875" style="59" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="59" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" style="59" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" style="59" customWidth="1"/>
     <col min="14" max="14" width="38" style="58" customWidth="1"/>
-    <col min="15" max="15" width="19.44140625" style="58" customWidth="1"/>
-    <col min="16" max="16" width="30.33203125" style="58" customWidth="1"/>
-    <col min="17" max="17" width="17.33203125" style="58" customWidth="1"/>
-    <col min="18" max="18" width="15.44140625" style="58" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" style="58" customWidth="1"/>
+    <col min="16" max="16" width="30.28515625" style="58" customWidth="1"/>
+    <col min="17" max="17" width="17.28515625" style="58" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" style="58" customWidth="1"/>
     <col min="19" max="19" width="13" style="58" customWidth="1"/>
-    <col min="20" max="21" width="9.6640625" style="58" customWidth="1"/>
-    <col min="22" max="22" width="9.44140625" style="58" customWidth="1"/>
+    <col min="20" max="21" width="9.7109375" style="58" customWidth="1"/>
+    <col min="22" max="22" width="9.42578125" style="58" customWidth="1"/>
     <col min="23" max="23" width="11" style="58" customWidth="1"/>
-    <col min="24" max="24" width="11.6640625" style="58" customWidth="1"/>
+    <col min="24" max="24" width="11.7109375" style="58" customWidth="1"/>
     <col min="25" max="30" width="9" style="58"/>
-    <col min="31" max="31" width="10.109375" style="58" customWidth="1"/>
+    <col min="31" max="31" width="10.140625" style="58" customWidth="1"/>
     <col min="32" max="16384" width="9" style="58"/>
   </cols>
   <sheetData>
@@ -6883,12 +6881,12 @@
   <sheetProtection algorithmName="SHA-512" hashValue="Sju3pjEnjegba3BrZLImZ+xscQ9MLEq+i8mDO7rXFn4S3yXv8zWb4HaF0uC2YruSs8wkV8FCIxY7a0fvnwVXFw==" saltValue="mZmUchosJ60PlKqUXOSzGQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A2:AF46"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="85" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen"/>
+      <selection activeCell="H23" sqref="H23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
-      <autoFilter ref="A2:AF46"/>
+      <autoFilter ref="A2:Y2"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen"/>
@@ -6897,12 +6895,12 @@
       <pageSetup paperSize="9" orientation="portrait"/>
       <autoFilter ref="A2:Y2"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen"/>
-      <selection activeCell="H23" sqref="H23"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="85" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
-      <autoFilter ref="A2:Y2"/>
+      <autoFilter ref="A2:AF46"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -6991,18 +6989,18 @@
       <selection activeCell="D173" sqref="D173"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="32" style="1" customWidth="1"/>
-    <col min="7" max="7" width="33.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="28.109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="33.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="28.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -7049,17 +7047,17 @@
       <c r="E111" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="F111" s="117" t="s">
+      <c r="F111" s="148" t="s">
         <v>140</v>
       </c>
-      <c r="G111" s="118"/>
-      <c r="H111" s="118"/>
-      <c r="I111" s="118"/>
-      <c r="J111" s="118"/>
-      <c r="K111" s="118"/>
-      <c r="L111" s="118"/>
-      <c r="M111" s="118"/>
-      <c r="N111" s="119"/>
+      <c r="G111" s="149"/>
+      <c r="H111" s="149"/>
+      <c r="I111" s="149"/>
+      <c r="J111" s="149"/>
+      <c r="K111" s="149"/>
+      <c r="L111" s="149"/>
+      <c r="M111" s="149"/>
+      <c r="N111" s="150"/>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="6" t="s">
@@ -7979,7 +7977,7 @@
       <c r="A149" s="19">
         <v>1</v>
       </c>
-      <c r="B149" s="148" t="s">
+      <c r="B149" s="117" t="s">
         <v>4</v>
       </c>
       <c r="C149" s="62" t="s">
@@ -8005,7 +8003,7 @@
       <c r="A150" s="19">
         <v>2</v>
       </c>
-      <c r="B150" s="149"/>
+      <c r="B150" s="119"/>
       <c r="C150" s="21" t="s">
         <v>173</v>
       </c>
@@ -8027,7 +8025,7 @@
       <c r="A151" s="19">
         <v>3</v>
       </c>
-      <c r="B151" s="149"/>
+      <c r="B151" s="119"/>
       <c r="C151" s="21" t="s">
         <v>18</v>
       </c>
@@ -8047,7 +8045,7 @@
       <c r="A152" s="19">
         <v>4</v>
       </c>
-      <c r="B152" s="149"/>
+      <c r="B152" s="119"/>
       <c r="C152" s="21" t="s">
         <v>175</v>
       </c>
@@ -8071,7 +8069,7 @@
       <c r="A153" s="19">
         <v>5</v>
       </c>
-      <c r="B153" s="149"/>
+      <c r="B153" s="119"/>
       <c r="C153" s="62" t="s">
         <v>177</v>
       </c>
@@ -8095,7 +8093,7 @@
       <c r="A154" s="19">
         <v>6</v>
       </c>
-      <c r="B154" s="149"/>
+      <c r="B154" s="119"/>
       <c r="C154" s="62" t="s">
         <v>181</v>
       </c>
@@ -8119,7 +8117,7 @@
       <c r="A155" s="19">
         <v>7</v>
       </c>
-      <c r="B155" s="149"/>
+      <c r="B155" s="119"/>
       <c r="C155" s="21" t="s">
         <v>183</v>
       </c>
@@ -8141,7 +8139,7 @@
       <c r="A156" s="19">
         <v>8</v>
       </c>
-      <c r="B156" s="149"/>
+      <c r="B156" s="119"/>
       <c r="C156" s="62" t="s">
         <v>184</v>
       </c>
@@ -8165,7 +8163,7 @@
       <c r="A157" s="19">
         <v>9</v>
       </c>
-      <c r="B157" s="149"/>
+      <c r="B157" s="119"/>
       <c r="C157" s="62" t="s">
         <v>185</v>
       </c>
@@ -8189,7 +8187,7 @@
       <c r="A158" s="19">
         <v>10</v>
       </c>
-      <c r="B158" s="149"/>
+      <c r="B158" s="119"/>
       <c r="C158" s="21" t="s">
         <v>186</v>
       </c>
@@ -8213,7 +8211,7 @@
       <c r="A159" s="112">
         <v>11</v>
       </c>
-      <c r="B159" s="149"/>
+      <c r="B159" s="119"/>
       <c r="C159" s="21" t="s">
         <v>187</v>
       </c>
@@ -8237,7 +8235,7 @@
       <c r="A160" s="112">
         <v>12</v>
       </c>
-      <c r="B160" s="149"/>
+      <c r="B160" s="119"/>
       <c r="C160" s="21" t="s">
         <v>189</v>
       </c>
@@ -8259,7 +8257,7 @@
       <c r="A161" s="112">
         <v>13</v>
       </c>
-      <c r="B161" s="149"/>
+      <c r="B161" s="119"/>
       <c r="C161" s="111" t="s">
         <v>400</v>
       </c>
@@ -8281,7 +8279,7 @@
       <c r="A162" s="112">
         <v>14</v>
       </c>
-      <c r="B162" s="134"/>
+      <c r="B162" s="126"/>
       <c r="C162" s="21" t="s">
         <v>193</v>
       </c>
@@ -8305,7 +8303,7 @@
       <c r="A163" s="112">
         <v>15</v>
       </c>
-      <c r="B163" s="129" t="s">
+      <c r="B163" s="127" t="s">
         <v>5</v>
       </c>
       <c r="C163" s="21" t="s">
@@ -8332,7 +8330,7 @@
       <c r="A164" s="112">
         <v>16</v>
       </c>
-      <c r="B164" s="129"/>
+      <c r="B164" s="127"/>
       <c r="C164" s="89" t="s">
         <v>341</v>
       </c>
@@ -8356,7 +8354,7 @@
       <c r="A165" s="112">
         <v>17</v>
       </c>
-      <c r="B165" s="129"/>
+      <c r="B165" s="127"/>
       <c r="C165" s="89" t="s">
         <v>344</v>
       </c>
@@ -8380,7 +8378,7 @@
       <c r="A166" s="112">
         <v>18</v>
       </c>
-      <c r="B166" s="129"/>
+      <c r="B166" s="127"/>
       <c r="C166" s="100" t="s">
         <v>377</v>
       </c>
@@ -8404,7 +8402,7 @@
       <c r="A167" s="112">
         <v>19</v>
       </c>
-      <c r="B167" s="129"/>
+      <c r="B167" s="127"/>
       <c r="C167" s="100" t="s">
         <v>378</v>
       </c>
@@ -8426,7 +8424,7 @@
       <c r="A168" s="112">
         <v>20</v>
       </c>
-      <c r="B168" s="129"/>
+      <c r="B168" s="127"/>
       <c r="C168" s="100" t="s">
         <v>379</v>
       </c>
@@ -8448,7 +8446,7 @@
       <c r="A169" s="112">
         <v>21</v>
       </c>
-      <c r="B169" s="130"/>
+      <c r="B169" s="124"/>
       <c r="C169" s="83" t="s">
         <v>200</v>
       </c>
@@ -8471,7 +8469,7 @@
       <c r="A170" s="112">
         <v>22</v>
       </c>
-      <c r="B170" s="148" t="s">
+      <c r="B170" s="117" t="s">
         <v>6</v>
       </c>
       <c r="C170" s="89" t="s">
@@ -8498,7 +8496,7 @@
       <c r="A171" s="112">
         <v>23</v>
       </c>
-      <c r="B171" s="150"/>
+      <c r="B171" s="118"/>
       <c r="C171" s="100" t="s">
         <v>347</v>
       </c>
@@ -8522,7 +8520,7 @@
       <c r="A172" s="112">
         <v>24</v>
       </c>
-      <c r="B172" s="150"/>
+      <c r="B172" s="118"/>
       <c r="C172" s="100" t="s">
         <v>348</v>
       </c>
@@ -8546,7 +8544,7 @@
       <c r="A173" s="112">
         <v>25</v>
       </c>
-      <c r="B173" s="150"/>
+      <c r="B173" s="118"/>
       <c r="C173" s="100" t="s">
         <v>382</v>
       </c>
@@ -8568,7 +8566,7 @@
       <c r="A174" s="112">
         <v>26</v>
       </c>
-      <c r="B174" s="150"/>
+      <c r="B174" s="118"/>
       <c r="C174" s="100" t="s">
         <v>369</v>
       </c>
@@ -8590,7 +8588,7 @@
       <c r="A175" s="112">
         <v>27</v>
       </c>
-      <c r="B175" s="150"/>
+      <c r="B175" s="118"/>
       <c r="C175" s="93" t="s">
         <v>366</v>
       </c>
@@ -8612,7 +8610,7 @@
       <c r="A176" s="112">
         <v>28</v>
       </c>
-      <c r="B176" s="150"/>
+      <c r="B176" s="118"/>
       <c r="C176" s="102" t="s">
         <v>376</v>
       </c>
@@ -8636,7 +8634,7 @@
       <c r="A177" s="112">
         <v>29</v>
       </c>
-      <c r="B177" s="150"/>
+      <c r="B177" s="118"/>
       <c r="C177" s="91" t="s">
         <v>364</v>
       </c>
@@ -8658,7 +8656,7 @@
       <c r="A178" s="112">
         <v>30</v>
       </c>
-      <c r="B178" s="150"/>
+      <c r="B178" s="118"/>
       <c r="C178" s="100" t="s">
         <v>372</v>
       </c>
@@ -8682,7 +8680,7 @@
       <c r="A179" s="112">
         <v>31</v>
       </c>
-      <c r="B179" s="150"/>
+      <c r="B179" s="118"/>
       <c r="C179" s="66" t="s">
         <v>304</v>
       </c>
@@ -8704,7 +8702,7 @@
       <c r="A180" s="112">
         <v>32</v>
       </c>
-      <c r="B180" s="134"/>
+      <c r="B180" s="126"/>
       <c r="C180" s="62" t="s">
         <v>204</v>
       </c>
@@ -8724,7 +8722,7 @@
       <c r="A181" s="112">
         <v>33</v>
       </c>
-      <c r="B181" s="129" t="s">
+      <c r="B181" s="127" t="s">
         <v>8</v>
       </c>
       <c r="C181" s="21" t="s">
@@ -8750,7 +8748,7 @@
       <c r="A182" s="112">
         <v>34</v>
       </c>
-      <c r="B182" s="130"/>
+      <c r="B182" s="124"/>
       <c r="C182" s="89" t="s">
         <v>354</v>
       </c>
@@ -8774,7 +8772,7 @@
       <c r="A183" s="112">
         <v>35</v>
       </c>
-      <c r="B183" s="130"/>
+      <c r="B183" s="124"/>
       <c r="C183" s="89" t="s">
         <v>209</v>
       </c>
@@ -8794,7 +8792,7 @@
       <c r="A184" s="112">
         <v>36</v>
       </c>
-      <c r="B184" s="130"/>
+      <c r="B184" s="124"/>
       <c r="C184" s="21" t="s">
         <v>210</v>
       </c>
@@ -8818,7 +8816,7 @@
       <c r="A185" s="112">
         <v>37</v>
       </c>
-      <c r="B185" s="130"/>
+      <c r="B185" s="124"/>
       <c r="C185" s="21" t="s">
         <v>211</v>
       </c>
@@ -8840,7 +8838,7 @@
       <c r="A186" s="112">
         <v>38</v>
       </c>
-      <c r="B186" s="130"/>
+      <c r="B186" s="124"/>
       <c r="C186" s="21" t="s">
         <v>212</v>
       </c>
@@ -8860,7 +8858,7 @@
       <c r="A187" s="112">
         <v>39</v>
       </c>
-      <c r="B187" s="130"/>
+      <c r="B187" s="124"/>
       <c r="C187" s="21" t="s">
         <v>213</v>
       </c>
@@ -8880,7 +8878,7 @@
       <c r="A188" s="112">
         <v>40</v>
       </c>
-      <c r="B188" s="130"/>
+      <c r="B188" s="124"/>
       <c r="C188" s="21" t="s">
         <v>47</v>
       </c>
@@ -8896,11 +8894,11 @@
       </c>
       <c r="H188" s="11"/>
     </row>
-    <row r="189" spans="1:8" ht="43.2">
+    <row r="189" spans="1:8" ht="45">
       <c r="A189" s="112">
         <v>41</v>
       </c>
-      <c r="B189" s="129" t="s">
+      <c r="B189" s="127" t="s">
         <v>9</v>
       </c>
       <c r="C189" s="21" t="s">
@@ -8924,7 +8922,7 @@
       <c r="A190" s="112">
         <v>42</v>
       </c>
-      <c r="B190" s="130"/>
+      <c r="B190" s="124"/>
       <c r="C190" s="62" t="s">
         <v>215</v>
       </c>
@@ -8946,7 +8944,7 @@
       <c r="A191" s="112">
         <v>43</v>
       </c>
-      <c r="B191" s="130"/>
+      <c r="B191" s="124"/>
       <c r="C191" s="78" t="s">
         <v>332</v>
       </c>
@@ -8968,7 +8966,7 @@
       <c r="A192" s="112">
         <v>44</v>
       </c>
-      <c r="B192" s="130"/>
+      <c r="B192" s="124"/>
       <c r="C192" s="78" t="s">
         <v>218</v>
       </c>
@@ -8990,7 +8988,7 @@
       <c r="A193" s="112">
         <v>45</v>
       </c>
-      <c r="B193" s="130"/>
+      <c r="B193" s="124"/>
       <c r="C193" s="78" t="s">
         <v>330</v>
       </c>
@@ -9012,7 +9010,7 @@
       <c r="A194" s="112">
         <v>46</v>
       </c>
-      <c r="B194" s="130"/>
+      <c r="B194" s="124"/>
       <c r="C194" s="104" t="s">
         <v>331</v>
       </c>
@@ -9034,7 +9032,7 @@
       <c r="A195" s="112">
         <v>47</v>
       </c>
-      <c r="B195" s="130"/>
+      <c r="B195" s="124"/>
       <c r="C195" s="104" t="s">
         <v>387</v>
       </c>
@@ -9056,7 +9054,7 @@
       <c r="A196" s="112">
         <v>48</v>
       </c>
-      <c r="B196" s="130"/>
+      <c r="B196" s="124"/>
       <c r="C196" s="104" t="s">
         <v>388</v>
       </c>
@@ -9078,7 +9076,7 @@
       <c r="A197" s="112">
         <v>49</v>
       </c>
-      <c r="B197" s="130"/>
+      <c r="B197" s="124"/>
       <c r="C197" s="78" t="s">
         <v>389</v>
       </c>
@@ -9100,7 +9098,7 @@
       <c r="A198" s="112">
         <v>50</v>
       </c>
-      <c r="B198" s="148" t="s">
+      <c r="B198" s="117" t="s">
         <v>10</v>
       </c>
       <c r="C198" s="21" t="s">
@@ -9126,7 +9124,7 @@
       <c r="A199" s="112">
         <v>51</v>
       </c>
-      <c r="B199" s="150"/>
+      <c r="B199" s="118"/>
       <c r="C199" s="80" t="s">
         <v>222</v>
       </c>
@@ -9150,7 +9148,7 @@
       <c r="A200" s="106">
         <v>52</v>
       </c>
-      <c r="B200" s="149"/>
+      <c r="B200" s="119"/>
       <c r="C200" s="79" t="s">
         <v>335</v>
       </c>
@@ -9174,7 +9172,7 @@
       <c r="A201" s="16">
         <v>53</v>
       </c>
-      <c r="B201" s="151" t="s">
+      <c r="B201" s="120" t="s">
         <v>156</v>
       </c>
       <c r="C201" s="63" t="s">
@@ -9198,7 +9196,7 @@
       <c r="A202" s="19">
         <v>54</v>
       </c>
-      <c r="B202" s="152"/>
+      <c r="B202" s="121"/>
       <c r="C202" s="62" t="s">
         <v>227</v>
       </c>
@@ -9220,7 +9218,7 @@
       <c r="A203" s="112">
         <v>55</v>
       </c>
-      <c r="B203" s="153"/>
+      <c r="B203" s="122"/>
       <c r="C203" s="64" t="s">
         <v>230</v>
       </c>
@@ -9242,7 +9240,7 @@
       <c r="A204" s="112">
         <v>56</v>
       </c>
-      <c r="B204" s="153"/>
+      <c r="B204" s="122"/>
       <c r="C204" s="64" t="s">
         <v>231</v>
       </c>
@@ -9264,7 +9262,7 @@
       <c r="A205" s="112">
         <v>57</v>
       </c>
-      <c r="B205" s="153"/>
+      <c r="B205" s="122"/>
       <c r="C205" s="70" t="s">
         <v>234</v>
       </c>
@@ -9284,7 +9282,7 @@
       <c r="A206" s="112">
         <v>58</v>
       </c>
-      <c r="B206" s="153"/>
+      <c r="B206" s="122"/>
       <c r="C206" s="70" t="s">
         <v>310</v>
       </c>
@@ -9306,7 +9304,7 @@
       <c r="A207" s="25">
         <v>59</v>
       </c>
-      <c r="B207" s="138"/>
+      <c r="B207" s="123"/>
       <c r="C207" s="26" t="s">
         <v>314</v>
       </c>
@@ -9372,11 +9370,11 @@
       <c r="B224" s="29" t="s">
         <v>241</v>
       </c>
-      <c r="C224" s="120" t="s">
+      <c r="C224" s="151" t="s">
         <v>242</v>
       </c>
-      <c r="D224" s="120"/>
-      <c r="E224" s="120"/>
+      <c r="D224" s="151"/>
+      <c r="E224" s="151"/>
       <c r="F224" s="30" t="s">
         <v>243</v>
       </c>
@@ -9385,17 +9383,17 @@
       </c>
     </row>
     <row r="225" spans="1:7">
-      <c r="A225" s="146" t="s">
+      <c r="A225" s="133" t="s">
         <v>245</v>
       </c>
-      <c r="B225" s="130" t="s">
+      <c r="B225" s="124" t="s">
         <v>246</v>
       </c>
-      <c r="C225" s="121" t="s">
+      <c r="C225" s="152" t="s">
         <v>247</v>
       </c>
-      <c r="D225" s="122"/>
-      <c r="E225" s="122"/>
+      <c r="D225" s="153"/>
+      <c r="E225" s="153"/>
       <c r="F225" s="21" t="s">
         <v>248</v>
       </c>
@@ -9404,13 +9402,13 @@
       </c>
     </row>
     <row r="226" spans="1:7">
-      <c r="A226" s="146"/>
-      <c r="B226" s="154"/>
-      <c r="C226" s="123" t="s">
+      <c r="A226" s="133"/>
+      <c r="B226" s="125"/>
+      <c r="C226" s="143" t="s">
         <v>247</v>
       </c>
-      <c r="D226" s="124"/>
-      <c r="E226" s="124"/>
+      <c r="D226" s="154"/>
+      <c r="E226" s="154"/>
       <c r="F226" s="20" t="s">
         <v>250</v>
       </c>
@@ -9419,15 +9417,15 @@
       </c>
     </row>
     <row r="227" spans="1:7">
-      <c r="A227" s="146"/>
-      <c r="B227" s="130" t="s">
+      <c r="A227" s="133"/>
+      <c r="B227" s="124" t="s">
         <v>251</v>
       </c>
-      <c r="C227" s="125" t="s">
+      <c r="C227" s="147" t="s">
         <v>252</v>
       </c>
-      <c r="D227" s="125"/>
-      <c r="E227" s="125"/>
+      <c r="D227" s="147"/>
+      <c r="E227" s="147"/>
       <c r="F227" s="21" t="s">
         <v>248</v>
       </c>
@@ -9436,13 +9434,13 @@
       </c>
     </row>
     <row r="228" spans="1:7">
-      <c r="A228" s="146"/>
-      <c r="B228" s="130"/>
-      <c r="C228" s="123" t="s">
+      <c r="A228" s="133"/>
+      <c r="B228" s="124"/>
+      <c r="C228" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="D228" s="123"/>
-      <c r="E228" s="123"/>
+      <c r="D228" s="143"/>
+      <c r="E228" s="143"/>
       <c r="F228" s="21" t="s">
         <v>250</v>
       </c>
@@ -9451,15 +9449,15 @@
       </c>
     </row>
     <row r="229" spans="1:7">
-      <c r="A229" s="146"/>
-      <c r="B229" s="154" t="s">
+      <c r="A229" s="133"/>
+      <c r="B229" s="125" t="s">
         <v>253</v>
       </c>
-      <c r="C229" s="126" t="s">
+      <c r="C229" s="144" t="s">
         <v>247</v>
       </c>
-      <c r="D229" s="127"/>
-      <c r="E229" s="128"/>
+      <c r="D229" s="145"/>
+      <c r="E229" s="146"/>
       <c r="F229" s="21" t="s">
         <v>248</v>
       </c>
@@ -9468,13 +9466,13 @@
       </c>
     </row>
     <row r="230" spans="1:7">
-      <c r="A230" s="146"/>
-      <c r="B230" s="134"/>
-      <c r="C230" s="126" t="s">
+      <c r="A230" s="133"/>
+      <c r="B230" s="126"/>
+      <c r="C230" s="144" t="s">
         <v>247</v>
       </c>
-      <c r="D230" s="127"/>
-      <c r="E230" s="128"/>
+      <c r="D230" s="145"/>
+      <c r="E230" s="146"/>
       <c r="F230" s="21" t="s">
         <v>250</v>
       </c>
@@ -9483,15 +9481,15 @@
       </c>
     </row>
     <row r="231" spans="1:7">
-      <c r="A231" s="146"/>
-      <c r="B231" s="130" t="s">
+      <c r="A231" s="133"/>
+      <c r="B231" s="124" t="s">
         <v>254</v>
       </c>
-      <c r="C231" s="125" t="s">
+      <c r="C231" s="147" t="s">
         <v>255</v>
       </c>
-      <c r="D231" s="125"/>
-      <c r="E231" s="125"/>
+      <c r="D231" s="147"/>
+      <c r="E231" s="147"/>
       <c r="F231" s="21" t="s">
         <v>248</v>
       </c>
@@ -9500,13 +9498,13 @@
       </c>
     </row>
     <row r="232" spans="1:7">
-      <c r="A232" s="146"/>
-      <c r="B232" s="130"/>
-      <c r="C232" s="125" t="s">
+      <c r="A232" s="133"/>
+      <c r="B232" s="124"/>
+      <c r="C232" s="147" t="s">
         <v>255</v>
       </c>
-      <c r="D232" s="125"/>
-      <c r="E232" s="125"/>
+      <c r="D232" s="147"/>
+      <c r="E232" s="147"/>
       <c r="F232" s="21" t="s">
         <v>250</v>
       </c>
@@ -9515,17 +9513,17 @@
       </c>
     </row>
     <row r="233" spans="1:7">
-      <c r="A233" s="146" t="s">
+      <c r="A233" s="133" t="s">
         <v>256</v>
       </c>
-      <c r="B233" s="130" t="s">
+      <c r="B233" s="124" t="s">
         <v>257</v>
       </c>
-      <c r="C233" s="129" t="s">
+      <c r="C233" s="127" t="s">
         <v>258</v>
       </c>
-      <c r="D233" s="130"/>
-      <c r="E233" s="130"/>
+      <c r="D233" s="124"/>
+      <c r="E233" s="124"/>
       <c r="F233" s="21" t="s">
         <v>248</v>
       </c>
@@ -9534,13 +9532,13 @@
       </c>
     </row>
     <row r="234" spans="1:7">
-      <c r="A234" s="146"/>
-      <c r="B234" s="130"/>
-      <c r="C234" s="130" t="s">
+      <c r="A234" s="133"/>
+      <c r="B234" s="124"/>
+      <c r="C234" s="124" t="s">
         <v>259</v>
       </c>
-      <c r="D234" s="130"/>
-      <c r="E234" s="130"/>
+      <c r="D234" s="124"/>
+      <c r="E234" s="124"/>
       <c r="F234" s="21" t="s">
         <v>250</v>
       </c>
@@ -9549,15 +9547,15 @@
       </c>
     </row>
     <row r="235" spans="1:7">
-      <c r="A235" s="146"/>
-      <c r="B235" s="130" t="s">
+      <c r="A235" s="133"/>
+      <c r="B235" s="124" t="s">
         <v>261</v>
       </c>
-      <c r="C235" s="130" t="s">
+      <c r="C235" s="124" t="s">
         <v>262</v>
       </c>
-      <c r="D235" s="130"/>
-      <c r="E235" s="130"/>
+      <c r="D235" s="124"/>
+      <c r="E235" s="124"/>
       <c r="F235" s="21" t="s">
         <v>248</v>
       </c>
@@ -9566,13 +9564,13 @@
       </c>
     </row>
     <row r="236" spans="1:7">
-      <c r="A236" s="146"/>
-      <c r="B236" s="130"/>
-      <c r="C236" s="130" t="s">
+      <c r="A236" s="133"/>
+      <c r="B236" s="124"/>
+      <c r="C236" s="124" t="s">
         <v>263</v>
       </c>
-      <c r="D236" s="130"/>
-      <c r="E236" s="130"/>
+      <c r="D236" s="124"/>
+      <c r="E236" s="124"/>
       <c r="F236" s="21" t="s">
         <v>250</v>
       </c>
@@ -9581,17 +9579,17 @@
       </c>
     </row>
     <row r="237" spans="1:7">
-      <c r="A237" s="146" t="s">
+      <c r="A237" s="133" t="s">
         <v>264</v>
       </c>
-      <c r="B237" s="130" t="s">
+      <c r="B237" s="124" t="s">
         <v>265</v>
       </c>
-      <c r="C237" s="129" t="s">
+      <c r="C237" s="127" t="s">
         <v>266</v>
       </c>
-      <c r="D237" s="130"/>
-      <c r="E237" s="130"/>
+      <c r="D237" s="124"/>
+      <c r="E237" s="124"/>
       <c r="F237" s="21" t="s">
         <v>248</v>
       </c>
@@ -9600,13 +9598,13 @@
       </c>
     </row>
     <row r="238" spans="1:7">
-      <c r="A238" s="146"/>
-      <c r="B238" s="130"/>
-      <c r="C238" s="130" t="s">
+      <c r="A238" s="133"/>
+      <c r="B238" s="124"/>
+      <c r="C238" s="124" t="s">
         <v>267</v>
       </c>
-      <c r="D238" s="130"/>
-      <c r="E238" s="130"/>
+      <c r="D238" s="124"/>
+      <c r="E238" s="124"/>
       <c r="F238" s="21" t="s">
         <v>250</v>
       </c>
@@ -9615,15 +9613,15 @@
       </c>
     </row>
     <row r="239" spans="1:7">
-      <c r="A239" s="146"/>
-      <c r="B239" s="130" t="s">
+      <c r="A239" s="133"/>
+      <c r="B239" s="124" t="s">
         <v>268</v>
       </c>
-      <c r="C239" s="129" t="s">
+      <c r="C239" s="127" t="s">
         <v>269</v>
       </c>
-      <c r="D239" s="130"/>
-      <c r="E239" s="130"/>
+      <c r="D239" s="124"/>
+      <c r="E239" s="124"/>
       <c r="F239" s="21" t="s">
         <v>248</v>
       </c>
@@ -9632,13 +9630,13 @@
       </c>
     </row>
     <row r="240" spans="1:7">
-      <c r="A240" s="147"/>
-      <c r="B240" s="131"/>
-      <c r="C240" s="131" t="s">
+      <c r="A240" s="134"/>
+      <c r="B240" s="135"/>
+      <c r="C240" s="135" t="s">
         <v>270</v>
       </c>
-      <c r="D240" s="131"/>
-      <c r="E240" s="131"/>
+      <c r="D240" s="135"/>
+      <c r="E240" s="135"/>
       <c r="F240" s="26" t="s">
         <v>250</v>
       </c>
@@ -9677,12 +9675,12 @@
       <c r="A245" s="35" t="s">
         <v>273</v>
       </c>
-      <c r="B245" s="132" t="s">
+      <c r="B245" s="141" t="s">
         <v>274</v>
       </c>
-      <c r="C245" s="132"/>
-      <c r="D245" s="132"/>
-      <c r="E245" s="132"/>
+      <c r="C245" s="141"/>
+      <c r="D245" s="141"/>
+      <c r="E245" s="141"/>
       <c r="F245" s="36" t="s">
         <v>275</v>
       </c>
@@ -9694,12 +9692,12 @@
       <c r="A246" s="38" t="s">
         <v>277</v>
       </c>
-      <c r="B246" s="133" t="s">
+      <c r="B246" s="142" t="s">
         <v>278</v>
       </c>
-      <c r="C246" s="134"/>
-      <c r="D246" s="134"/>
-      <c r="E246" s="134"/>
+      <c r="C246" s="126"/>
+      <c r="D246" s="126"/>
+      <c r="E246" s="126"/>
       <c r="F246" s="39" t="s">
         <v>154</v>
       </c>
@@ -9711,12 +9709,12 @@
       <c r="A247" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="B247" s="135" t="s">
+      <c r="B247" s="137" t="s">
         <v>280</v>
       </c>
-      <c r="C247" s="136"/>
-      <c r="D247" s="136"/>
-      <c r="E247" s="137"/>
+      <c r="C247" s="138"/>
+      <c r="D247" s="138"/>
+      <c r="E247" s="139"/>
       <c r="F247" s="9" t="s">
         <v>249</v>
       </c>
@@ -9728,12 +9726,12 @@
       <c r="A248" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="B248" s="135" t="s">
+      <c r="B248" s="137" t="s">
         <v>282</v>
       </c>
-      <c r="C248" s="136"/>
-      <c r="D248" s="136"/>
-      <c r="E248" s="137"/>
+      <c r="C248" s="138"/>
+      <c r="D248" s="138"/>
+      <c r="E248" s="139"/>
       <c r="F248" s="13" t="s">
         <v>249</v>
       </c>
@@ -9745,12 +9743,12 @@
       <c r="A249" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="B249" s="138" t="s">
+      <c r="B249" s="123" t="s">
         <v>284</v>
       </c>
-      <c r="C249" s="131"/>
-      <c r="D249" s="131"/>
-      <c r="E249" s="131"/>
+      <c r="C249" s="135"/>
+      <c r="D249" s="135"/>
+      <c r="E249" s="135"/>
       <c r="F249" s="15" t="s">
         <v>249</v>
       </c>
@@ -9795,11 +9793,11 @@
       <c r="C254" s="17" t="s">
         <v>289</v>
       </c>
-      <c r="D254" s="139" t="s">
+      <c r="D254" s="140" t="s">
         <v>290</v>
       </c>
-      <c r="E254" s="139"/>
-      <c r="F254" s="139"/>
+      <c r="E254" s="140"/>
+      <c r="F254" s="140"/>
       <c r="G254" s="47"/>
     </row>
     <row r="255" spans="1:7">
@@ -9812,11 +9810,11 @@
       <c r="C255" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="D255" s="140" t="s">
+      <c r="D255" s="136" t="s">
         <v>291</v>
       </c>
-      <c r="E255" s="140"/>
-      <c r="F255" s="140"/>
+      <c r="E255" s="136"/>
+      <c r="F255" s="136"/>
       <c r="G255" s="32"/>
     </row>
     <row r="256" spans="1:7">
@@ -9829,11 +9827,11 @@
       <c r="C256" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="D256" s="140" t="s">
+      <c r="D256" s="136" t="s">
         <v>292</v>
       </c>
-      <c r="E256" s="140"/>
-      <c r="F256" s="140"/>
+      <c r="E256" s="136"/>
+      <c r="F256" s="136"/>
       <c r="G256" s="32"/>
     </row>
     <row r="257" spans="1:7">
@@ -9846,11 +9844,11 @@
       <c r="C257" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="D257" s="140" t="s">
+      <c r="D257" s="136" t="s">
         <v>293</v>
       </c>
-      <c r="E257" s="140"/>
-      <c r="F257" s="140"/>
+      <c r="E257" s="136"/>
+      <c r="F257" s="136"/>
       <c r="G257" s="32"/>
     </row>
     <row r="258" spans="1:7">
@@ -9863,11 +9861,11 @@
       <c r="C258" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="D258" s="140" t="s">
+      <c r="D258" s="136" t="s">
         <v>294</v>
       </c>
-      <c r="E258" s="140"/>
-      <c r="F258" s="140"/>
+      <c r="E258" s="136"/>
+      <c r="F258" s="136"/>
       <c r="G258" s="32"/>
     </row>
     <row r="259" spans="1:7">
@@ -9880,11 +9878,11 @@
       <c r="C259" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="D259" s="140" t="s">
+      <c r="D259" s="136" t="s">
         <v>295</v>
       </c>
-      <c r="E259" s="140"/>
-      <c r="F259" s="140"/>
+      <c r="E259" s="136"/>
+      <c r="F259" s="136"/>
       <c r="G259" s="32"/>
     </row>
     <row r="260" spans="1:7">
@@ -9897,11 +9895,11 @@
       <c r="C260" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="D260" s="141" t="s">
+      <c r="D260" s="128" t="s">
         <v>296</v>
       </c>
-      <c r="E260" s="142"/>
-      <c r="F260" s="143"/>
+      <c r="E260" s="129"/>
+      <c r="F260" s="130"/>
       <c r="G260" s="33"/>
     </row>
     <row r="261" spans="1:7">
@@ -9914,11 +9912,11 @@
       <c r="C261" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="D261" s="141" t="s">
+      <c r="D261" s="128" t="s">
         <v>297</v>
       </c>
-      <c r="E261" s="142"/>
-      <c r="F261" s="143"/>
+      <c r="E261" s="129"/>
+      <c r="F261" s="130"/>
       <c r="G261" s="33"/>
     </row>
     <row r="262" spans="1:7">
@@ -9931,11 +9929,11 @@
       <c r="C262" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="D262" s="141" t="s">
+      <c r="D262" s="128" t="s">
         <v>298</v>
       </c>
-      <c r="E262" s="142"/>
-      <c r="F262" s="143"/>
+      <c r="E262" s="129"/>
+      <c r="F262" s="130"/>
       <c r="G262" s="33"/>
     </row>
     <row r="263" spans="1:7">
@@ -10135,11 +10133,11 @@
       <c r="C274" s="26" t="s">
         <v>289</v>
       </c>
-      <c r="D274" s="144" t="s">
+      <c r="D274" s="131" t="s">
         <v>399</v>
       </c>
-      <c r="E274" s="145"/>
-      <c r="F274" s="145"/>
+      <c r="E274" s="132"/>
+      <c r="F274" s="132"/>
       <c r="G274" s="34"/>
     </row>
   </sheetData>
@@ -10152,16 +10150,31 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="51">
-    <mergeCell ref="B198:B200"/>
-    <mergeCell ref="B201:B207"/>
-    <mergeCell ref="B225:B226"/>
-    <mergeCell ref="B227:B228"/>
-    <mergeCell ref="B229:B230"/>
-    <mergeCell ref="B149:B162"/>
-    <mergeCell ref="B163:B169"/>
-    <mergeCell ref="B170:B180"/>
-    <mergeCell ref="B181:B188"/>
-    <mergeCell ref="B189:B197"/>
+    <mergeCell ref="F111:N111"/>
+    <mergeCell ref="C224:E224"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C226:E226"/>
+    <mergeCell ref="C227:E227"/>
+    <mergeCell ref="C228:E228"/>
+    <mergeCell ref="C229:E229"/>
+    <mergeCell ref="C230:E230"/>
+    <mergeCell ref="C231:E231"/>
+    <mergeCell ref="C232:E232"/>
+    <mergeCell ref="C233:E233"/>
+    <mergeCell ref="C234:E234"/>
+    <mergeCell ref="C235:E235"/>
+    <mergeCell ref="C236:E236"/>
+    <mergeCell ref="C237:E237"/>
+    <mergeCell ref="C238:E238"/>
+    <mergeCell ref="C239:E239"/>
+    <mergeCell ref="C240:E240"/>
+    <mergeCell ref="B245:E245"/>
+    <mergeCell ref="B246:E246"/>
+    <mergeCell ref="B247:E247"/>
+    <mergeCell ref="B248:E248"/>
+    <mergeCell ref="B249:E249"/>
+    <mergeCell ref="D254:F254"/>
+    <mergeCell ref="D255:F255"/>
     <mergeCell ref="D261:F261"/>
     <mergeCell ref="D262:F262"/>
     <mergeCell ref="D274:F274"/>
@@ -10178,31 +10191,16 @@
     <mergeCell ref="D258:F258"/>
     <mergeCell ref="D259:F259"/>
     <mergeCell ref="D260:F260"/>
-    <mergeCell ref="B247:E247"/>
-    <mergeCell ref="B248:E248"/>
-    <mergeCell ref="B249:E249"/>
-    <mergeCell ref="D254:F254"/>
-    <mergeCell ref="D255:F255"/>
-    <mergeCell ref="C238:E238"/>
-    <mergeCell ref="C239:E239"/>
-    <mergeCell ref="C240:E240"/>
-    <mergeCell ref="B245:E245"/>
-    <mergeCell ref="B246:E246"/>
-    <mergeCell ref="C233:E233"/>
-    <mergeCell ref="C234:E234"/>
-    <mergeCell ref="C235:E235"/>
-    <mergeCell ref="C236:E236"/>
-    <mergeCell ref="C237:E237"/>
-    <mergeCell ref="C228:E228"/>
-    <mergeCell ref="C229:E229"/>
-    <mergeCell ref="C230:E230"/>
-    <mergeCell ref="C231:E231"/>
-    <mergeCell ref="C232:E232"/>
-    <mergeCell ref="F111:N111"/>
-    <mergeCell ref="C224:E224"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C226:E226"/>
-    <mergeCell ref="C227:E227"/>
+    <mergeCell ref="B149:B162"/>
+    <mergeCell ref="B163:B169"/>
+    <mergeCell ref="B170:B180"/>
+    <mergeCell ref="B181:B188"/>
+    <mergeCell ref="B189:B197"/>
+    <mergeCell ref="B198:B200"/>
+    <mergeCell ref="B201:B207"/>
+    <mergeCell ref="B225:B226"/>
+    <mergeCell ref="B227:B228"/>
+    <mergeCell ref="B229:B230"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -10219,7 +10217,7 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -10228,16 +10226,16 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="D24" sqref="D24"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="E26" sqref="E26"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="D24" sqref="D24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
i420--auto greed mode and local env override update
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_example/standard_suite/diamond_regression.xlsx
+++ b/tmp_client/doc/TMP_example/standard_suite/diamond_regression.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\repository\tmp_client\doc\TMP_example\standard_suite\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2059E9-9BBB-4807-8736-50210267FECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="suite" sheetId="1" r:id="rId1"/>
@@ -25,15 +26,15 @@
   </definedNames>
   <calcPr calcId="144525"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="2391" yWindow="-9" windowWidth="2418" windowHeight="1318" activeSheetId="3" showComments="commIndAndComment"/>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
     <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
-    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="2391" yWindow="-9" windowWidth="2418" windowHeight="1318" activeSheetId="3" showComments="commIndAndComment"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="408">
   <si>
     <t>[suite_info]</t>
   </si>
@@ -1269,21 +1270,49 @@
   <si>
     <t>est_mem</t>
   </si>
+  <si>
+    <t>greed_mode</t>
+  </si>
+  <si>
+    <t>false,true, auto</t>
+  </si>
+  <si>
+    <t>Task/case will be take and run no matter system resource ready or not</t>
+  </si>
+  <si>
+    <t>greed mode support for client task take</t>
+  </si>
+  <si>
+    <t>local</t>
+  </si>
+  <si>
+    <t>With this option, force override</t>
+  </si>
+  <si>
+    <t>Works for cmd like options, for other options: case &gt; suite</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00_);[Red]\(0.00\)"/>
     <numFmt numFmtId="165" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1862,189 +1891,189 @@
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="37" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="37" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="5" applyNumberFormat="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="5" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="5" applyNumberFormat="1">
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="5" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="5" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="7" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="7" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="12" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="12" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="13" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="13" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="14" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="14" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="15" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="15" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
@@ -2056,10 +2085,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2071,7 +2100,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2089,11 +2118,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
@@ -2102,10 +2131,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2114,19 +2143,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1">
@@ -2135,10 +2164,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2148,7 +2177,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2157,185 +2186,216 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="5" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="5" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="5" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="5" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="5" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="5" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="33" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="34" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="36" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="33" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="34" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="36" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Check Cell" xfId="4" builtinId="23"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="5"/>
-    <cellStyle name="Normal 3" xfId="6"/>
-    <cellStyle name="Normal 4" xfId="7"/>
-    <cellStyle name="Normal 5" xfId="8"/>
-    <cellStyle name="Normal 6" xfId="3"/>
-    <cellStyle name="Note 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 5" xfId="8" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 6" xfId="3" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Note 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -2367,7 +2427,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4564,7 +4630,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -4619,7 +4691,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="Add Test Case - TestRail - Mozilla Firefox"/>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Add Test Case - TestRail - Mozilla Firefox">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4653,24 +4731,30 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>213</xdr:row>
+      <xdr:row>215</xdr:row>
       <xdr:rowOff>140970</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>904875</xdr:colOff>
-      <xdr:row>221</xdr:row>
+      <xdr:row>223</xdr:row>
       <xdr:rowOff>102870</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1341755" y="34699575"/>
-          <a:ext cx="6244590" cy="1424940"/>
+          <a:off x="1302854" y="41404927"/>
+          <a:ext cx="6509717" cy="1485900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4783,7 +4867,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="6" name="Straight Arrow Connector 5"/>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -4830,7 +4920,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Straight Arrow Connector 6"/>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -4863,27 +4959,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{77E4B79D-4F2B-4D50-B486-0C91AC1CF622}">
-  <header guid="{77E4B79D-4F2B-4D50-B486-0C91AC1CF622}" dateTime="2021-12-29T10:58:06" maxSheetId="5" userName="Jason Wang" r:id="rId1">
-    <sheetIdMap count="4">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
-</headers>
-</file>
-
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
-</file>
-
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4962,6 +5037,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -4997,6 +5089,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5172,13 +5281,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15" style="58" customWidth="1"/>
     <col min="2" max="2" width="28" style="58" customWidth="1"/>
@@ -5261,8 +5372,8 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="B4" sqref="B4"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="B41" sqref="B41"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -5271,8 +5382,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="B41" sqref="B41"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="B4" sqref="B4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -5283,7 +5394,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AF46"/>
   <sheetViews>
@@ -5294,73 +5405,73 @@
       <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="58" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="58" customWidth="1"/>
     <col min="2" max="2" width="9" style="58" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" style="58" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="58" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" style="58" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="58" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" style="58" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" style="58" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" style="58" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="58" customWidth="1"/>
     <col min="7" max="7" width="24" style="58" customWidth="1"/>
     <col min="8" max="8" width="37" style="58" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="58" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" style="58" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" style="58" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" style="58" customWidth="1"/>
     <col min="11" max="11" width="12" style="58" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" style="59" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" style="59" customWidth="1"/>
+    <col min="12" max="12" width="9.5546875" style="59" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" style="59" customWidth="1"/>
     <col min="14" max="14" width="38" style="58" customWidth="1"/>
-    <col min="15" max="15" width="19.42578125" style="58" customWidth="1"/>
-    <col min="16" max="16" width="30.28515625" style="58" customWidth="1"/>
-    <col min="17" max="17" width="17.28515625" style="58" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" style="58" customWidth="1"/>
+    <col min="15" max="15" width="19.44140625" style="58" customWidth="1"/>
+    <col min="16" max="16" width="30.33203125" style="58" customWidth="1"/>
+    <col min="17" max="17" width="17.33203125" style="58" customWidth="1"/>
+    <col min="18" max="18" width="15.44140625" style="58" customWidth="1"/>
     <col min="19" max="19" width="13" style="58" customWidth="1"/>
-    <col min="20" max="21" width="9.7109375" style="58" customWidth="1"/>
-    <col min="22" max="22" width="9.42578125" style="58" customWidth="1"/>
+    <col min="20" max="21" width="9.6640625" style="58" customWidth="1"/>
+    <col min="22" max="22" width="9.44140625" style="58" customWidth="1"/>
     <col min="23" max="23" width="11" style="58" customWidth="1"/>
-    <col min="24" max="24" width="11.7109375" style="58" customWidth="1"/>
+    <col min="24" max="24" width="11.6640625" style="58" customWidth="1"/>
     <col min="25" max="30" width="9" style="58"/>
-    <col min="31" max="31" width="10.140625" style="58" customWidth="1"/>
+    <col min="31" max="31" width="10.109375" style="58" customWidth="1"/>
     <col min="32" max="16384" width="9" style="58"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" s="57" customFormat="1">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="123" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114"/>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="114"/>
-      <c r="N1" s="114"/>
-      <c r="O1" s="114"/>
-      <c r="P1" s="114"/>
-      <c r="Q1" s="114"/>
-      <c r="R1" s="114"/>
-      <c r="S1" s="114"/>
-      <c r="T1" s="114"/>
-      <c r="U1" s="114"/>
-      <c r="V1" s="114"/>
-      <c r="W1" s="114"/>
-      <c r="X1" s="115"/>
-      <c r="Y1" s="116" t="s">
+      <c r="B1" s="124"/>
+      <c r="C1" s="124"/>
+      <c r="D1" s="124"/>
+      <c r="E1" s="124"/>
+      <c r="F1" s="124"/>
+      <c r="G1" s="124"/>
+      <c r="H1" s="124"/>
+      <c r="I1" s="124"/>
+      <c r="J1" s="124"/>
+      <c r="K1" s="124"/>
+      <c r="L1" s="124"/>
+      <c r="M1" s="124"/>
+      <c r="N1" s="124"/>
+      <c r="O1" s="124"/>
+      <c r="P1" s="124"/>
+      <c r="Q1" s="124"/>
+      <c r="R1" s="124"/>
+      <c r="S1" s="124"/>
+      <c r="T1" s="124"/>
+      <c r="U1" s="124"/>
+      <c r="V1" s="124"/>
+      <c r="W1" s="124"/>
+      <c r="X1" s="125"/>
+      <c r="Y1" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="Z1" s="116"/>
-      <c r="AA1" s="116"/>
-      <c r="AB1" s="116"/>
-      <c r="AC1" s="116"/>
-      <c r="AD1" s="116"/>
-      <c r="AE1" s="116"/>
-      <c r="AF1" s="116"/>
+      <c r="Z1" s="126"/>
+      <c r="AA1" s="126"/>
+      <c r="AB1" s="126"/>
+      <c r="AC1" s="126"/>
+      <c r="AD1" s="126"/>
+      <c r="AE1" s="126"/>
+      <c r="AF1" s="126"/>
     </row>
     <row r="2" spans="1:32" s="57" customFormat="1">
       <c r="A2" s="60" t="s">
@@ -6879,28 +6990,28 @@
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="Sju3pjEnjegba3BrZLImZ+xscQ9MLEq+i8mDO7rXFn4S3yXv8zWb4HaF0uC2YruSs8wkV8FCIxY7a0fvnwVXFw==" saltValue="mZmUchosJ60PlKqUXOSzGQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <autoFilter ref="A2:AF46"/>
+  <autoFilter ref="A2:AF46" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <customSheetViews>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen"/>
-      <selection activeCell="H23" sqref="H23"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="85" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
-      <autoFilter ref="A2:Y2"/>
+      <autoFilter ref="A2:AF46" xr:uid="{8BA986C3-86FF-43CA-A524-ABF0F8318CAE}"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen"/>
       <selection activeCell="C23" sqref="C23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
-      <autoFilter ref="A2:Y2"/>
+      <autoFilter ref="A2:Y2" xr:uid="{0BFEF7DE-702D-4114-BA09-6A436D06221C}"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="85" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen"/>
+      <selection activeCell="H23" sqref="H23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
-      <autoFilter ref="A2:AF46"/>
+      <autoFilter ref="A2:Y2" xr:uid="{20938BFE-4123-429A-828B-1E4E93851D08}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -6908,10 +7019,10 @@
     <mergeCell ref="Y1:AF1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:I1 N1:X1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:I1 N1:X1" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$F$119:$J$119</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y1:AC1 AF1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y1:AC1 AF1" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -6920,55 +7031,55 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>description!$F$122:$H$122</xm:f>
           </x14:formula1>
           <xm:sqref>K1:K1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
           <x14:formula1>
             <xm:f>description!$F$113:$G$113</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
           <x14:formula1>
             <xm:f>description!$F$123:$H$123</xm:f>
           </x14:formula1>
           <xm:sqref>L1:L1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
           <x14:formula1>
             <xm:f>description!$F$117:$H$117</xm:f>
           </x14:formula1>
           <xm:sqref>F2:F1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
           <x14:formula1>
             <xm:f>description!$F$142:$H$142</xm:f>
           </x14:formula1>
           <xm:sqref>AD1:AD1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000007000000}">
           <x14:formula1>
             <xm:f>description!$F$120:$K$120</xm:f>
           </x14:formula1>
           <xm:sqref>I2:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000008000000}">
           <x14:formula1>
             <xm:f>description!$E$121:$K$121</xm:f>
           </x14:formula1>
           <xm:sqref>J1:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000009000000}">
           <x14:formula1>
             <xm:f>description!$F$143:$H$143</xm:f>
           </x14:formula1>
           <xm:sqref>AE1:AE1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000A000000}">
           <x14:formula1>
             <xm:f>description!$F$124:$H$124</xm:f>
           </x14:formula1>
@@ -6981,26 +7092,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:N274"/>
+  <dimension ref="A1:N277"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D173" sqref="D173"/>
+    <sheetView topLeftCell="A170" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A189" sqref="A189"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.88671875" style="1" customWidth="1"/>
     <col min="6" max="6" width="32" style="1" customWidth="1"/>
-    <col min="7" max="7" width="33.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="28.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="33.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="28.109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -7009,7 +7120,7 @@
         <v>133</v>
       </c>
       <c r="B1" s="2">
-        <v>1.24</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -7017,7 +7128,7 @@
         <v>29</v>
       </c>
       <c r="B2" s="3">
-        <v>44559</v>
+        <v>44755</v>
       </c>
     </row>
     <row r="107" spans="1:14" ht="12.75" customHeight="1"/>
@@ -7047,17 +7158,17 @@
       <c r="E111" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="F111" s="148" t="s">
+      <c r="F111" s="127" t="s">
         <v>140</v>
       </c>
-      <c r="G111" s="149"/>
-      <c r="H111" s="149"/>
-      <c r="I111" s="149"/>
-      <c r="J111" s="149"/>
-      <c r="K111" s="149"/>
-      <c r="L111" s="149"/>
-      <c r="M111" s="149"/>
-      <c r="N111" s="150"/>
+      <c r="G111" s="128"/>
+      <c r="H111" s="128"/>
+      <c r="I111" s="128"/>
+      <c r="J111" s="128"/>
+      <c r="K111" s="128"/>
+      <c r="L111" s="128"/>
+      <c r="M111" s="128"/>
+      <c r="N111" s="129"/>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="6" t="s">
@@ -7977,7 +8088,7 @@
       <c r="A149" s="19">
         <v>1</v>
       </c>
-      <c r="B149" s="117" t="s">
+      <c r="B149" s="158" t="s">
         <v>4</v>
       </c>
       <c r="C149" s="62" t="s">
@@ -8003,7 +8114,7 @@
       <c r="A150" s="19">
         <v>2</v>
       </c>
-      <c r="B150" s="119"/>
+      <c r="B150" s="159"/>
       <c r="C150" s="21" t="s">
         <v>173</v>
       </c>
@@ -8025,7 +8136,7 @@
       <c r="A151" s="19">
         <v>3</v>
       </c>
-      <c r="B151" s="119"/>
+      <c r="B151" s="159"/>
       <c r="C151" s="21" t="s">
         <v>18</v>
       </c>
@@ -8045,7 +8156,7 @@
       <c r="A152" s="19">
         <v>4</v>
       </c>
-      <c r="B152" s="119"/>
+      <c r="B152" s="159"/>
       <c r="C152" s="21" t="s">
         <v>175</v>
       </c>
@@ -8069,7 +8180,7 @@
       <c r="A153" s="19">
         <v>5</v>
       </c>
-      <c r="B153" s="119"/>
+      <c r="B153" s="159"/>
       <c r="C153" s="62" t="s">
         <v>177</v>
       </c>
@@ -8093,7 +8204,7 @@
       <c r="A154" s="19">
         <v>6</v>
       </c>
-      <c r="B154" s="119"/>
+      <c r="B154" s="159"/>
       <c r="C154" s="62" t="s">
         <v>181</v>
       </c>
@@ -8117,7 +8228,7 @@
       <c r="A155" s="19">
         <v>7</v>
       </c>
-      <c r="B155" s="119"/>
+      <c r="B155" s="159"/>
       <c r="C155" s="21" t="s">
         <v>183</v>
       </c>
@@ -8139,7 +8250,7 @@
       <c r="A156" s="19">
         <v>8</v>
       </c>
-      <c r="B156" s="119"/>
+      <c r="B156" s="159"/>
       <c r="C156" s="62" t="s">
         <v>184</v>
       </c>
@@ -8163,7 +8274,7 @@
       <c r="A157" s="19">
         <v>9</v>
       </c>
-      <c r="B157" s="119"/>
+      <c r="B157" s="159"/>
       <c r="C157" s="62" t="s">
         <v>185</v>
       </c>
@@ -8187,7 +8298,7 @@
       <c r="A158" s="19">
         <v>10</v>
       </c>
-      <c r="B158" s="119"/>
+      <c r="B158" s="159"/>
       <c r="C158" s="21" t="s">
         <v>186</v>
       </c>
@@ -8211,7 +8322,7 @@
       <c r="A159" s="112">
         <v>11</v>
       </c>
-      <c r="B159" s="119"/>
+      <c r="B159" s="159"/>
       <c r="C159" s="21" t="s">
         <v>187</v>
       </c>
@@ -8235,7 +8346,7 @@
       <c r="A160" s="112">
         <v>12</v>
       </c>
-      <c r="B160" s="119"/>
+      <c r="B160" s="159"/>
       <c r="C160" s="21" t="s">
         <v>189</v>
       </c>
@@ -8257,7 +8368,7 @@
       <c r="A161" s="112">
         <v>13</v>
       </c>
-      <c r="B161" s="119"/>
+      <c r="B161" s="159"/>
       <c r="C161" s="111" t="s">
         <v>400</v>
       </c>
@@ -8279,7 +8390,7 @@
       <c r="A162" s="112">
         <v>14</v>
       </c>
-      <c r="B162" s="126"/>
+      <c r="B162" s="144"/>
       <c r="C162" s="21" t="s">
         <v>193</v>
       </c>
@@ -8303,7 +8414,7 @@
       <c r="A163" s="112">
         <v>15</v>
       </c>
-      <c r="B163" s="127" t="s">
+      <c r="B163" s="139" t="s">
         <v>5</v>
       </c>
       <c r="C163" s="21" t="s">
@@ -8330,7 +8441,7 @@
       <c r="A164" s="112">
         <v>16</v>
       </c>
-      <c r="B164" s="127"/>
+      <c r="B164" s="139"/>
       <c r="C164" s="89" t="s">
         <v>341</v>
       </c>
@@ -8354,7 +8465,7 @@
       <c r="A165" s="112">
         <v>17</v>
       </c>
-      <c r="B165" s="127"/>
+      <c r="B165" s="139"/>
       <c r="C165" s="89" t="s">
         <v>344</v>
       </c>
@@ -8378,7 +8489,7 @@
       <c r="A166" s="112">
         <v>18</v>
       </c>
-      <c r="B166" s="127"/>
+      <c r="B166" s="139"/>
       <c r="C166" s="100" t="s">
         <v>377</v>
       </c>
@@ -8402,7 +8513,7 @@
       <c r="A167" s="112">
         <v>19</v>
       </c>
-      <c r="B167" s="127"/>
+      <c r="B167" s="139"/>
       <c r="C167" s="100" t="s">
         <v>378</v>
       </c>
@@ -8424,7 +8535,7 @@
       <c r="A168" s="112">
         <v>20</v>
       </c>
-      <c r="B168" s="127"/>
+      <c r="B168" s="139"/>
       <c r="C168" s="100" t="s">
         <v>379</v>
       </c>
@@ -8443,424 +8554,430 @@
       <c r="H168" s="68"/>
     </row>
     <row r="169" spans="1:9">
-      <c r="A169" s="112">
+      <c r="A169" s="118">
         <v>21</v>
       </c>
-      <c r="B169" s="124"/>
-      <c r="C169" s="83" t="s">
+      <c r="B169" s="139"/>
+      <c r="C169" s="121" t="s">
         <v>200</v>
       </c>
-      <c r="D169" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E169" s="87" t="s">
-        <v>169</v>
-      </c>
-      <c r="F169" s="90"/>
-      <c r="G169" s="89" t="s">
+      <c r="D169" s="117" t="s">
+        <v>169</v>
+      </c>
+      <c r="E169" s="117" t="s">
+        <v>169</v>
+      </c>
+      <c r="F169" s="116"/>
+      <c r="G169" s="100" t="s">
         <v>171</v>
       </c>
       <c r="H169" s="68" t="s">
         <v>201</v>
       </c>
-      <c r="I169" s="85"/>
     </row>
     <row r="170" spans="1:9">
-      <c r="A170" s="112">
+      <c r="A170" s="118">
         <v>22</v>
       </c>
-      <c r="B170" s="117" t="s">
+      <c r="B170" s="140"/>
+      <c r="C170" s="83" t="s">
+        <v>204</v>
+      </c>
+      <c r="D170" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E170" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="F170" s="90" t="s">
+        <v>405</v>
+      </c>
+      <c r="G170" s="89" t="s">
+        <v>205</v>
+      </c>
+      <c r="H170" s="122" t="s">
+        <v>406</v>
+      </c>
+      <c r="I170" s="85"/>
+    </row>
+    <row r="171" spans="1:9">
+      <c r="A171" s="118">
+        <v>23</v>
+      </c>
+      <c r="B171" s="158" t="s">
         <v>6</v>
       </c>
-      <c r="C170" s="89" t="s">
+      <c r="C171" s="89" t="s">
         <v>202</v>
       </c>
-      <c r="D170" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E170" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F170" s="89" t="s">
+      <c r="D171" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E171" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F171" s="89" t="s">
         <v>203</v>
       </c>
-      <c r="G170" s="66" t="s">
+      <c r="G171" s="66" t="s">
         <v>171</v>
       </c>
-      <c r="H170" s="68" t="s">
+      <c r="H171" s="68" t="s">
         <v>353</v>
       </c>
-      <c r="I170" s="85"/>
-    </row>
-    <row r="171" spans="1:9">
-      <c r="A171" s="112">
-        <v>23</v>
-      </c>
-      <c r="B171" s="118"/>
-      <c r="C171" s="100" t="s">
+      <c r="I171" s="85"/>
+    </row>
+    <row r="172" spans="1:9">
+      <c r="A172" s="118">
+        <v>24</v>
+      </c>
+      <c r="B172" s="160"/>
+      <c r="C172" s="100" t="s">
         <v>347</v>
       </c>
-      <c r="D171" s="87" t="s">
-        <v>169</v>
-      </c>
-      <c r="E171" s="87" t="s">
-        <v>169</v>
-      </c>
-      <c r="F171" s="89" t="s">
+      <c r="D172" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="E172" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="F172" s="89" t="s">
         <v>349</v>
-      </c>
-      <c r="G171" s="89" t="s">
-        <v>171</v>
-      </c>
-      <c r="H171" s="68" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="172" spans="1:9">
-      <c r="A172" s="112">
-        <v>24</v>
-      </c>
-      <c r="B172" s="118"/>
-      <c r="C172" s="100" t="s">
-        <v>348</v>
-      </c>
-      <c r="D172" s="87" t="s">
-        <v>169</v>
-      </c>
-      <c r="E172" s="87" t="s">
-        <v>169</v>
-      </c>
-      <c r="F172" s="89" t="s">
-        <v>350</v>
       </c>
       <c r="G172" s="89" t="s">
         <v>171</v>
       </c>
-      <c r="H172" s="96" t="s">
+      <c r="H172" s="68" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9">
+      <c r="A173" s="118">
+        <v>25</v>
+      </c>
+      <c r="B173" s="160"/>
+      <c r="C173" s="100" t="s">
+        <v>348</v>
+      </c>
+      <c r="D173" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="E173" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="F173" s="89" t="s">
+        <v>350</v>
+      </c>
+      <c r="G173" s="89" t="s">
+        <v>171</v>
+      </c>
+      <c r="H173" s="96" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="173" spans="1:9">
-      <c r="A173" s="112">
-        <v>25</v>
-      </c>
-      <c r="B173" s="118"/>
-      <c r="C173" s="100" t="s">
+    <row r="174" spans="1:9">
+      <c r="A174" s="118">
+        <v>26</v>
+      </c>
+      <c r="B174" s="160"/>
+      <c r="C174" s="100" t="s">
         <v>382</v>
       </c>
-      <c r="D173" s="97" t="s">
-        <v>169</v>
-      </c>
-      <c r="E173" s="97" t="s">
-        <v>169</v>
-      </c>
-      <c r="F173" s="98" t="s">
+      <c r="D174" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="E174" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="F174" s="98" t="s">
         <v>350</v>
       </c>
-      <c r="G173" s="98" t="s">
+      <c r="G174" s="98" t="s">
         <v>171</v>
       </c>
-      <c r="H173" s="96"/>
-    </row>
-    <row r="174" spans="1:9">
-      <c r="A174" s="112">
-        <v>26</v>
-      </c>
-      <c r="B174" s="118"/>
-      <c r="C174" s="100" t="s">
+      <c r="H174" s="96"/>
+    </row>
+    <row r="175" spans="1:9">
+      <c r="A175" s="118">
+        <v>27</v>
+      </c>
+      <c r="B175" s="160"/>
+      <c r="C175" s="100" t="s">
         <v>369</v>
       </c>
-      <c r="D174" s="87" t="s">
-        <v>169</v>
-      </c>
-      <c r="E174" s="87" t="s">
-        <v>169</v>
-      </c>
-      <c r="F174" s="89" t="s">
+      <c r="D175" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="E175" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="F175" s="89" t="s">
         <v>350</v>
       </c>
-      <c r="G174" s="89" t="s">
+      <c r="G175" s="89" t="s">
         <v>171</v>
       </c>
-      <c r="H174" s="68"/>
-    </row>
-    <row r="175" spans="1:9">
-      <c r="A175" s="112">
-        <v>27</v>
-      </c>
-      <c r="B175" s="118"/>
-      <c r="C175" s="93" t="s">
+      <c r="H175" s="68"/>
+    </row>
+    <row r="176" spans="1:9">
+      <c r="A176" s="118">
+        <v>28</v>
+      </c>
+      <c r="B176" s="160"/>
+      <c r="C176" s="93" t="s">
         <v>366</v>
       </c>
-      <c r="D175" s="92"/>
-      <c r="E175" s="92" t="s">
-        <v>169</v>
-      </c>
-      <c r="F175" s="93" t="s">
+      <c r="D176" s="92"/>
+      <c r="E176" s="92" t="s">
+        <v>169</v>
+      </c>
+      <c r="F176" s="93" t="s">
         <v>367</v>
       </c>
-      <c r="G175" s="93" t="s">
+      <c r="G176" s="93" t="s">
         <v>171</v>
       </c>
-      <c r="H175" s="96" t="s">
+      <c r="H176" s="96" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="176" spans="1:9">
-      <c r="A176" s="112">
-        <v>28</v>
-      </c>
-      <c r="B176" s="118"/>
-      <c r="C176" s="102" t="s">
+    <row r="177" spans="1:8">
+      <c r="A177" s="118">
+        <v>29</v>
+      </c>
+      <c r="B177" s="160"/>
+      <c r="C177" s="102" t="s">
         <v>376</v>
       </c>
-      <c r="D176" s="97" t="s">
-        <v>169</v>
-      </c>
-      <c r="E176" s="97" t="s">
-        <v>169</v>
-      </c>
-      <c r="F176" s="102" t="s">
+      <c r="D177" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="E177" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="F177" s="102" t="s">
         <v>373</v>
       </c>
-      <c r="G176" s="108" t="s">
+      <c r="G177" s="108" t="s">
         <v>386</v>
       </c>
-      <c r="H176" s="96" t="s">
+      <c r="H177" s="96" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="177" spans="1:8">
-      <c r="A177" s="112">
-        <v>29</v>
-      </c>
-      <c r="B177" s="118"/>
-      <c r="C177" s="91" t="s">
+    <row r="178" spans="1:8">
+      <c r="A178" s="118">
+        <v>30</v>
+      </c>
+      <c r="B178" s="160"/>
+      <c r="C178" s="91" t="s">
         <v>364</v>
       </c>
-      <c r="D177" s="100" t="s">
-        <v>169</v>
-      </c>
-      <c r="E177" s="94"/>
-      <c r="F177" s="91" t="s">
+      <c r="D178" s="100" t="s">
+        <v>169</v>
+      </c>
+      <c r="E178" s="94"/>
+      <c r="F178" s="91" t="s">
         <v>228</v>
       </c>
-      <c r="G177" s="91" t="s">
+      <c r="G178" s="91" t="s">
         <v>229</v>
       </c>
-      <c r="H177" s="68" t="s">
+      <c r="H178" s="68" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="178" spans="1:8">
-      <c r="A178" s="112">
-        <v>30</v>
-      </c>
-      <c r="B178" s="118"/>
-      <c r="C178" s="100" t="s">
+    <row r="179" spans="1:8">
+      <c r="A179" s="118">
+        <v>31</v>
+      </c>
+      <c r="B179" s="160"/>
+      <c r="C179" s="100" t="s">
         <v>372</v>
       </c>
-      <c r="D178" s="100" t="s">
-        <v>169</v>
-      </c>
-      <c r="E178" s="100" t="s">
-        <v>169</v>
-      </c>
-      <c r="F178" s="102" t="s">
+      <c r="D179" s="100" t="s">
+        <v>169</v>
+      </c>
+      <c r="E179" s="100" t="s">
+        <v>169</v>
+      </c>
+      <c r="F179" s="102" t="s">
         <v>385</v>
       </c>
-      <c r="G178" s="102" t="s">
+      <c r="G179" s="102" t="s">
         <v>383</v>
       </c>
-      <c r="H178" s="103" t="s">
+      <c r="H179" s="103" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="179" spans="1:8">
-      <c r="A179" s="112">
-        <v>31</v>
-      </c>
-      <c r="B179" s="118"/>
-      <c r="C179" s="66" t="s">
+    <row r="180" spans="1:8">
+      <c r="A180" s="118">
+        <v>32</v>
+      </c>
+      <c r="B180" s="160"/>
+      <c r="C180" s="66" t="s">
         <v>304</v>
       </c>
-      <c r="D179" s="65" t="s">
-        <v>169</v>
-      </c>
-      <c r="E179" s="65" t="s">
-        <v>169</v>
-      </c>
-      <c r="F179" s="65"/>
-      <c r="G179" s="66" t="s">
+      <c r="D180" s="65" t="s">
+        <v>169</v>
+      </c>
+      <c r="E180" s="65" t="s">
+        <v>169</v>
+      </c>
+      <c r="F180" s="65"/>
+      <c r="G180" s="66" t="s">
         <v>171</v>
       </c>
-      <c r="H179" s="68" t="s">
+      <c r="H180" s="68" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="180" spans="1:8">
-      <c r="A180" s="112">
-        <v>32</v>
-      </c>
-      <c r="B180" s="126"/>
-      <c r="C180" s="62" t="s">
+    <row r="181" spans="1:8">
+      <c r="A181" s="118">
+        <v>33</v>
+      </c>
+      <c r="B181" s="144"/>
+      <c r="C181" s="62" t="s">
         <v>204</v>
       </c>
-      <c r="D180" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E180" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F180" s="21"/>
-      <c r="G180" s="21" t="s">
+      <c r="D181" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E181" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F181" s="21"/>
+      <c r="G181" s="21" t="s">
         <v>205</v>
       </c>
-      <c r="H180" s="11"/>
-    </row>
-    <row r="181" spans="1:8">
-      <c r="A181" s="112">
-        <v>33</v>
-      </c>
-      <c r="B181" s="127" t="s">
+      <c r="H181" s="96" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8">
+      <c r="A182" s="118">
+        <v>34</v>
+      </c>
+      <c r="B182" s="139" t="s">
         <v>8</v>
       </c>
-      <c r="C181" s="21" t="s">
+      <c r="C182" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="D181" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E181" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F181" s="89" t="s">
+      <c r="D182" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E182" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F182" s="89" t="s">
         <v>207</v>
       </c>
-      <c r="G181" s="89" t="s">
+      <c r="G182" s="89" t="s">
         <v>358</v>
       </c>
-      <c r="H181" s="68" t="s">
+      <c r="H182" s="68" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="182" spans="1:8">
-      <c r="A182" s="112">
-        <v>34</v>
-      </c>
-      <c r="B182" s="124"/>
-      <c r="C182" s="89" t="s">
+    <row r="183" spans="1:8">
+      <c r="A183" s="118">
+        <v>35</v>
+      </c>
+      <c r="B183" s="140"/>
+      <c r="C183" s="89" t="s">
         <v>354</v>
       </c>
-      <c r="D182" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E182" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F182" s="89" t="s">
+      <c r="D183" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E183" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F183" s="89" t="s">
         <v>355</v>
       </c>
-      <c r="G182" s="100" t="s">
+      <c r="G183" s="100" t="s">
         <v>356</v>
       </c>
-      <c r="H182" s="68" t="s">
+      <c r="H183" s="68" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="183" spans="1:8">
-      <c r="A183" s="112">
-        <v>35</v>
-      </c>
-      <c r="B183" s="124"/>
-      <c r="C183" s="89" t="s">
+    <row r="184" spans="1:8">
+      <c r="A184" s="118">
+        <v>36</v>
+      </c>
+      <c r="B184" s="140"/>
+      <c r="C184" s="89" t="s">
         <v>209</v>
       </c>
-      <c r="D183" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E183" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F183" s="21"/>
-      <c r="G183" s="21" t="s">
+      <c r="D184" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E184" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F184" s="21"/>
+      <c r="G184" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="H183" s="11"/>
-    </row>
-    <row r="184" spans="1:8">
-      <c r="A184" s="112">
-        <v>36</v>
-      </c>
-      <c r="B184" s="124"/>
-      <c r="C184" s="21" t="s">
+      <c r="H184" s="11"/>
+    </row>
+    <row r="185" spans="1:8">
+      <c r="A185" s="118">
+        <v>37</v>
+      </c>
+      <c r="B185" s="140"/>
+      <c r="C185" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="D184" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E184" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F184" s="21">
+      <c r="D185" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E185" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F185" s="21">
         <v>20.03</v>
       </c>
-      <c r="G184" s="89">
+      <c r="G185" s="89">
         <v>20.03</v>
       </c>
-      <c r="H184" s="68" t="s">
+      <c r="H185" s="68" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="185" spans="1:8">
-      <c r="A185" s="112">
-        <v>37</v>
-      </c>
-      <c r="B185" s="124"/>
-      <c r="C185" s="21" t="s">
+    <row r="186" spans="1:8">
+      <c r="A186" s="118">
+        <v>38</v>
+      </c>
+      <c r="B186" s="140"/>
+      <c r="C186" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="D185" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E185" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F185" s="21">
+      <c r="D186" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E186" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F186" s="21">
         <v>20.04</v>
       </c>
-      <c r="G185" s="21" t="s">
-        <v>208</v>
-      </c>
-      <c r="H185" s="11"/>
-    </row>
-    <row r="186" spans="1:8">
-      <c r="A186" s="112">
-        <v>38</v>
-      </c>
-      <c r="B186" s="124"/>
-      <c r="C186" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="D186" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E186" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F186" s="21"/>
       <c r="G186" s="21" t="s">
         <v>208</v>
       </c>
       <c r="H186" s="11"/>
     </row>
     <row r="187" spans="1:8">
-      <c r="A187" s="112">
+      <c r="A187" s="118">
         <v>39</v>
       </c>
-      <c r="B187" s="124"/>
+      <c r="B187" s="140"/>
       <c r="C187" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D187" s="21" t="s">
         <v>169</v>
@@ -8875,12 +8992,12 @@
       <c r="H187" s="11"/>
     </row>
     <row r="188" spans="1:8">
-      <c r="A188" s="112">
+      <c r="A188" s="118">
         <v>40</v>
       </c>
-      <c r="B188" s="124"/>
+      <c r="B188" s="140"/>
       <c r="C188" s="21" t="s">
-        <v>47</v>
+        <v>213</v>
       </c>
       <c r="D188" s="21" t="s">
         <v>169</v>
@@ -8894,169 +9011,167 @@
       </c>
       <c r="H188" s="11"/>
     </row>
-    <row r="189" spans="1:8" ht="45">
-      <c r="A189" s="112">
+    <row r="189" spans="1:8">
+      <c r="A189" s="118">
         <v>41</v>
       </c>
-      <c r="B189" s="127" t="s">
+      <c r="B189" s="140"/>
+      <c r="C189" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D189" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E189" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F189" s="21"/>
+      <c r="G189" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="H189" s="11"/>
+    </row>
+    <row r="190" spans="1:8" ht="43.2">
+      <c r="A190" s="118">
+        <v>42</v>
+      </c>
+      <c r="B190" s="139" t="s">
         <v>9</v>
       </c>
-      <c r="C189" s="21" t="s">
+      <c r="C190" s="21" t="s">
         <v>214</v>
       </c>
-      <c r="D189" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E189" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F189" s="67" t="s">
+      <c r="D190" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E190" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F190" s="67" t="s">
         <v>327</v>
       </c>
-      <c r="G189" s="81" t="s">
+      <c r="G190" s="81" t="s">
         <v>363</v>
       </c>
-      <c r="H189" s="11"/>
-    </row>
-    <row r="190" spans="1:8">
-      <c r="A190" s="112">
-        <v>42</v>
-      </c>
-      <c r="B190" s="124"/>
-      <c r="C190" s="62" t="s">
+      <c r="H190" s="11"/>
+    </row>
+    <row r="191" spans="1:8">
+      <c r="A191" s="118">
+        <v>43</v>
+      </c>
+      <c r="B191" s="140"/>
+      <c r="C191" s="62" t="s">
         <v>215</v>
       </c>
-      <c r="D190" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E190" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F190" s="62" t="s">
+      <c r="D191" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E191" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F191" s="62" t="s">
         <v>216</v>
       </c>
-      <c r="G190" s="62" t="s">
+      <c r="G191" s="62" t="s">
         <v>217</v>
       </c>
-      <c r="H190" s="11"/>
-    </row>
-    <row r="191" spans="1:8">
-      <c r="A191" s="112">
-        <v>43</v>
-      </c>
-      <c r="B191" s="124"/>
-      <c r="C191" s="78" t="s">
+      <c r="H191" s="11"/>
+    </row>
+    <row r="192" spans="1:8">
+      <c r="A192" s="118">
+        <v>44</v>
+      </c>
+      <c r="B192" s="140"/>
+      <c r="C192" s="78" t="s">
         <v>332</v>
       </c>
-      <c r="D191" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="E191" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="F191" s="78" t="s">
+      <c r="D192" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="E192" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="F192" s="78" t="s">
         <v>216</v>
       </c>
-      <c r="G191" s="78" t="s">
+      <c r="G192" s="78" t="s">
         <v>333</v>
       </c>
-      <c r="H191" s="11"/>
-    </row>
-    <row r="192" spans="1:8">
-      <c r="A192" s="112">
-        <v>44</v>
-      </c>
-      <c r="B192" s="124"/>
-      <c r="C192" s="78" t="s">
+      <c r="H192" s="11"/>
+    </row>
+    <row r="193" spans="1:8">
+      <c r="A193" s="118">
+        <v>45</v>
+      </c>
+      <c r="B193" s="140"/>
+      <c r="C193" s="78" t="s">
         <v>218</v>
       </c>
-      <c r="D192" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="E192" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="F192" s="78" t="s">
+      <c r="D193" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="E193" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="F193" s="78" t="s">
         <v>328</v>
       </c>
-      <c r="G192" s="78" t="s">
+      <c r="G193" s="78" t="s">
         <v>328</v>
       </c>
-      <c r="H192" s="11"/>
-    </row>
-    <row r="193" spans="1:8">
-      <c r="A193" s="112">
-        <v>45</v>
-      </c>
-      <c r="B193" s="124"/>
-      <c r="C193" s="78" t="s">
+      <c r="H193" s="11"/>
+    </row>
+    <row r="194" spans="1:8">
+      <c r="A194" s="118">
+        <v>46</v>
+      </c>
+      <c r="B194" s="140"/>
+      <c r="C194" s="78" t="s">
         <v>330</v>
       </c>
-      <c r="D193" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="E193" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="F193" s="78">
+      <c r="D194" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="E194" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="F194" s="78">
         <v>64</v>
       </c>
-      <c r="G193" s="78" t="s">
+      <c r="G194" s="78" t="s">
         <v>329</v>
       </c>
-      <c r="H193" s="11"/>
-    </row>
-    <row r="194" spans="1:8">
-      <c r="A194" s="112">
-        <v>46</v>
-      </c>
-      <c r="B194" s="124"/>
-      <c r="C194" s="104" t="s">
+      <c r="H194" s="11"/>
+    </row>
+    <row r="195" spans="1:8">
+      <c r="A195" s="118">
+        <v>47</v>
+      </c>
+      <c r="B195" s="140"/>
+      <c r="C195" s="104" t="s">
         <v>331</v>
       </c>
-      <c r="D194" s="105" t="s">
-        <v>169</v>
-      </c>
-      <c r="E194" s="105" t="s">
-        <v>169</v>
-      </c>
-      <c r="F194" s="104">
+      <c r="D195" s="105" t="s">
+        <v>169</v>
+      </c>
+      <c r="E195" s="105" t="s">
+        <v>169</v>
+      </c>
+      <c r="F195" s="104">
         <v>7.9</v>
       </c>
-      <c r="G194" s="104" t="s">
+      <c r="G195" s="104" t="s">
         <v>334</v>
       </c>
-      <c r="H194" s="11"/>
-    </row>
-    <row r="195" spans="1:8">
-      <c r="A195" s="112">
-        <v>47</v>
-      </c>
-      <c r="B195" s="124"/>
-      <c r="C195" s="104" t="s">
+      <c r="H195" s="11"/>
+    </row>
+    <row r="196" spans="1:8">
+      <c r="A196" s="118">
+        <v>48</v>
+      </c>
+      <c r="B196" s="140"/>
+      <c r="C196" s="104" t="s">
         <v>387</v>
-      </c>
-      <c r="D195" s="105" t="s">
-        <v>169</v>
-      </c>
-      <c r="E195" s="105"/>
-      <c r="F195" s="104">
-        <v>50</v>
-      </c>
-      <c r="G195" s="104" t="s">
-        <v>390</v>
-      </c>
-      <c r="H195" s="68" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="196" spans="1:8">
-      <c r="A196" s="112">
-        <v>48</v>
-      </c>
-      <c r="B196" s="124"/>
-      <c r="C196" s="104" t="s">
-        <v>388</v>
       </c>
       <c r="D196" s="105" t="s">
         <v>169</v>
@@ -9069,363 +9184,375 @@
         <v>390</v>
       </c>
       <c r="H196" s="68" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8">
+      <c r="A197" s="118">
+        <v>49</v>
+      </c>
+      <c r="B197" s="140"/>
+      <c r="C197" s="104" t="s">
+        <v>388</v>
+      </c>
+      <c r="D197" s="105" t="s">
+        <v>169</v>
+      </c>
+      <c r="E197" s="105"/>
+      <c r="F197" s="104">
+        <v>50</v>
+      </c>
+      <c r="G197" s="104" t="s">
+        <v>390</v>
+      </c>
+      <c r="H197" s="68" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="197" spans="1:8">
-      <c r="A197" s="112">
-        <v>49</v>
-      </c>
-      <c r="B197" s="124"/>
-      <c r="C197" s="78" t="s">
+    <row r="198" spans="1:8">
+      <c r="A198" s="118">
+        <v>50</v>
+      </c>
+      <c r="B198" s="140"/>
+      <c r="C198" s="78" t="s">
         <v>389</v>
       </c>
-      <c r="D197" s="105" t="s">
-        <v>169</v>
-      </c>
-      <c r="E197" s="105"/>
-      <c r="F197" s="21">
+      <c r="D198" s="105" t="s">
+        <v>169</v>
+      </c>
+      <c r="E198" s="105"/>
+      <c r="F198" s="21">
         <v>10</v>
       </c>
-      <c r="G197" s="78" t="s">
+      <c r="G198" s="78" t="s">
         <v>391</v>
       </c>
-      <c r="H197" s="68" t="s">
+      <c r="H198" s="68" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="198" spans="1:8">
-      <c r="A198" s="112">
-        <v>50</v>
-      </c>
-      <c r="B198" s="117" t="s">
+    <row r="199" spans="1:8">
+      <c r="A199" s="118">
+        <v>51</v>
+      </c>
+      <c r="B199" s="158" t="s">
         <v>10</v>
       </c>
-      <c r="C198" s="21" t="s">
+      <c r="C199" s="21" t="s">
         <v>219</v>
       </c>
-      <c r="D198" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E198" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F198" s="21" t="s">
+      <c r="D199" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E199" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F199" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="G198" s="21" t="s">
+      <c r="G199" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="H198" s="11" t="s">
+      <c r="H199" s="11" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="199" spans="1:8">
-      <c r="A199" s="112">
-        <v>51</v>
-      </c>
-      <c r="B199" s="118"/>
-      <c r="C199" s="80" t="s">
+    <row r="200" spans="1:8">
+      <c r="A200" s="118">
+        <v>52</v>
+      </c>
+      <c r="B200" s="160"/>
+      <c r="C200" s="80" t="s">
         <v>222</v>
       </c>
-      <c r="D199" s="80" t="s">
-        <v>169</v>
-      </c>
-      <c r="E199" s="80" t="s">
-        <v>169</v>
-      </c>
-      <c r="F199" s="80" t="s">
+      <c r="D200" s="80" t="s">
+        <v>169</v>
+      </c>
+      <c r="E200" s="80" t="s">
+        <v>169</v>
+      </c>
+      <c r="F200" s="80" t="s">
         <v>223</v>
       </c>
-      <c r="G199" s="80" t="s">
+      <c r="G200" s="80" t="s">
         <v>171</v>
       </c>
-      <c r="H199" s="24" t="s">
+      <c r="H200" s="24" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="200" spans="1:8">
-      <c r="A200" s="106">
-        <v>52</v>
-      </c>
-      <c r="B200" s="119"/>
-      <c r="C200" s="79" t="s">
+    <row r="201" spans="1:8">
+      <c r="A201" s="106">
+        <v>53</v>
+      </c>
+      <c r="B201" s="159"/>
+      <c r="C201" s="79" t="s">
         <v>335</v>
       </c>
-      <c r="D200" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="E200" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="F200" s="79" t="s">
+      <c r="D201" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="E201" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="F201" s="79" t="s">
         <v>336</v>
       </c>
-      <c r="G200" s="20" t="s">
+      <c r="G201" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="H200" s="22" t="s">
+      <c r="H201" s="22" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="201" spans="1:8">
-      <c r="A201" s="16">
-        <v>53</v>
-      </c>
-      <c r="B201" s="120" t="s">
+    <row r="202" spans="1:8">
+      <c r="A202" s="16">
+        <v>54</v>
+      </c>
+      <c r="B202" s="161" t="s">
         <v>156</v>
       </c>
-      <c r="C201" s="63" t="s">
+      <c r="C202" s="63" t="s">
         <v>224</v>
       </c>
-      <c r="D201" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="E201" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="F201" s="17" t="s">
+      <c r="D202" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="E202" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="F202" s="17" t="s">
         <v>225</v>
       </c>
-      <c r="G201" s="63" t="s">
+      <c r="G202" s="63" t="s">
         <v>226</v>
       </c>
-      <c r="H201" s="10"/>
-    </row>
-    <row r="202" spans="1:8">
-      <c r="A202" s="19">
-        <v>54</v>
-      </c>
-      <c r="B202" s="121"/>
-      <c r="C202" s="62" t="s">
+      <c r="H202" s="10"/>
+    </row>
+    <row r="203" spans="1:8">
+      <c r="A203" s="119">
+        <v>55</v>
+      </c>
+      <c r="B203" s="162"/>
+      <c r="C203" s="120" t="s">
+        <v>401</v>
+      </c>
+      <c r="D203" s="115" t="s">
+        <v>169</v>
+      </c>
+      <c r="E203" s="115"/>
+      <c r="F203" s="115" t="s">
+        <v>232</v>
+      </c>
+      <c r="G203" s="113" t="s">
+        <v>402</v>
+      </c>
+      <c r="H203" s="40" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8">
+      <c r="A204" s="119">
+        <v>56</v>
+      </c>
+      <c r="B204" s="163"/>
+      <c r="C204" s="62" t="s">
         <v>227</v>
       </c>
-      <c r="D202" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E202" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F202" s="21" t="s">
+      <c r="D204" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E204" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F204" s="21" t="s">
         <v>228</v>
       </c>
-      <c r="G202" s="64" t="s">
+      <c r="G204" s="64" t="s">
         <v>229</v>
       </c>
-      <c r="H202" s="11"/>
-    </row>
-    <row r="203" spans="1:8">
-      <c r="A203" s="112">
-        <v>55</v>
-      </c>
-      <c r="B203" s="122"/>
-      <c r="C203" s="64" t="s">
+      <c r="H204" s="11"/>
+    </row>
+    <row r="205" spans="1:8">
+      <c r="A205" s="119">
+        <v>57</v>
+      </c>
+      <c r="B205" s="164"/>
+      <c r="C205" s="64" t="s">
         <v>230</v>
       </c>
-      <c r="D203" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E203" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F203" s="21" t="s">
+      <c r="D205" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E205" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F205" s="21" t="s">
         <v>228</v>
       </c>
-      <c r="G203" s="20" t="s">
+      <c r="G205" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="H203" s="22"/>
-    </row>
-    <row r="204" spans="1:8">
-      <c r="A204" s="112">
-        <v>56</v>
-      </c>
-      <c r="B204" s="122"/>
-      <c r="C204" s="64" t="s">
+      <c r="H205" s="22"/>
+    </row>
+    <row r="206" spans="1:8">
+      <c r="A206" s="119">
+        <v>58</v>
+      </c>
+      <c r="B206" s="164"/>
+      <c r="C206" s="64" t="s">
         <v>231</v>
       </c>
-      <c r="D204" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="E204" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="F204" s="23" t="s">
+      <c r="D206" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="E206" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="F206" s="23" t="s">
         <v>232</v>
       </c>
-      <c r="G204" s="64" t="s">
+      <c r="G206" s="64" t="s">
         <v>233</v>
       </c>
-      <c r="H204" s="24"/>
-    </row>
-    <row r="205" spans="1:8">
-      <c r="A205" s="112">
-        <v>57</v>
-      </c>
-      <c r="B205" s="122"/>
-      <c r="C205" s="70" t="s">
+      <c r="H206" s="24"/>
+    </row>
+    <row r="207" spans="1:8">
+      <c r="A207" s="119">
+        <v>59</v>
+      </c>
+      <c r="B207" s="164"/>
+      <c r="C207" s="70" t="s">
         <v>234</v>
       </c>
-      <c r="D205" s="71" t="s">
-        <v>169</v>
-      </c>
-      <c r="E205" s="71" t="s">
-        <v>169</v>
-      </c>
-      <c r="F205" s="71"/>
-      <c r="G205" s="72" t="s">
+      <c r="D207" s="71" t="s">
+        <v>169</v>
+      </c>
+      <c r="E207" s="71" t="s">
+        <v>169</v>
+      </c>
+      <c r="F207" s="71"/>
+      <c r="G207" s="72" t="s">
         <v>316</v>
       </c>
-      <c r="H205" s="24"/>
-    </row>
-    <row r="206" spans="1:8">
-      <c r="A206" s="112">
-        <v>58</v>
-      </c>
-      <c r="B206" s="122"/>
-      <c r="C206" s="70" t="s">
+      <c r="H207" s="24"/>
+    </row>
+    <row r="208" spans="1:8">
+      <c r="A208" s="119">
+        <v>60</v>
+      </c>
+      <c r="B208" s="164"/>
+      <c r="C208" s="70" t="s">
         <v>310</v>
       </c>
-      <c r="D206" s="71" t="s">
-        <v>169</v>
-      </c>
-      <c r="E206" s="71"/>
-      <c r="F206" s="71" t="s">
+      <c r="D208" s="71" t="s">
+        <v>169</v>
+      </c>
+      <c r="E208" s="71"/>
+      <c r="F208" s="71" t="s">
         <v>311</v>
       </c>
-      <c r="G206" s="70" t="s">
+      <c r="G208" s="70" t="s">
         <v>312</v>
       </c>
-      <c r="H206" s="24" t="s">
+      <c r="H208" s="24" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="207" spans="1:8">
-      <c r="A207" s="25">
-        <v>59</v>
-      </c>
-      <c r="B207" s="123"/>
-      <c r="C207" s="26" t="s">
+    <row r="209" spans="1:8">
+      <c r="A209" s="25">
+        <v>61</v>
+      </c>
+      <c r="B209" s="148"/>
+      <c r="C209" s="26" t="s">
         <v>314</v>
       </c>
-      <c r="D207" s="26" t="s">
-        <v>169</v>
-      </c>
-      <c r="E207" s="26"/>
-      <c r="F207" s="26" t="s">
+      <c r="D209" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="E209" s="26"/>
+      <c r="F209" s="26" t="s">
         <v>228</v>
       </c>
-      <c r="G207" s="26" t="s">
+      <c r="G209" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="H207" s="27" t="s">
+      <c r="H209" s="27" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="208" spans="1:8">
-      <c r="A208" s="1" t="s">
+    <row r="210" spans="1:8">
+      <c r="A210" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B208" s="1" t="s">
+      <c r="B210" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="209" spans="1:7">
-      <c r="B209" s="28" t="s">
+    <row r="211" spans="1:8">
+      <c r="B211" s="28" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="210" spans="1:7">
-      <c r="B210" s="85" t="s">
+    <row r="212" spans="1:8">
+      <c r="B212" s="85" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="211" spans="1:7">
-      <c r="B211" s="85" t="s">
+    <row r="213" spans="1:8">
+      <c r="B213" s="85" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="212" spans="1:7">
-      <c r="B212" s="95" t="s">
+    <row r="214" spans="1:8">
+      <c r="B214" s="95" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="213" spans="1:7">
-      <c r="B213" s="85" t="s">
+    <row r="215" spans="1:8">
+      <c r="B215" s="85" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="223" spans="1:7">
-      <c r="A223" s="1" t="s">
+    <row r="225" spans="1:7">
+      <c r="A225" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B223" s="1" t="s">
+      <c r="B225" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="224" spans="1:7">
-      <c r="A224" s="4" t="s">
+    <row r="226" spans="1:7">
+      <c r="A226" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="B224" s="29" t="s">
+      <c r="B226" s="29" t="s">
         <v>241</v>
       </c>
-      <c r="C224" s="151" t="s">
+      <c r="C226" s="130" t="s">
         <v>242</v>
       </c>
-      <c r="D224" s="151"/>
-      <c r="E224" s="151"/>
-      <c r="F224" s="30" t="s">
+      <c r="D226" s="130"/>
+      <c r="E226" s="130"/>
+      <c r="F226" s="30" t="s">
         <v>243</v>
       </c>
-      <c r="G224" s="31" t="s">
+      <c r="G226" s="31" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="225" spans="1:7">
-      <c r="A225" s="133" t="s">
+    <row r="227" spans="1:7">
+      <c r="A227" s="156" t="s">
         <v>245</v>
       </c>
-      <c r="B225" s="124" t="s">
+      <c r="B227" s="140" t="s">
         <v>246</v>
       </c>
-      <c r="C225" s="152" t="s">
+      <c r="C227" s="131" t="s">
         <v>247</v>
       </c>
-      <c r="D225" s="153"/>
-      <c r="E225" s="153"/>
-      <c r="F225" s="21" t="s">
-        <v>248</v>
-      </c>
-      <c r="G225" s="32" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="226" spans="1:7">
-      <c r="A226" s="133"/>
-      <c r="B226" s="125"/>
-      <c r="C226" s="143" t="s">
-        <v>247</v>
-      </c>
-      <c r="D226" s="154"/>
-      <c r="E226" s="154"/>
-      <c r="F226" s="20" t="s">
-        <v>250</v>
-      </c>
-      <c r="G226" s="33" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="227" spans="1:7">
-      <c r="A227" s="133"/>
-      <c r="B227" s="124" t="s">
-        <v>251</v>
-      </c>
-      <c r="C227" s="147" t="s">
-        <v>252</v>
-      </c>
-      <c r="D227" s="147"/>
-      <c r="E227" s="147"/>
+      <c r="D227" s="132"/>
+      <c r="E227" s="132"/>
       <c r="F227" s="21" t="s">
         <v>248</v>
       </c>
@@ -9434,30 +9561,30 @@
       </c>
     </row>
     <row r="228" spans="1:7">
-      <c r="A228" s="133"/>
-      <c r="B228" s="124"/>
-      <c r="C228" s="143" t="s">
+      <c r="A228" s="156"/>
+      <c r="B228" s="165"/>
+      <c r="C228" s="133" t="s">
+        <v>247</v>
+      </c>
+      <c r="D228" s="134"/>
+      <c r="E228" s="134"/>
+      <c r="F228" s="20" t="s">
+        <v>250</v>
+      </c>
+      <c r="G228" s="33" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7">
+      <c r="A229" s="156"/>
+      <c r="B229" s="140" t="s">
+        <v>251</v>
+      </c>
+      <c r="C229" s="135" t="s">
         <v>252</v>
       </c>
-      <c r="D228" s="143"/>
-      <c r="E228" s="143"/>
-      <c r="F228" s="21" t="s">
-        <v>250</v>
-      </c>
-      <c r="G228" s="32" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="229" spans="1:7">
-      <c r="A229" s="133"/>
-      <c r="B229" s="125" t="s">
-        <v>253</v>
-      </c>
-      <c r="C229" s="144" t="s">
-        <v>247</v>
-      </c>
-      <c r="D229" s="145"/>
-      <c r="E229" s="146"/>
+      <c r="D229" s="135"/>
+      <c r="E229" s="135"/>
       <c r="F229" s="21" t="s">
         <v>248</v>
       </c>
@@ -9466,13 +9593,13 @@
       </c>
     </row>
     <row r="230" spans="1:7">
-      <c r="A230" s="133"/>
-      <c r="B230" s="126"/>
-      <c r="C230" s="144" t="s">
-        <v>247</v>
-      </c>
-      <c r="D230" s="145"/>
-      <c r="E230" s="146"/>
+      <c r="A230" s="156"/>
+      <c r="B230" s="140"/>
+      <c r="C230" s="133" t="s">
+        <v>252</v>
+      </c>
+      <c r="D230" s="133"/>
+      <c r="E230" s="133"/>
       <c r="F230" s="21" t="s">
         <v>250</v>
       </c>
@@ -9481,15 +9608,15 @@
       </c>
     </row>
     <row r="231" spans="1:7">
-      <c r="A231" s="133"/>
-      <c r="B231" s="124" t="s">
-        <v>254</v>
-      </c>
-      <c r="C231" s="147" t="s">
-        <v>255</v>
-      </c>
-      <c r="D231" s="147"/>
-      <c r="E231" s="147"/>
+      <c r="A231" s="156"/>
+      <c r="B231" s="165" t="s">
+        <v>253</v>
+      </c>
+      <c r="C231" s="136" t="s">
+        <v>247</v>
+      </c>
+      <c r="D231" s="137"/>
+      <c r="E231" s="138"/>
       <c r="F231" s="21" t="s">
         <v>248</v>
       </c>
@@ -9498,13 +9625,13 @@
       </c>
     </row>
     <row r="232" spans="1:7">
-      <c r="A232" s="133"/>
-      <c r="B232" s="124"/>
-      <c r="C232" s="147" t="s">
-        <v>255</v>
-      </c>
-      <c r="D232" s="147"/>
-      <c r="E232" s="147"/>
+      <c r="A232" s="156"/>
+      <c r="B232" s="144"/>
+      <c r="C232" s="136" t="s">
+        <v>247</v>
+      </c>
+      <c r="D232" s="137"/>
+      <c r="E232" s="138"/>
       <c r="F232" s="21" t="s">
         <v>250</v>
       </c>
@@ -9513,17 +9640,15 @@
       </c>
     </row>
     <row r="233" spans="1:7">
-      <c r="A233" s="133" t="s">
-        <v>256</v>
-      </c>
-      <c r="B233" s="124" t="s">
-        <v>257</v>
-      </c>
-      <c r="C233" s="127" t="s">
-        <v>258</v>
-      </c>
-      <c r="D233" s="124"/>
-      <c r="E233" s="124"/>
+      <c r="A233" s="156"/>
+      <c r="B233" s="140" t="s">
+        <v>254</v>
+      </c>
+      <c r="C233" s="135" t="s">
+        <v>255</v>
+      </c>
+      <c r="D233" s="135"/>
+      <c r="E233" s="135"/>
       <c r="F233" s="21" t="s">
         <v>248</v>
       </c>
@@ -9532,30 +9657,32 @@
       </c>
     </row>
     <row r="234" spans="1:7">
-      <c r="A234" s="133"/>
-      <c r="B234" s="124"/>
-      <c r="C234" s="124" t="s">
-        <v>259</v>
-      </c>
-      <c r="D234" s="124"/>
-      <c r="E234" s="124"/>
+      <c r="A234" s="156"/>
+      <c r="B234" s="140"/>
+      <c r="C234" s="135" t="s">
+        <v>255</v>
+      </c>
+      <c r="D234" s="135"/>
+      <c r="E234" s="135"/>
       <c r="F234" s="21" t="s">
         <v>250</v>
       </c>
       <c r="G234" s="32" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
     </row>
     <row r="235" spans="1:7">
-      <c r="A235" s="133"/>
-      <c r="B235" s="124" t="s">
-        <v>261</v>
-      </c>
-      <c r="C235" s="124" t="s">
-        <v>262</v>
-      </c>
-      <c r="D235" s="124"/>
-      <c r="E235" s="124"/>
+      <c r="A235" s="156" t="s">
+        <v>256</v>
+      </c>
+      <c r="B235" s="140" t="s">
+        <v>257</v>
+      </c>
+      <c r="C235" s="139" t="s">
+        <v>258</v>
+      </c>
+      <c r="D235" s="140"/>
+      <c r="E235" s="140"/>
       <c r="F235" s="21" t="s">
         <v>248</v>
       </c>
@@ -9564,32 +9691,30 @@
       </c>
     </row>
     <row r="236" spans="1:7">
-      <c r="A236" s="133"/>
-      <c r="B236" s="124"/>
-      <c r="C236" s="124" t="s">
-        <v>263</v>
-      </c>
-      <c r="D236" s="124"/>
-      <c r="E236" s="124"/>
+      <c r="A236" s="156"/>
+      <c r="B236" s="140"/>
+      <c r="C236" s="140" t="s">
+        <v>259</v>
+      </c>
+      <c r="D236" s="140"/>
+      <c r="E236" s="140"/>
       <c r="F236" s="21" t="s">
         <v>250</v>
       </c>
       <c r="G236" s="32" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
     </row>
     <row r="237" spans="1:7">
-      <c r="A237" s="133" t="s">
-        <v>264</v>
-      </c>
-      <c r="B237" s="124" t="s">
-        <v>265</v>
-      </c>
-      <c r="C237" s="127" t="s">
-        <v>266</v>
-      </c>
-      <c r="D237" s="124"/>
-      <c r="E237" s="124"/>
+      <c r="A237" s="156"/>
+      <c r="B237" s="140" t="s">
+        <v>261</v>
+      </c>
+      <c r="C237" s="140" t="s">
+        <v>262</v>
+      </c>
+      <c r="D237" s="140"/>
+      <c r="E237" s="140"/>
       <c r="F237" s="21" t="s">
         <v>248</v>
       </c>
@@ -9598,13 +9723,13 @@
       </c>
     </row>
     <row r="238" spans="1:7">
-      <c r="A238" s="133"/>
-      <c r="B238" s="124"/>
-      <c r="C238" s="124" t="s">
-        <v>267</v>
-      </c>
-      <c r="D238" s="124"/>
-      <c r="E238" s="124"/>
+      <c r="A238" s="156"/>
+      <c r="B238" s="140"/>
+      <c r="C238" s="140" t="s">
+        <v>263</v>
+      </c>
+      <c r="D238" s="140"/>
+      <c r="E238" s="140"/>
       <c r="F238" s="21" t="s">
         <v>250</v>
       </c>
@@ -9613,15 +9738,17 @@
       </c>
     </row>
     <row r="239" spans="1:7">
-      <c r="A239" s="133"/>
-      <c r="B239" s="124" t="s">
-        <v>268</v>
-      </c>
-      <c r="C239" s="127" t="s">
-        <v>269</v>
-      </c>
-      <c r="D239" s="124"/>
-      <c r="E239" s="124"/>
+      <c r="A239" s="156" t="s">
+        <v>264</v>
+      </c>
+      <c r="B239" s="140" t="s">
+        <v>265</v>
+      </c>
+      <c r="C239" s="139" t="s">
+        <v>266</v>
+      </c>
+      <c r="D239" s="140"/>
+      <c r="E239" s="140"/>
       <c r="F239" s="21" t="s">
         <v>248</v>
       </c>
@@ -9630,358 +9757,356 @@
       </c>
     </row>
     <row r="240" spans="1:7">
-      <c r="A240" s="134"/>
-      <c r="B240" s="135"/>
-      <c r="C240" s="135" t="s">
+      <c r="A240" s="156"/>
+      <c r="B240" s="140"/>
+      <c r="C240" s="140" t="s">
+        <v>267</v>
+      </c>
+      <c r="D240" s="140"/>
+      <c r="E240" s="140"/>
+      <c r="F240" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="G240" s="32" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7">
+      <c r="A241" s="156"/>
+      <c r="B241" s="140" t="s">
+        <v>268</v>
+      </c>
+      <c r="C241" s="139" t="s">
+        <v>269</v>
+      </c>
+      <c r="D241" s="140"/>
+      <c r="E241" s="140"/>
+      <c r="F241" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="G241" s="32" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="242" spans="1:7">
+      <c r="A242" s="157"/>
+      <c r="B242" s="141"/>
+      <c r="C242" s="141" t="s">
         <v>270</v>
       </c>
-      <c r="D240" s="135"/>
-      <c r="E240" s="135"/>
-      <c r="F240" s="26" t="s">
+      <c r="D242" s="141"/>
+      <c r="E242" s="141"/>
+      <c r="F242" s="26" t="s">
         <v>250</v>
       </c>
-      <c r="G240" s="34" t="s">
+      <c r="G242" s="34" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="241" spans="1:7">
-      <c r="A241" s="1" t="s">
+    <row r="243" spans="1:7">
+      <c r="A243" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="C241" s="28"/>
-      <c r="D241" s="28"/>
-      <c r="E241" s="28"/>
-      <c r="F241" s="28"/>
-    </row>
-    <row r="242" spans="1:7">
-      <c r="C242" s="28"/>
-      <c r="D242" s="28"/>
-      <c r="E242" s="28"/>
-    </row>
-    <row r="243" spans="1:7">
       <c r="C243" s="28"/>
       <c r="D243" s="28"/>
       <c r="E243" s="28"/>
+      <c r="F243" s="28"/>
     </row>
     <row r="244" spans="1:7">
-      <c r="A244" s="1" t="s">
-        <v>272</v>
-      </c>
       <c r="C244" s="28"/>
       <c r="D244" s="28"/>
       <c r="E244" s="28"/>
     </row>
     <row r="245" spans="1:7">
-      <c r="A245" s="35" t="s">
+      <c r="C245" s="28"/>
+      <c r="D245" s="28"/>
+      <c r="E245" s="28"/>
+    </row>
+    <row r="246" spans="1:7">
+      <c r="A246" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C246" s="28"/>
+      <c r="D246" s="28"/>
+      <c r="E246" s="28"/>
+    </row>
+    <row r="247" spans="1:7">
+      <c r="A247" s="35" t="s">
         <v>273</v>
       </c>
-      <c r="B245" s="141" t="s">
+      <c r="B247" s="142" t="s">
         <v>274</v>
       </c>
-      <c r="C245" s="141"/>
-      <c r="D245" s="141"/>
-      <c r="E245" s="141"/>
-      <c r="F245" s="36" t="s">
+      <c r="C247" s="142"/>
+      <c r="D247" s="142"/>
+      <c r="E247" s="142"/>
+      <c r="F247" s="36" t="s">
         <v>275</v>
       </c>
-      <c r="G245" s="37" t="s">
+      <c r="G247" s="37" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="246" spans="1:7" ht="93" customHeight="1">
-      <c r="A246" s="38" t="s">
+    <row r="248" spans="1:7" ht="93" customHeight="1">
+      <c r="A248" s="38" t="s">
         <v>277</v>
       </c>
-      <c r="B246" s="142" t="s">
+      <c r="B248" s="143" t="s">
         <v>278</v>
       </c>
-      <c r="C246" s="126"/>
-      <c r="D246" s="126"/>
-      <c r="E246" s="126"/>
-      <c r="F246" s="39" t="s">
+      <c r="C248" s="144"/>
+      <c r="D248" s="144"/>
+      <c r="E248" s="144"/>
+      <c r="F248" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="G246" s="40" t="s">
+      <c r="G248" s="40" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="247" spans="1:7" ht="57" customHeight="1">
-      <c r="A247" s="8" t="s">
+    <row r="249" spans="1:7" ht="57" customHeight="1">
+      <c r="A249" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="B247" s="137" t="s">
+      <c r="B249" s="145" t="s">
         <v>280</v>
       </c>
-      <c r="C247" s="138"/>
-      <c r="D247" s="138"/>
-      <c r="E247" s="139"/>
-      <c r="F247" s="9" t="s">
+      <c r="C249" s="146"/>
+      <c r="D249" s="146"/>
+      <c r="E249" s="147"/>
+      <c r="F249" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="G247" s="11" t="s">
+      <c r="G249" s="11" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="248" spans="1:7" ht="57" customHeight="1">
-      <c r="A248" s="12" t="s">
+    <row r="250" spans="1:7" ht="57" customHeight="1">
+      <c r="A250" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="B248" s="137" t="s">
+      <c r="B250" s="145" t="s">
         <v>282</v>
       </c>
-      <c r="C248" s="138"/>
-      <c r="D248" s="138"/>
-      <c r="E248" s="139"/>
-      <c r="F248" s="13" t="s">
+      <c r="C250" s="146"/>
+      <c r="D250" s="146"/>
+      <c r="E250" s="147"/>
+      <c r="F250" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="G248" s="22" t="s">
+      <c r="G250" s="22" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="249" spans="1:7" ht="69" customHeight="1">
-      <c r="A249" s="14" t="s">
+    <row r="251" spans="1:7" ht="69" customHeight="1">
+      <c r="A251" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="B249" s="123" t="s">
+      <c r="B251" s="148" t="s">
         <v>284</v>
       </c>
-      <c r="C249" s="135"/>
-      <c r="D249" s="135"/>
-      <c r="E249" s="135"/>
-      <c r="F249" s="15" t="s">
+      <c r="C251" s="141"/>
+      <c r="D251" s="141"/>
+      <c r="E251" s="141"/>
+      <c r="F251" s="15" t="s">
         <v>249</v>
       </c>
-      <c r="G249" s="27" t="s">
+      <c r="G251" s="27" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="250" spans="1:7">
-      <c r="C250" s="41"/>
-    </row>
     <row r="252" spans="1:7">
-      <c r="A252" s="1" t="s">
+      <c r="C252" s="41"/>
+    </row>
+    <row r="254" spans="1:7">
+      <c r="A254" s="1" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="253" spans="1:7">
-      <c r="A253" s="4" t="s">
+    <row r="255" spans="1:7">
+      <c r="A255" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="B253" s="29" t="s">
+      <c r="B255" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="C253" s="42" t="s">
+      <c r="C255" s="42" t="s">
         <v>287</v>
       </c>
-      <c r="D253" s="43" t="s">
+      <c r="D255" s="43" t="s">
         <v>274</v>
       </c>
-      <c r="E253" s="43"/>
-      <c r="F253" s="44"/>
-      <c r="G253" s="31" t="s">
+      <c r="E255" s="43"/>
+      <c r="F255" s="44"/>
+      <c r="G255" s="31" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="254" spans="1:7">
-      <c r="A254" s="45">
+    <row r="256" spans="1:7">
+      <c r="A256" s="45">
         <v>42682</v>
       </c>
-      <c r="B254" s="46">
+      <c r="B256" s="46">
         <v>1.04</v>
       </c>
-      <c r="C254" s="17" t="s">
+      <c r="C256" s="17" t="s">
         <v>289</v>
       </c>
-      <c r="D254" s="140" t="s">
+      <c r="D256" s="149" t="s">
         <v>290</v>
       </c>
-      <c r="E254" s="140"/>
-      <c r="F254" s="140"/>
-      <c r="G254" s="47"/>
-    </row>
-    <row r="255" spans="1:7">
-      <c r="A255" s="48">
-        <v>42692</v>
-      </c>
-      <c r="B255" s="49">
-        <v>1.05</v>
-      </c>
-      <c r="C255" s="21" t="s">
-        <v>289</v>
-      </c>
-      <c r="D255" s="136" t="s">
-        <v>291</v>
-      </c>
-      <c r="E255" s="136"/>
-      <c r="F255" s="136"/>
-      <c r="G255" s="32"/>
-    </row>
-    <row r="256" spans="1:7">
-      <c r="A256" s="48">
-        <v>42955</v>
-      </c>
-      <c r="B256" s="49">
-        <v>1.06</v>
-      </c>
-      <c r="C256" s="21" t="s">
-        <v>289</v>
-      </c>
-      <c r="D256" s="136" t="s">
-        <v>292</v>
-      </c>
-      <c r="E256" s="136"/>
-      <c r="F256" s="136"/>
-      <c r="G256" s="32"/>
+      <c r="E256" s="149"/>
+      <c r="F256" s="149"/>
+      <c r="G256" s="47"/>
     </row>
     <row r="257" spans="1:7">
       <c r="A257" s="48">
-        <v>42991</v>
+        <v>42692</v>
       </c>
       <c r="B257" s="49">
-        <v>1.07</v>
+        <v>1.05</v>
       </c>
       <c r="C257" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="D257" s="136" t="s">
-        <v>293</v>
-      </c>
-      <c r="E257" s="136"/>
-      <c r="F257" s="136"/>
+      <c r="D257" s="150" t="s">
+        <v>291</v>
+      </c>
+      <c r="E257" s="150"/>
+      <c r="F257" s="150"/>
       <c r="G257" s="32"/>
     </row>
     <row r="258" spans="1:7">
       <c r="A258" s="48">
-        <v>43026</v>
+        <v>42955</v>
       </c>
       <c r="B258" s="49">
-        <v>1.08</v>
+        <v>1.06</v>
       </c>
       <c r="C258" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="D258" s="136" t="s">
-        <v>294</v>
-      </c>
-      <c r="E258" s="136"/>
-      <c r="F258" s="136"/>
+      <c r="D258" s="150" t="s">
+        <v>292</v>
+      </c>
+      <c r="E258" s="150"/>
+      <c r="F258" s="150"/>
       <c r="G258" s="32"/>
     </row>
     <row r="259" spans="1:7">
       <c r="A259" s="48">
-        <v>43069</v>
+        <v>42991</v>
       </c>
       <c r="B259" s="49">
-        <v>1.0900000000000001</v>
+        <v>1.07</v>
       </c>
       <c r="C259" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="D259" s="136" t="s">
+      <c r="D259" s="150" t="s">
+        <v>293</v>
+      </c>
+      <c r="E259" s="150"/>
+      <c r="F259" s="150"/>
+      <c r="G259" s="32"/>
+    </row>
+    <row r="260" spans="1:7">
+      <c r="A260" s="48">
+        <v>43026</v>
+      </c>
+      <c r="B260" s="49">
+        <v>1.08</v>
+      </c>
+      <c r="C260" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="D260" s="150" t="s">
+        <v>294</v>
+      </c>
+      <c r="E260" s="150"/>
+      <c r="F260" s="150"/>
+      <c r="G260" s="32"/>
+    </row>
+    <row r="261" spans="1:7">
+      <c r="A261" s="48">
+        <v>43069</v>
+      </c>
+      <c r="B261" s="49">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="C261" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="D261" s="150" t="s">
         <v>295</v>
       </c>
-      <c r="E259" s="136"/>
-      <c r="F259" s="136"/>
-      <c r="G259" s="32"/>
-    </row>
-    <row r="260" spans="1:7">
-      <c r="A260" s="50">
-        <v>43248</v>
-      </c>
-      <c r="B260" s="51">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C260" s="20" t="s">
-        <v>289</v>
-      </c>
-      <c r="D260" s="128" t="s">
-        <v>296</v>
-      </c>
-      <c r="E260" s="129"/>
-      <c r="F260" s="130"/>
-      <c r="G260" s="33"/>
-    </row>
-    <row r="261" spans="1:7">
-      <c r="A261" s="50">
-        <v>43339</v>
-      </c>
-      <c r="B261" s="51">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="C261" s="20" t="s">
-        <v>289</v>
-      </c>
-      <c r="D261" s="128" t="s">
-        <v>297</v>
-      </c>
-      <c r="E261" s="129"/>
-      <c r="F261" s="130"/>
-      <c r="G261" s="33"/>
+      <c r="E261" s="150"/>
+      <c r="F261" s="150"/>
+      <c r="G261" s="32"/>
     </row>
     <row r="262" spans="1:7">
       <c r="A262" s="50">
-        <v>43542</v>
+        <v>43248</v>
       </c>
       <c r="B262" s="51">
-        <v>1.1200000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C262" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="D262" s="128" t="s">
-        <v>298</v>
-      </c>
-      <c r="E262" s="129"/>
-      <c r="F262" s="130"/>
+      <c r="D262" s="151" t="s">
+        <v>296</v>
+      </c>
+      <c r="E262" s="152"/>
+      <c r="F262" s="153"/>
       <c r="G262" s="33"/>
     </row>
     <row r="263" spans="1:7">
       <c r="A263" s="50">
-        <v>43599</v>
+        <v>43339</v>
       </c>
       <c r="B263" s="51">
-        <v>1.1299999999999999</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="C263" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="D263" s="52" t="s">
-        <v>299</v>
-      </c>
-      <c r="E263" s="53"/>
-      <c r="F263" s="54"/>
+      <c r="D263" s="151" t="s">
+        <v>297</v>
+      </c>
+      <c r="E263" s="152"/>
+      <c r="F263" s="153"/>
       <c r="G263" s="33"/>
     </row>
     <row r="264" spans="1:7">
       <c r="A264" s="50">
-        <v>43643</v>
+        <v>43542</v>
       </c>
       <c r="B264" s="51">
-        <v>1.1399999999999999</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="C264" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="D264" s="52" t="s">
-        <v>300</v>
-      </c>
-      <c r="E264" s="53"/>
-      <c r="F264" s="54"/>
+      <c r="D264" s="151" t="s">
+        <v>298</v>
+      </c>
+      <c r="E264" s="152"/>
+      <c r="F264" s="153"/>
       <c r="G264" s="33"/>
     </row>
     <row r="265" spans="1:7">
       <c r="A265" s="50">
-        <v>43894</v>
+        <v>43599</v>
       </c>
       <c r="B265" s="51">
-        <v>1.1499999999999999</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="C265" s="20" t="s">
         <v>289</v>
       </c>
       <c r="D265" s="52" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E265" s="53"/>
       <c r="F265" s="54"/>
@@ -9989,16 +10114,16 @@
     </row>
     <row r="266" spans="1:7">
       <c r="A266" s="50">
-        <v>44017</v>
+        <v>43643</v>
       </c>
       <c r="B266" s="51">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="C266" s="71" t="s">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="C266" s="20" t="s">
         <v>289</v>
       </c>
       <c r="D266" s="52" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E266" s="53"/>
       <c r="F266" s="54"/>
@@ -10006,16 +10131,16 @@
     </row>
     <row r="267" spans="1:7">
       <c r="A267" s="50">
-        <v>44118</v>
+        <v>43894</v>
       </c>
       <c r="B267" s="51">
-        <v>1.17</v>
-      </c>
-      <c r="C267" s="73" t="s">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C267" s="20" t="s">
         <v>289</v>
       </c>
       <c r="D267" s="52" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="E267" s="53"/>
       <c r="F267" s="54"/>
@@ -10023,16 +10148,16 @@
     </row>
     <row r="268" spans="1:7">
       <c r="A268" s="50">
-        <v>44209</v>
+        <v>44017</v>
       </c>
       <c r="B268" s="51">
-        <v>1.18</v>
-      </c>
-      <c r="C268" s="77" t="s">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="C268" s="71" t="s">
         <v>289</v>
       </c>
-      <c r="D268" s="86" t="s">
-        <v>320</v>
+      <c r="D268" s="52" t="s">
+        <v>302</v>
       </c>
       <c r="E268" s="53"/>
       <c r="F268" s="54"/>
@@ -10040,16 +10165,16 @@
     </row>
     <row r="269" spans="1:7">
       <c r="A269" s="50">
-        <v>44258</v>
+        <v>44118</v>
       </c>
       <c r="B269" s="51">
-        <v>1.19</v>
-      </c>
-      <c r="C269" s="80" t="s">
+        <v>1.17</v>
+      </c>
+      <c r="C269" s="73" t="s">
         <v>289</v>
       </c>
       <c r="D269" s="52" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="E269" s="53"/>
       <c r="F269" s="54"/>
@@ -10057,16 +10182,16 @@
     </row>
     <row r="270" spans="1:7">
       <c r="A270" s="50">
-        <v>44357</v>
+        <v>44209</v>
       </c>
       <c r="B270" s="51">
-        <v>1.2</v>
-      </c>
-      <c r="C270" s="82" t="s">
+        <v>1.18</v>
+      </c>
+      <c r="C270" s="77" t="s">
         <v>289</v>
       </c>
-      <c r="D270" s="52" t="s">
-        <v>337</v>
+      <c r="D270" s="86" t="s">
+        <v>320</v>
       </c>
       <c r="E270" s="53"/>
       <c r="F270" s="54"/>
@@ -10074,16 +10199,16 @@
     </row>
     <row r="271" spans="1:7">
       <c r="A271" s="50">
-        <v>44487</v>
+        <v>44258</v>
       </c>
       <c r="B271" s="51">
-        <v>1.21</v>
-      </c>
-      <c r="C271" s="88" t="s">
+        <v>1.19</v>
+      </c>
+      <c r="C271" s="80" t="s">
         <v>289</v>
       </c>
       <c r="D271" s="52" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="E271" s="53"/>
       <c r="F271" s="54"/>
@@ -10091,16 +10216,16 @@
     </row>
     <row r="272" spans="1:7">
       <c r="A272" s="50">
-        <v>44518</v>
+        <v>44357</v>
       </c>
       <c r="B272" s="51">
-        <v>1.22</v>
-      </c>
-      <c r="C272" s="107" t="s">
+        <v>1.2</v>
+      </c>
+      <c r="C272" s="82" t="s">
         <v>289</v>
       </c>
       <c r="D272" s="52" t="s">
-        <v>361</v>
+        <v>337</v>
       </c>
       <c r="E272" s="53"/>
       <c r="F272" s="54"/>
@@ -10108,40 +10233,91 @@
     </row>
     <row r="273" spans="1:7">
       <c r="A273" s="50">
-        <v>44530</v>
+        <v>44487</v>
       </c>
       <c r="B273" s="51">
-        <v>1.23</v>
-      </c>
-      <c r="C273" s="110" t="s">
+        <v>1.21</v>
+      </c>
+      <c r="C273" s="88" t="s">
         <v>289</v>
       </c>
       <c r="D273" s="52" t="s">
-        <v>395</v>
+        <v>340</v>
       </c>
       <c r="E273" s="53"/>
       <c r="F273" s="54"/>
       <c r="G273" s="33"/>
     </row>
     <row r="274" spans="1:7">
-      <c r="A274" s="55">
+      <c r="A274" s="50">
+        <v>44518</v>
+      </c>
+      <c r="B274" s="51">
+        <v>1.22</v>
+      </c>
+      <c r="C274" s="107" t="s">
+        <v>289</v>
+      </c>
+      <c r="D274" s="52" t="s">
+        <v>361</v>
+      </c>
+      <c r="E274" s="53"/>
+      <c r="F274" s="54"/>
+      <c r="G274" s="33"/>
+    </row>
+    <row r="275" spans="1:7">
+      <c r="A275" s="50">
+        <v>44530</v>
+      </c>
+      <c r="B275" s="51">
+        <v>1.23</v>
+      </c>
+      <c r="C275" s="110" t="s">
+        <v>289</v>
+      </c>
+      <c r="D275" s="52" t="s">
+        <v>395</v>
+      </c>
+      <c r="E275" s="53"/>
+      <c r="F275" s="54"/>
+      <c r="G275" s="33"/>
+    </row>
+    <row r="276" spans="1:7">
+      <c r="A276" s="50">
         <v>44559</v>
       </c>
-      <c r="B274" s="56">
+      <c r="B276" s="51">
         <v>1.24</v>
       </c>
-      <c r="C274" s="26" t="s">
+      <c r="C276" s="114" t="s">
         <v>289</v>
       </c>
-      <c r="D274" s="131" t="s">
+      <c r="D276" s="52" t="s">
         <v>399</v>
       </c>
-      <c r="E274" s="132"/>
-      <c r="F274" s="132"/>
-      <c r="G274" s="34"/>
+      <c r="E276" s="53"/>
+      <c r="F276" s="54"/>
+      <c r="G276" s="33"/>
+    </row>
+    <row r="277" spans="1:7">
+      <c r="A277" s="55">
+        <v>44755</v>
+      </c>
+      <c r="B277" s="56">
+        <v>1.25</v>
+      </c>
+      <c r="C277" s="26" t="s">
+        <v>289</v>
+      </c>
+      <c r="D277" s="154" t="s">
+        <v>404</v>
+      </c>
+      <c r="E277" s="155"/>
+      <c r="F277" s="155"/>
+      <c r="G277" s="34"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="apWuLBIlzSrG8yzhsN6NRNuUMxPsVv6nh9x2ibQ2WTXetoAj2BIKJUf55DVFWNeEvBrjPDVHqwNr8Lr9q27wyQ==" saltValue="38Ewv6vELDf+Pf6Dvr7g9A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="7MNpesOG1rZ2LnPtxhNxmcf/+7u/H7WIeQiis60EcC11Lcg2hAZBo+Fy1qouALu83/cgX8zW69Zdd9X5yJU6mw==" saltValue="J1j/ZnlHpA3xx+2QC3XePw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <customSheetViews>
     <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115" topLeftCell="A139">
       <selection activeCell="D163" sqref="D163"/>
@@ -10150,57 +10326,57 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="51">
-    <mergeCell ref="F111:N111"/>
-    <mergeCell ref="C224:E224"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C226:E226"/>
-    <mergeCell ref="C227:E227"/>
-    <mergeCell ref="C228:E228"/>
-    <mergeCell ref="C229:E229"/>
+    <mergeCell ref="B199:B201"/>
+    <mergeCell ref="B202:B209"/>
+    <mergeCell ref="B227:B228"/>
+    <mergeCell ref="B229:B230"/>
+    <mergeCell ref="B231:B232"/>
+    <mergeCell ref="B149:B162"/>
+    <mergeCell ref="B163:B170"/>
+    <mergeCell ref="B171:B181"/>
+    <mergeCell ref="B182:B189"/>
+    <mergeCell ref="B190:B198"/>
+    <mergeCell ref="D263:F263"/>
+    <mergeCell ref="D264:F264"/>
+    <mergeCell ref="D277:F277"/>
+    <mergeCell ref="A227:A234"/>
+    <mergeCell ref="A235:A238"/>
+    <mergeCell ref="A239:A242"/>
+    <mergeCell ref="B233:B234"/>
+    <mergeCell ref="B235:B236"/>
+    <mergeCell ref="B237:B238"/>
+    <mergeCell ref="B239:B240"/>
+    <mergeCell ref="B241:B242"/>
+    <mergeCell ref="D258:F258"/>
+    <mergeCell ref="D259:F259"/>
+    <mergeCell ref="D260:F260"/>
+    <mergeCell ref="D261:F261"/>
+    <mergeCell ref="D262:F262"/>
+    <mergeCell ref="B249:E249"/>
+    <mergeCell ref="B250:E250"/>
+    <mergeCell ref="B251:E251"/>
+    <mergeCell ref="D256:F256"/>
+    <mergeCell ref="D257:F257"/>
+    <mergeCell ref="C240:E240"/>
+    <mergeCell ref="C241:E241"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="B247:E247"/>
+    <mergeCell ref="B248:E248"/>
+    <mergeCell ref="C235:E235"/>
+    <mergeCell ref="C236:E236"/>
+    <mergeCell ref="C237:E237"/>
+    <mergeCell ref="C238:E238"/>
+    <mergeCell ref="C239:E239"/>
     <mergeCell ref="C230:E230"/>
     <mergeCell ref="C231:E231"/>
     <mergeCell ref="C232:E232"/>
     <mergeCell ref="C233:E233"/>
     <mergeCell ref="C234:E234"/>
-    <mergeCell ref="C235:E235"/>
-    <mergeCell ref="C236:E236"/>
-    <mergeCell ref="C237:E237"/>
-    <mergeCell ref="C238:E238"/>
-    <mergeCell ref="C239:E239"/>
-    <mergeCell ref="C240:E240"/>
-    <mergeCell ref="B245:E245"/>
-    <mergeCell ref="B246:E246"/>
-    <mergeCell ref="B247:E247"/>
-    <mergeCell ref="B248:E248"/>
-    <mergeCell ref="B249:E249"/>
-    <mergeCell ref="D254:F254"/>
-    <mergeCell ref="D255:F255"/>
-    <mergeCell ref="D261:F261"/>
-    <mergeCell ref="D262:F262"/>
-    <mergeCell ref="D274:F274"/>
-    <mergeCell ref="A225:A232"/>
-    <mergeCell ref="A233:A236"/>
-    <mergeCell ref="A237:A240"/>
-    <mergeCell ref="B231:B232"/>
-    <mergeCell ref="B233:B234"/>
-    <mergeCell ref="B235:B236"/>
-    <mergeCell ref="B237:B238"/>
-    <mergeCell ref="B239:B240"/>
-    <mergeCell ref="D256:F256"/>
-    <mergeCell ref="D257:F257"/>
-    <mergeCell ref="D258:F258"/>
-    <mergeCell ref="D259:F259"/>
-    <mergeCell ref="D260:F260"/>
-    <mergeCell ref="B149:B162"/>
-    <mergeCell ref="B163:B169"/>
-    <mergeCell ref="B170:B180"/>
-    <mergeCell ref="B181:B188"/>
-    <mergeCell ref="B189:B197"/>
-    <mergeCell ref="B198:B200"/>
-    <mergeCell ref="B201:B207"/>
-    <mergeCell ref="B225:B226"/>
-    <mergeCell ref="B227:B228"/>
-    <mergeCell ref="B229:B230"/>
+    <mergeCell ref="F111:N111"/>
+    <mergeCell ref="C226:E226"/>
+    <mergeCell ref="C227:E227"/>
+    <mergeCell ref="C228:E228"/>
+    <mergeCell ref="C229:E229"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -10209,7 +10385,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -10217,7 +10393,7 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -10226,16 +10402,16 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="E26" sqref="E26"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="D24" sqref="D24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="D24" sqref="D24"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
i434--squish run record environment update
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_example/standard_suite/diamond_regression.xlsx
+++ b/tmp_client/doc/TMP_example/standard_suite/diamond_regression.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\repository\tmp_client\doc\TMP_example\standard_suite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3294B8-563E-4F51-8847-CDD17A8E75B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24DF3DF5-072E-49EB-9683-52A3528C8934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,15 +26,15 @@
   </definedNames>
   <calcPr calcId="144525"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="2391" yWindow="-9" windowWidth="2418" windowHeight="1318" activeSheetId="3" showComments="commIndAndComment"/>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
     <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
-    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="2391" yWindow="-9" windowWidth="2418" windowHeight="1318" activeSheetId="3" showComments="commIndAndComment"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="413">
   <si>
     <t>[suite_info]</t>
   </si>
@@ -1297,6 +1297,15 @@
   <si>
     <t>video record support for client tasks</t>
   </si>
+  <si>
+    <t>SQUISH_RECORD = 1</t>
+  </si>
+  <si>
+    <t>Any</t>
+  </si>
+  <si>
+    <t>Client only check this variable exists or not</t>
+  </si>
 </sst>
 </file>
 
@@ -1306,12 +1315,19 @@
     <numFmt numFmtId="164" formatCode="0.00_);[Red]\(0.00\)"/>
     <numFmt numFmtId="165" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1401,7 +1417,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -1894,203 +1910,192 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="37" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="37" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="171">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="5" applyNumberFormat="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="5" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="5" applyNumberFormat="1">
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="5" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="5" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="5" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="7" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="7" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="12" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="12" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="13" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="13" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="14" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="14" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="15" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="15" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
@@ -2102,10 +2107,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2117,7 +2122,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2135,11 +2140,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
@@ -2148,10 +2153,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2160,19 +2165,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1">
@@ -2181,10 +2186,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2194,7 +2199,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2203,212 +2208,216 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="5" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="5" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="5" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="5" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="5" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="5" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="5" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="33" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="33" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="34" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="34" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="36" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="36" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4757,13 +4766,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>216</xdr:row>
+      <xdr:row>217</xdr:row>
       <xdr:rowOff>140970</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>904875</xdr:colOff>
-      <xdr:row>224</xdr:row>
+      <xdr:row>225</xdr:row>
       <xdr:rowOff>102870</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5398,8 +5407,8 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="B4" sqref="B4"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="B41" sqref="B41"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -5408,8 +5417,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="B41" sqref="B41"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="B4" sqref="B4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -5462,42 +5471,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" s="57" customFormat="1">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="127" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
-      <c r="H1" s="126"/>
-      <c r="I1" s="126"/>
-      <c r="J1" s="126"/>
-      <c r="K1" s="126"/>
-      <c r="L1" s="126"/>
-      <c r="M1" s="126"/>
-      <c r="N1" s="126"/>
-      <c r="O1" s="126"/>
-      <c r="P1" s="126"/>
-      <c r="Q1" s="126"/>
-      <c r="R1" s="126"/>
-      <c r="S1" s="126"/>
-      <c r="T1" s="126"/>
-      <c r="U1" s="126"/>
-      <c r="V1" s="126"/>
-      <c r="W1" s="126"/>
-      <c r="X1" s="127"/>
-      <c r="Y1" s="128" t="s">
+      <c r="B1" s="128"/>
+      <c r="C1" s="128"/>
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="128"/>
+      <c r="H1" s="128"/>
+      <c r="I1" s="128"/>
+      <c r="J1" s="128"/>
+      <c r="K1" s="128"/>
+      <c r="L1" s="128"/>
+      <c r="M1" s="128"/>
+      <c r="N1" s="128"/>
+      <c r="O1" s="128"/>
+      <c r="P1" s="128"/>
+      <c r="Q1" s="128"/>
+      <c r="R1" s="128"/>
+      <c r="S1" s="128"/>
+      <c r="T1" s="128"/>
+      <c r="U1" s="128"/>
+      <c r="V1" s="128"/>
+      <c r="W1" s="128"/>
+      <c r="X1" s="129"/>
+      <c r="Y1" s="130" t="s">
         <v>13</v>
       </c>
-      <c r="Z1" s="128"/>
-      <c r="AA1" s="128"/>
-      <c r="AB1" s="128"/>
-      <c r="AC1" s="128"/>
-      <c r="AD1" s="128"/>
-      <c r="AE1" s="128"/>
-      <c r="AF1" s="128"/>
+      <c r="Z1" s="130"/>
+      <c r="AA1" s="130"/>
+      <c r="AB1" s="130"/>
+      <c r="AC1" s="130"/>
+      <c r="AD1" s="130"/>
+      <c r="AE1" s="130"/>
+      <c r="AF1" s="130"/>
     </row>
     <row r="2" spans="1:32" s="57" customFormat="1">
       <c r="A2" s="60" t="s">
@@ -7018,26 +7027,26 @@
   <sheetProtection algorithmName="SHA-512" hashValue="Sju3pjEnjegba3BrZLImZ+xscQ9MLEq+i8mDO7rXFn4S3yXv8zWb4HaF0uC2YruSs8wkV8FCIxY7a0fvnwVXFw==" saltValue="mZmUchosJ60PlKqUXOSzGQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A2:AF46" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <customSheetViews>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen"/>
-      <selection activeCell="H23" sqref="H23"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="85" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
-      <autoFilter ref="A2:Y2" xr:uid="{67DA3D03-4751-4353-B230-F152739151D6}"/>
+      <autoFilter ref="A2:AF46" xr:uid="{B09CBBEF-D706-4648-BE3A-906C2B40087F}"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen"/>
       <selection activeCell="C23" sqref="C23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
-      <autoFilter ref="A2:Y2" xr:uid="{9580C794-B700-473D-BC71-633D862FAD88}"/>
+      <autoFilter ref="A2:Y2" xr:uid="{53CB5A60-F92A-4B8D-9E7A-73846FA9D12C}"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="85" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen"/>
+      <selection activeCell="H23" sqref="H23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
-      <autoFilter ref="A2:AF46" xr:uid="{2927C4EC-9E6E-4DD8-9EA6-CA16B9D44144}"/>
+      <autoFilter ref="A2:Y2" xr:uid="{0CC67152-D474-4B02-9AF2-919DF322C933}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -7120,10 +7129,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:N279"/>
+  <dimension ref="A1:N280"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A191" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G169" sqref="G169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -7184,17 +7193,17 @@
       <c r="E111" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="F111" s="161" t="s">
+      <c r="F111" s="131" t="s">
         <v>140</v>
       </c>
-      <c r="G111" s="162"/>
-      <c r="H111" s="162"/>
-      <c r="I111" s="162"/>
-      <c r="J111" s="162"/>
-      <c r="K111" s="162"/>
-      <c r="L111" s="162"/>
-      <c r="M111" s="162"/>
-      <c r="N111" s="163"/>
+      <c r="G111" s="132"/>
+      <c r="H111" s="132"/>
+      <c r="I111" s="132"/>
+      <c r="J111" s="132"/>
+      <c r="K111" s="132"/>
+      <c r="L111" s="132"/>
+      <c r="M111" s="132"/>
+      <c r="N111" s="133"/>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="6" t="s">
@@ -8114,7 +8123,7 @@
       <c r="A149" s="19">
         <v>1</v>
       </c>
-      <c r="B149" s="129" t="s">
+      <c r="B149" s="162" t="s">
         <v>4</v>
       </c>
       <c r="C149" s="62" t="s">
@@ -8140,7 +8149,7 @@
       <c r="A150" s="19">
         <v>2</v>
       </c>
-      <c r="B150" s="131"/>
+      <c r="B150" s="163"/>
       <c r="C150" s="21" t="s">
         <v>173</v>
       </c>
@@ -8162,7 +8171,7 @@
       <c r="A151" s="19">
         <v>3</v>
       </c>
-      <c r="B151" s="131"/>
+      <c r="B151" s="163"/>
       <c r="C151" s="21" t="s">
         <v>18</v>
       </c>
@@ -8182,7 +8191,7 @@
       <c r="A152" s="19">
         <v>4</v>
       </c>
-      <c r="B152" s="131"/>
+      <c r="B152" s="163"/>
       <c r="C152" s="21" t="s">
         <v>175</v>
       </c>
@@ -8206,7 +8215,7 @@
       <c r="A153" s="19">
         <v>5</v>
       </c>
-      <c r="B153" s="131"/>
+      <c r="B153" s="163"/>
       <c r="C153" s="62" t="s">
         <v>177</v>
       </c>
@@ -8230,7 +8239,7 @@
       <c r="A154" s="19">
         <v>6</v>
       </c>
-      <c r="B154" s="131"/>
+      <c r="B154" s="163"/>
       <c r="C154" s="62" t="s">
         <v>181</v>
       </c>
@@ -8254,7 +8263,7 @@
       <c r="A155" s="19">
         <v>7</v>
       </c>
-      <c r="B155" s="131"/>
+      <c r="B155" s="163"/>
       <c r="C155" s="21" t="s">
         <v>183</v>
       </c>
@@ -8276,7 +8285,7 @@
       <c r="A156" s="19">
         <v>8</v>
       </c>
-      <c r="B156" s="131"/>
+      <c r="B156" s="163"/>
       <c r="C156" s="62" t="s">
         <v>184</v>
       </c>
@@ -8300,7 +8309,7 @@
       <c r="A157" s="19">
         <v>9</v>
       </c>
-      <c r="B157" s="131"/>
+      <c r="B157" s="163"/>
       <c r="C157" s="62" t="s">
         <v>185</v>
       </c>
@@ -8324,7 +8333,7 @@
       <c r="A158" s="19">
         <v>10</v>
       </c>
-      <c r="B158" s="131"/>
+      <c r="B158" s="163"/>
       <c r="C158" s="21" t="s">
         <v>186</v>
       </c>
@@ -8348,7 +8357,7 @@
       <c r="A159" s="112">
         <v>11</v>
       </c>
-      <c r="B159" s="131"/>
+      <c r="B159" s="163"/>
       <c r="C159" s="21" t="s">
         <v>187</v>
       </c>
@@ -8372,7 +8381,7 @@
       <c r="A160" s="112">
         <v>12</v>
       </c>
-      <c r="B160" s="131"/>
+      <c r="B160" s="163"/>
       <c r="C160" s="21" t="s">
         <v>189</v>
       </c>
@@ -8394,7 +8403,7 @@
       <c r="A161" s="112">
         <v>13</v>
       </c>
-      <c r="B161" s="131"/>
+      <c r="B161" s="163"/>
       <c r="C161" s="111" t="s">
         <v>400</v>
       </c>
@@ -8416,7 +8425,7 @@
       <c r="A162" s="112">
         <v>14</v>
       </c>
-      <c r="B162" s="139"/>
+      <c r="B162" s="148"/>
       <c r="C162" s="21" t="s">
         <v>193</v>
       </c>
@@ -8440,7 +8449,7 @@
       <c r="A163" s="112">
         <v>15</v>
       </c>
-      <c r="B163" s="140" t="s">
+      <c r="B163" s="143" t="s">
         <v>5</v>
       </c>
       <c r="C163" s="21" t="s">
@@ -8467,7 +8476,7 @@
       <c r="A164" s="112">
         <v>16</v>
       </c>
-      <c r="B164" s="140"/>
+      <c r="B164" s="143"/>
       <c r="C164" s="89" t="s">
         <v>341</v>
       </c>
@@ -8491,7 +8500,7 @@
       <c r="A165" s="112">
         <v>17</v>
       </c>
-      <c r="B165" s="140"/>
+      <c r="B165" s="143"/>
       <c r="C165" s="89" t="s">
         <v>344</v>
       </c>
@@ -8515,7 +8524,7 @@
       <c r="A166" s="112">
         <v>18</v>
       </c>
-      <c r="B166" s="140"/>
+      <c r="B166" s="143"/>
       <c r="C166" s="100" t="s">
         <v>377</v>
       </c>
@@ -8539,7 +8548,7 @@
       <c r="A167" s="112">
         <v>19</v>
       </c>
-      <c r="B167" s="140"/>
+      <c r="B167" s="143"/>
       <c r="C167" s="100" t="s">
         <v>378</v>
       </c>
@@ -8558,10 +8567,10 @@
       <c r="H167" s="101"/>
     </row>
     <row r="168" spans="1:9">
-      <c r="A168" s="112">
+      <c r="A168" s="125">
         <v>20</v>
       </c>
-      <c r="B168" s="140"/>
+      <c r="B168" s="143"/>
       <c r="C168" s="100" t="s">
         <v>379</v>
       </c>
@@ -8580,450 +8589,454 @@
       <c r="H168" s="68"/>
     </row>
     <row r="169" spans="1:9">
-      <c r="A169" s="118">
+      <c r="A169" s="125">
         <v>21</v>
       </c>
-      <c r="B169" s="140"/>
-      <c r="C169" s="121" t="s">
+      <c r="B169" s="143"/>
+      <c r="C169" s="170" t="s">
+        <v>410</v>
+      </c>
+      <c r="D169" s="124" t="s">
+        <v>169</v>
+      </c>
+      <c r="E169" s="124" t="s">
+        <v>169</v>
+      </c>
+      <c r="F169" s="126">
+        <v>1</v>
+      </c>
+      <c r="G169" s="170" t="s">
+        <v>411</v>
+      </c>
+      <c r="H169" s="68" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9">
+      <c r="A170" s="125">
+        <v>22</v>
+      </c>
+      <c r="B170" s="143"/>
+      <c r="C170" s="120" t="s">
         <v>200</v>
       </c>
-      <c r="D169" s="117" t="s">
-        <v>169</v>
-      </c>
-      <c r="E169" s="117" t="s">
-        <v>169</v>
-      </c>
-      <c r="F169" s="116"/>
-      <c r="G169" s="100" t="s">
+      <c r="D170" s="117" t="s">
+        <v>169</v>
+      </c>
+      <c r="E170" s="117" t="s">
+        <v>169</v>
+      </c>
+      <c r="F170" s="116"/>
+      <c r="G170" s="100" t="s">
         <v>171</v>
       </c>
-      <c r="H169" s="68" t="s">
+      <c r="H170" s="68" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="170" spans="1:9">
-      <c r="A170" s="118">
-        <v>22</v>
-      </c>
-      <c r="B170" s="137"/>
-      <c r="C170" s="83" t="s">
+    <row r="171" spans="1:9">
+      <c r="A171" s="125">
+        <v>23</v>
+      </c>
+      <c r="B171" s="144"/>
+      <c r="C171" s="83" t="s">
         <v>204</v>
       </c>
-      <c r="D170" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E170" s="87" t="s">
-        <v>169</v>
-      </c>
-      <c r="F170" s="90" t="s">
+      <c r="D171" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E171" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="F171" s="90" t="s">
         <v>405</v>
       </c>
-      <c r="G170" s="89" t="s">
+      <c r="G171" s="89" t="s">
         <v>205</v>
       </c>
-      <c r="H170" s="122" t="s">
+      <c r="H171" s="121" t="s">
         <v>406</v>
       </c>
-      <c r="I170" s="85"/>
-    </row>
-    <row r="171" spans="1:9">
-      <c r="A171" s="118">
-        <v>23</v>
-      </c>
-      <c r="B171" s="129" t="s">
+      <c r="I171" s="85"/>
+    </row>
+    <row r="172" spans="1:9">
+      <c r="A172" s="125">
+        <v>24</v>
+      </c>
+      <c r="B172" s="162" t="s">
         <v>6</v>
       </c>
-      <c r="C171" s="89" t="s">
+      <c r="C172" s="89" t="s">
         <v>202</v>
       </c>
-      <c r="D171" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E171" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F171" s="89" t="s">
+      <c r="D172" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E172" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F172" s="89" t="s">
         <v>203</v>
       </c>
-      <c r="G171" s="66" t="s">
+      <c r="G172" s="66" t="s">
         <v>171</v>
       </c>
-      <c r="H171" s="68" t="s">
+      <c r="H172" s="68" t="s">
         <v>353</v>
       </c>
-      <c r="I171" s="85"/>
-    </row>
-    <row r="172" spans="1:9">
-      <c r="A172" s="118">
-        <v>24</v>
-      </c>
-      <c r="B172" s="130"/>
-      <c r="C172" s="100" t="s">
+      <c r="I172" s="85"/>
+    </row>
+    <row r="173" spans="1:9">
+      <c r="A173" s="125">
+        <v>25</v>
+      </c>
+      <c r="B173" s="164"/>
+      <c r="C173" s="100" t="s">
         <v>347</v>
       </c>
-      <c r="D172" s="87" t="s">
-        <v>169</v>
-      </c>
-      <c r="E172" s="87" t="s">
-        <v>169</v>
-      </c>
-      <c r="F172" s="89" t="s">
+      <c r="D173" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="E173" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="F173" s="89" t="s">
         <v>349</v>
-      </c>
-      <c r="G172" s="89" t="s">
-        <v>171</v>
-      </c>
-      <c r="H172" s="68" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="173" spans="1:9">
-      <c r="A173" s="118">
-        <v>25</v>
-      </c>
-      <c r="B173" s="130"/>
-      <c r="C173" s="100" t="s">
-        <v>348</v>
-      </c>
-      <c r="D173" s="87" t="s">
-        <v>169</v>
-      </c>
-      <c r="E173" s="87" t="s">
-        <v>169</v>
-      </c>
-      <c r="F173" s="89" t="s">
-        <v>350</v>
       </c>
       <c r="G173" s="89" t="s">
         <v>171</v>
       </c>
-      <c r="H173" s="96" t="s">
+      <c r="H173" s="68" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9">
+      <c r="A174" s="125">
+        <v>26</v>
+      </c>
+      <c r="B174" s="164"/>
+      <c r="C174" s="100" t="s">
+        <v>348</v>
+      </c>
+      <c r="D174" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="E174" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="F174" s="89" t="s">
+        <v>350</v>
+      </c>
+      <c r="G174" s="89" t="s">
+        <v>171</v>
+      </c>
+      <c r="H174" s="96" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="174" spans="1:9">
-      <c r="A174" s="118">
-        <v>26</v>
-      </c>
-      <c r="B174" s="130"/>
-      <c r="C174" s="100" t="s">
+    <row r="175" spans="1:9">
+      <c r="A175" s="125">
+        <v>27</v>
+      </c>
+      <c r="B175" s="164"/>
+      <c r="C175" s="100" t="s">
         <v>382</v>
       </c>
-      <c r="D174" s="97" t="s">
-        <v>169</v>
-      </c>
-      <c r="E174" s="97" t="s">
-        <v>169</v>
-      </c>
-      <c r="F174" s="98" t="s">
+      <c r="D175" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="E175" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="F175" s="98" t="s">
         <v>350</v>
       </c>
-      <c r="G174" s="98" t="s">
+      <c r="G175" s="98" t="s">
         <v>171</v>
       </c>
-      <c r="H174" s="96"/>
-    </row>
-    <row r="175" spans="1:9">
-      <c r="A175" s="118">
-        <v>27</v>
-      </c>
-      <c r="B175" s="130"/>
-      <c r="C175" s="100" t="s">
+      <c r="H175" s="96"/>
+    </row>
+    <row r="176" spans="1:9">
+      <c r="A176" s="125">
+        <v>28</v>
+      </c>
+      <c r="B176" s="164"/>
+      <c r="C176" s="100" t="s">
         <v>369</v>
       </c>
-      <c r="D175" s="87" t="s">
-        <v>169</v>
-      </c>
-      <c r="E175" s="87" t="s">
-        <v>169</v>
-      </c>
-      <c r="F175" s="89" t="s">
+      <c r="D176" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="E176" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="F176" s="89" t="s">
         <v>350</v>
       </c>
-      <c r="G175" s="89" t="s">
+      <c r="G176" s="89" t="s">
         <v>171</v>
       </c>
-      <c r="H175" s="68"/>
-    </row>
-    <row r="176" spans="1:9">
-      <c r="A176" s="118">
-        <v>28</v>
-      </c>
-      <c r="B176" s="130"/>
-      <c r="C176" s="93" t="s">
+      <c r="H176" s="68"/>
+    </row>
+    <row r="177" spans="1:8">
+      <c r="A177" s="125">
+        <v>29</v>
+      </c>
+      <c r="B177" s="164"/>
+      <c r="C177" s="93" t="s">
         <v>366</v>
       </c>
-      <c r="D176" s="92"/>
-      <c r="E176" s="92" t="s">
-        <v>169</v>
-      </c>
-      <c r="F176" s="93" t="s">
+      <c r="D177" s="92"/>
+      <c r="E177" s="92" t="s">
+        <v>169</v>
+      </c>
+      <c r="F177" s="93" t="s">
         <v>367</v>
       </c>
-      <c r="G176" s="93" t="s">
+      <c r="G177" s="93" t="s">
         <v>171</v>
       </c>
-      <c r="H176" s="96" t="s">
+      <c r="H177" s="96" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="177" spans="1:8">
-      <c r="A177" s="118">
-        <v>29</v>
-      </c>
-      <c r="B177" s="130"/>
-      <c r="C177" s="102" t="s">
+    <row r="178" spans="1:8">
+      <c r="A178" s="125">
+        <v>30</v>
+      </c>
+      <c r="B178" s="164"/>
+      <c r="C178" s="102" t="s">
         <v>376</v>
       </c>
-      <c r="D177" s="97" t="s">
-        <v>169</v>
-      </c>
-      <c r="E177" s="97" t="s">
-        <v>169</v>
-      </c>
-      <c r="F177" s="102" t="s">
+      <c r="D178" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="E178" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="F178" s="102" t="s">
         <v>373</v>
       </c>
-      <c r="G177" s="108" t="s">
+      <c r="G178" s="108" t="s">
         <v>386</v>
       </c>
-      <c r="H177" s="96" t="s">
+      <c r="H178" s="96" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="178" spans="1:8">
-      <c r="A178" s="118">
-        <v>30</v>
-      </c>
-      <c r="B178" s="130"/>
-      <c r="C178" s="91" t="s">
+    <row r="179" spans="1:8">
+      <c r="A179" s="125">
+        <v>31</v>
+      </c>
+      <c r="B179" s="164"/>
+      <c r="C179" s="91" t="s">
         <v>364</v>
       </c>
-      <c r="D178" s="100" t="s">
-        <v>169</v>
-      </c>
-      <c r="E178" s="94"/>
-      <c r="F178" s="91" t="s">
+      <c r="D179" s="100" t="s">
+        <v>169</v>
+      </c>
+      <c r="E179" s="94"/>
+      <c r="F179" s="91" t="s">
         <v>228</v>
       </c>
-      <c r="G178" s="91" t="s">
+      <c r="G179" s="91" t="s">
         <v>229</v>
       </c>
-      <c r="H178" s="68" t="s">
+      <c r="H179" s="68" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="179" spans="1:8">
-      <c r="A179" s="118">
-        <v>31</v>
-      </c>
-      <c r="B179" s="130"/>
-      <c r="C179" s="100" t="s">
+    <row r="180" spans="1:8">
+      <c r="A180" s="125">
+        <v>32</v>
+      </c>
+      <c r="B180" s="164"/>
+      <c r="C180" s="100" t="s">
         <v>372</v>
       </c>
-      <c r="D179" s="100" t="s">
-        <v>169</v>
-      </c>
-      <c r="E179" s="100" t="s">
-        <v>169</v>
-      </c>
-      <c r="F179" s="102" t="s">
+      <c r="D180" s="100" t="s">
+        <v>169</v>
+      </c>
+      <c r="E180" s="100" t="s">
+        <v>169</v>
+      </c>
+      <c r="F180" s="102" t="s">
         <v>385</v>
       </c>
-      <c r="G179" s="102" t="s">
+      <c r="G180" s="102" t="s">
         <v>383</v>
       </c>
-      <c r="H179" s="103" t="s">
+      <c r="H180" s="103" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="180" spans="1:8">
-      <c r="A180" s="118">
-        <v>32</v>
-      </c>
-      <c r="B180" s="130"/>
-      <c r="C180" s="66" t="s">
+    <row r="181" spans="1:8">
+      <c r="A181" s="125">
+        <v>33</v>
+      </c>
+      <c r="B181" s="164"/>
+      <c r="C181" s="66" t="s">
         <v>304</v>
       </c>
-      <c r="D180" s="65" t="s">
-        <v>169</v>
-      </c>
-      <c r="E180" s="65" t="s">
-        <v>169</v>
-      </c>
-      <c r="F180" s="65"/>
-      <c r="G180" s="66" t="s">
+      <c r="D181" s="65" t="s">
+        <v>169</v>
+      </c>
+      <c r="E181" s="65" t="s">
+        <v>169</v>
+      </c>
+      <c r="F181" s="65"/>
+      <c r="G181" s="66" t="s">
         <v>171</v>
       </c>
-      <c r="H180" s="68" t="s">
+      <c r="H181" s="68" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="181" spans="1:8">
-      <c r="A181" s="118">
-        <v>33</v>
-      </c>
-      <c r="B181" s="139"/>
-      <c r="C181" s="62" t="s">
+    <row r="182" spans="1:8">
+      <c r="A182" s="125">
+        <v>34</v>
+      </c>
+      <c r="B182" s="148"/>
+      <c r="C182" s="62" t="s">
         <v>204</v>
       </c>
-      <c r="D181" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E181" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F181" s="21"/>
-      <c r="G181" s="21" t="s">
+      <c r="D182" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E182" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F182" s="21"/>
+      <c r="G182" s="21" t="s">
         <v>205</v>
       </c>
-      <c r="H181" s="96" t="s">
+      <c r="H182" s="96" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="182" spans="1:8">
-      <c r="A182" s="118">
-        <v>34</v>
-      </c>
-      <c r="B182" s="140" t="s">
+    <row r="183" spans="1:8">
+      <c r="A183" s="125">
+        <v>35</v>
+      </c>
+      <c r="B183" s="143" t="s">
         <v>8</v>
       </c>
-      <c r="C182" s="21" t="s">
+      <c r="C183" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="D182" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E182" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F182" s="89" t="s">
+      <c r="D183" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E183" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F183" s="89" t="s">
         <v>207</v>
       </c>
-      <c r="G182" s="89" t="s">
+      <c r="G183" s="89" t="s">
         <v>358</v>
       </c>
-      <c r="H182" s="68" t="s">
+      <c r="H183" s="68" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="183" spans="1:8">
-      <c r="A183" s="118">
-        <v>35</v>
-      </c>
-      <c r="B183" s="137"/>
-      <c r="C183" s="89" t="s">
+    <row r="184" spans="1:8">
+      <c r="A184" s="125">
+        <v>36</v>
+      </c>
+      <c r="B184" s="144"/>
+      <c r="C184" s="89" t="s">
         <v>354</v>
       </c>
-      <c r="D183" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E183" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F183" s="89" t="s">
+      <c r="D184" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E184" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F184" s="89" t="s">
         <v>355</v>
       </c>
-      <c r="G183" s="100" t="s">
+      <c r="G184" s="100" t="s">
         <v>356</v>
       </c>
-      <c r="H183" s="68" t="s">
+      <c r="H184" s="68" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="184" spans="1:8">
-      <c r="A184" s="118">
-        <v>36</v>
-      </c>
-      <c r="B184" s="137"/>
-      <c r="C184" s="89" t="s">
+    <row r="185" spans="1:8">
+      <c r="A185" s="125">
+        <v>37</v>
+      </c>
+      <c r="B185" s="144"/>
+      <c r="C185" s="89" t="s">
         <v>209</v>
       </c>
-      <c r="D184" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E184" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F184" s="21"/>
-      <c r="G184" s="21" t="s">
+      <c r="D185" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E185" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F185" s="21"/>
+      <c r="G185" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="H184" s="11"/>
-    </row>
-    <row r="185" spans="1:8">
-      <c r="A185" s="118">
-        <v>37</v>
-      </c>
-      <c r="B185" s="137"/>
-      <c r="C185" s="21" t="s">
+      <c r="H185" s="11"/>
+    </row>
+    <row r="186" spans="1:8">
+      <c r="A186" s="125">
+        <v>38</v>
+      </c>
+      <c r="B186" s="144"/>
+      <c r="C186" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="D185" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E185" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F185" s="21">
+      <c r="D186" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E186" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F186" s="21">
         <v>20.03</v>
       </c>
-      <c r="G185" s="89">
+      <c r="G186" s="89">
         <v>20.03</v>
       </c>
-      <c r="H185" s="68" t="s">
+      <c r="H186" s="68" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="186" spans="1:8">
-      <c r="A186" s="118">
-        <v>38</v>
-      </c>
-      <c r="B186" s="137"/>
-      <c r="C186" s="21" t="s">
+    <row r="187" spans="1:8">
+      <c r="A187" s="125">
+        <v>39</v>
+      </c>
+      <c r="B187" s="144"/>
+      <c r="C187" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="D186" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E186" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F186" s="21">
+      <c r="D187" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E187" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F187" s="21">
         <v>20.04</v>
       </c>
-      <c r="G186" s="21" t="s">
-        <v>208</v>
-      </c>
-      <c r="H186" s="11"/>
-    </row>
-    <row r="187" spans="1:8">
-      <c r="A187" s="118">
-        <v>39</v>
-      </c>
-      <c r="B187" s="137"/>
-      <c r="C187" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="D187" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E187" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F187" s="21"/>
       <c r="G187" s="21" t="s">
         <v>208</v>
       </c>
       <c r="H187" s="11"/>
     </row>
     <row r="188" spans="1:8">
-      <c r="A188" s="118">
+      <c r="A188" s="125">
         <v>40</v>
       </c>
-      <c r="B188" s="137"/>
+      <c r="B188" s="144"/>
       <c r="C188" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D188" s="21" t="s">
         <v>169</v>
@@ -9038,12 +9051,12 @@
       <c r="H188" s="11"/>
     </row>
     <row r="189" spans="1:8">
-      <c r="A189" s="118">
+      <c r="A189" s="125">
         <v>41</v>
       </c>
-      <c r="B189" s="137"/>
+      <c r="B189" s="144"/>
       <c r="C189" s="21" t="s">
-        <v>47</v>
+        <v>213</v>
       </c>
       <c r="D189" s="21" t="s">
         <v>169</v>
@@ -9057,169 +9070,167 @@
       </c>
       <c r="H189" s="11"/>
     </row>
-    <row r="190" spans="1:8" ht="45">
-      <c r="A190" s="118">
+    <row r="190" spans="1:8">
+      <c r="A190" s="125">
         <v>42</v>
       </c>
-      <c r="B190" s="140" t="s">
+      <c r="B190" s="144"/>
+      <c r="C190" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D190" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E190" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F190" s="21"/>
+      <c r="G190" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="H190" s="11"/>
+    </row>
+    <row r="191" spans="1:8" ht="45">
+      <c r="A191" s="125">
+        <v>43</v>
+      </c>
+      <c r="B191" s="143" t="s">
         <v>9</v>
       </c>
-      <c r="C190" s="21" t="s">
+      <c r="C191" s="21" t="s">
         <v>214</v>
       </c>
-      <c r="D190" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E190" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F190" s="67" t="s">
+      <c r="D191" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E191" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F191" s="67" t="s">
         <v>327</v>
       </c>
-      <c r="G190" s="81" t="s">
+      <c r="G191" s="81" t="s">
         <v>363</v>
       </c>
-      <c r="H190" s="11"/>
-    </row>
-    <row r="191" spans="1:8">
-      <c r="A191" s="118">
-        <v>43</v>
-      </c>
-      <c r="B191" s="137"/>
-      <c r="C191" s="62" t="s">
+      <c r="H191" s="11"/>
+    </row>
+    <row r="192" spans="1:8">
+      <c r="A192" s="125">
+        <v>44</v>
+      </c>
+      <c r="B192" s="144"/>
+      <c r="C192" s="62" t="s">
         <v>215</v>
       </c>
-      <c r="D191" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E191" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F191" s="62" t="s">
+      <c r="D192" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E192" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F192" s="62" t="s">
         <v>216</v>
       </c>
-      <c r="G191" s="62" t="s">
+      <c r="G192" s="62" t="s">
         <v>217</v>
       </c>
-      <c r="H191" s="11"/>
-    </row>
-    <row r="192" spans="1:8">
-      <c r="A192" s="118">
-        <v>44</v>
-      </c>
-      <c r="B192" s="137"/>
-      <c r="C192" s="78" t="s">
+      <c r="H192" s="11"/>
+    </row>
+    <row r="193" spans="1:8">
+      <c r="A193" s="125">
+        <v>45</v>
+      </c>
+      <c r="B193" s="144"/>
+      <c r="C193" s="78" t="s">
         <v>332</v>
       </c>
-      <c r="D192" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="E192" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="F192" s="78" t="s">
+      <c r="D193" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="E193" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="F193" s="78" t="s">
         <v>216</v>
       </c>
-      <c r="G192" s="78" t="s">
+      <c r="G193" s="78" t="s">
         <v>333</v>
       </c>
-      <c r="H192" s="11"/>
-    </row>
-    <row r="193" spans="1:8">
-      <c r="A193" s="118">
-        <v>45</v>
-      </c>
-      <c r="B193" s="137"/>
-      <c r="C193" s="78" t="s">
+      <c r="H193" s="11"/>
+    </row>
+    <row r="194" spans="1:8">
+      <c r="A194" s="125">
+        <v>46</v>
+      </c>
+      <c r="B194" s="144"/>
+      <c r="C194" s="78" t="s">
         <v>218</v>
       </c>
-      <c r="D193" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="E193" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="F193" s="78" t="s">
+      <c r="D194" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="E194" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="F194" s="78" t="s">
         <v>328</v>
       </c>
-      <c r="G193" s="78" t="s">
+      <c r="G194" s="78" t="s">
         <v>328</v>
       </c>
-      <c r="H193" s="11"/>
-    </row>
-    <row r="194" spans="1:8">
-      <c r="A194" s="118">
-        <v>46</v>
-      </c>
-      <c r="B194" s="137"/>
-      <c r="C194" s="78" t="s">
+      <c r="H194" s="11"/>
+    </row>
+    <row r="195" spans="1:8">
+      <c r="A195" s="125">
+        <v>47</v>
+      </c>
+      <c r="B195" s="144"/>
+      <c r="C195" s="78" t="s">
         <v>330</v>
       </c>
-      <c r="D194" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="E194" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="F194" s="78">
+      <c r="D195" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="E195" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="F195" s="78">
         <v>64</v>
       </c>
-      <c r="G194" s="78" t="s">
+      <c r="G195" s="78" t="s">
         <v>329</v>
       </c>
-      <c r="H194" s="11"/>
-    </row>
-    <row r="195" spans="1:8">
-      <c r="A195" s="118">
-        <v>47</v>
-      </c>
-      <c r="B195" s="137"/>
-      <c r="C195" s="104" t="s">
+      <c r="H195" s="11"/>
+    </row>
+    <row r="196" spans="1:8">
+      <c r="A196" s="125">
+        <v>48</v>
+      </c>
+      <c r="B196" s="144"/>
+      <c r="C196" s="104" t="s">
         <v>331</v>
       </c>
-      <c r="D195" s="105" t="s">
-        <v>169</v>
-      </c>
-      <c r="E195" s="105" t="s">
-        <v>169</v>
-      </c>
-      <c r="F195" s="104">
+      <c r="D196" s="105" t="s">
+        <v>169</v>
+      </c>
+      <c r="E196" s="105" t="s">
+        <v>169</v>
+      </c>
+      <c r="F196" s="104">
         <v>7.9</v>
       </c>
-      <c r="G195" s="104" t="s">
+      <c r="G196" s="104" t="s">
         <v>334</v>
       </c>
-      <c r="H195" s="11"/>
-    </row>
-    <row r="196" spans="1:8">
-      <c r="A196" s="118">
-        <v>48</v>
-      </c>
-      <c r="B196" s="137"/>
-      <c r="C196" s="104" t="s">
+      <c r="H196" s="11"/>
+    </row>
+    <row r="197" spans="1:8">
+      <c r="A197" s="125">
+        <v>49</v>
+      </c>
+      <c r="B197" s="144"/>
+      <c r="C197" s="104" t="s">
         <v>387</v>
-      </c>
-      <c r="D196" s="105" t="s">
-        <v>169</v>
-      </c>
-      <c r="E196" s="105"/>
-      <c r="F196" s="104">
-        <v>50</v>
-      </c>
-      <c r="G196" s="104" t="s">
-        <v>390</v>
-      </c>
-      <c r="H196" s="68" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="197" spans="1:8">
-      <c r="A197" s="118">
-        <v>49</v>
-      </c>
-      <c r="B197" s="137"/>
-      <c r="C197" s="104" t="s">
-        <v>388</v>
       </c>
       <c r="D197" s="105" t="s">
         <v>169</v>
@@ -9232,180 +9243,180 @@
         <v>390</v>
       </c>
       <c r="H197" s="68" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8">
+      <c r="A198" s="125">
+        <v>50</v>
+      </c>
+      <c r="B198" s="144"/>
+      <c r="C198" s="104" t="s">
+        <v>388</v>
+      </c>
+      <c r="D198" s="105" t="s">
+        <v>169</v>
+      </c>
+      <c r="E198" s="105"/>
+      <c r="F198" s="104">
+        <v>50</v>
+      </c>
+      <c r="G198" s="104" t="s">
+        <v>390</v>
+      </c>
+      <c r="H198" s="68" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="198" spans="1:8">
-      <c r="A198" s="118">
-        <v>50</v>
-      </c>
-      <c r="B198" s="137"/>
-      <c r="C198" s="78" t="s">
+    <row r="199" spans="1:8">
+      <c r="A199" s="125">
+        <v>51</v>
+      </c>
+      <c r="B199" s="144"/>
+      <c r="C199" s="78" t="s">
         <v>389</v>
       </c>
-      <c r="D198" s="105" t="s">
-        <v>169</v>
-      </c>
-      <c r="E198" s="105"/>
-      <c r="F198" s="21">
+      <c r="D199" s="105" t="s">
+        <v>169</v>
+      </c>
+      <c r="E199" s="105"/>
+      <c r="F199" s="21">
         <v>10</v>
       </c>
-      <c r="G198" s="78" t="s">
+      <c r="G199" s="78" t="s">
         <v>391</v>
       </c>
-      <c r="H198" s="68" t="s">
+      <c r="H199" s="68" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="199" spans="1:8">
-      <c r="A199" s="118">
-        <v>51</v>
-      </c>
-      <c r="B199" s="129" t="s">
+    <row r="200" spans="1:8">
+      <c r="A200" s="125">
+        <v>52</v>
+      </c>
+      <c r="B200" s="162" t="s">
         <v>10</v>
       </c>
-      <c r="C199" s="21" t="s">
+      <c r="C200" s="21" t="s">
         <v>219</v>
       </c>
-      <c r="D199" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E199" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F199" s="21" t="s">
+      <c r="D200" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E200" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F200" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="G199" s="21" t="s">
+      <c r="G200" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="H199" s="11" t="s">
+      <c r="H200" s="11" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="200" spans="1:8">
-      <c r="A200" s="118">
-        <v>52</v>
-      </c>
-      <c r="B200" s="130"/>
-      <c r="C200" s="80" t="s">
+    <row r="201" spans="1:8">
+      <c r="A201" s="125">
+        <v>53</v>
+      </c>
+      <c r="B201" s="164"/>
+      <c r="C201" s="80" t="s">
         <v>222</v>
       </c>
-      <c r="D200" s="80" t="s">
-        <v>169</v>
-      </c>
-      <c r="E200" s="80" t="s">
-        <v>169</v>
-      </c>
-      <c r="F200" s="80" t="s">
+      <c r="D201" s="80" t="s">
+        <v>169</v>
+      </c>
+      <c r="E201" s="80" t="s">
+        <v>169</v>
+      </c>
+      <c r="F201" s="80" t="s">
         <v>223</v>
       </c>
-      <c r="G200" s="80" t="s">
+      <c r="G201" s="80" t="s">
         <v>171</v>
       </c>
-      <c r="H200" s="24" t="s">
+      <c r="H201" s="24" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="201" spans="1:8">
-      <c r="A201" s="106">
-        <v>53</v>
-      </c>
-      <c r="B201" s="131"/>
-      <c r="C201" s="79" t="s">
+    <row r="202" spans="1:8">
+      <c r="A202" s="106">
+        <v>54</v>
+      </c>
+      <c r="B202" s="163"/>
+      <c r="C202" s="79" t="s">
         <v>335</v>
       </c>
-      <c r="D201" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="E201" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="F201" s="79" t="s">
+      <c r="D202" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="E202" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="F202" s="79" t="s">
         <v>336</v>
       </c>
-      <c r="G201" s="20" t="s">
+      <c r="G202" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="H201" s="22" t="s">
+      <c r="H202" s="22" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="202" spans="1:8">
-      <c r="A202" s="16">
-        <v>54</v>
-      </c>
-      <c r="B202" s="132" t="s">
+    <row r="203" spans="1:8">
+      <c r="A203" s="16">
+        <v>55</v>
+      </c>
+      <c r="B203" s="165" t="s">
         <v>156</v>
       </c>
-      <c r="C202" s="63" t="s">
+      <c r="C203" s="63" t="s">
         <v>224</v>
       </c>
-      <c r="D202" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="E202" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="F202" s="17" t="s">
+      <c r="D203" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="E203" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="F203" s="17" t="s">
         <v>225</v>
       </c>
-      <c r="G202" s="63" t="s">
+      <c r="G203" s="63" t="s">
         <v>226</v>
       </c>
-      <c r="H202" s="10"/>
-    </row>
-    <row r="203" spans="1:8">
-      <c r="A203" s="119">
-        <v>55</v>
-      </c>
-      <c r="B203" s="133"/>
-      <c r="C203" s="120" t="s">
+      <c r="H203" s="10"/>
+    </row>
+    <row r="204" spans="1:8">
+      <c r="A204" s="118">
+        <v>56</v>
+      </c>
+      <c r="B204" s="166"/>
+      <c r="C204" s="119" t="s">
         <v>401</v>
       </c>
-      <c r="D203" s="115" t="s">
-        <v>169</v>
-      </c>
-      <c r="E203" s="115"/>
-      <c r="F203" s="115" t="s">
+      <c r="D204" s="115" t="s">
+        <v>169</v>
+      </c>
+      <c r="E204" s="115"/>
+      <c r="F204" s="115" t="s">
         <v>232</v>
       </c>
-      <c r="G203" s="113" t="s">
+      <c r="G204" s="113" t="s">
         <v>402</v>
       </c>
-      <c r="H203" s="40" t="s">
+      <c r="H204" s="40" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="204" spans="1:8">
-      <c r="A204" s="119">
-        <v>56</v>
-      </c>
-      <c r="B204" s="134"/>
-      <c r="C204" s="62" t="s">
+    <row r="205" spans="1:8">
+      <c r="A205" s="118">
+        <v>57</v>
+      </c>
+      <c r="B205" s="167"/>
+      <c r="C205" s="62" t="s">
         <v>227</v>
-      </c>
-      <c r="D204" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E204" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="F204" s="21" t="s">
-        <v>228</v>
-      </c>
-      <c r="G204" s="64" t="s">
-        <v>229</v>
-      </c>
-      <c r="H204" s="11"/>
-    </row>
-    <row r="205" spans="1:8">
-      <c r="A205" s="119">
-        <v>57</v>
-      </c>
-      <c r="B205" s="135"/>
-      <c r="C205" s="64" t="s">
-        <v>230</v>
       </c>
       <c r="D205" s="21" t="s">
         <v>169</v>
@@ -9416,454 +9427,471 @@
       <c r="F205" s="21" t="s">
         <v>228</v>
       </c>
-      <c r="G205" s="20" t="s">
+      <c r="G205" s="64" t="s">
         <v>229</v>
       </c>
-      <c r="H205" s="22"/>
+      <c r="H205" s="11"/>
     </row>
     <row r="206" spans="1:8">
-      <c r="A206" s="119">
+      <c r="A206" s="118">
         <v>58</v>
       </c>
-      <c r="B206" s="135"/>
+      <c r="B206" s="168"/>
       <c r="C206" s="64" t="s">
+        <v>230</v>
+      </c>
+      <c r="D206" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E206" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F206" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="G206" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="H206" s="22"/>
+    </row>
+    <row r="207" spans="1:8">
+      <c r="A207" s="118">
+        <v>59</v>
+      </c>
+      <c r="B207" s="168"/>
+      <c r="C207" s="64" t="s">
         <v>231</v>
       </c>
-      <c r="D206" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="E206" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="F206" s="23" t="s">
+      <c r="D207" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="E207" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="F207" s="23" t="s">
         <v>232</v>
       </c>
-      <c r="G206" s="64" t="s">
+      <c r="G207" s="64" t="s">
         <v>233</v>
       </c>
-      <c r="H206" s="24"/>
-    </row>
-    <row r="207" spans="1:8">
-      <c r="A207" s="119">
-        <v>59</v>
-      </c>
-      <c r="B207" s="135"/>
-      <c r="C207" s="70" t="s">
+      <c r="H207" s="24"/>
+    </row>
+    <row r="208" spans="1:8">
+      <c r="A208" s="118">
+        <v>60</v>
+      </c>
+      <c r="B208" s="168"/>
+      <c r="C208" s="70" t="s">
         <v>234</v>
       </c>
-      <c r="D207" s="71" t="s">
-        <v>169</v>
-      </c>
-      <c r="E207" s="71" t="s">
-        <v>169</v>
-      </c>
-      <c r="F207" s="71"/>
-      <c r="G207" s="72" t="s">
+      <c r="D208" s="71" t="s">
+        <v>169</v>
+      </c>
+      <c r="E208" s="71" t="s">
+        <v>169</v>
+      </c>
+      <c r="F208" s="71"/>
+      <c r="G208" s="72" t="s">
         <v>316</v>
       </c>
-      <c r="H207" s="24"/>
-    </row>
-    <row r="208" spans="1:8">
-      <c r="A208" s="119">
-        <v>60</v>
-      </c>
-      <c r="B208" s="135"/>
-      <c r="C208" s="70" t="s">
+      <c r="H208" s="24"/>
+    </row>
+    <row r="209" spans="1:8">
+      <c r="A209" s="118">
+        <v>61</v>
+      </c>
+      <c r="B209" s="168"/>
+      <c r="C209" s="70" t="s">
         <v>310</v>
       </c>
-      <c r="D208" s="71" t="s">
-        <v>169</v>
-      </c>
-      <c r="E208" s="71"/>
-      <c r="F208" s="71" t="s">
+      <c r="D209" s="71" t="s">
+        <v>169</v>
+      </c>
+      <c r="E209" s="71"/>
+      <c r="F209" s="71" t="s">
         <v>311</v>
       </c>
-      <c r="G208" s="70" t="s">
+      <c r="G209" s="70" t="s">
         <v>312</v>
       </c>
-      <c r="H208" s="24" t="s">
+      <c r="H209" s="24" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="209" spans="1:8">
-      <c r="A209" s="168">
-        <v>61</v>
-      </c>
-      <c r="B209" s="135"/>
-      <c r="C209" s="123" t="s">
+    <row r="210" spans="1:8">
+      <c r="A210" s="118">
+        <v>62</v>
+      </c>
+      <c r="B210" s="168"/>
+      <c r="C210" s="122" t="s">
         <v>314</v>
       </c>
-      <c r="D209" s="124" t="s">
-        <v>169</v>
-      </c>
-      <c r="E209" s="124"/>
-      <c r="F209" s="124" t="s">
+      <c r="D210" s="123" t="s">
+        <v>169</v>
+      </c>
+      <c r="E210" s="123"/>
+      <c r="F210" s="123" t="s">
         <v>228</v>
       </c>
-      <c r="G209" s="123" t="s">
+      <c r="G210" s="122" t="s">
         <v>229</v>
       </c>
-      <c r="H209" s="24" t="s">
+      <c r="H210" s="24" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="210" spans="1:8">
-      <c r="A210" s="25">
-        <v>62</v>
-      </c>
-      <c r="B210" s="136"/>
-      <c r="C210" s="26" t="s">
+    <row r="211" spans="1:8">
+      <c r="A211" s="25">
+        <v>63</v>
+      </c>
+      <c r="B211" s="152"/>
+      <c r="C211" s="26" t="s">
         <v>408</v>
       </c>
-      <c r="D210" s="26" t="s">
-        <v>169</v>
-      </c>
-      <c r="E210" s="26" t="s">
-        <v>169</v>
-      </c>
-      <c r="F210" s="26" t="s">
+      <c r="D211" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="E211" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="F211" s="26" t="s">
         <v>228</v>
       </c>
-      <c r="G210" s="26" t="s">
+      <c r="G211" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="H210" s="27"/>
-    </row>
-    <row r="211" spans="1:8">
-      <c r="A211" s="1" t="s">
+      <c r="H211" s="27"/>
+    </row>
+    <row r="212" spans="1:8">
+      <c r="A212" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B211" s="1" t="s">
+      <c r="B212" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="212" spans="1:8">
-      <c r="B212" s="28" t="s">
+    <row r="213" spans="1:8">
+      <c r="B213" s="28" t="s">
         <v>237</v>
-      </c>
-    </row>
-    <row r="213" spans="1:8">
-      <c r="B213" s="85" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="214" spans="1:8">
       <c r="B214" s="85" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8">
+      <c r="B215" s="85" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="215" spans="1:8">
-      <c r="B215" s="95" t="s">
+    <row r="216" spans="1:8">
+      <c r="B216" s="95" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="216" spans="1:8">
-      <c r="B216" s="85" t="s">
+    <row r="217" spans="1:8">
+      <c r="B217" s="85" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="226" spans="1:7">
-      <c r="A226" s="1" t="s">
+    <row r="227" spans="1:7">
+      <c r="A227" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B226" s="1" t="s">
+      <c r="B227" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="227" spans="1:7">
-      <c r="A227" s="4" t="s">
+    <row r="228" spans="1:7">
+      <c r="A228" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="B227" s="29" t="s">
+      <c r="B228" s="29" t="s">
         <v>241</v>
       </c>
-      <c r="C227" s="164" t="s">
+      <c r="C228" s="134" t="s">
         <v>242</v>
       </c>
-      <c r="D227" s="164"/>
-      <c r="E227" s="164"/>
-      <c r="F227" s="30" t="s">
+      <c r="D228" s="134"/>
+      <c r="E228" s="134"/>
+      <c r="F228" s="30" t="s">
         <v>243</v>
       </c>
-      <c r="G227" s="31" t="s">
+      <c r="G228" s="31" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="228" spans="1:7">
-      <c r="A228" s="146" t="s">
+    <row r="229" spans="1:7">
+      <c r="A229" s="160" t="s">
         <v>245</v>
       </c>
-      <c r="B228" s="137" t="s">
+      <c r="B229" s="144" t="s">
         <v>246</v>
       </c>
-      <c r="C228" s="165" t="s">
+      <c r="C229" s="135" t="s">
         <v>247</v>
       </c>
-      <c r="D228" s="166"/>
-      <c r="E228" s="166"/>
-      <c r="F228" s="21" t="s">
+      <c r="D229" s="136"/>
+      <c r="E229" s="136"/>
+      <c r="F229" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="G228" s="32" t="s">
+      <c r="G229" s="32" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="229" spans="1:7">
-      <c r="A229" s="146"/>
-      <c r="B229" s="138"/>
-      <c r="C229" s="156" t="s">
+    <row r="230" spans="1:7">
+      <c r="A230" s="160"/>
+      <c r="B230" s="169"/>
+      <c r="C230" s="137" t="s">
         <v>247</v>
       </c>
-      <c r="D229" s="167"/>
-      <c r="E229" s="167"/>
-      <c r="F229" s="20" t="s">
+      <c r="D230" s="138"/>
+      <c r="E230" s="138"/>
+      <c r="F230" s="20" t="s">
         <v>250</v>
       </c>
-      <c r="G229" s="33" t="s">
+      <c r="G230" s="33" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="230" spans="1:7">
-      <c r="A230" s="146"/>
-      <c r="B230" s="137" t="s">
+    <row r="231" spans="1:7">
+      <c r="A231" s="160"/>
+      <c r="B231" s="144" t="s">
         <v>251</v>
       </c>
-      <c r="C230" s="160" t="s">
+      <c r="C231" s="139" t="s">
         <v>252</v>
       </c>
-      <c r="D230" s="160"/>
-      <c r="E230" s="160"/>
-      <c r="F230" s="21" t="s">
+      <c r="D231" s="139"/>
+      <c r="E231" s="139"/>
+      <c r="F231" s="21" t="s">
         <v>248</v>
-      </c>
-      <c r="G230" s="32" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="231" spans="1:7">
-      <c r="A231" s="146"/>
-      <c r="B231" s="137"/>
-      <c r="C231" s="156" t="s">
-        <v>252</v>
-      </c>
-      <c r="D231" s="156"/>
-      <c r="E231" s="156"/>
-      <c r="F231" s="21" t="s">
-        <v>250</v>
       </c>
       <c r="G231" s="32" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="232" spans="1:7">
-      <c r="A232" s="146"/>
-      <c r="B232" s="138" t="s">
-        <v>253</v>
-      </c>
-      <c r="C232" s="157" t="s">
-        <v>247</v>
-      </c>
-      <c r="D232" s="158"/>
-      <c r="E232" s="159"/>
+      <c r="A232" s="160"/>
+      <c r="B232" s="144"/>
+      <c r="C232" s="137" t="s">
+        <v>252</v>
+      </c>
+      <c r="D232" s="137"/>
+      <c r="E232" s="137"/>
       <c r="F232" s="21" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="G232" s="32" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="233" spans="1:7">
-      <c r="A233" s="146"/>
-      <c r="B233" s="139"/>
-      <c r="C233" s="157" t="s">
+      <c r="A233" s="160"/>
+      <c r="B233" s="169" t="s">
+        <v>253</v>
+      </c>
+      <c r="C233" s="140" t="s">
         <v>247</v>
       </c>
-      <c r="D233" s="158"/>
-      <c r="E233" s="159"/>
+      <c r="D233" s="141"/>
+      <c r="E233" s="142"/>
       <c r="F233" s="21" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G233" s="32" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="234" spans="1:7">
-      <c r="A234" s="146"/>
-      <c r="B234" s="137" t="s">
-        <v>254</v>
-      </c>
-      <c r="C234" s="160" t="s">
-        <v>255</v>
-      </c>
-      <c r="D234" s="160"/>
-      <c r="E234" s="160"/>
+      <c r="A234" s="160"/>
+      <c r="B234" s="148"/>
+      <c r="C234" s="140" t="s">
+        <v>247</v>
+      </c>
+      <c r="D234" s="141"/>
+      <c r="E234" s="142"/>
       <c r="F234" s="21" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="G234" s="32" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="235" spans="1:7">
-      <c r="A235" s="146"/>
-      <c r="B235" s="137"/>
-      <c r="C235" s="160" t="s">
+      <c r="A235" s="160"/>
+      <c r="B235" s="144" t="s">
+        <v>254</v>
+      </c>
+      <c r="C235" s="139" t="s">
         <v>255</v>
       </c>
-      <c r="D235" s="160"/>
-      <c r="E235" s="160"/>
+      <c r="D235" s="139"/>
+      <c r="E235" s="139"/>
       <c r="F235" s="21" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G235" s="32" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="236" spans="1:7">
-      <c r="A236" s="146" t="s">
-        <v>256</v>
-      </c>
-      <c r="B236" s="137" t="s">
-        <v>257</v>
-      </c>
-      <c r="C236" s="140" t="s">
-        <v>258</v>
-      </c>
-      <c r="D236" s="137"/>
-      <c r="E236" s="137"/>
+      <c r="A236" s="160"/>
+      <c r="B236" s="144"/>
+      <c r="C236" s="139" t="s">
+        <v>255</v>
+      </c>
+      <c r="D236" s="139"/>
+      <c r="E236" s="139"/>
       <c r="F236" s="21" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="G236" s="32" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="237" spans="1:7">
-      <c r="A237" s="146"/>
-      <c r="B237" s="137"/>
-      <c r="C237" s="137" t="s">
+      <c r="A237" s="160" t="s">
+        <v>256</v>
+      </c>
+      <c r="B237" s="144" t="s">
+        <v>257</v>
+      </c>
+      <c r="C237" s="143" t="s">
+        <v>258</v>
+      </c>
+      <c r="D237" s="144"/>
+      <c r="E237" s="144"/>
+      <c r="F237" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="G237" s="32" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7">
+      <c r="A238" s="160"/>
+      <c r="B238" s="144"/>
+      <c r="C238" s="144" t="s">
         <v>259</v>
       </c>
-      <c r="D237" s="137"/>
-      <c r="E237" s="137"/>
-      <c r="F237" s="21" t="s">
+      <c r="D238" s="144"/>
+      <c r="E238" s="144"/>
+      <c r="F238" s="21" t="s">
         <v>250</v>
       </c>
-      <c r="G237" s="32" t="s">
+      <c r="G238" s="32" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="238" spans="1:7">
-      <c r="A238" s="146"/>
-      <c r="B238" s="137" t="s">
+    <row r="239" spans="1:7">
+      <c r="A239" s="160"/>
+      <c r="B239" s="144" t="s">
         <v>261</v>
       </c>
-      <c r="C238" s="137" t="s">
+      <c r="C239" s="144" t="s">
         <v>262</v>
       </c>
-      <c r="D238" s="137"/>
-      <c r="E238" s="137"/>
-      <c r="F238" s="21" t="s">
+      <c r="D239" s="144"/>
+      <c r="E239" s="144"/>
+      <c r="F239" s="21" t="s">
         <v>248</v>
-      </c>
-      <c r="G238" s="32" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="239" spans="1:7">
-      <c r="A239" s="146"/>
-      <c r="B239" s="137"/>
-      <c r="C239" s="137" t="s">
-        <v>263</v>
-      </c>
-      <c r="D239" s="137"/>
-      <c r="E239" s="137"/>
-      <c r="F239" s="21" t="s">
-        <v>250</v>
       </c>
       <c r="G239" s="32" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="240" spans="1:7">
-      <c r="A240" s="146" t="s">
-        <v>264</v>
-      </c>
-      <c r="B240" s="137" t="s">
-        <v>265</v>
-      </c>
-      <c r="C240" s="140" t="s">
-        <v>266</v>
-      </c>
-      <c r="D240" s="137"/>
-      <c r="E240" s="137"/>
+      <c r="A240" s="160"/>
+      <c r="B240" s="144"/>
+      <c r="C240" s="144" t="s">
+        <v>263</v>
+      </c>
+      <c r="D240" s="144"/>
+      <c r="E240" s="144"/>
       <c r="F240" s="21" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="G240" s="32" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="241" spans="1:7">
-      <c r="A241" s="146"/>
-      <c r="B241" s="137"/>
-      <c r="C241" s="137" t="s">
-        <v>267</v>
-      </c>
-      <c r="D241" s="137"/>
-      <c r="E241" s="137"/>
+      <c r="A241" s="160" t="s">
+        <v>264</v>
+      </c>
+      <c r="B241" s="144" t="s">
+        <v>265</v>
+      </c>
+      <c r="C241" s="143" t="s">
+        <v>266</v>
+      </c>
+      <c r="D241" s="144"/>
+      <c r="E241" s="144"/>
       <c r="F241" s="21" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G241" s="32" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="242" spans="1:7">
-      <c r="A242" s="146"/>
-      <c r="B242" s="137" t="s">
-        <v>268</v>
-      </c>
-      <c r="C242" s="140" t="s">
-        <v>269</v>
-      </c>
-      <c r="D242" s="137"/>
-      <c r="E242" s="137"/>
+      <c r="A242" s="160"/>
+      <c r="B242" s="144"/>
+      <c r="C242" s="144" t="s">
+        <v>267</v>
+      </c>
+      <c r="D242" s="144"/>
+      <c r="E242" s="144"/>
       <c r="F242" s="21" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="G242" s="32" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="243" spans="1:7">
-      <c r="A243" s="147"/>
-      <c r="B243" s="148"/>
-      <c r="C243" s="148" t="s">
+      <c r="A243" s="160"/>
+      <c r="B243" s="144" t="s">
+        <v>268</v>
+      </c>
+      <c r="C243" s="143" t="s">
+        <v>269</v>
+      </c>
+      <c r="D243" s="144"/>
+      <c r="E243" s="144"/>
+      <c r="F243" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="G243" s="32" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7">
+      <c r="A244" s="161"/>
+      <c r="B244" s="145"/>
+      <c r="C244" s="145" t="s">
         <v>270</v>
       </c>
-      <c r="D243" s="148"/>
-      <c r="E243" s="148"/>
-      <c r="F243" s="26" t="s">
+      <c r="D244" s="145"/>
+      <c r="E244" s="145"/>
+      <c r="F244" s="26" t="s">
         <v>250</v>
       </c>
-      <c r="G243" s="34" t="s">
+      <c r="G244" s="34" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="244" spans="1:7">
-      <c r="A244" s="1" t="s">
+    <row r="245" spans="1:7">
+      <c r="A245" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="C244" s="28"/>
-      <c r="D244" s="28"/>
-      <c r="E244" s="28"/>
-      <c r="F244" s="28"/>
-    </row>
-    <row r="245" spans="1:7">
       <c r="C245" s="28"/>
       <c r="D245" s="28"/>
       <c r="E245" s="28"/>
+      <c r="F245" s="28"/>
     </row>
     <row r="246" spans="1:7">
       <c r="C246" s="28"/>
@@ -9871,307 +9899,295 @@
       <c r="E246" s="28"/>
     </row>
     <row r="247" spans="1:7">
-      <c r="A247" s="1" t="s">
-        <v>272</v>
-      </c>
       <c r="C247" s="28"/>
       <c r="D247" s="28"/>
       <c r="E247" s="28"/>
     </row>
     <row r="248" spans="1:7">
-      <c r="A248" s="35" t="s">
+      <c r="A248" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C248" s="28"/>
+      <c r="D248" s="28"/>
+      <c r="E248" s="28"/>
+    </row>
+    <row r="249" spans="1:7">
+      <c r="A249" s="35" t="s">
         <v>273</v>
       </c>
-      <c r="B248" s="154" t="s">
+      <c r="B249" s="146" t="s">
         <v>274</v>
       </c>
-      <c r="C248" s="154"/>
-      <c r="D248" s="154"/>
-      <c r="E248" s="154"/>
-      <c r="F248" s="36" t="s">
+      <c r="C249" s="146"/>
+      <c r="D249" s="146"/>
+      <c r="E249" s="146"/>
+      <c r="F249" s="36" t="s">
         <v>275</v>
       </c>
-      <c r="G248" s="37" t="s">
+      <c r="G249" s="37" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="249" spans="1:7" ht="93" customHeight="1">
-      <c r="A249" s="38" t="s">
+    <row r="250" spans="1:7" ht="93" customHeight="1">
+      <c r="A250" s="38" t="s">
         <v>277</v>
       </c>
-      <c r="B249" s="155" t="s">
+      <c r="B250" s="147" t="s">
         <v>278</v>
       </c>
-      <c r="C249" s="139"/>
-      <c r="D249" s="139"/>
-      <c r="E249" s="139"/>
-      <c r="F249" s="39" t="s">
+      <c r="C250" s="148"/>
+      <c r="D250" s="148"/>
+      <c r="E250" s="148"/>
+      <c r="F250" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="G249" s="40" t="s">
+      <c r="G250" s="40" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="250" spans="1:7" ht="57" customHeight="1">
-      <c r="A250" s="8" t="s">
+    <row r="251" spans="1:7" ht="57" customHeight="1">
+      <c r="A251" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="B250" s="150" t="s">
+      <c r="B251" s="149" t="s">
         <v>280</v>
       </c>
-      <c r="C250" s="151"/>
-      <c r="D250" s="151"/>
-      <c r="E250" s="152"/>
-      <c r="F250" s="9" t="s">
+      <c r="C251" s="150"/>
+      <c r="D251" s="150"/>
+      <c r="E251" s="151"/>
+      <c r="F251" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="G250" s="11" t="s">
+      <c r="G251" s="11" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="251" spans="1:7" ht="57" customHeight="1">
-      <c r="A251" s="12" t="s">
+    <row r="252" spans="1:7" ht="57" customHeight="1">
+      <c r="A252" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="B251" s="150" t="s">
+      <c r="B252" s="149" t="s">
         <v>282</v>
       </c>
-      <c r="C251" s="151"/>
-      <c r="D251" s="151"/>
-      <c r="E251" s="152"/>
-      <c r="F251" s="13" t="s">
+      <c r="C252" s="150"/>
+      <c r="D252" s="150"/>
+      <c r="E252" s="151"/>
+      <c r="F252" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="G251" s="22" t="s">
+      <c r="G252" s="22" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="252" spans="1:7" ht="69" customHeight="1">
-      <c r="A252" s="14" t="s">
+    <row r="253" spans="1:7" ht="69" customHeight="1">
+      <c r="A253" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="B252" s="136" t="s">
+      <c r="B253" s="152" t="s">
         <v>284</v>
       </c>
-      <c r="C252" s="148"/>
-      <c r="D252" s="148"/>
-      <c r="E252" s="148"/>
-      <c r="F252" s="15" t="s">
+      <c r="C253" s="145"/>
+      <c r="D253" s="145"/>
+      <c r="E253" s="145"/>
+      <c r="F253" s="15" t="s">
         <v>249</v>
       </c>
-      <c r="G252" s="27" t="s">
+      <c r="G253" s="27" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="253" spans="1:7">
-      <c r="C253" s="41"/>
-    </row>
-    <row r="255" spans="1:7">
-      <c r="A255" s="1" t="s">
+    <row r="254" spans="1:7">
+      <c r="C254" s="41"/>
+    </row>
+    <row r="256" spans="1:7">
+      <c r="A256" s="1" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="256" spans="1:7">
-      <c r="A256" s="4" t="s">
+    <row r="257" spans="1:7">
+      <c r="A257" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="B256" s="29" t="s">
+      <c r="B257" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="C256" s="42" t="s">
+      <c r="C257" s="42" t="s">
         <v>287</v>
       </c>
-      <c r="D256" s="43" t="s">
+      <c r="D257" s="43" t="s">
         <v>274</v>
       </c>
-      <c r="E256" s="43"/>
-      <c r="F256" s="44"/>
-      <c r="G256" s="31" t="s">
+      <c r="E257" s="43"/>
+      <c r="F257" s="44"/>
+      <c r="G257" s="31" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="257" spans="1:7">
-      <c r="A257" s="45">
+    <row r="258" spans="1:7">
+      <c r="A258" s="45">
         <v>42682</v>
       </c>
-      <c r="B257" s="46">
+      <c r="B258" s="46">
         <v>1.04</v>
       </c>
-      <c r="C257" s="17" t="s">
+      <c r="C258" s="17" t="s">
         <v>289</v>
       </c>
-      <c r="D257" s="153" t="s">
+      <c r="D258" s="153" t="s">
         <v>290</v>
       </c>
-      <c r="E257" s="153"/>
-      <c r="F257" s="153"/>
-      <c r="G257" s="47"/>
-    </row>
-    <row r="258" spans="1:7">
-      <c r="A258" s="48">
-        <v>42692</v>
-      </c>
-      <c r="B258" s="49">
-        <v>1.05</v>
-      </c>
-      <c r="C258" s="21" t="s">
-        <v>289</v>
-      </c>
-      <c r="D258" s="149" t="s">
-        <v>291</v>
-      </c>
-      <c r="E258" s="149"/>
-      <c r="F258" s="149"/>
-      <c r="G258" s="32"/>
+      <c r="E258" s="153"/>
+      <c r="F258" s="153"/>
+      <c r="G258" s="47"/>
     </row>
     <row r="259" spans="1:7">
       <c r="A259" s="48">
-        <v>42955</v>
+        <v>42692</v>
       </c>
       <c r="B259" s="49">
-        <v>1.06</v>
+        <v>1.05</v>
       </c>
       <c r="C259" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="D259" s="149" t="s">
-        <v>292</v>
-      </c>
-      <c r="E259" s="149"/>
-      <c r="F259" s="149"/>
+      <c r="D259" s="154" t="s">
+        <v>291</v>
+      </c>
+      <c r="E259" s="154"/>
+      <c r="F259" s="154"/>
       <c r="G259" s="32"/>
     </row>
     <row r="260" spans="1:7">
       <c r="A260" s="48">
-        <v>42991</v>
+        <v>42955</v>
       </c>
       <c r="B260" s="49">
-        <v>1.07</v>
+        <v>1.06</v>
       </c>
       <c r="C260" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="D260" s="149" t="s">
-        <v>293</v>
-      </c>
-      <c r="E260" s="149"/>
-      <c r="F260" s="149"/>
+      <c r="D260" s="154" t="s">
+        <v>292</v>
+      </c>
+      <c r="E260" s="154"/>
+      <c r="F260" s="154"/>
       <c r="G260" s="32"/>
     </row>
     <row r="261" spans="1:7">
       <c r="A261" s="48">
-        <v>43026</v>
+        <v>42991</v>
       </c>
       <c r="B261" s="49">
-        <v>1.08</v>
+        <v>1.07</v>
       </c>
       <c r="C261" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="D261" s="149" t="s">
-        <v>294</v>
-      </c>
-      <c r="E261" s="149"/>
-      <c r="F261" s="149"/>
+      <c r="D261" s="154" t="s">
+        <v>293</v>
+      </c>
+      <c r="E261" s="154"/>
+      <c r="F261" s="154"/>
       <c r="G261" s="32"/>
     </row>
     <row r="262" spans="1:7">
       <c r="A262" s="48">
-        <v>43069</v>
+        <v>43026</v>
       </c>
       <c r="B262" s="49">
-        <v>1.0900000000000001</v>
+        <v>1.08</v>
       </c>
       <c r="C262" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="D262" s="149" t="s">
+      <c r="D262" s="154" t="s">
+        <v>294</v>
+      </c>
+      <c r="E262" s="154"/>
+      <c r="F262" s="154"/>
+      <c r="G262" s="32"/>
+    </row>
+    <row r="263" spans="1:7">
+      <c r="A263" s="48">
+        <v>43069</v>
+      </c>
+      <c r="B263" s="49">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="C263" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="D263" s="154" t="s">
         <v>295</v>
       </c>
-      <c r="E262" s="149"/>
-      <c r="F262" s="149"/>
-      <c r="G262" s="32"/>
-    </row>
-    <row r="263" spans="1:7">
-      <c r="A263" s="50">
-        <v>43248</v>
-      </c>
-      <c r="B263" s="51">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C263" s="20" t="s">
-        <v>289</v>
-      </c>
-      <c r="D263" s="141" t="s">
-        <v>296</v>
-      </c>
-      <c r="E263" s="142"/>
-      <c r="F263" s="143"/>
-      <c r="G263" s="33"/>
+      <c r="E263" s="154"/>
+      <c r="F263" s="154"/>
+      <c r="G263" s="32"/>
     </row>
     <row r="264" spans="1:7">
       <c r="A264" s="50">
-        <v>43339</v>
+        <v>43248</v>
       </c>
       <c r="B264" s="51">
-        <v>1.1100000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C264" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="D264" s="141" t="s">
-        <v>297</v>
-      </c>
-      <c r="E264" s="142"/>
-      <c r="F264" s="143"/>
+      <c r="D264" s="155" t="s">
+        <v>296</v>
+      </c>
+      <c r="E264" s="156"/>
+      <c r="F264" s="157"/>
       <c r="G264" s="33"/>
     </row>
     <row r="265" spans="1:7">
       <c r="A265" s="50">
-        <v>43542</v>
+        <v>43339</v>
       </c>
       <c r="B265" s="51">
-        <v>1.1200000000000001</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="C265" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="D265" s="141" t="s">
-        <v>298</v>
-      </c>
-      <c r="E265" s="142"/>
-      <c r="F265" s="143"/>
+      <c r="D265" s="155" t="s">
+        <v>297</v>
+      </c>
+      <c r="E265" s="156"/>
+      <c r="F265" s="157"/>
       <c r="G265" s="33"/>
     </row>
     <row r="266" spans="1:7">
       <c r="A266" s="50">
-        <v>43599</v>
+        <v>43542</v>
       </c>
       <c r="B266" s="51">
-        <v>1.1299999999999999</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="C266" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="D266" s="52" t="s">
-        <v>299</v>
-      </c>
-      <c r="E266" s="53"/>
-      <c r="F266" s="54"/>
+      <c r="D266" s="155" t="s">
+        <v>298</v>
+      </c>
+      <c r="E266" s="156"/>
+      <c r="F266" s="157"/>
       <c r="G266" s="33"/>
     </row>
     <row r="267" spans="1:7">
       <c r="A267" s="50">
-        <v>43643</v>
+        <v>43599</v>
       </c>
       <c r="B267" s="51">
-        <v>1.1399999999999999</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="C267" s="20" t="s">
         <v>289</v>
       </c>
       <c r="D267" s="52" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E267" s="53"/>
       <c r="F267" s="54"/>
@@ -10179,16 +10195,16 @@
     </row>
     <row r="268" spans="1:7">
       <c r="A268" s="50">
-        <v>43894</v>
+        <v>43643</v>
       </c>
       <c r="B268" s="51">
-        <v>1.1499999999999999</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="C268" s="20" t="s">
         <v>289</v>
       </c>
       <c r="D268" s="52" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E268" s="53"/>
       <c r="F268" s="54"/>
@@ -10196,16 +10212,16 @@
     </row>
     <row r="269" spans="1:7">
       <c r="A269" s="50">
-        <v>44017</v>
+        <v>43894</v>
       </c>
       <c r="B269" s="51">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="C269" s="71" t="s">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C269" s="20" t="s">
         <v>289</v>
       </c>
       <c r="D269" s="52" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E269" s="53"/>
       <c r="F269" s="54"/>
@@ -10213,16 +10229,16 @@
     </row>
     <row r="270" spans="1:7">
       <c r="A270" s="50">
-        <v>44118</v>
+        <v>44017</v>
       </c>
       <c r="B270" s="51">
-        <v>1.17</v>
-      </c>
-      <c r="C270" s="73" t="s">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="C270" s="71" t="s">
         <v>289</v>
       </c>
       <c r="D270" s="52" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="E270" s="53"/>
       <c r="F270" s="54"/>
@@ -10230,16 +10246,16 @@
     </row>
     <row r="271" spans="1:7">
       <c r="A271" s="50">
-        <v>44209</v>
+        <v>44118</v>
       </c>
       <c r="B271" s="51">
-        <v>1.18</v>
-      </c>
-      <c r="C271" s="77" t="s">
+        <v>1.17</v>
+      </c>
+      <c r="C271" s="73" t="s">
         <v>289</v>
       </c>
-      <c r="D271" s="86" t="s">
-        <v>320</v>
+      <c r="D271" s="52" t="s">
+        <v>317</v>
       </c>
       <c r="E271" s="53"/>
       <c r="F271" s="54"/>
@@ -10247,16 +10263,16 @@
     </row>
     <row r="272" spans="1:7">
       <c r="A272" s="50">
-        <v>44258</v>
+        <v>44209</v>
       </c>
       <c r="B272" s="51">
-        <v>1.19</v>
-      </c>
-      <c r="C272" s="80" t="s">
+        <v>1.18</v>
+      </c>
+      <c r="C272" s="77" t="s">
         <v>289</v>
       </c>
-      <c r="D272" s="52" t="s">
-        <v>326</v>
+      <c r="D272" s="86" t="s">
+        <v>320</v>
       </c>
       <c r="E272" s="53"/>
       <c r="F272" s="54"/>
@@ -10264,16 +10280,16 @@
     </row>
     <row r="273" spans="1:7">
       <c r="A273" s="50">
-        <v>44357</v>
+        <v>44258</v>
       </c>
       <c r="B273" s="51">
-        <v>1.2</v>
-      </c>
-      <c r="C273" s="82" t="s">
+        <v>1.19</v>
+      </c>
+      <c r="C273" s="80" t="s">
         <v>289</v>
       </c>
       <c r="D273" s="52" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="E273" s="53"/>
       <c r="F273" s="54"/>
@@ -10281,16 +10297,16 @@
     </row>
     <row r="274" spans="1:7">
       <c r="A274" s="50">
-        <v>44487</v>
+        <v>44357</v>
       </c>
       <c r="B274" s="51">
-        <v>1.21</v>
-      </c>
-      <c r="C274" s="88" t="s">
+        <v>1.2</v>
+      </c>
+      <c r="C274" s="82" t="s">
         <v>289</v>
       </c>
       <c r="D274" s="52" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E274" s="53"/>
       <c r="F274" s="54"/>
@@ -10298,16 +10314,16 @@
     </row>
     <row r="275" spans="1:7">
       <c r="A275" s="50">
-        <v>44518</v>
+        <v>44487</v>
       </c>
       <c r="B275" s="51">
-        <v>1.22</v>
-      </c>
-      <c r="C275" s="107" t="s">
+        <v>1.21</v>
+      </c>
+      <c r="C275" s="88" t="s">
         <v>289</v>
       </c>
       <c r="D275" s="52" t="s">
-        <v>361</v>
+        <v>340</v>
       </c>
       <c r="E275" s="53"/>
       <c r="F275" s="54"/>
@@ -10315,16 +10331,16 @@
     </row>
     <row r="276" spans="1:7">
       <c r="A276" s="50">
-        <v>44530</v>
+        <v>44518</v>
       </c>
       <c r="B276" s="51">
-        <v>1.23</v>
-      </c>
-      <c r="C276" s="110" t="s">
+        <v>1.22</v>
+      </c>
+      <c r="C276" s="107" t="s">
         <v>289</v>
       </c>
       <c r="D276" s="52" t="s">
-        <v>395</v>
+        <v>361</v>
       </c>
       <c r="E276" s="53"/>
       <c r="F276" s="54"/>
@@ -10332,16 +10348,16 @@
     </row>
     <row r="277" spans="1:7">
       <c r="A277" s="50">
-        <v>44559</v>
+        <v>44530</v>
       </c>
       <c r="B277" s="51">
-        <v>1.24</v>
-      </c>
-      <c r="C277" s="114" t="s">
+        <v>1.23</v>
+      </c>
+      <c r="C277" s="110" t="s">
         <v>289</v>
       </c>
       <c r="D277" s="52" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="E277" s="53"/>
       <c r="F277" s="54"/>
@@ -10349,40 +10365,57 @@
     </row>
     <row r="278" spans="1:7">
       <c r="A278" s="50">
-        <v>44755</v>
+        <v>44559</v>
       </c>
       <c r="B278" s="51">
-        <v>1.25</v>
-      </c>
-      <c r="C278" s="124" t="s">
+        <v>1.24</v>
+      </c>
+      <c r="C278" s="114" t="s">
         <v>289</v>
       </c>
       <c r="D278" s="52" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="E278" s="53"/>
       <c r="F278" s="54"/>
       <c r="G278" s="33"/>
     </row>
     <row r="279" spans="1:7">
-      <c r="A279" s="55">
+      <c r="A279" s="50">
+        <v>44755</v>
+      </c>
+      <c r="B279" s="51">
+        <v>1.25</v>
+      </c>
+      <c r="C279" s="123" t="s">
+        <v>289</v>
+      </c>
+      <c r="D279" s="52" t="s">
+        <v>404</v>
+      </c>
+      <c r="E279" s="53"/>
+      <c r="F279" s="54"/>
+      <c r="G279" s="33"/>
+    </row>
+    <row r="280" spans="1:7">
+      <c r="A280" s="55">
         <v>44881</v>
       </c>
-      <c r="B279" s="56">
+      <c r="B280" s="56">
         <v>1.26</v>
       </c>
-      <c r="C279" s="26" t="s">
+      <c r="C280" s="26" t="s">
         <v>289</v>
       </c>
-      <c r="D279" s="144" t="s">
+      <c r="D280" s="158" t="s">
         <v>409</v>
       </c>
-      <c r="E279" s="145"/>
-      <c r="F279" s="145"/>
-      <c r="G279" s="34"/>
+      <c r="E280" s="159"/>
+      <c r="F280" s="159"/>
+      <c r="G280" s="34"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="RKleJfTh3COi3AqYGGEAXXG/BsFKLGh0DoKeR9DrTzQ9sC/gEJm6Qq6PwFunSfvBkyT00OkAWa3rLDuhCZQN6A==" saltValue="jfo4474+J2OqjsbqZlpDoQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="P09gLXyZsqbqOLtV1gUANmS3s7Is4tkaKk2Gzdi+CKugZQMkEweB8COIgM6pJS+Tup2x549jLDbUn9S0eSNeqA==" saltValue="KXPVp+hGaHmf30gQz9LGKg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <customSheetViews>
     <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115" topLeftCell="A139">
       <selection activeCell="D163" sqref="D163"/>
@@ -10391,57 +10424,57 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="51">
-    <mergeCell ref="F111:N111"/>
-    <mergeCell ref="C227:E227"/>
-    <mergeCell ref="C228:E228"/>
-    <mergeCell ref="C229:E229"/>
-    <mergeCell ref="C230:E230"/>
-    <mergeCell ref="C231:E231"/>
+    <mergeCell ref="B200:B202"/>
+    <mergeCell ref="B203:B211"/>
+    <mergeCell ref="B229:B230"/>
+    <mergeCell ref="B231:B232"/>
+    <mergeCell ref="B233:B234"/>
+    <mergeCell ref="B149:B162"/>
+    <mergeCell ref="B163:B171"/>
+    <mergeCell ref="B172:B182"/>
+    <mergeCell ref="B183:B190"/>
+    <mergeCell ref="B191:B199"/>
+    <mergeCell ref="D265:F265"/>
+    <mergeCell ref="D266:F266"/>
+    <mergeCell ref="D280:F280"/>
+    <mergeCell ref="A229:A236"/>
+    <mergeCell ref="A237:A240"/>
+    <mergeCell ref="A241:A244"/>
+    <mergeCell ref="B235:B236"/>
+    <mergeCell ref="B237:B238"/>
+    <mergeCell ref="B239:B240"/>
+    <mergeCell ref="B241:B242"/>
+    <mergeCell ref="B243:B244"/>
+    <mergeCell ref="D260:F260"/>
+    <mergeCell ref="D261:F261"/>
+    <mergeCell ref="D262:F262"/>
+    <mergeCell ref="D263:F263"/>
+    <mergeCell ref="D264:F264"/>
+    <mergeCell ref="B251:E251"/>
+    <mergeCell ref="B252:E252"/>
+    <mergeCell ref="B253:E253"/>
+    <mergeCell ref="D258:F258"/>
+    <mergeCell ref="D259:F259"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C243:E243"/>
+    <mergeCell ref="C244:E244"/>
+    <mergeCell ref="B249:E249"/>
+    <mergeCell ref="B250:E250"/>
+    <mergeCell ref="C237:E237"/>
+    <mergeCell ref="C238:E238"/>
+    <mergeCell ref="C239:E239"/>
+    <mergeCell ref="C240:E240"/>
+    <mergeCell ref="C241:E241"/>
     <mergeCell ref="C232:E232"/>
     <mergeCell ref="C233:E233"/>
     <mergeCell ref="C234:E234"/>
     <mergeCell ref="C235:E235"/>
     <mergeCell ref="C236:E236"/>
-    <mergeCell ref="C237:E237"/>
-    <mergeCell ref="C238:E238"/>
-    <mergeCell ref="C239:E239"/>
-    <mergeCell ref="C240:E240"/>
-    <mergeCell ref="C241:E241"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C243:E243"/>
-    <mergeCell ref="B248:E248"/>
-    <mergeCell ref="B249:E249"/>
-    <mergeCell ref="B250:E250"/>
-    <mergeCell ref="B251:E251"/>
-    <mergeCell ref="B252:E252"/>
-    <mergeCell ref="D257:F257"/>
-    <mergeCell ref="D258:F258"/>
-    <mergeCell ref="D264:F264"/>
-    <mergeCell ref="D265:F265"/>
-    <mergeCell ref="D279:F279"/>
-    <mergeCell ref="A228:A235"/>
-    <mergeCell ref="A236:A239"/>
-    <mergeCell ref="A240:A243"/>
-    <mergeCell ref="B234:B235"/>
-    <mergeCell ref="B236:B237"/>
-    <mergeCell ref="B238:B239"/>
-    <mergeCell ref="B240:B241"/>
-    <mergeCell ref="B242:B243"/>
-    <mergeCell ref="D259:F259"/>
-    <mergeCell ref="D260:F260"/>
-    <mergeCell ref="D261:F261"/>
-    <mergeCell ref="D262:F262"/>
-    <mergeCell ref="D263:F263"/>
-    <mergeCell ref="B149:B162"/>
-    <mergeCell ref="B163:B170"/>
-    <mergeCell ref="B171:B181"/>
-    <mergeCell ref="B182:B189"/>
-    <mergeCell ref="B190:B198"/>
-    <mergeCell ref="B199:B201"/>
-    <mergeCell ref="B202:B210"/>
-    <mergeCell ref="B228:B229"/>
-    <mergeCell ref="B230:B231"/>
-    <mergeCell ref="B232:B233"/>
+    <mergeCell ref="F111:N111"/>
+    <mergeCell ref="C228:E228"/>
+    <mergeCell ref="C229:E229"/>
+    <mergeCell ref="C230:E230"/>
+    <mergeCell ref="C231:E231"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -10467,16 +10500,16 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="E26" sqref="E26"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="D24" sqref="D24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="D24" sqref="D24"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
i458--estimate memory register method update
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_example/standard_suite/diamond_regression.xlsx
+++ b/tmp_client/doc/TMP_example/standard_suite/diamond_regression.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\repository\tmp_client\doc\TMP_example\standard_suite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FC01F6-3918-48E4-867D-58CEAA386DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C0BECB-D67B-4DF3-83EC-59595CBC39A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,15 +26,15 @@
   </definedNames>
   <calcPr calcId="144525"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="2391" yWindow="-9" windowWidth="2418" windowHeight="1318" activeSheetId="3" showComments="commIndAndComment"/>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
     <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
-    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="2391" yWindow="-9" windowWidth="2418" windowHeight="1318" activeSheetId="3" showComments="commIndAndComment"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="419">
   <si>
     <t>[suite_info]</t>
   </si>
@@ -1253,15 +1253,6 @@
     <t>System dynamic status(CPU, MEM, space) attribute update</t>
   </si>
   <si>
-    <t>1~16</t>
-  </si>
-  <si>
-    <t>1(G, default)</t>
-  </si>
-  <si>
-    <t>estimated memory usage for task case run</t>
-  </si>
-  <si>
     <t>estimated memory usage info added for a test suite/case</t>
   </si>
   <si>
@@ -1320,6 +1311,18 @@
   </si>
   <si>
     <t>estimated space usage support</t>
+  </si>
+  <si>
+    <t>2(G, default)</t>
+  </si>
+  <si>
+    <t>1~32</t>
+  </si>
+  <si>
+    <t>1~16(G, dynamic)</t>
+  </si>
+  <si>
+    <t>estimated memory usage for task case run, dynamic based on current system available memoroy</t>
   </si>
 </sst>
 </file>
@@ -2229,6 +2232,15 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="5" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="39" xfId="5" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="5" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="33" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2241,118 +2253,109 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="5" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="5" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="39" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -5364,7 +5367,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -5449,8 +5454,8 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="B4" sqref="B4"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="B41" sqref="B41"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -5459,8 +5464,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="B41" sqref="B41"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="B4" sqref="B4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -5513,42 +5518,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" s="51" customFormat="1">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
-      <c r="K1" s="85"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="85"/>
-      <c r="N1" s="85"/>
-      <c r="O1" s="85"/>
-      <c r="P1" s="85"/>
-      <c r="Q1" s="85"/>
-      <c r="R1" s="85"/>
-      <c r="S1" s="85"/>
-      <c r="T1" s="85"/>
-      <c r="U1" s="85"/>
-      <c r="V1" s="85"/>
-      <c r="W1" s="85"/>
-      <c r="X1" s="86"/>
-      <c r="Y1" s="87" t="s">
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="88"/>
+      <c r="J1" s="88"/>
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
+      <c r="M1" s="88"/>
+      <c r="N1" s="88"/>
+      <c r="O1" s="88"/>
+      <c r="P1" s="88"/>
+      <c r="Q1" s="88"/>
+      <c r="R1" s="88"/>
+      <c r="S1" s="88"/>
+      <c r="T1" s="88"/>
+      <c r="U1" s="88"/>
+      <c r="V1" s="88"/>
+      <c r="W1" s="88"/>
+      <c r="X1" s="89"/>
+      <c r="Y1" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="Z1" s="87"/>
-      <c r="AA1" s="87"/>
-      <c r="AB1" s="87"/>
-      <c r="AC1" s="87"/>
-      <c r="AD1" s="87"/>
-      <c r="AE1" s="87"/>
-      <c r="AF1" s="87"/>
+      <c r="Z1" s="90"/>
+      <c r="AA1" s="90"/>
+      <c r="AB1" s="90"/>
+      <c r="AC1" s="90"/>
+      <c r="AD1" s="90"/>
+      <c r="AE1" s="90"/>
+      <c r="AF1" s="90"/>
     </row>
     <row r="2" spans="1:32" s="51" customFormat="1">
       <c r="A2" s="54" t="s">
@@ -7069,26 +7074,26 @@
   <sheetProtection algorithmName="SHA-512" hashValue="Sju3pjEnjegba3BrZLImZ+xscQ9MLEq+i8mDO7rXFn4S3yXv8zWb4HaF0uC2YruSs8wkV8FCIxY7a0fvnwVXFw==" saltValue="mZmUchosJ60PlKqUXOSzGQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A2:AF46" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <customSheetViews>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen"/>
-      <selection activeCell="H23" sqref="H23"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="85" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
-      <autoFilter ref="A2:Y2" xr:uid="{E30A4C14-A46D-4576-8328-F5D5A6C1B662}"/>
+      <autoFilter ref="A2:AF46" xr:uid="{2D77DE8A-ECF3-4CAD-B615-2BA955344E49}"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen"/>
       <selection activeCell="C23" sqref="C23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
-      <autoFilter ref="A2:Y2" xr:uid="{DE78499B-1EDA-4087-8EF4-BF963FF8942A}"/>
+      <autoFilter ref="A2:Y2" xr:uid="{DE42DF3A-9453-4457-969D-933CA4754FD7}"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="85" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen"/>
+      <selection activeCell="H23" sqref="H23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
-      <autoFilter ref="A2:AF46" xr:uid="{5E0980F9-12E2-4913-80E8-2BD79DEA48D4}"/>
+      <autoFilter ref="A2:Y2" xr:uid="{30755886-FF43-4FA4-80FA-C88BF216D825}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -7173,8 +7178,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:N283"/>
   <sheetViews>
-    <sheetView topLeftCell="A260" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C277" sqref="C277"/>
+    <sheetView topLeftCell="A141" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F161" sqref="F161:H161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -7235,17 +7240,17 @@
       <c r="E111" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="F111" s="119" t="s">
+      <c r="F111" s="91" t="s">
         <v>140</v>
       </c>
-      <c r="G111" s="120"/>
-      <c r="H111" s="120"/>
-      <c r="I111" s="120"/>
-      <c r="J111" s="120"/>
-      <c r="K111" s="120"/>
-      <c r="L111" s="120"/>
-      <c r="M111" s="120"/>
-      <c r="N111" s="121"/>
+      <c r="G111" s="92"/>
+      <c r="H111" s="92"/>
+      <c r="I111" s="92"/>
+      <c r="J111" s="92"/>
+      <c r="K111" s="92"/>
+      <c r="L111" s="92"/>
+      <c r="M111" s="92"/>
+      <c r="N111" s="93"/>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="6" t="s">
@@ -8165,7 +8170,7 @@
       <c r="A149" s="75">
         <v>1</v>
       </c>
-      <c r="B149" s="89" t="s">
+      <c r="B149" s="121" t="s">
         <v>4</v>
       </c>
       <c r="C149" s="76" t="s">
@@ -8191,7 +8196,7 @@
       <c r="A150" s="19">
         <v>2</v>
       </c>
-      <c r="B150" s="90"/>
+      <c r="B150" s="122"/>
       <c r="C150" s="21" t="s">
         <v>173</v>
       </c>
@@ -8213,7 +8218,7 @@
       <c r="A151" s="19">
         <v>3</v>
       </c>
-      <c r="B151" s="90"/>
+      <c r="B151" s="122"/>
       <c r="C151" s="21" t="s">
         <v>18</v>
       </c>
@@ -8233,7 +8238,7 @@
       <c r="A152" s="19">
         <v>4</v>
       </c>
-      <c r="B152" s="90"/>
+      <c r="B152" s="122"/>
       <c r="C152" s="21" t="s">
         <v>175</v>
       </c>
@@ -8257,7 +8262,7 @@
       <c r="A153" s="19">
         <v>5</v>
       </c>
-      <c r="B153" s="90"/>
+      <c r="B153" s="122"/>
       <c r="C153" s="56" t="s">
         <v>177</v>
       </c>
@@ -8281,7 +8286,7 @@
       <c r="A154" s="19">
         <v>6</v>
       </c>
-      <c r="B154" s="90"/>
+      <c r="B154" s="122"/>
       <c r="C154" s="56" t="s">
         <v>181</v>
       </c>
@@ -8305,7 +8310,7 @@
       <c r="A155" s="19">
         <v>7</v>
       </c>
-      <c r="B155" s="90"/>
+      <c r="B155" s="122"/>
       <c r="C155" s="21" t="s">
         <v>183</v>
       </c>
@@ -8327,7 +8332,7 @@
       <c r="A156" s="19">
         <v>8</v>
       </c>
-      <c r="B156" s="90"/>
+      <c r="B156" s="122"/>
       <c r="C156" s="56" t="s">
         <v>184</v>
       </c>
@@ -8351,7 +8356,7 @@
       <c r="A157" s="19">
         <v>9</v>
       </c>
-      <c r="B157" s="90"/>
+      <c r="B157" s="122"/>
       <c r="C157" s="56" t="s">
         <v>185</v>
       </c>
@@ -8375,7 +8380,7 @@
       <c r="A158" s="19">
         <v>10</v>
       </c>
-      <c r="B158" s="90"/>
+      <c r="B158" s="122"/>
       <c r="C158" s="21" t="s">
         <v>186</v>
       </c>
@@ -8399,7 +8404,7 @@
       <c r="A159" s="19">
         <v>11</v>
       </c>
-      <c r="B159" s="90"/>
+      <c r="B159" s="122"/>
       <c r="C159" s="21" t="s">
         <v>187</v>
       </c>
@@ -8423,7 +8428,7 @@
       <c r="A160" s="19">
         <v>12</v>
       </c>
-      <c r="B160" s="90"/>
+      <c r="B160" s="122"/>
       <c r="C160" s="21" t="s">
         <v>189</v>
       </c>
@@ -8445,51 +8450,51 @@
       <c r="A161" s="19">
         <v>13</v>
       </c>
-      <c r="B161" s="90"/>
+      <c r="B161" s="122"/>
       <c r="C161" s="56" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="D161" s="21" t="s">
         <v>169</v>
       </c>
       <c r="E161" s="21"/>
       <c r="F161" s="56" t="s">
-        <v>396</v>
+        <v>417</v>
       </c>
       <c r="G161" s="56" t="s">
-        <v>395</v>
+        <v>416</v>
       </c>
       <c r="H161" s="59" t="s">
-        <v>397</v>
+        <v>418</v>
       </c>
     </row>
     <row r="162" spans="1:9">
       <c r="A162" s="19">
         <v>14</v>
       </c>
-      <c r="B162" s="90"/>
+      <c r="B162" s="122"/>
       <c r="C162" s="56" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D162" s="21" t="s">
         <v>169</v>
       </c>
       <c r="E162" s="21"/>
       <c r="F162" s="56" t="s">
-        <v>396</v>
+        <v>415</v>
       </c>
       <c r="G162" s="56" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="H162" s="59" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="163" spans="1:9">
       <c r="A163" s="19">
         <v>15</v>
       </c>
-      <c r="B163" s="96"/>
+      <c r="B163" s="114"/>
       <c r="C163" s="21" t="s">
         <v>193</v>
       </c>
@@ -8513,7 +8518,7 @@
       <c r="A164" s="19">
         <v>16</v>
       </c>
-      <c r="B164" s="99" t="s">
+      <c r="B164" s="103" t="s">
         <v>5</v>
       </c>
       <c r="C164" s="21" t="s">
@@ -8540,7 +8545,7 @@
       <c r="A165" s="19">
         <v>17</v>
       </c>
-      <c r="B165" s="99"/>
+      <c r="B165" s="103"/>
       <c r="C165" s="56" t="s">
         <v>340</v>
       </c>
@@ -8564,7 +8569,7 @@
       <c r="A166" s="19">
         <v>18</v>
       </c>
-      <c r="B166" s="99"/>
+      <c r="B166" s="103"/>
       <c r="C166" s="56" t="s">
         <v>343</v>
       </c>
@@ -8588,7 +8593,7 @@
       <c r="A167" s="19">
         <v>19</v>
       </c>
-      <c r="B167" s="99"/>
+      <c r="B167" s="103"/>
       <c r="C167" s="68" t="s">
         <v>376</v>
       </c>
@@ -8612,7 +8617,7 @@
       <c r="A168" s="19">
         <v>20</v>
       </c>
-      <c r="B168" s="99"/>
+      <c r="B168" s="103"/>
       <c r="C168" s="68" t="s">
         <v>377</v>
       </c>
@@ -8634,7 +8639,7 @@
       <c r="A169" s="19">
         <v>21</v>
       </c>
-      <c r="B169" s="99"/>
+      <c r="B169" s="103"/>
       <c r="C169" s="68" t="s">
         <v>378</v>
       </c>
@@ -8656,9 +8661,9 @@
       <c r="A170" s="19">
         <v>22</v>
       </c>
-      <c r="B170" s="99"/>
+      <c r="B170" s="103"/>
       <c r="C170" s="79" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D170" s="21" t="s">
         <v>169</v>
@@ -8670,17 +8675,17 @@
         <v>1</v>
       </c>
       <c r="G170" s="79" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="H170" s="59" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="171" spans="1:9">
       <c r="A171" s="19">
         <v>23</v>
       </c>
-      <c r="B171" s="99"/>
+      <c r="B171" s="103"/>
       <c r="C171" s="77" t="s">
         <v>200</v>
       </c>
@@ -8702,7 +8707,7 @@
       <c r="A172" s="19">
         <v>24</v>
       </c>
-      <c r="B172" s="98"/>
+      <c r="B172" s="104"/>
       <c r="C172" s="56" t="s">
         <v>204</v>
       </c>
@@ -8713,13 +8718,13 @@
         <v>169</v>
       </c>
       <c r="F172" s="60" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="G172" s="56" t="s">
         <v>205</v>
       </c>
       <c r="H172" s="78" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="I172" s="64"/>
     </row>
@@ -8727,7 +8732,7 @@
       <c r="A173" s="19">
         <v>25</v>
       </c>
-      <c r="B173" s="88" t="s">
+      <c r="B173" s="123" t="s">
         <v>6</v>
       </c>
       <c r="C173" s="56" t="s">
@@ -8754,7 +8759,7 @@
       <c r="A174" s="19">
         <v>26</v>
       </c>
-      <c r="B174" s="89"/>
+      <c r="B174" s="121"/>
       <c r="C174" s="68" t="s">
         <v>346</v>
       </c>
@@ -8778,7 +8783,7 @@
       <c r="A175" s="19">
         <v>27</v>
       </c>
-      <c r="B175" s="89"/>
+      <c r="B175" s="121"/>
       <c r="C175" s="68" t="s">
         <v>347</v>
       </c>
@@ -8802,7 +8807,7 @@
       <c r="A176" s="19">
         <v>28</v>
       </c>
-      <c r="B176" s="89"/>
+      <c r="B176" s="121"/>
       <c r="C176" s="68" t="s">
         <v>381</v>
       </c>
@@ -8824,7 +8829,7 @@
       <c r="A177" s="19">
         <v>29</v>
       </c>
-      <c r="B177" s="89"/>
+      <c r="B177" s="121"/>
       <c r="C177" s="68" t="s">
         <v>368</v>
       </c>
@@ -8846,7 +8851,7 @@
       <c r="A178" s="19">
         <v>30</v>
       </c>
-      <c r="B178" s="89"/>
+      <c r="B178" s="121"/>
       <c r="C178" s="56" t="s">
         <v>365</v>
       </c>
@@ -8868,7 +8873,7 @@
       <c r="A179" s="19">
         <v>31</v>
       </c>
-      <c r="B179" s="89"/>
+      <c r="B179" s="121"/>
       <c r="C179" s="70" t="s">
         <v>375</v>
       </c>
@@ -8892,7 +8897,7 @@
       <c r="A180" s="19">
         <v>32</v>
       </c>
-      <c r="B180" s="89"/>
+      <c r="B180" s="121"/>
       <c r="C180" s="56" t="s">
         <v>363</v>
       </c>
@@ -8914,7 +8919,7 @@
       <c r="A181" s="19">
         <v>33</v>
       </c>
-      <c r="B181" s="89"/>
+      <c r="B181" s="121"/>
       <c r="C181" s="68" t="s">
         <v>371</v>
       </c>
@@ -8938,7 +8943,7 @@
       <c r="A182" s="19">
         <v>34</v>
       </c>
-      <c r="B182" s="89"/>
+      <c r="B182" s="121"/>
       <c r="C182" s="56" t="s">
         <v>303</v>
       </c>
@@ -8960,7 +8965,7 @@
       <c r="A183" s="19">
         <v>35</v>
       </c>
-      <c r="B183" s="96"/>
+      <c r="B183" s="114"/>
       <c r="C183" s="56" t="s">
         <v>204</v>
       </c>
@@ -8975,14 +8980,14 @@
         <v>205</v>
       </c>
       <c r="H183" s="67" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="184" spans="1:8">
       <c r="A184" s="19">
         <v>36</v>
       </c>
-      <c r="B184" s="99" t="s">
+      <c r="B184" s="103" t="s">
         <v>8</v>
       </c>
       <c r="C184" s="21" t="s">
@@ -9008,7 +9013,7 @@
       <c r="A185" s="19">
         <v>37</v>
       </c>
-      <c r="B185" s="98"/>
+      <c r="B185" s="104"/>
       <c r="C185" s="56" t="s">
         <v>353</v>
       </c>
@@ -9032,7 +9037,7 @@
       <c r="A186" s="19">
         <v>38</v>
       </c>
-      <c r="B186" s="98"/>
+      <c r="B186" s="104"/>
       <c r="C186" s="56" t="s">
         <v>209</v>
       </c>
@@ -9052,7 +9057,7 @@
       <c r="A187" s="19">
         <v>39</v>
       </c>
-      <c r="B187" s="98"/>
+      <c r="B187" s="104"/>
       <c r="C187" s="21" t="s">
         <v>210</v>
       </c>
@@ -9076,7 +9081,7 @@
       <c r="A188" s="19">
         <v>40</v>
       </c>
-      <c r="B188" s="98"/>
+      <c r="B188" s="104"/>
       <c r="C188" s="21" t="s">
         <v>211</v>
       </c>
@@ -9098,7 +9103,7 @@
       <c r="A189" s="19">
         <v>41</v>
       </c>
-      <c r="B189" s="98"/>
+      <c r="B189" s="104"/>
       <c r="C189" s="21" t="s">
         <v>212</v>
       </c>
@@ -9118,7 +9123,7 @@
       <c r="A190" s="19">
         <v>42</v>
       </c>
-      <c r="B190" s="98"/>
+      <c r="B190" s="104"/>
       <c r="C190" s="21" t="s">
         <v>213</v>
       </c>
@@ -9138,7 +9143,7 @@
       <c r="A191" s="19">
         <v>43</v>
       </c>
-      <c r="B191" s="98"/>
+      <c r="B191" s="104"/>
       <c r="C191" s="21" t="s">
         <v>47</v>
       </c>
@@ -9158,7 +9163,7 @@
       <c r="A192" s="19">
         <v>44</v>
       </c>
-      <c r="B192" s="99" t="s">
+      <c r="B192" s="103" t="s">
         <v>9</v>
       </c>
       <c r="C192" s="21" t="s">
@@ -9182,7 +9187,7 @@
       <c r="A193" s="19">
         <v>45</v>
       </c>
-      <c r="B193" s="98"/>
+      <c r="B193" s="104"/>
       <c r="C193" s="56" t="s">
         <v>215</v>
       </c>
@@ -9204,7 +9209,7 @@
       <c r="A194" s="19">
         <v>46</v>
       </c>
-      <c r="B194" s="98"/>
+      <c r="B194" s="104"/>
       <c r="C194" s="56" t="s">
         <v>331</v>
       </c>
@@ -9226,7 +9231,7 @@
       <c r="A195" s="19">
         <v>47</v>
       </c>
-      <c r="B195" s="98"/>
+      <c r="B195" s="104"/>
       <c r="C195" s="56" t="s">
         <v>218</v>
       </c>
@@ -9248,7 +9253,7 @@
       <c r="A196" s="19">
         <v>48</v>
       </c>
-      <c r="B196" s="98"/>
+      <c r="B196" s="104"/>
       <c r="C196" s="56" t="s">
         <v>329</v>
       </c>
@@ -9270,7 +9275,7 @@
       <c r="A197" s="19">
         <v>49</v>
       </c>
-      <c r="B197" s="98"/>
+      <c r="B197" s="104"/>
       <c r="C197" s="56" t="s">
         <v>330</v>
       </c>
@@ -9292,7 +9297,7 @@
       <c r="A198" s="19">
         <v>50</v>
       </c>
-      <c r="B198" s="98"/>
+      <c r="B198" s="104"/>
       <c r="C198" s="56" t="s">
         <v>386</v>
       </c>
@@ -9314,7 +9319,7 @@
       <c r="A199" s="19">
         <v>51</v>
       </c>
-      <c r="B199" s="98"/>
+      <c r="B199" s="104"/>
       <c r="C199" s="56" t="s">
         <v>387</v>
       </c>
@@ -9336,7 +9341,7 @@
       <c r="A200" s="19">
         <v>52</v>
       </c>
-      <c r="B200" s="98"/>
+      <c r="B200" s="104"/>
       <c r="C200" s="56" t="s">
         <v>388</v>
       </c>
@@ -9358,7 +9363,7 @@
       <c r="A201" s="19">
         <v>53</v>
       </c>
-      <c r="B201" s="88" t="s">
+      <c r="B201" s="123" t="s">
         <v>10</v>
       </c>
       <c r="C201" s="21" t="s">
@@ -9384,7 +9389,7 @@
       <c r="A202" s="19">
         <v>54</v>
       </c>
-      <c r="B202" s="89"/>
+      <c r="B202" s="121"/>
       <c r="C202" s="20" t="s">
         <v>222</v>
       </c>
@@ -9408,7 +9413,7 @@
       <c r="A203" s="19">
         <v>55</v>
       </c>
-      <c r="B203" s="90"/>
+      <c r="B203" s="122"/>
       <c r="C203" s="58" t="s">
         <v>334</v>
       </c>
@@ -9432,7 +9437,7 @@
       <c r="A204" s="16">
         <v>56</v>
       </c>
-      <c r="B204" s="91" t="s">
+      <c r="B204" s="124" t="s">
         <v>156</v>
       </c>
       <c r="C204" s="57" t="s">
@@ -9456,9 +9461,9 @@
       <c r="A205" s="75">
         <v>57</v>
       </c>
-      <c r="B205" s="92"/>
+      <c r="B205" s="125"/>
       <c r="C205" s="76" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="D205" s="74" t="s">
         <v>169</v>
@@ -9468,17 +9473,17 @@
         <v>232</v>
       </c>
       <c r="G205" s="73" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="H205" s="36" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="206" spans="1:8">
       <c r="A206" s="75">
         <v>58</v>
       </c>
-      <c r="B206" s="93"/>
+      <c r="B206" s="126"/>
       <c r="C206" s="56" t="s">
         <v>227</v>
       </c>
@@ -9500,7 +9505,7 @@
       <c r="A207" s="75">
         <v>59</v>
       </c>
-      <c r="B207" s="94"/>
+      <c r="B207" s="127"/>
       <c r="C207" s="58" t="s">
         <v>230</v>
       </c>
@@ -9522,7 +9527,7 @@
       <c r="A208" s="75">
         <v>60</v>
       </c>
-      <c r="B208" s="94"/>
+      <c r="B208" s="127"/>
       <c r="C208" s="58" t="s">
         <v>231</v>
       </c>
@@ -9544,7 +9549,7 @@
       <c r="A209" s="75">
         <v>61</v>
       </c>
-      <c r="B209" s="94"/>
+      <c r="B209" s="127"/>
       <c r="C209" s="58" t="s">
         <v>234</v>
       </c>
@@ -9564,7 +9569,7 @@
       <c r="A210" s="75">
         <v>62</v>
       </c>
-      <c r="B210" s="94"/>
+      <c r="B210" s="127"/>
       <c r="C210" s="58" t="s">
         <v>309</v>
       </c>
@@ -9586,7 +9591,7 @@
       <c r="A211" s="75">
         <v>63</v>
       </c>
-      <c r="B211" s="94"/>
+      <c r="B211" s="127"/>
       <c r="C211" s="58" t="s">
         <v>313</v>
       </c>
@@ -9608,9 +9613,9 @@
       <c r="A212" s="23">
         <v>64</v>
       </c>
-      <c r="B212" s="95"/>
+      <c r="B212" s="108"/>
       <c r="C212" s="24" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D212" s="24" t="s">
         <v>169</v>
@@ -9664,7 +9669,7 @@
         <v>238</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="229" spans="1:7" ht="15.75" thickBot="1">
@@ -9674,11 +9679,11 @@
       <c r="B229" s="32" t="s">
         <v>240</v>
       </c>
-      <c r="C229" s="122" t="s">
+      <c r="C229" s="94" t="s">
         <v>241</v>
       </c>
-      <c r="D229" s="122"/>
-      <c r="E229" s="122"/>
+      <c r="D229" s="94"/>
+      <c r="E229" s="94"/>
       <c r="F229" s="32" t="s">
         <v>242</v>
       </c>
@@ -9687,17 +9692,17 @@
       </c>
     </row>
     <row r="230" spans="1:7">
-      <c r="A230" s="103" t="s">
+      <c r="A230" s="118" t="s">
         <v>244</v>
       </c>
-      <c r="B230" s="96" t="s">
+      <c r="B230" s="114" t="s">
         <v>245</v>
       </c>
-      <c r="C230" s="123" t="s">
+      <c r="C230" s="95" t="s">
         <v>246</v>
       </c>
-      <c r="D230" s="124"/>
-      <c r="E230" s="124"/>
+      <c r="D230" s="96"/>
+      <c r="E230" s="96"/>
       <c r="F230" s="74" t="s">
         <v>247</v>
       </c>
@@ -9706,13 +9711,13 @@
       </c>
     </row>
     <row r="231" spans="1:7">
-      <c r="A231" s="104"/>
-      <c r="B231" s="97"/>
-      <c r="C231" s="114" t="s">
+      <c r="A231" s="119"/>
+      <c r="B231" s="128"/>
+      <c r="C231" s="97" t="s">
         <v>246</v>
       </c>
-      <c r="D231" s="125"/>
-      <c r="E231" s="125"/>
+      <c r="D231" s="98"/>
+      <c r="E231" s="98"/>
       <c r="F231" s="20" t="s">
         <v>249</v>
       </c>
@@ -9721,15 +9726,15 @@
       </c>
     </row>
     <row r="232" spans="1:7">
-      <c r="A232" s="104"/>
-      <c r="B232" s="98" t="s">
+      <c r="A232" s="119"/>
+      <c r="B232" s="104" t="s">
         <v>250</v>
       </c>
-      <c r="C232" s="118" t="s">
+      <c r="C232" s="99" t="s">
         <v>251</v>
       </c>
-      <c r="D232" s="118"/>
-      <c r="E232" s="118"/>
+      <c r="D232" s="99"/>
+      <c r="E232" s="99"/>
       <c r="F232" s="21" t="s">
         <v>247</v>
       </c>
@@ -9738,13 +9743,13 @@
       </c>
     </row>
     <row r="233" spans="1:7">
-      <c r="A233" s="104"/>
-      <c r="B233" s="98"/>
-      <c r="C233" s="114" t="s">
+      <c r="A233" s="119"/>
+      <c r="B233" s="104"/>
+      <c r="C233" s="97" t="s">
         <v>251</v>
       </c>
-      <c r="D233" s="114"/>
-      <c r="E233" s="114"/>
+      <c r="D233" s="97"/>
+      <c r="E233" s="97"/>
       <c r="F233" s="21" t="s">
         <v>249</v>
       </c>
@@ -9753,15 +9758,15 @@
       </c>
     </row>
     <row r="234" spans="1:7">
-      <c r="A234" s="104"/>
-      <c r="B234" s="97" t="s">
+      <c r="A234" s="119"/>
+      <c r="B234" s="128" t="s">
         <v>252</v>
       </c>
-      <c r="C234" s="115" t="s">
+      <c r="C234" s="100" t="s">
         <v>246</v>
       </c>
-      <c r="D234" s="116"/>
-      <c r="E234" s="117"/>
+      <c r="D234" s="101"/>
+      <c r="E234" s="102"/>
       <c r="F234" s="21" t="s">
         <v>247</v>
       </c>
@@ -9770,13 +9775,13 @@
       </c>
     </row>
     <row r="235" spans="1:7">
-      <c r="A235" s="104"/>
-      <c r="B235" s="96"/>
-      <c r="C235" s="115" t="s">
+      <c r="A235" s="119"/>
+      <c r="B235" s="114"/>
+      <c r="C235" s="100" t="s">
         <v>246</v>
       </c>
-      <c r="D235" s="116"/>
-      <c r="E235" s="117"/>
+      <c r="D235" s="101"/>
+      <c r="E235" s="102"/>
       <c r="F235" s="21" t="s">
         <v>249</v>
       </c>
@@ -9785,15 +9790,15 @@
       </c>
     </row>
     <row r="236" spans="1:7">
-      <c r="A236" s="104"/>
-      <c r="B236" s="98" t="s">
+      <c r="A236" s="119"/>
+      <c r="B236" s="104" t="s">
         <v>253</v>
       </c>
-      <c r="C236" s="118" t="s">
+      <c r="C236" s="99" t="s">
         <v>254</v>
       </c>
-      <c r="D236" s="118"/>
-      <c r="E236" s="118"/>
+      <c r="D236" s="99"/>
+      <c r="E236" s="99"/>
       <c r="F236" s="21" t="s">
         <v>247</v>
       </c>
@@ -9802,13 +9807,13 @@
       </c>
     </row>
     <row r="237" spans="1:7">
-      <c r="A237" s="104"/>
-      <c r="B237" s="98"/>
-      <c r="C237" s="118" t="s">
+      <c r="A237" s="119"/>
+      <c r="B237" s="104"/>
+      <c r="C237" s="99" t="s">
         <v>254</v>
       </c>
-      <c r="D237" s="118"/>
-      <c r="E237" s="118"/>
+      <c r="D237" s="99"/>
+      <c r="E237" s="99"/>
       <c r="F237" s="21" t="s">
         <v>249</v>
       </c>
@@ -9817,17 +9822,17 @@
       </c>
     </row>
     <row r="238" spans="1:7">
-      <c r="A238" s="104" t="s">
+      <c r="A238" s="119" t="s">
         <v>255</v>
       </c>
-      <c r="B238" s="98" t="s">
+      <c r="B238" s="104" t="s">
         <v>256</v>
       </c>
-      <c r="C238" s="99" t="s">
+      <c r="C238" s="103" t="s">
         <v>257</v>
       </c>
-      <c r="D238" s="98"/>
-      <c r="E238" s="98"/>
+      <c r="D238" s="104"/>
+      <c r="E238" s="104"/>
       <c r="F238" s="21" t="s">
         <v>247</v>
       </c>
@@ -9836,13 +9841,13 @@
       </c>
     </row>
     <row r="239" spans="1:7">
-      <c r="A239" s="104"/>
-      <c r="B239" s="98"/>
-      <c r="C239" s="98" t="s">
+      <c r="A239" s="119"/>
+      <c r="B239" s="104"/>
+      <c r="C239" s="104" t="s">
         <v>258</v>
       </c>
-      <c r="D239" s="98"/>
-      <c r="E239" s="98"/>
+      <c r="D239" s="104"/>
+      <c r="E239" s="104"/>
       <c r="F239" s="21" t="s">
         <v>249</v>
       </c>
@@ -9851,15 +9856,15 @@
       </c>
     </row>
     <row r="240" spans="1:7">
-      <c r="A240" s="104"/>
-      <c r="B240" s="98" t="s">
+      <c r="A240" s="119"/>
+      <c r="B240" s="104" t="s">
         <v>260</v>
       </c>
-      <c r="C240" s="98" t="s">
+      <c r="C240" s="104" t="s">
         <v>261</v>
       </c>
-      <c r="D240" s="98"/>
-      <c r="E240" s="98"/>
+      <c r="D240" s="104"/>
+      <c r="E240" s="104"/>
       <c r="F240" s="21" t="s">
         <v>247</v>
       </c>
@@ -9868,13 +9873,13 @@
       </c>
     </row>
     <row r="241" spans="1:7">
-      <c r="A241" s="104"/>
-      <c r="B241" s="98"/>
-      <c r="C241" s="98" t="s">
+      <c r="A241" s="119"/>
+      <c r="B241" s="104"/>
+      <c r="C241" s="104" t="s">
         <v>262</v>
       </c>
-      <c r="D241" s="98"/>
-      <c r="E241" s="98"/>
+      <c r="D241" s="104"/>
+      <c r="E241" s="104"/>
       <c r="F241" s="21" t="s">
         <v>249</v>
       </c>
@@ -9883,17 +9888,17 @@
       </c>
     </row>
     <row r="242" spans="1:7">
-      <c r="A242" s="104" t="s">
+      <c r="A242" s="119" t="s">
         <v>263</v>
       </c>
-      <c r="B242" s="98" t="s">
+      <c r="B242" s="104" t="s">
         <v>264</v>
       </c>
-      <c r="C242" s="99" t="s">
+      <c r="C242" s="103" t="s">
         <v>265</v>
       </c>
-      <c r="D242" s="98"/>
-      <c r="E242" s="98"/>
+      <c r="D242" s="104"/>
+      <c r="E242" s="104"/>
       <c r="F242" s="21" t="s">
         <v>247</v>
       </c>
@@ -9902,13 +9907,13 @@
       </c>
     </row>
     <row r="243" spans="1:7">
-      <c r="A243" s="104"/>
-      <c r="B243" s="98"/>
-      <c r="C243" s="98" t="s">
+      <c r="A243" s="119"/>
+      <c r="B243" s="104"/>
+      <c r="C243" s="104" t="s">
         <v>266</v>
       </c>
-      <c r="D243" s="98"/>
-      <c r="E243" s="98"/>
+      <c r="D243" s="104"/>
+      <c r="E243" s="104"/>
       <c r="F243" s="21" t="s">
         <v>249</v>
       </c>
@@ -9917,15 +9922,15 @@
       </c>
     </row>
     <row r="244" spans="1:7">
-      <c r="A244" s="104"/>
-      <c r="B244" s="98" t="s">
+      <c r="A244" s="119"/>
+      <c r="B244" s="104" t="s">
         <v>267</v>
       </c>
-      <c r="C244" s="99" t="s">
+      <c r="C244" s="103" t="s">
         <v>268</v>
       </c>
-      <c r="D244" s="98"/>
-      <c r="E244" s="98"/>
+      <c r="D244" s="104"/>
+      <c r="E244" s="104"/>
       <c r="F244" s="21" t="s">
         <v>247</v>
       </c>
@@ -9934,13 +9939,13 @@
       </c>
     </row>
     <row r="245" spans="1:7">
-      <c r="A245" s="105"/>
-      <c r="B245" s="106"/>
-      <c r="C245" s="106" t="s">
+      <c r="A245" s="120"/>
+      <c r="B245" s="109"/>
+      <c r="C245" s="109" t="s">
         <v>269</v>
       </c>
-      <c r="D245" s="106"/>
-      <c r="E245" s="106"/>
+      <c r="D245" s="109"/>
+      <c r="E245" s="109"/>
       <c r="F245" s="24" t="s">
         <v>249</v>
       </c>
@@ -9982,9 +9987,9 @@
       <c r="B251" s="113" t="s">
         <v>277</v>
       </c>
-      <c r="C251" s="96"/>
-      <c r="D251" s="96"/>
-      <c r="E251" s="96"/>
+      <c r="C251" s="114"/>
+      <c r="D251" s="114"/>
+      <c r="E251" s="114"/>
       <c r="F251" s="35" t="s">
         <v>154</v>
       </c>
@@ -9996,12 +10001,12 @@
       <c r="A252" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="B252" s="108" t="s">
+      <c r="B252" s="105" t="s">
         <v>279</v>
       </c>
-      <c r="C252" s="109"/>
-      <c r="D252" s="109"/>
-      <c r="E252" s="110"/>
+      <c r="C252" s="106"/>
+      <c r="D252" s="106"/>
+      <c r="E252" s="107"/>
       <c r="F252" s="9" t="s">
         <v>248</v>
       </c>
@@ -10013,12 +10018,12 @@
       <c r="A253" s="12" t="s">
         <v>280</v>
       </c>
-      <c r="B253" s="108" t="s">
+      <c r="B253" s="105" t="s">
         <v>281</v>
       </c>
-      <c r="C253" s="109"/>
-      <c r="D253" s="109"/>
-      <c r="E253" s="110"/>
+      <c r="C253" s="106"/>
+      <c r="D253" s="106"/>
+      <c r="E253" s="107"/>
       <c r="F253" s="13" t="s">
         <v>248</v>
       </c>
@@ -10030,12 +10035,12 @@
       <c r="A254" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="B254" s="95" t="s">
+      <c r="B254" s="108" t="s">
         <v>283</v>
       </c>
-      <c r="C254" s="106"/>
-      <c r="D254" s="106"/>
-      <c r="E254" s="106"/>
+      <c r="C254" s="109"/>
+      <c r="D254" s="109"/>
+      <c r="E254" s="109"/>
       <c r="F254" s="15" t="s">
         <v>248</v>
       </c>
@@ -10080,11 +10085,11 @@
       <c r="C259" s="17" t="s">
         <v>288</v>
       </c>
-      <c r="D259" s="111" t="s">
+      <c r="D259" s="110" t="s">
         <v>289</v>
       </c>
-      <c r="E259" s="111"/>
-      <c r="F259" s="111"/>
+      <c r="E259" s="110"/>
+      <c r="F259" s="110"/>
       <c r="G259" s="18"/>
     </row>
     <row r="260" spans="1:7">
@@ -10097,11 +10102,11 @@
       <c r="C260" s="21" t="s">
         <v>288</v>
       </c>
-      <c r="D260" s="107" t="s">
+      <c r="D260" s="111" t="s">
         <v>290</v>
       </c>
-      <c r="E260" s="107"/>
-      <c r="F260" s="107"/>
+      <c r="E260" s="111"/>
+      <c r="F260" s="111"/>
       <c r="G260" s="28"/>
     </row>
     <row r="261" spans="1:7">
@@ -10114,11 +10119,11 @@
       <c r="C261" s="21" t="s">
         <v>288</v>
       </c>
-      <c r="D261" s="107" t="s">
+      <c r="D261" s="111" t="s">
         <v>291</v>
       </c>
-      <c r="E261" s="107"/>
-      <c r="F261" s="107"/>
+      <c r="E261" s="111"/>
+      <c r="F261" s="111"/>
       <c r="G261" s="28"/>
     </row>
     <row r="262" spans="1:7">
@@ -10131,11 +10136,11 @@
       <c r="C262" s="21" t="s">
         <v>288</v>
       </c>
-      <c r="D262" s="107" t="s">
+      <c r="D262" s="111" t="s">
         <v>292</v>
       </c>
-      <c r="E262" s="107"/>
-      <c r="F262" s="107"/>
+      <c r="E262" s="111"/>
+      <c r="F262" s="111"/>
       <c r="G262" s="28"/>
     </row>
     <row r="263" spans="1:7">
@@ -10148,11 +10153,11 @@
       <c r="C263" s="21" t="s">
         <v>288</v>
       </c>
-      <c r="D263" s="107" t="s">
+      <c r="D263" s="111" t="s">
         <v>293</v>
       </c>
-      <c r="E263" s="107"/>
-      <c r="F263" s="107"/>
+      <c r="E263" s="111"/>
+      <c r="F263" s="111"/>
       <c r="G263" s="28"/>
     </row>
     <row r="264" spans="1:7">
@@ -10165,11 +10170,11 @@
       <c r="C264" s="21" t="s">
         <v>288</v>
       </c>
-      <c r="D264" s="107" t="s">
+      <c r="D264" s="111" t="s">
         <v>294</v>
       </c>
-      <c r="E264" s="107"/>
-      <c r="F264" s="107"/>
+      <c r="E264" s="111"/>
+      <c r="F264" s="111"/>
       <c r="G264" s="28"/>
     </row>
     <row r="265" spans="1:7">
@@ -10182,11 +10187,11 @@
       <c r="C265" s="20" t="s">
         <v>288</v>
       </c>
-      <c r="D265" s="100" t="s">
+      <c r="D265" s="115" t="s">
         <v>295</v>
       </c>
-      <c r="E265" s="101"/>
-      <c r="F265" s="102"/>
+      <c r="E265" s="116"/>
+      <c r="F265" s="117"/>
       <c r="G265" s="29"/>
     </row>
     <row r="266" spans="1:7">
@@ -10199,11 +10204,11 @@
       <c r="C266" s="20" t="s">
         <v>288</v>
       </c>
-      <c r="D266" s="100" t="s">
+      <c r="D266" s="115" t="s">
         <v>296</v>
       </c>
-      <c r="E266" s="101"/>
-      <c r="F266" s="102"/>
+      <c r="E266" s="116"/>
+      <c r="F266" s="117"/>
       <c r="G266" s="29"/>
     </row>
     <row r="267" spans="1:7">
@@ -10216,11 +10221,11 @@
       <c r="C267" s="20" t="s">
         <v>288</v>
       </c>
-      <c r="D267" s="100" t="s">
+      <c r="D267" s="115" t="s">
         <v>297</v>
       </c>
-      <c r="E267" s="101"/>
-      <c r="F267" s="102"/>
+      <c r="E267" s="116"/>
+      <c r="F267" s="117"/>
       <c r="G267" s="29"/>
     </row>
     <row r="268" spans="1:7">
@@ -10421,7 +10426,7 @@
         <v>288</v>
       </c>
       <c r="D279" s="46" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="E279" s="47"/>
       <c r="F279" s="48"/>
@@ -10438,7 +10443,7 @@
         <v>288</v>
       </c>
       <c r="D280" s="46" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="E280" s="47"/>
       <c r="F280" s="48"/>
@@ -10455,7 +10460,7 @@
         <v>288</v>
       </c>
       <c r="D281" s="46" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="E281" s="47"/>
       <c r="F281" s="48"/>
@@ -10472,7 +10477,7 @@
         <v>288</v>
       </c>
       <c r="D282" s="46" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="E282" s="47"/>
       <c r="F282" s="48"/>
@@ -10488,15 +10493,15 @@
       <c r="C283" s="24" t="s">
         <v>288</v>
       </c>
-      <c r="D283" s="126" t="s">
-        <v>417</v>
-      </c>
-      <c r="E283" s="127"/>
-      <c r="F283" s="128"/>
+      <c r="D283" s="84" t="s">
+        <v>414</v>
+      </c>
+      <c r="E283" s="85"/>
+      <c r="F283" s="86"/>
       <c r="G283" s="30"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="MU3YfW5kMaQw/S5LoiPWsjBdgUtBYGwjSAbDm5FkjYZ5eZAn78p0p5h+E7z/Lo441UI34edXKptC/ui5Db0odA==" saltValue="7FWOTUptA7IDZijSpC1TBA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="/HVI315p0oCUENVcikYWZVDK2qm22Ddvoh9ExcWjLbp81ydRCXqzzl9GvxwMXSQrkfo64Vjt+cWzFsR3r7r9/Q==" saltValue="oIynV72Uh6cBEcLBFZqbwQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <customSheetViews>
     <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115" topLeftCell="A139">
       <selection activeCell="D163" sqref="D163"/>
@@ -10505,31 +10510,16 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="50">
-    <mergeCell ref="F111:N111"/>
-    <mergeCell ref="C229:E229"/>
-    <mergeCell ref="C230:E230"/>
-    <mergeCell ref="C231:E231"/>
-    <mergeCell ref="C232:E232"/>
-    <mergeCell ref="C233:E233"/>
-    <mergeCell ref="C234:E234"/>
-    <mergeCell ref="C235:E235"/>
-    <mergeCell ref="C236:E236"/>
-    <mergeCell ref="C237:E237"/>
-    <mergeCell ref="C238:E238"/>
-    <mergeCell ref="C239:E239"/>
-    <mergeCell ref="C240:E240"/>
-    <mergeCell ref="C241:E241"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C243:E243"/>
-    <mergeCell ref="C244:E244"/>
-    <mergeCell ref="C245:E245"/>
-    <mergeCell ref="B250:E250"/>
-    <mergeCell ref="B251:E251"/>
-    <mergeCell ref="B252:E252"/>
-    <mergeCell ref="B253:E253"/>
-    <mergeCell ref="B254:E254"/>
-    <mergeCell ref="D259:F259"/>
-    <mergeCell ref="D260:F260"/>
+    <mergeCell ref="B201:B203"/>
+    <mergeCell ref="B204:B212"/>
+    <mergeCell ref="B230:B231"/>
+    <mergeCell ref="B232:B233"/>
+    <mergeCell ref="B234:B235"/>
+    <mergeCell ref="B149:B163"/>
+    <mergeCell ref="B164:B172"/>
+    <mergeCell ref="B173:B183"/>
+    <mergeCell ref="B184:B191"/>
+    <mergeCell ref="B192:B200"/>
     <mergeCell ref="D266:F266"/>
     <mergeCell ref="D267:F267"/>
     <mergeCell ref="A230:A237"/>
@@ -10545,16 +10535,31 @@
     <mergeCell ref="D263:F263"/>
     <mergeCell ref="D264:F264"/>
     <mergeCell ref="D265:F265"/>
-    <mergeCell ref="B149:B163"/>
-    <mergeCell ref="B164:B172"/>
-    <mergeCell ref="B173:B183"/>
-    <mergeCell ref="B184:B191"/>
-    <mergeCell ref="B192:B200"/>
-    <mergeCell ref="B201:B203"/>
-    <mergeCell ref="B204:B212"/>
-    <mergeCell ref="B230:B231"/>
-    <mergeCell ref="B232:B233"/>
-    <mergeCell ref="B234:B235"/>
+    <mergeCell ref="B252:E252"/>
+    <mergeCell ref="B253:E253"/>
+    <mergeCell ref="B254:E254"/>
+    <mergeCell ref="D259:F259"/>
+    <mergeCell ref="D260:F260"/>
+    <mergeCell ref="C243:E243"/>
+    <mergeCell ref="C244:E244"/>
+    <mergeCell ref="C245:E245"/>
+    <mergeCell ref="B250:E250"/>
+    <mergeCell ref="B251:E251"/>
+    <mergeCell ref="C238:E238"/>
+    <mergeCell ref="C239:E239"/>
+    <mergeCell ref="C240:E240"/>
+    <mergeCell ref="C241:E241"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C233:E233"/>
+    <mergeCell ref="C234:E234"/>
+    <mergeCell ref="C235:E235"/>
+    <mergeCell ref="C236:E236"/>
+    <mergeCell ref="C237:E237"/>
+    <mergeCell ref="F111:N111"/>
+    <mergeCell ref="C229:E229"/>
+    <mergeCell ref="C230:E230"/>
+    <mergeCell ref="C231:E231"/>
+    <mergeCell ref="C232:E232"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -10580,16 +10585,16 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="E26" sqref="E26"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="D24" sqref="D24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="D24" sqref="D24"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>